<commit_message>
Contest 2 DC vs MI and Contest 3 PBKS vs RCB
</commit_message>
<xml_diff>
--- a/2022/EBE Boys 2022.xlsx
+++ b/2022/EBE Boys 2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEFDB333-ABB1-3F46-905E-F5CBA85614A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3FDA240-6183-6941-9464-563005C62414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="520" windowWidth="35840" windowHeight="20420" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -1391,41 +1391,55 @@
       <c r="C13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="3" t="str">
+      <c r="D13" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E13, ($W13,$T13,$Q13,$N13,$K13,$H13,$E13), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E13, ($W13,$T13,$Q13,$N13,$K13,$H13,$E13), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="G13" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="E13" s="1">
+        <v>60</v>
+      </c>
+      <c r="G13" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H13, ($W13,$T13,$Q13,$N13,$K13,$H13,$E13), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H13, ($W13,$T13,$Q13,$N13,$K13,$H13,$E13), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H13" s="1"/>
-      <c r="J13" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="H13" s="1">
+        <v>100</v>
+      </c>
+      <c r="J13" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K13, ($W13,$T13,$Q13,$N13,$K13,$H13,$E13), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K13, ($W13,$T13,$Q13,$N13,$K13,$H13,$E13), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K13" s="1"/>
-      <c r="M13" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="K13" s="1">
+        <v>40</v>
+      </c>
+      <c r="M13" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N13, ($W13,$T13,$Q13,$N13,$K13,$H13,$E13), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N13, ($W13,$T13,$Q13,$N13,$K13,$H13,$E13), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N13" s="1"/>
-      <c r="P13" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="N13" s="1">
+        <v>0</v>
+      </c>
+      <c r="P13" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q13, ($W13,$T13,$Q13,$N13,$K13,$H13,$E13), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q13, ($W13,$T13,$Q13,$N13,$K13,$H13,$E13), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q13" s="1"/>
-      <c r="S13" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>70</v>
+      </c>
+      <c r="S13" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T13, ($W13,$T13,$Q13,$N13,$K13,$H13,$E13), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T13, ($W13,$T13,$Q13,$N13,$K13,$H13,$E13), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T13" s="1"/>
-      <c r="V13" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="T13" s="1">
+        <v>50</v>
+      </c>
+      <c r="V13" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W13, ($W13,$T13,$Q13,$N13,$K13,$H13,$E13), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W13, ($W13,$T13,$Q13,$N13,$K13,$H13,$E13), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W13" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="W13" s="1">
+        <v>80</v>
+      </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
@@ -1437,41 +1451,55 @@
       <c r="C14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="3" t="str">
+      <c r="D14" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E14, ($W14,$T14,$Q14,$N14,$K14,$H14,$E14), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E14, ($W14,$T14,$Q14,$N14,$K14,$H14,$E14), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="G14" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H14, ($W14,$T14,$Q14,$N14,$K14,$H14,$E14), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H14, ($W14,$T14,$Q14,$N14,$K14,$H14,$E14), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H14" s="1"/>
-      <c r="J14" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>70</v>
+      </c>
+      <c r="J14" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K14, ($W14,$T14,$Q14,$N14,$K14,$H14,$E14), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K14, ($W14,$T14,$Q14,$N14,$K14,$H14,$E14), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K14" s="1"/>
-      <c r="M14" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="K14" s="1">
+        <v>50</v>
+      </c>
+      <c r="M14" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N14, ($W14,$T14,$Q14,$N14,$K14,$H14,$E14), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N14, ($W14,$T14,$Q14,$N14,$K14,$H14,$E14), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N14" s="1"/>
-      <c r="P14" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="N14" s="1">
+        <v>80</v>
+      </c>
+      <c r="P14" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q14, ($W14,$T14,$Q14,$N14,$K14,$H14,$E14), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q14, ($W14,$T14,$Q14,$N14,$K14,$H14,$E14), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q14" s="1"/>
-      <c r="S14" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>40</v>
+      </c>
+      <c r="S14" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T14, ($W14,$T14,$Q14,$N14,$K14,$H14,$E14), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T14, ($W14,$T14,$Q14,$N14,$K14,$H14,$E14), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T14" s="1"/>
-      <c r="V14" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="T14" s="1">
+        <v>60</v>
+      </c>
+      <c r="V14" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W14, ($W14,$T14,$Q14,$N14,$K14,$H14,$E14), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W14, ($W14,$T14,$Q14,$N14,$K14,$H14,$E14), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W14" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="W14" s="1">
+        <v>100</v>
+      </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
@@ -1483,41 +1511,55 @@
       <c r="C15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="3" t="str">
+      <c r="D15" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E15, ($W15,$T15,$Q15,$N15,$K15,$H15,$E15), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E15, ($W15,$T15,$Q15,$N15,$K15,$H15,$E15), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E15" s="1"/>
-      <c r="G15" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="E15" s="1">
+        <v>60</v>
+      </c>
+      <c r="G15" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H15, ($W15,$T15,$Q15,$N15,$K15,$H15,$E15), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H15, ($W15,$T15,$Q15,$N15,$K15,$H15,$E15), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H15" s="1"/>
-      <c r="J15" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="H15" s="1">
+        <v>50</v>
+      </c>
+      <c r="J15" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K15, ($W15,$T15,$Q15,$N15,$K15,$H15,$E15), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K15, ($W15,$T15,$Q15,$N15,$K15,$H15,$E15), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K15" s="1"/>
-      <c r="M15" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="K15" s="1">
+        <v>40</v>
+      </c>
+      <c r="M15" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N15, ($W15,$T15,$Q15,$N15,$K15,$H15,$E15), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N15, ($W15,$T15,$Q15,$N15,$K15,$H15,$E15), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N15" s="1"/>
-      <c r="P15" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="N15" s="1">
+        <v>70</v>
+      </c>
+      <c r="P15" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q15, ($W15,$T15,$Q15,$N15,$K15,$H15,$E15), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q15, ($W15,$T15,$Q15,$N15,$K15,$H15,$E15), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q15" s="1"/>
-      <c r="S15" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>80</v>
+      </c>
+      <c r="S15" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T15, ($W15,$T15,$Q15,$N15,$K15,$H15,$E15), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T15, ($W15,$T15,$Q15,$N15,$K15,$H15,$E15), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T15" s="1"/>
-      <c r="V15" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="T15" s="1">
+        <v>0</v>
+      </c>
+      <c r="V15" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W15, ($W15,$T15,$Q15,$N15,$K15,$H15,$E15), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W15, ($W15,$T15,$Q15,$N15,$K15,$H15,$E15), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W15" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="W15" s="1">
+        <v>100</v>
+      </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
@@ -2385,28 +2427,28 @@
       </c>
       <c r="E35" s="12">
         <f>SUM(D13:D32)</f>
-        <v>0</v>
+        <v>-45</v>
       </c>
       <c r="G35" s="7" t="s">
         <v>7</v>
       </c>
       <c r="H35" s="12">
         <f>SUM(G13:G32)</f>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="J35" s="7" t="s">
         <v>7</v>
       </c>
       <c r="K35" s="12">
         <f>SUM(J13:J32)</f>
-        <v>0</v>
+        <v>-55</v>
       </c>
       <c r="M35" s="7" t="s">
         <v>7</v>
       </c>
       <c r="N35" s="12">
         <f>SUM(M13:M32)</f>
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="P35" s="7" t="s">
         <v>7</v>
@@ -2420,14 +2462,14 @@
       </c>
       <c r="T35" s="12">
         <f>SUM(S13:S32)</f>
-        <v>0</v>
+        <v>-50</v>
       </c>
       <c r="V35" s="7" t="s">
         <v>7</v>
       </c>
       <c r="W35" s="12">
         <f>SUM(V13:V32)</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="X35" s="1">
         <f>SUM(E35,H35,K35,N35,Q35,T35,W35)</f>

</xml_diff>

<commit_message>
Contest 5 SRH vs RR
</commit_message>
<xml_diff>
--- a/2022/EBE Boys 2022.xlsx
+++ b/2022/EBE Boys 2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3FDA240-6183-6941-9464-563005C62414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18FB8F6F-1520-6141-AE2C-DDA435CCB563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="520" windowWidth="35840" windowHeight="20420" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -1571,41 +1571,55 @@
       <c r="C16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="3" t="str">
+      <c r="D16" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E16, ($W16,$T16,$Q16,$N16,$K16,$H16,$E16), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E16, ($W16,$T16,$Q16,$N16,$K16,$H16,$E16), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="G16" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <v>70</v>
+      </c>
+      <c r="G16" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H16, ($W16,$T16,$Q16,$N16,$K16,$H16,$E16), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H16, ($W16,$T16,$Q16,$N16,$K16,$H16,$E16), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H16" s="1"/>
-      <c r="J16" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="H16" s="1">
+        <v>50</v>
+      </c>
+      <c r="J16" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K16, ($W16,$T16,$Q16,$N16,$K16,$H16,$E16), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K16, ($W16,$T16,$Q16,$N16,$K16,$H16,$E16), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K16" s="1"/>
-      <c r="M16" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="K16" s="1">
+        <v>100</v>
+      </c>
+      <c r="M16" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N16, ($W16,$T16,$Q16,$N16,$K16,$H16,$E16), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N16, ($W16,$T16,$Q16,$N16,$K16,$H16,$E16), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N16" s="1"/>
-      <c r="P16" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="N16" s="1">
+        <v>0</v>
+      </c>
+      <c r="P16" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q16, ($W16,$T16,$Q16,$N16,$K16,$H16,$E16), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q16, ($W16,$T16,$Q16,$N16,$K16,$H16,$E16), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q16" s="1"/>
-      <c r="S16" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>40</v>
+      </c>
+      <c r="S16" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T16, ($W16,$T16,$Q16,$N16,$K16,$H16,$E16), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T16, ($W16,$T16,$Q16,$N16,$K16,$H16,$E16), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T16" s="1"/>
-      <c r="V16" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="T16" s="1">
+        <v>80</v>
+      </c>
+      <c r="V16" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W16, ($W16,$T16,$Q16,$N16,$K16,$H16,$E16), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W16, ($W16,$T16,$Q16,$N16,$K16,$H16,$E16), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W16" s="1"/>
+        <v>-10</v>
+      </c>
+      <c r="W16" s="1">
+        <v>60</v>
+      </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
@@ -1617,41 +1631,55 @@
       <c r="C17" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="3" t="str">
+      <c r="D17" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E17, ($W17,$T17,$Q17,$N17,$K17,$H17,$E17), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E17, ($W17,$T17,$Q17,$N17,$K17,$H17,$E17), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E17" s="1"/>
-      <c r="G17" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H17, ($W17,$T17,$Q17,$N17,$K17,$H17,$E17), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H17, ($W17,$T17,$Q17,$N17,$K17,$H17,$E17), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H17" s="1"/>
-      <c r="J17" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="H17" s="1">
+        <v>50</v>
+      </c>
+      <c r="J17" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K17, ($W17,$T17,$Q17,$N17,$K17,$H17,$E17), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K17, ($W17,$T17,$Q17,$N17,$K17,$H17,$E17), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K17" s="1"/>
-      <c r="M17" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K17" s="1">
+        <v>60</v>
+      </c>
+      <c r="M17" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N17, ($W17,$T17,$Q17,$N17,$K17,$H17,$E17), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N17, ($W17,$T17,$Q17,$N17,$K17,$H17,$E17), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N17" s="1"/>
-      <c r="P17" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="N17" s="1">
+        <v>70</v>
+      </c>
+      <c r="P17" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q17, ($W17,$T17,$Q17,$N17,$K17,$H17,$E17), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q17, ($W17,$T17,$Q17,$N17,$K17,$H17,$E17), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q17" s="1"/>
-      <c r="S17" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>100</v>
+      </c>
+      <c r="S17" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T17, ($W17,$T17,$Q17,$N17,$K17,$H17,$E17), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T17, ($W17,$T17,$Q17,$N17,$K17,$H17,$E17), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T17" s="1"/>
-      <c r="V17" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="T17" s="1">
+        <v>40</v>
+      </c>
+      <c r="V17" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W17, ($W17,$T17,$Q17,$N17,$K17,$H17,$E17), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W17, ($W17,$T17,$Q17,$N17,$K17,$H17,$E17), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W17" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="W17" s="1">
+        <v>80</v>
+      </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
@@ -2427,35 +2455,35 @@
       </c>
       <c r="E35" s="12">
         <f>SUM(D13:D32)</f>
-        <v>-45</v>
+        <v>-70</v>
       </c>
       <c r="G35" s="7" t="s">
         <v>7</v>
       </c>
       <c r="H35" s="12">
         <f>SUM(G13:G32)</f>
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="J35" s="7" t="s">
         <v>7</v>
       </c>
       <c r="K35" s="12">
         <f>SUM(J13:J32)</f>
-        <v>-55</v>
+        <v>-15</v>
       </c>
       <c r="M35" s="7" t="s">
         <v>7</v>
       </c>
       <c r="N35" s="12">
         <f>SUM(M13:M32)</f>
-        <v>-5</v>
+        <v>-30</v>
       </c>
       <c r="P35" s="7" t="s">
         <v>7</v>
       </c>
       <c r="Q35" s="12">
         <f>SUM(P13:P32)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="S35" s="7" t="s">
         <v>7</v>
@@ -2469,7 +2497,7 @@
       </c>
       <c r="W35" s="12">
         <f>SUM(V13:V32)</f>
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="X35" s="1">
         <f>SUM(E35,H35,K35,N35,Q35,T35,W35)</f>

</xml_diff>

<commit_message>
Contest 6 RCB vs KKR.
</commit_message>
<xml_diff>
--- a/2022/EBE Boys 2022.xlsx
+++ b/2022/EBE Boys 2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18FB8F6F-1520-6141-AE2C-DDA435CCB563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E20B73-C13F-5940-A244-447649312BBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="520" windowWidth="35840" windowHeight="20420" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -1691,41 +1691,55 @@
       <c r="C18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="3" t="str">
+      <c r="D18" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E18, ($W18,$T18,$Q18,$N18,$K18,$H18,$E18), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E18, ($W18,$T18,$Q18,$N18,$K18,$H18,$E18), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E18" s="1"/>
-      <c r="G18" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="E18" s="1">
+        <v>50</v>
+      </c>
+      <c r="G18" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H18, ($W18,$T18,$Q18,$N18,$K18,$H18,$E18), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H18, ($W18,$T18,$Q18,$N18,$K18,$H18,$E18), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H18" s="1"/>
-      <c r="J18" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1">
+        <v>70</v>
+      </c>
+      <c r="J18" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K18, ($W18,$T18,$Q18,$N18,$K18,$H18,$E18), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K18, ($W18,$T18,$Q18,$N18,$K18,$H18,$E18), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K18" s="1"/>
-      <c r="M18" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="K18" s="1">
+        <v>80</v>
+      </c>
+      <c r="M18" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N18, ($W18,$T18,$Q18,$N18,$K18,$H18,$E18), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N18, ($W18,$T18,$Q18,$N18,$K18,$H18,$E18), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N18" s="1"/>
-      <c r="P18" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="N18" s="1">
+        <v>40</v>
+      </c>
+      <c r="P18" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q18, ($W18,$T18,$Q18,$N18,$K18,$H18,$E18), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q18, ($W18,$T18,$Q18,$N18,$K18,$H18,$E18), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q18" s="1"/>
-      <c r="S18" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>100</v>
+      </c>
+      <c r="S18" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T18, ($W18,$T18,$Q18,$N18,$K18,$H18,$E18), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T18, ($W18,$T18,$Q18,$N18,$K18,$H18,$E18), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T18" s="1"/>
-      <c r="V18" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="T18" s="1">
+        <v>60</v>
+      </c>
+      <c r="V18" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W18, ($W18,$T18,$Q18,$N18,$K18,$H18,$E18), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W18, ($W18,$T18,$Q18,$N18,$K18,$H18,$E18), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W18" s="1"/>
+        <v>-25</v>
+      </c>
+      <c r="W18" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
@@ -2455,7 +2469,7 @@
       </c>
       <c r="E35" s="12">
         <f>SUM(D13:D32)</f>
-        <v>-70</v>
+        <v>-85</v>
       </c>
       <c r="G35" s="7" t="s">
         <v>7</v>
@@ -2469,35 +2483,35 @@
       </c>
       <c r="K35" s="12">
         <f>SUM(J13:J32)</f>
-        <v>-15</v>
+        <v>5</v>
       </c>
       <c r="M35" s="7" t="s">
         <v>7</v>
       </c>
       <c r="N35" s="12">
         <f>SUM(M13:M32)</f>
-        <v>-30</v>
+        <v>-50</v>
       </c>
       <c r="P35" s="7" t="s">
         <v>7</v>
       </c>
       <c r="Q35" s="12">
         <f>SUM(P13:P32)</f>
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="S35" s="7" t="s">
         <v>7</v>
       </c>
       <c r="T35" s="12">
         <f>SUM(S13:S32)</f>
-        <v>-50</v>
+        <v>-60</v>
       </c>
       <c r="V35" s="7" t="s">
         <v>7</v>
       </c>
       <c r="W35" s="12">
         <f>SUM(V13:V32)</f>
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="X35" s="1">
         <f>SUM(E35,H35,K35,N35,Q35,T35,W35)</f>

</xml_diff>

<commit_message>
Contest 7 LSG vs CSK
</commit_message>
<xml_diff>
--- a/2022/EBE Boys 2022.xlsx
+++ b/2022/EBE Boys 2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E20B73-C13F-5940-A244-447649312BBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE4F20F-27B3-CB46-9CCF-4B0FFF744E78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="520" windowWidth="35840" windowHeight="20420" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -1751,41 +1751,55 @@
       <c r="C19" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="3" t="str">
+      <c r="D19" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E19, ($W19,$T19,$Q19,$N19,$K19,$H19,$E19), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E19, ($W19,$T19,$Q19,$N19,$K19,$H19,$E19), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E19" s="1"/>
-      <c r="G19" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="E19" s="1">
+        <v>80</v>
+      </c>
+      <c r="G19" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H19, ($W19,$T19,$Q19,$N19,$K19,$H19,$E19), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H19, ($W19,$T19,$Q19,$N19,$K19,$H19,$E19), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H19" s="1"/>
-      <c r="J19" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0</v>
+      </c>
+      <c r="J19" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K19, ($W19,$T19,$Q19,$N19,$K19,$H19,$E19), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K19, ($W19,$T19,$Q19,$N19,$K19,$H19,$E19), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K19" s="1"/>
-      <c r="M19" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="K19" s="1">
+        <v>50</v>
+      </c>
+      <c r="M19" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N19, ($W19,$T19,$Q19,$N19,$K19,$H19,$E19), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N19, ($W19,$T19,$Q19,$N19,$K19,$H19,$E19), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N19" s="1"/>
-      <c r="P19" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="N19" s="1">
+        <v>40</v>
+      </c>
+      <c r="P19" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q19, ($W19,$T19,$Q19,$N19,$K19,$H19,$E19), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q19, ($W19,$T19,$Q19,$N19,$K19,$H19,$E19), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q19" s="1"/>
-      <c r="S19" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>60</v>
+      </c>
+      <c r="S19" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T19, ($W19,$T19,$Q19,$N19,$K19,$H19,$E19), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T19, ($W19,$T19,$Q19,$N19,$K19,$H19,$E19), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T19" s="1"/>
-      <c r="V19" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="T19" s="1">
+        <v>70</v>
+      </c>
+      <c r="V19" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W19, ($W19,$T19,$Q19,$N19,$K19,$H19,$E19), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W19, ($W19,$T19,$Q19,$N19,$K19,$H19,$E19), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W19" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="W19" s="1">
+        <v>100</v>
+      </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
@@ -2469,35 +2483,35 @@
       </c>
       <c r="E35" s="12">
         <f>SUM(D13:D32)</f>
-        <v>-85</v>
+        <v>-65</v>
       </c>
       <c r="G35" s="7" t="s">
         <v>7</v>
       </c>
       <c r="H35" s="12">
         <f>SUM(G13:G32)</f>
-        <v>5</v>
+        <v>-20</v>
       </c>
       <c r="J35" s="7" t="s">
         <v>7</v>
       </c>
       <c r="K35" s="12">
         <f>SUM(J13:J32)</f>
-        <v>5</v>
+        <v>-10</v>
       </c>
       <c r="M35" s="7" t="s">
         <v>7</v>
       </c>
       <c r="N35" s="12">
         <f>SUM(M13:M32)</f>
-        <v>-50</v>
+        <v>-70</v>
       </c>
       <c r="P35" s="7" t="s">
         <v>7</v>
       </c>
       <c r="Q35" s="12">
         <f>SUM(P13:P32)</f>
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="S35" s="7" t="s">
         <v>7</v>
@@ -2511,7 +2525,7 @@
       </c>
       <c r="W35" s="12">
         <f>SUM(V13:V32)</f>
-        <v>105</v>
+        <v>155</v>
       </c>
       <c r="X35" s="1">
         <f>SUM(E35,H35,K35,N35,Q35,T35,W35)</f>

</xml_diff>

<commit_message>
Results till contest 13 RR vs RCB
</commit_message>
<xml_diff>
--- a/2022/EBE Boys 2022.xlsx
+++ b/2022/EBE Boys 2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE4F20F-27B3-CB46-9CCF-4B0FFF744E78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA63219-2B16-074E-8E7A-37AD02DF02DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="520" windowWidth="35840" windowHeight="20420" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -1811,41 +1811,55 @@
       <c r="C20" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="3" t="str">
+      <c r="D20" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E20, ($W20,$T20,$Q20,$N20,$K20,$H20,$E20), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E20, ($W20,$T20,$Q20,$N20,$K20,$H20,$E20), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E20" s="1"/>
-      <c r="G20" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="E20" s="1">
+        <v>40</v>
+      </c>
+      <c r="G20" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H20, ($W20,$T20,$Q20,$N20,$K20,$H20,$E20), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H20, ($W20,$T20,$Q20,$N20,$K20,$H20,$E20), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H20" s="1"/>
-      <c r="J20" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1">
+        <v>70</v>
+      </c>
+      <c r="J20" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K20, ($W20,$T20,$Q20,$N20,$K20,$H20,$E20), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K20, ($W20,$T20,$Q20,$N20,$K20,$H20,$E20), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K20" s="1"/>
-      <c r="M20" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="K20" s="1">
+        <v>80</v>
+      </c>
+      <c r="M20" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N20, ($W20,$T20,$Q20,$N20,$K20,$H20,$E20), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N20, ($W20,$T20,$Q20,$N20,$K20,$H20,$E20), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N20" s="1"/>
-      <c r="P20" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="N20" s="1">
+        <v>60</v>
+      </c>
+      <c r="P20" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q20, ($W20,$T20,$Q20,$N20,$K20,$H20,$E20), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q20, ($W20,$T20,$Q20,$N20,$K20,$H20,$E20), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q20" s="1"/>
-      <c r="S20" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>100</v>
+      </c>
+      <c r="S20" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T20, ($W20,$T20,$Q20,$N20,$K20,$H20,$E20), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T20, ($W20,$T20,$Q20,$N20,$K20,$H20,$E20), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T20" s="1"/>
-      <c r="V20" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="T20" s="1">
+        <v>0</v>
+      </c>
+      <c r="V20" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W20, ($W20,$T20,$Q20,$N20,$K20,$H20,$E20), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W20, ($W20,$T20,$Q20,$N20,$K20,$H20,$E20), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W20" s="1"/>
+        <v>-15</v>
+      </c>
+      <c r="W20" s="1">
+        <v>50</v>
+      </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
@@ -1857,41 +1871,55 @@
       <c r="C21" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="3" t="str">
+      <c r="D21" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E21, ($W21,$T21,$Q21,$N21,$K21,$H21,$E21), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E21, ($W21,$T21,$Q21,$N21,$K21,$H21,$E21), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E21" s="4"/>
-      <c r="G21" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="E21" s="4">
+        <v>100</v>
+      </c>
+      <c r="G21" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H21, ($W21,$T21,$Q21,$N21,$K21,$H21,$E21), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H21, ($W21,$T21,$Q21,$N21,$K21,$H21,$E21), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H21" s="4"/>
-      <c r="J21" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="H21" s="4">
+        <v>50</v>
+      </c>
+      <c r="J21" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K21, ($W21,$T21,$Q21,$N21,$K21,$H21,$E21), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K21, ($W21,$T21,$Q21,$N21,$K21,$H21,$E21), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K21" s="4"/>
-      <c r="M21" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="K21" s="4">
+        <v>40</v>
+      </c>
+      <c r="M21" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N21, ($W21,$T21,$Q21,$N21,$K21,$H21,$E21), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N21, ($W21,$T21,$Q21,$N21,$K21,$H21,$E21), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N21" s="4"/>
-      <c r="P21" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="N21" s="4">
+        <v>80</v>
+      </c>
+      <c r="P21" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q21, ($W21,$T21,$Q21,$N21,$K21,$H21,$E21), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q21, ($W21,$T21,$Q21,$N21,$K21,$H21,$E21), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q21" s="4"/>
-      <c r="S21" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="Q21" s="4">
+        <v>60</v>
+      </c>
+      <c r="S21" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T21, ($W21,$T21,$Q21,$N21,$K21,$H21,$E21), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T21, ($W21,$T21,$Q21,$N21,$K21,$H21,$E21), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T21" s="4"/>
-      <c r="V21" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="T21" s="4">
+        <v>70</v>
+      </c>
+      <c r="V21" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W21, ($W21,$T21,$Q21,$N21,$K21,$H21,$E21), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W21, ($W21,$T21,$Q21,$N21,$K21,$H21,$E21), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W21" s="4"/>
+        <v>-25</v>
+      </c>
+      <c r="W21" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
@@ -1903,41 +1931,55 @@
       <c r="C22" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="3" t="str">
+      <c r="D22" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E22, ($W22,$T22,$Q22,$N22,$K22,$H22,$E22), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E22, ($W22,$T22,$Q22,$N22,$K22,$H22,$E22), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E22" s="4"/>
-      <c r="G22" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="E22" s="4">
+        <v>60</v>
+      </c>
+      <c r="G22" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H22, ($W22,$T22,$Q22,$N22,$K22,$H22,$E22), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H22, ($W22,$T22,$Q22,$N22,$K22,$H22,$E22), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H22" s="4"/>
-      <c r="J22" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="H22" s="4">
+        <v>0</v>
+      </c>
+      <c r="J22" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K22, ($W22,$T22,$Q22,$N22,$K22,$H22,$E22), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K22, ($W22,$T22,$Q22,$N22,$K22,$H22,$E22), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K22" s="4"/>
-      <c r="M22" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="K22" s="4">
+        <v>70</v>
+      </c>
+      <c r="M22" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N22, ($W22,$T22,$Q22,$N22,$K22,$H22,$E22), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N22, ($W22,$T22,$Q22,$N22,$K22,$H22,$E22), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N22" s="4"/>
-      <c r="P22" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="N22" s="4">
+        <v>100</v>
+      </c>
+      <c r="P22" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q22, ($W22,$T22,$Q22,$N22,$K22,$H22,$E22), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q22, ($W22,$T22,$Q22,$N22,$K22,$H22,$E22), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q22" s="4"/>
-      <c r="S22" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="Q22" s="4">
+        <v>50</v>
+      </c>
+      <c r="S22" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T22, ($W22,$T22,$Q22,$N22,$K22,$H22,$E22), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T22, ($W22,$T22,$Q22,$N22,$K22,$H22,$E22), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T22" s="4"/>
-      <c r="V22" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="T22" s="4">
+        <v>40</v>
+      </c>
+      <c r="V22" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W22, ($W22,$T22,$Q22,$N22,$K22,$H22,$E22), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W22, ($W22,$T22,$Q22,$N22,$K22,$H22,$E22), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W22" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="W22" s="4">
+        <v>80</v>
+      </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
@@ -1949,41 +1991,55 @@
       <c r="C23" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="3" t="str">
+      <c r="D23" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E23, ($W23,$T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E23, ($W23,$T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E23" s="4"/>
-      <c r="G23" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="E23" s="4">
+        <v>70</v>
+      </c>
+      <c r="G23" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H23, ($W23,$T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H23, ($W23,$T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H23" s="4"/>
-      <c r="J23" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="H23" s="4">
+        <v>0</v>
+      </c>
+      <c r="J23" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K23, ($W23,$T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K23, ($W23,$T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K23" s="4"/>
-      <c r="M23" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="K23" s="4">
+        <v>50</v>
+      </c>
+      <c r="M23" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N23, ($W23,$T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N23, ($W23,$T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N23" s="4"/>
-      <c r="P23" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="N23" s="4">
+        <v>100</v>
+      </c>
+      <c r="P23" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q23, ($W23,$T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q23, ($W23,$T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q23" s="4"/>
-      <c r="S23" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="Q23" s="4">
+        <v>40</v>
+      </c>
+      <c r="S23" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T23, ($W23,$T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T23, ($W23,$T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T23" s="4"/>
-      <c r="V23" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="T23" s="4">
+        <v>60</v>
+      </c>
+      <c r="V23" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W23, ($W23,$T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W23, ($W23,$T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W23" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="W23" s="4">
+        <v>80</v>
+      </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
@@ -1995,41 +2051,55 @@
       <c r="C24" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D24" s="3" t="str">
+      <c r="D24" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E24, ($W24,$T24,$Q24,$N24,$K24,$H24,$E24), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E24, ($W24,$T24,$Q24,$N24,$K24,$H24,$E24), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E24" s="4"/>
-      <c r="G24" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="E24" s="4">
+        <v>100</v>
+      </c>
+      <c r="G24" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H24, ($W24,$T24,$Q24,$N24,$K24,$H24,$E24), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H24, ($W24,$T24,$Q24,$N24,$K24,$H24,$E24), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H24" s="4"/>
-      <c r="J24" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="H24" s="4">
+        <v>70</v>
+      </c>
+      <c r="J24" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K24, ($W24,$T24,$Q24,$N24,$K24,$H24,$E24), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K24, ($W24,$T24,$Q24,$N24,$K24,$H24,$E24), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K24" s="4"/>
-      <c r="M24" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="K24" s="4">
+        <v>40</v>
+      </c>
+      <c r="M24" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N24, ($W24,$T24,$Q24,$N24,$K24,$H24,$E24), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N24, ($W24,$T24,$Q24,$N24,$K24,$H24,$E24), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N24" s="4"/>
-      <c r="P24" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="N24" s="4">
+        <v>50</v>
+      </c>
+      <c r="P24" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q24, ($W24,$T24,$Q24,$N24,$K24,$H24,$E24), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q24, ($W24,$T24,$Q24,$N24,$K24,$H24,$E24), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q24" s="4"/>
-      <c r="S24" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="Q24" s="4">
+        <v>0</v>
+      </c>
+      <c r="S24" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T24, ($W24,$T24,$Q24,$N24,$K24,$H24,$E24), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T24, ($W24,$T24,$Q24,$N24,$K24,$H24,$E24), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T24" s="4"/>
-      <c r="V24" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="T24" s="4">
+        <v>80</v>
+      </c>
+      <c r="V24" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W24, ($W24,$T24,$Q24,$N24,$K24,$H24,$E24), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W24, ($W24,$T24,$Q24,$N24,$K24,$H24,$E24), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W24" s="4"/>
+        <v>-10</v>
+      </c>
+      <c r="W24" s="4">
+        <v>60</v>
+      </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
@@ -2041,41 +2111,53 @@
       <c r="C25" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="3" t="str">
+      <c r="D25" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E25, ($W25,$T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E25, ($W25,$T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E25" s="4"/>
-      <c r="G25" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="E25" s="4">
+        <v>70</v>
+      </c>
+      <c r="G25" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H25, ($W25,$T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H25, ($W25,$T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H25" s="4"/>
-      <c r="J25" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(K25, ($W25,$T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K25, ($W25,$T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K25" s="4"/>
-      <c r="M25" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="H25" s="4">
+        <v>100</v>
+      </c>
+      <c r="J25" s="3">
+        <v>-22.5</v>
+      </c>
+      <c r="K25" s="4">
+        <v>40</v>
+      </c>
+      <c r="M25" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N25, ($W25,$T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N25, ($W25,$T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N25" s="4"/>
-      <c r="P25" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="N25" s="4">
+        <v>80</v>
+      </c>
+      <c r="P25" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q25, ($W25,$T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q25, ($W25,$T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q25" s="4"/>
-      <c r="S25" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="Q25" s="4">
+        <v>60</v>
+      </c>
+      <c r="S25" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T25, ($W25,$T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T25, ($W25,$T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T25" s="4"/>
-      <c r="V25" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(W25, ($W25,$T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W25, ($W25,$T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W25" s="4"/>
+        <v>-15</v>
+      </c>
+      <c r="T25" s="4">
+        <v>50</v>
+      </c>
+      <c r="V25" s="3">
+        <v>-22.5</v>
+      </c>
+      <c r="W25" s="4">
+        <v>40</v>
+      </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
@@ -2483,49 +2565,49 @@
       </c>
       <c r="E35" s="12">
         <f>SUM(D13:D32)</f>
-        <v>-65</v>
+        <v>5</v>
       </c>
       <c r="G35" s="7" t="s">
         <v>7</v>
       </c>
       <c r="H35" s="12">
         <f>SUM(G13:G32)</f>
-        <v>-20</v>
+        <v>-35</v>
       </c>
       <c r="J35" s="7" t="s">
         <v>7</v>
       </c>
       <c r="K35" s="12">
         <f>SUM(J13:J32)</f>
-        <v>-10</v>
+        <v>-67.5</v>
       </c>
       <c r="M35" s="7" t="s">
         <v>7</v>
       </c>
       <c r="N35" s="12">
         <f>SUM(M13:M32)</f>
-        <v>-70</v>
+        <v>45</v>
       </c>
       <c r="P35" s="7" t="s">
         <v>7</v>
       </c>
       <c r="Q35" s="12">
         <f>SUM(P13:P32)</f>
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="S35" s="7" t="s">
         <v>7</v>
       </c>
       <c r="T35" s="12">
         <f>SUM(S13:S32)</f>
-        <v>-60</v>
+        <v>-110</v>
       </c>
       <c r="V35" s="7" t="s">
         <v>7</v>
       </c>
       <c r="W35" s="12">
         <f>SUM(V13:V32)</f>
-        <v>155</v>
+        <v>122.5</v>
       </c>
       <c r="X35" s="1">
         <f>SUM(E35,H35,K35,N35,Q35,T35,W35)</f>

</xml_diff>

<commit_message>
Results: Contest 14 through 21
</commit_message>
<xml_diff>
--- a/2022/EBE Boys 2022.xlsx
+++ b/2022/EBE Boys 2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA63219-2B16-074E-8E7A-37AD02DF02DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD1B85EB-A1BE-624E-BA0C-83B44F078F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="520" windowWidth="35840" windowHeight="20420" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
   <si>
     <t>Points</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>RR vs LSG</t>
+  </si>
+  <si>
+    <t>SRH vs GT</t>
   </si>
 </sst>
 </file>
@@ -477,7 +480,187 @@
     <cellStyle name="20% - Accent6" xfId="1" builtinId="50"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="48">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1093,11 +1276,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
-  <dimension ref="A1:Z66"/>
+  <dimension ref="A1:Z81"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X35" sqref="X35"/>
+      <pane ySplit="11" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X50" sqref="X50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2169,41 +2352,55 @@
       <c r="C26" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="3" t="str">
+      <c r="D26" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E26, ($W26,$T26,$Q26,$N26,$K26,$H26,$E26), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E26, ($W26,$T26,$Q26,$N26,$K26,$H26,$E26), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E26" s="4"/>
-      <c r="G26" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="E26" s="4">
+        <v>50</v>
+      </c>
+      <c r="G26" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H26, ($W26,$T26,$Q26,$N26,$K26,$H26,$E26), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H26, ($W26,$T26,$Q26,$N26,$K26,$H26,$E26), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H26" s="4"/>
-      <c r="J26" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="H26" s="4">
+        <v>100</v>
+      </c>
+      <c r="J26" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K26, ($W26,$T26,$Q26,$N26,$K26,$H26,$E26), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K26, ($W26,$T26,$Q26,$N26,$K26,$H26,$E26), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K26" s="4"/>
-      <c r="M26" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="K26" s="4">
+        <v>0</v>
+      </c>
+      <c r="M26" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N26, ($W26,$T26,$Q26,$N26,$K26,$H26,$E26), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N26, ($W26,$T26,$Q26,$N26,$K26,$H26,$E26), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N26" s="4"/>
-      <c r="P26" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="N26" s="4">
+        <v>80</v>
+      </c>
+      <c r="P26" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q26, ($W26,$T26,$Q26,$N26,$K26,$H26,$E26), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q26, ($W26,$T26,$Q26,$N26,$K26,$H26,$E26), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q26" s="4"/>
-      <c r="S26" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="4">
+        <v>70</v>
+      </c>
+      <c r="S26" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T26, ($W26,$T26,$Q26,$N26,$K26,$H26,$E26), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T26, ($W26,$T26,$Q26,$N26,$K26,$H26,$E26), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T26" s="4"/>
-      <c r="V26" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="T26" s="4">
+        <v>60</v>
+      </c>
+      <c r="V26" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W26, ($W26,$T26,$Q26,$N26,$K26,$H26,$E26), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W26, ($W26,$T26,$Q26,$N26,$K26,$H26,$E26), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W26" s="4"/>
+        <v>-20</v>
+      </c>
+      <c r="W26" s="4">
+        <v>40</v>
+      </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
@@ -2215,41 +2412,55 @@
       <c r="C27" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="3" t="str">
+      <c r="D27" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E27, ($W27,$T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E27, ($W27,$T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E27" s="4"/>
-      <c r="G27" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="E27" s="4">
+        <v>60</v>
+      </c>
+      <c r="G27" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H27, ($W27,$T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H27, ($W27,$T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H27" s="4"/>
-      <c r="J27" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="H27" s="4">
+        <v>50</v>
+      </c>
+      <c r="J27" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K27, ($W27,$T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K27, ($W27,$T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K27" s="4"/>
-      <c r="M27" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="K27" s="4">
+        <v>0</v>
+      </c>
+      <c r="M27" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N27, ($W27,$T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N27, ($W27,$T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N27" s="4"/>
-      <c r="P27" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="N27" s="4">
+        <v>100</v>
+      </c>
+      <c r="P27" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q27, ($W27,$T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q27, ($W27,$T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q27" s="4"/>
-      <c r="S27" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="Q27" s="4">
+        <v>40</v>
+      </c>
+      <c r="S27" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T27, ($W27,$T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T27, ($W27,$T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T27" s="4"/>
-      <c r="V27" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="T27" s="4">
+        <v>80</v>
+      </c>
+      <c r="V27" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W27, ($W27,$T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W27, ($W27,$T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W27" s="4"/>
+        <v>0</v>
+      </c>
+      <c r="W27" s="4">
+        <v>70</v>
+      </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
@@ -2261,41 +2472,55 @@
       <c r="C28" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D28" s="3" t="str">
+      <c r="D28" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E28, ($W28,$T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E28, ($W28,$T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E28" s="1"/>
-      <c r="G28" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1">
+        <v>70</v>
+      </c>
+      <c r="G28" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H28, ($W28,$T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H28, ($W28,$T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H28" s="1"/>
-      <c r="J28" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="H28" s="1">
+        <v>40</v>
+      </c>
+      <c r="J28" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K28, ($W28,$T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K28, ($W28,$T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K28" s="1"/>
-      <c r="M28" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="K28" s="1">
+        <v>50</v>
+      </c>
+      <c r="M28" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N28, ($W28,$T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N28, ($W28,$T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N28" s="1"/>
-      <c r="P28" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="N28" s="1">
+        <v>100</v>
+      </c>
+      <c r="P28" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q28, ($W28,$T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q28, ($W28,$T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q28" s="1"/>
-      <c r="S28" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>60</v>
+      </c>
+      <c r="S28" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T28, ($W28,$T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T28, ($W28,$T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T28" s="1"/>
-      <c r="V28" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="T28" s="1">
+        <v>80</v>
+      </c>
+      <c r="V28" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W28, ($W28,$T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W28, ($W28,$T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W28" s="1"/>
+        <v>-25</v>
+      </c>
+      <c r="W28" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
@@ -2307,41 +2532,55 @@
       <c r="C29" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="3" t="str">
+      <c r="D29" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E29, ($W29,$T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E29, ($W29,$T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E29" s="1"/>
-      <c r="G29" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="E29" s="1">
+        <v>50</v>
+      </c>
+      <c r="G29" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H29, ($W29,$T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H29, ($W29,$T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H29" s="1"/>
-      <c r="J29" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="H29" s="1">
+        <v>100</v>
+      </c>
+      <c r="J29" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K29, ($W29,$T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K29, ($W29,$T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K29" s="1"/>
-      <c r="M29" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="K29" s="1">
+        <v>80</v>
+      </c>
+      <c r="M29" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N29, ($W29,$T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N29, ($W29,$T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N29" s="1"/>
-      <c r="P29" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="N29" s="1">
+        <v>60</v>
+      </c>
+      <c r="P29" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q29, ($W29,$T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q29, ($W29,$T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q29" s="1"/>
-      <c r="S29" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>0</v>
+      </c>
+      <c r="S29" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T29, ($W29,$T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T29, ($W29,$T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T29" s="1"/>
-      <c r="V29" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="T29" s="1">
+        <v>40</v>
+      </c>
+      <c r="V29" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W29, ($W29,$T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W29, ($W29,$T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W29" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="W29" s="1">
+        <v>70</v>
+      </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
@@ -2353,41 +2592,55 @@
       <c r="C30" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="3" t="str">
+      <c r="D30" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E30, ($W30,$T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E30, ($W30,$T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E30" s="1"/>
-      <c r="G30" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="E30" s="1">
+        <v>40</v>
+      </c>
+      <c r="G30" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H30, ($W30,$T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H30, ($W30,$T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H30" s="1"/>
-      <c r="J30" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="H30" s="1">
+        <v>60</v>
+      </c>
+      <c r="J30" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K30, ($W30,$T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K30, ($W30,$T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K30" s="1"/>
-      <c r="M30" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="K30" s="1">
+        <v>80</v>
+      </c>
+      <c r="M30" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N30, ($W30,$T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N30, ($W30,$T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N30" s="1"/>
-      <c r="P30" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="N30" s="1">
+        <v>70</v>
+      </c>
+      <c r="P30" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q30, ($W30,$T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q30, ($W30,$T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q30" s="1"/>
-      <c r="S30" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>50</v>
+      </c>
+      <c r="S30" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T30, ($W30,$T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T30, ($W30,$T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T30" s="1"/>
-      <c r="V30" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="T30" s="1">
+        <v>100</v>
+      </c>
+      <c r="V30" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W30, ($W30,$T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W30, ($W30,$T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W30" s="1"/>
+        <v>-25</v>
+      </c>
+      <c r="W30" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
@@ -2399,41 +2652,55 @@
       <c r="C31" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D31" s="3" t="str">
+      <c r="D31" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E31, ($W31,$T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E31, ($W31,$T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E31" s="1"/>
-      <c r="G31" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="E31" s="1">
+        <v>50</v>
+      </c>
+      <c r="G31" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H31, ($W31,$T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H31, ($W31,$T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H31" s="1"/>
-      <c r="J31" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="H31" s="1">
+        <v>70</v>
+      </c>
+      <c r="J31" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K31, ($W31,$T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K31, ($W31,$T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K31" s="1"/>
-      <c r="M31" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="K31" s="1">
+        <v>80</v>
+      </c>
+      <c r="M31" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N31, ($W31,$T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N31, ($W31,$T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N31" s="1"/>
-      <c r="P31" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="N31" s="1">
+        <v>100</v>
+      </c>
+      <c r="P31" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q31, ($W31,$T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q31, ($W31,$T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q31" s="1"/>
-      <c r="S31" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>0</v>
+      </c>
+      <c r="S31" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T31, ($W31,$T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T31, ($W31,$T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T31" s="1"/>
-      <c r="V31" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="T31" s="1">
+        <v>60</v>
+      </c>
+      <c r="V31" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W31, ($W31,$T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W31, ($W31,$T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W31" s="1"/>
+        <v>-20</v>
+      </c>
+      <c r="W31" s="1">
+        <v>40</v>
+      </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
@@ -2445,600 +2712,561 @@
       <c r="C32" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D32" s="3" t="str">
+      <c r="D32" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E32, ($W32,$T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E32, ($W32,$T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E32" s="1"/>
-      <c r="G32" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(H32, ($W32,$T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H32, ($W32,$T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H32" s="1"/>
-      <c r="J32" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="E32" s="1">
+        <v>100</v>
+      </c>
+      <c r="G32" s="3">
+        <v>10</v>
+      </c>
+      <c r="H32" s="1">
+        <v>80</v>
+      </c>
+      <c r="J32" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K32, ($W32,$T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K32, ($W32,$T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K32" s="1"/>
-      <c r="M32" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(N32, ($W32,$T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N32, ($W32,$T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N32" s="1"/>
-      <c r="P32" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="K32" s="1">
+        <v>50</v>
+      </c>
+      <c r="M32" s="3">
+        <v>10</v>
+      </c>
+      <c r="N32" s="1">
+        <v>80</v>
+      </c>
+      <c r="P32" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q32, ($W32,$T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q32, ($W32,$T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q32" s="1"/>
-      <c r="S32" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="Q32" s="1">
+        <v>40</v>
+      </c>
+      <c r="S32" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T32, ($W32,$T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T32, ($W32,$T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T32" s="1"/>
-      <c r="V32" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="T32" s="1">
+        <v>0</v>
+      </c>
+      <c r="V32" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W32, ($W32,$T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W32, ($W32,$T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W32" s="1"/>
-    </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A33" s="6"/>
-      <c r="B33" s="1" t="s">
+        <v>-10</v>
+      </c>
+      <c r="W32" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A33" s="6">
+        <v>21</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D33" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(E33, ($W33,$T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E33, ($W33,$T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="E33" s="1">
+        <v>70</v>
+      </c>
+      <c r="G33" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(H33, ($W33,$T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H33, ($W33,$T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-20</v>
+      </c>
+      <c r="H33" s="1">
+        <v>40</v>
+      </c>
+      <c r="J33" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(K33, ($W33,$T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K33, ($W33,$T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-10</v>
+      </c>
+      <c r="K33" s="1">
+        <v>60</v>
+      </c>
+      <c r="M33" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(N33, ($W33,$T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N33, ($W33,$T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-15</v>
+      </c>
+      <c r="N33" s="1">
+        <v>50</v>
+      </c>
+      <c r="P33" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q33, ($W33,$T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q33, ($W33,$T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>20</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>80</v>
+      </c>
+      <c r="S33" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(T33, ($W33,$T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T33, ($W33,$T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>50</v>
+      </c>
+      <c r="T33" s="1">
+        <v>100</v>
+      </c>
+      <c r="V33" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(W33, ($W33,$T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W33, ($W33,$T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-25</v>
+      </c>
+      <c r="W33" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>22</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="1"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="1"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="1"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="1"/>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="1"/>
+      <c r="S34" s="3"/>
+      <c r="T34" s="1"/>
+      <c r="V34" s="3"/>
+      <c r="W34" s="1"/>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A35" s="6">
+        <v>23</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="1"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="1"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="1"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="1"/>
+      <c r="P35" s="3"/>
+      <c r="Q35" s="1"/>
+      <c r="S35" s="3"/>
+      <c r="T35" s="1"/>
+      <c r="V35" s="3"/>
+      <c r="W35" s="1"/>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>24</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="1"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="1"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="1"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="1"/>
+      <c r="P36" s="3"/>
+      <c r="Q36" s="1"/>
+      <c r="S36" s="3"/>
+      <c r="T36" s="1"/>
+      <c r="V36" s="3"/>
+      <c r="W36" s="1"/>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A37" s="6">
+        <v>25</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="1"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="1"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="1"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="1"/>
+      <c r="P37" s="3"/>
+      <c r="Q37" s="1"/>
+      <c r="S37" s="3"/>
+      <c r="T37" s="1"/>
+      <c r="V37" s="3"/>
+      <c r="W37" s="1"/>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>26</v>
+      </c>
+      <c r="B38" s="1"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="1"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="1"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="1"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="1"/>
+      <c r="P38" s="3"/>
+      <c r="Q38" s="1"/>
+      <c r="S38" s="3"/>
+      <c r="T38" s="1"/>
+      <c r="V38" s="3"/>
+      <c r="W38" s="1"/>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A39" s="6">
+        <v>27</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="1"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="1"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="1"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="1"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="1"/>
+      <c r="S39" s="3"/>
+      <c r="T39" s="1"/>
+      <c r="V39" s="3"/>
+      <c r="W39" s="1"/>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>28</v>
+      </c>
+      <c r="B40" s="1"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="1"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="1"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="1"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="1"/>
+      <c r="P40" s="3"/>
+      <c r="Q40" s="1"/>
+      <c r="S40" s="3"/>
+      <c r="T40" s="1"/>
+      <c r="V40" s="3"/>
+      <c r="W40" s="1"/>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A41" s="6">
+        <v>29</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="1"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="1"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="1"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="1"/>
+      <c r="P41" s="3"/>
+      <c r="Q41" s="1"/>
+      <c r="S41" s="3"/>
+      <c r="T41" s="1"/>
+      <c r="V41" s="3"/>
+      <c r="W41" s="1"/>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>30</v>
+      </c>
+      <c r="B42" s="1"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="1"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="1"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="1"/>
+      <c r="M42" s="3"/>
+      <c r="N42" s="1"/>
+      <c r="P42" s="3"/>
+      <c r="Q42" s="1"/>
+      <c r="S42" s="3"/>
+      <c r="T42" s="1"/>
+      <c r="V42" s="3"/>
+      <c r="W42" s="1"/>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A43" s="6">
+        <v>31</v>
+      </c>
+      <c r="B43" s="1"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="1"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="1"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="1"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="1"/>
+      <c r="P43" s="3"/>
+      <c r="Q43" s="1"/>
+      <c r="S43" s="3"/>
+      <c r="T43" s="1"/>
+      <c r="V43" s="3"/>
+      <c r="W43" s="1"/>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>32</v>
+      </c>
+      <c r="B44" s="1"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="1"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="1"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="1"/>
+      <c r="M44" s="3"/>
+      <c r="N44" s="1"/>
+      <c r="P44" s="3"/>
+      <c r="Q44" s="1"/>
+      <c r="S44" s="3"/>
+      <c r="T44" s="1"/>
+      <c r="V44" s="3"/>
+      <c r="W44" s="1"/>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A45" s="6">
+        <v>33</v>
+      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="1"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="1"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="1"/>
+      <c r="M45" s="3"/>
+      <c r="N45" s="1"/>
+      <c r="P45" s="3"/>
+      <c r="Q45" s="1"/>
+      <c r="S45" s="3"/>
+      <c r="T45" s="1"/>
+      <c r="V45" s="3"/>
+      <c r="W45" s="1"/>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>34</v>
+      </c>
+      <c r="B46" s="1"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="1"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="1"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="1"/>
+      <c r="M46" s="3"/>
+      <c r="N46" s="1"/>
+      <c r="P46" s="3"/>
+      <c r="Q46" s="1"/>
+      <c r="S46" s="3"/>
+      <c r="T46" s="1"/>
+      <c r="V46" s="3"/>
+      <c r="W46" s="1"/>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A47" s="6">
+        <v>35</v>
+      </c>
+      <c r="B47" s="1"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="1"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="1"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="1"/>
+      <c r="M47" s="3"/>
+      <c r="N47" s="1"/>
+      <c r="P47" s="3"/>
+      <c r="Q47" s="1"/>
+      <c r="S47" s="3"/>
+      <c r="T47" s="1"/>
+      <c r="V47" s="3"/>
+      <c r="W47" s="1"/>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A48" s="6"/>
+      <c r="B48" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C33" s="10"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="9" t="s">
+      <c r="C48" s="10"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G33" s="1"/>
-      <c r="H33" s="9" t="s">
+      <c r="G48" s="1"/>
+      <c r="H48" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J33" s="1"/>
-      <c r="K33" s="9" t="s">
+      <c r="J48" s="1"/>
+      <c r="K48" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="M33" s="1"/>
-      <c r="N33" s="9" t="s">
+      <c r="M48" s="1"/>
+      <c r="N48" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="P33" s="1"/>
-      <c r="Q33" s="9" t="s">
+      <c r="P48" s="1"/>
+      <c r="Q48" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="S33" s="1"/>
-      <c r="T33" s="9" t="s">
+      <c r="S48" s="1"/>
+      <c r="T48" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="V33" s="1"/>
-      <c r="W33" s="9" t="s">
+      <c r="V48" s="1"/>
+      <c r="W48" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="11" t="str">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="11" t="str">
         <f>D12</f>
         <v>Jaya</v>
       </c>
-      <c r="G34" s="1"/>
-      <c r="H34" s="11" t="str">
+      <c r="G49" s="1"/>
+      <c r="H49" s="11" t="str">
         <f>G12</f>
         <v>Justin</v>
       </c>
-      <c r="J34" s="1"/>
-      <c r="K34" s="11" t="str">
+      <c r="J49" s="1"/>
+      <c r="K49" s="11" t="str">
         <f>J12</f>
         <v>Ram</v>
       </c>
-      <c r="M34" s="1"/>
-      <c r="N34" s="11" t="str">
+      <c r="M49" s="1"/>
+      <c r="N49" s="11" t="str">
         <f>M12</f>
         <v>Sibi</v>
       </c>
-      <c r="P34" s="1"/>
-      <c r="Q34" s="11" t="str">
+      <c r="P49" s="1"/>
+      <c r="Q49" s="11" t="str">
         <f>P12</f>
         <v>Sundar</v>
       </c>
-      <c r="S34" s="1"/>
-      <c r="T34" s="11" t="str">
+      <c r="S49" s="1"/>
+      <c r="T49" s="11" t="str">
         <f>S12</f>
         <v>Upili</v>
       </c>
-      <c r="V34" s="1"/>
-      <c r="W34" s="11" t="str">
+      <c r="V49" s="1"/>
+      <c r="W49" s="11" t="str">
         <f>V12</f>
         <v>Vicky</v>
       </c>
     </row>
-    <row r="35" spans="1:26" ht="21" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E35" s="12">
-        <f>SUM(D13:D32)</f>
-        <v>5</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H35" s="12">
-        <f>SUM(G13:G32)</f>
-        <v>-35</v>
-      </c>
-      <c r="J35" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="K35" s="12">
-        <f>SUM(J13:J32)</f>
-        <v>-67.5</v>
-      </c>
-      <c r="M35" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="N35" s="12">
-        <f>SUM(M13:M32)</f>
-        <v>45</v>
-      </c>
-      <c r="P35" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q35" s="12">
-        <f>SUM(P13:P32)</f>
-        <v>40</v>
-      </c>
-      <c r="S35" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="T35" s="12">
-        <f>SUM(S13:S32)</f>
-        <v>-110</v>
-      </c>
-      <c r="V35" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="W35" s="12">
-        <f>SUM(V13:V32)</f>
-        <v>122.5</v>
-      </c>
-      <c r="X35" s="1">
-        <f>SUM(E35,H35,K35,N35,Q35,T35,W35)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="S36" s="5"/>
-      <c r="T36" s="5"/>
-    </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="S37" s="5"/>
-      <c r="T37" s="5"/>
-    </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A38" s="5"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="5"/>
-      <c r="J38" s="5"/>
-      <c r="K38" s="5"/>
-      <c r="L38" s="5"/>
-      <c r="M38" s="5"/>
-      <c r="N38" s="5"/>
-      <c r="O38" s="5"/>
-      <c r="P38" s="5"/>
-      <c r="Q38" s="5"/>
-      <c r="R38" s="5"/>
-      <c r="S38" s="5"/>
-      <c r="T38" s="5"/>
-      <c r="U38" s="5"/>
-      <c r="V38" s="5"/>
-      <c r="W38" s="5"/>
-      <c r="X38" s="5"/>
-      <c r="Y38" s="5"/>
-      <c r="Z38" s="5"/>
-    </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="5"/>
-      <c r="J39" s="5"/>
-      <c r="K39" s="5"/>
-      <c r="L39" s="5"/>
-      <c r="M39" s="5"/>
-      <c r="N39" s="5"/>
-      <c r="O39" s="5"/>
-      <c r="P39" s="5"/>
-      <c r="Q39" s="5"/>
-      <c r="R39" s="5"/>
-      <c r="S39" s="5"/>
-      <c r="T39" s="5"/>
-      <c r="U39" s="5"/>
-      <c r="V39" s="5"/>
-      <c r="W39" s="5"/>
-      <c r="X39" s="5"/>
-      <c r="Y39" s="5"/>
-      <c r="Z39" s="5"/>
-    </row>
-    <row r="40" spans="1:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="19"/>
-      <c r="G40" s="19"/>
-      <c r="H40" s="19"/>
-      <c r="I40" s="20"/>
-      <c r="J40" s="5"/>
-      <c r="K40" s="5"/>
-      <c r="L40" s="5"/>
-      <c r="M40" s="5"/>
-      <c r="N40" s="5"/>
-      <c r="O40" s="5"/>
-      <c r="P40" s="5"/>
-      <c r="Q40" s="5"/>
-      <c r="R40" s="5"/>
-      <c r="S40" s="5"/>
-      <c r="T40" s="5"/>
-      <c r="U40" s="5"/>
-      <c r="V40" s="5"/>
-      <c r="W40" s="5"/>
-      <c r="X40" s="5"/>
-      <c r="Y40" s="5"/>
-      <c r="Z40" s="5"/>
-    </row>
-    <row r="41" spans="1:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21"/>
-      <c r="G41" s="21"/>
-      <c r="H41" s="21"/>
-      <c r="I41" s="22"/>
-      <c r="J41" s="5"/>
-      <c r="K41" s="5"/>
-      <c r="L41" s="5"/>
-      <c r="M41" s="5"/>
-      <c r="N41" s="5"/>
-      <c r="O41" s="5"/>
-      <c r="P41" s="5"/>
-      <c r="Q41" s="5"/>
-      <c r="R41" s="5"/>
-      <c r="S41" s="5"/>
-      <c r="T41" s="5"/>
-      <c r="U41" s="5"/>
-      <c r="V41" s="5"/>
-      <c r="W41" s="5"/>
-      <c r="X41" s="5"/>
-      <c r="Y41" s="5"/>
-      <c r="Z41" s="5"/>
-    </row>
-    <row r="42" spans="1:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
-      <c r="I42" s="21"/>
-      <c r="J42" s="5"/>
-      <c r="K42" s="5"/>
-      <c r="L42" s="5"/>
-      <c r="M42" s="5"/>
-      <c r="N42" s="5"/>
-      <c r="O42" s="5"/>
-      <c r="P42" s="5"/>
-      <c r="Q42" s="5"/>
-      <c r="R42" s="5"/>
-      <c r="S42" s="5"/>
-      <c r="T42" s="5"/>
-      <c r="U42" s="5"/>
-      <c r="V42" s="5"/>
-      <c r="W42" s="5"/>
-      <c r="X42" s="5"/>
-      <c r="Y42" s="5"/>
-      <c r="Z42" s="5"/>
-    </row>
-    <row r="43" spans="1:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="21"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5"/>
-      <c r="I43" s="21"/>
-      <c r="J43" s="5"/>
-      <c r="K43" s="5"/>
-      <c r="L43" s="5"/>
-      <c r="M43" s="5"/>
-      <c r="N43" s="5"/>
-      <c r="O43" s="5"/>
-      <c r="P43" s="5"/>
-      <c r="Q43" s="5"/>
-      <c r="R43" s="5"/>
-      <c r="S43" s="5"/>
-      <c r="T43" s="5"/>
-      <c r="U43" s="5"/>
-      <c r="V43" s="5"/>
-      <c r="W43" s="5"/>
-      <c r="X43" s="5"/>
-      <c r="Y43" s="5"/>
-      <c r="Z43" s="5"/>
-    </row>
-    <row r="44" spans="1:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="21"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
-      <c r="H44" s="5"/>
-      <c r="I44" s="21"/>
-      <c r="J44" s="5"/>
-      <c r="K44" s="5"/>
-      <c r="L44" s="5"/>
-      <c r="M44" s="5"/>
-      <c r="N44" s="5"/>
-      <c r="O44" s="5"/>
-      <c r="P44" s="5"/>
-      <c r="Q44" s="5"/>
-      <c r="R44" s="5"/>
-      <c r="S44" s="5"/>
-      <c r="T44" s="5"/>
-      <c r="U44" s="5"/>
-      <c r="V44" s="5"/>
-      <c r="W44" s="5"/>
-      <c r="X44" s="5"/>
-      <c r="Y44" s="5"/>
-      <c r="Z44" s="5"/>
-    </row>
-    <row r="45" spans="1:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="21"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
-      <c r="I45" s="21"/>
-      <c r="J45" s="5"/>
-      <c r="K45" s="5"/>
-      <c r="L45" s="5"/>
-      <c r="M45" s="5"/>
-      <c r="N45" s="5"/>
-      <c r="O45" s="5"/>
-      <c r="P45" s="5"/>
-      <c r="Q45" s="5"/>
-      <c r="R45" s="5"/>
-      <c r="S45" s="5"/>
-      <c r="T45" s="5"/>
-      <c r="U45" s="5"/>
-      <c r="V45" s="5"/>
-      <c r="W45" s="5"/>
-      <c r="X45" s="5"/>
-      <c r="Y45" s="5"/>
-      <c r="Z45" s="5"/>
-    </row>
-    <row r="46" spans="1:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="21"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
-      <c r="H46" s="5"/>
-      <c r="I46" s="21"/>
-      <c r="J46" s="5"/>
-      <c r="K46" s="5"/>
-      <c r="L46" s="5"/>
-      <c r="M46" s="5"/>
-      <c r="N46" s="5"/>
-      <c r="O46" s="5"/>
-      <c r="P46" s="5"/>
-      <c r="Q46" s="5"/>
-      <c r="R46" s="5"/>
-      <c r="S46" s="5"/>
-      <c r="T46" s="5"/>
-      <c r="U46" s="5"/>
-      <c r="V46" s="5"/>
-      <c r="W46" s="5"/>
-      <c r="X46" s="5"/>
-      <c r="Y46" s="5"/>
-      <c r="Z46" s="5"/>
-    </row>
-    <row r="47" spans="1:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="21"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
-      <c r="I47" s="21"/>
-      <c r="J47" s="5"/>
-      <c r="K47" s="5"/>
-      <c r="L47" s="5"/>
-      <c r="M47" s="5"/>
-      <c r="N47" s="5"/>
-      <c r="O47" s="5"/>
-      <c r="P47" s="5"/>
-      <c r="Q47" s="5"/>
-      <c r="R47" s="5"/>
-      <c r="S47" s="5"/>
-      <c r="T47" s="5"/>
-      <c r="U47" s="5"/>
-      <c r="V47" s="5"/>
-      <c r="W47" s="5"/>
-      <c r="X47" s="5"/>
-      <c r="Y47" s="5"/>
-      <c r="Z47" s="5"/>
-    </row>
-    <row r="48" spans="1:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="21"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
-      <c r="H48" s="5"/>
-      <c r="I48" s="21"/>
-      <c r="J48" s="5"/>
-      <c r="K48" s="5"/>
-      <c r="L48" s="5"/>
-      <c r="M48" s="5"/>
-      <c r="N48" s="5"/>
-      <c r="O48" s="5"/>
-      <c r="P48" s="5"/>
-      <c r="Q48" s="5"/>
-      <c r="R48" s="5"/>
-      <c r="S48" s="5"/>
-      <c r="T48" s="5"/>
-      <c r="U48" s="5"/>
-      <c r="V48" s="5"/>
-      <c r="W48" s="5"/>
-      <c r="X48" s="5"/>
-      <c r="Y48" s="5"/>
-      <c r="Z48" s="5"/>
-    </row>
-    <row r="49" spans="2:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="21"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
-      <c r="H49" s="5"/>
-      <c r="I49" s="21"/>
-      <c r="J49" s="5"/>
-      <c r="K49" s="5"/>
-      <c r="L49" s="5"/>
-      <c r="M49" s="5"/>
-      <c r="N49" s="5"/>
-      <c r="O49" s="5"/>
-      <c r="P49" s="5"/>
-      <c r="Q49" s="5"/>
-      <c r="R49" s="5"/>
-      <c r="S49" s="5"/>
-      <c r="T49" s="5"/>
-      <c r="U49" s="5"/>
-      <c r="V49" s="5"/>
-      <c r="W49" s="5"/>
-      <c r="X49" s="5"/>
-      <c r="Y49" s="5"/>
-      <c r="Z49" s="5"/>
-    </row>
-    <row r="50" spans="2:26" ht="19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" ht="21" x14ac:dyDescent="0.25">
+      <c r="A50" s="5"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
-      <c r="H50" s="5"/>
-      <c r="I50" s="21"/>
-      <c r="J50" s="5"/>
-      <c r="K50" s="5"/>
-      <c r="L50" s="5"/>
-      <c r="M50" s="5"/>
-      <c r="N50" s="5"/>
-      <c r="O50" s="5"/>
-      <c r="P50" s="5"/>
-      <c r="Q50" s="5"/>
-      <c r="R50" s="5"/>
-      <c r="S50" s="5"/>
-      <c r="T50" s="5"/>
-      <c r="U50" s="5"/>
-      <c r="V50" s="5"/>
-      <c r="W50" s="5"/>
-      <c r="X50" s="5"/>
-      <c r="Y50" s="5"/>
-      <c r="Z50" s="5"/>
-    </row>
-    <row r="51" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="D50" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" s="12">
+        <f>SUM(D13:D47)</f>
+        <v>-20</v>
+      </c>
+      <c r="G50" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H50" s="12">
+        <f>SUM(G13:G47)</f>
+        <v>10</v>
+      </c>
+      <c r="J50" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K50" s="12">
+        <f>SUM(J13:J47)</f>
+        <v>-97.5</v>
+      </c>
+      <c r="M50" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="N50" s="12">
+        <f>SUM(M13:M47)</f>
+        <v>200</v>
+      </c>
+      <c r="P50" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q50" s="12">
+        <f>SUM(P13:P47)</f>
+        <v>-55</v>
+      </c>
+      <c r="S50" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="T50" s="12">
+        <f>SUM(S13:S47)</f>
+        <v>-35</v>
+      </c>
+      <c r="V50" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="W50" s="12">
+        <f>SUM(V13:V47)</f>
+        <v>-2.5</v>
+      </c>
+      <c r="X50" s="1">
+        <f>SUM(E50,H50,K50,N50,Q50,T50,W50)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A51" s="5"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
-      <c r="H51" s="5"/>
-      <c r="I51" s="5"/>
-      <c r="J51" s="5"/>
-      <c r="K51" s="5"/>
-      <c r="L51" s="5"/>
-      <c r="M51" s="5"/>
-      <c r="N51" s="5"/>
-      <c r="O51" s="5"/>
-      <c r="P51" s="5"/>
-      <c r="Q51" s="5"/>
-      <c r="R51" s="5"/>
       <c r="S51" s="5"/>
       <c r="T51" s="5"/>
-      <c r="U51" s="5"/>
-      <c r="V51" s="5"/>
-      <c r="W51" s="5"/>
-      <c r="X51" s="5"/>
-      <c r="Y51" s="5"/>
-      <c r="Z51" s="5"/>
-    </row>
-    <row r="52" spans="2:26" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A52" s="5"/>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
-      <c r="H52" s="5"/>
-      <c r="I52" s="5"/>
-      <c r="J52" s="5"/>
-      <c r="K52" s="5"/>
-      <c r="L52" s="5"/>
-      <c r="M52" s="5"/>
-      <c r="N52" s="5"/>
-      <c r="O52" s="5"/>
-      <c r="P52" s="5"/>
-      <c r="Q52" s="5"/>
-      <c r="R52" s="5"/>
       <c r="S52" s="5"/>
       <c r="T52" s="5"/>
-      <c r="U52" s="5"/>
-      <c r="V52" s="5"/>
-      <c r="W52" s="5"/>
-      <c r="X52" s="5"/>
-      <c r="Y52" s="5"/>
-      <c r="Z52" s="5"/>
-    </row>
-    <row r="53" spans="2:26" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A53" s="5"/>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
@@ -3065,7 +3293,7 @@
       <c r="Y53" s="5"/>
       <c r="Z53" s="5"/>
     </row>
-    <row r="54" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
@@ -3092,15 +3320,15 @@
       <c r="Y54" s="5"/>
       <c r="Z54" s="5"/>
     </row>
-    <row r="55" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
-      <c r="F55" s="5"/>
-      <c r="G55" s="5"/>
-      <c r="H55" s="5"/>
-      <c r="I55" s="5"/>
+      <c r="E55" s="19"/>
+      <c r="F55" s="19"/>
+      <c r="G55" s="19"/>
+      <c r="H55" s="19"/>
+      <c r="I55" s="20"/>
       <c r="J55" s="5"/>
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
@@ -3119,15 +3347,15 @@
       <c r="Y55" s="5"/>
       <c r="Z55" s="5"/>
     </row>
-    <row r="56" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
-      <c r="E56" s="5"/>
-      <c r="F56" s="5"/>
-      <c r="G56" s="5"/>
-      <c r="H56" s="5"/>
-      <c r="I56" s="5"/>
+      <c r="E56" s="21"/>
+      <c r="F56" s="21"/>
+      <c r="G56" s="21"/>
+      <c r="H56" s="21"/>
+      <c r="I56" s="22"/>
       <c r="J56" s="5"/>
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
@@ -3146,15 +3374,15 @@
       <c r="Y56" s="5"/>
       <c r="Z56" s="5"/>
     </row>
-    <row r="57" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
+      <c r="D57" s="21"/>
       <c r="E57" s="5"/>
       <c r="F57" s="5"/>
       <c r="G57" s="5"/>
       <c r="H57" s="5"/>
-      <c r="I57" s="5"/>
+      <c r="I57" s="21"/>
       <c r="J57" s="5"/>
       <c r="K57" s="5"/>
       <c r="L57" s="5"/>
@@ -3173,15 +3401,15 @@
       <c r="Y57" s="5"/>
       <c r="Z57" s="5"/>
     </row>
-    <row r="58" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
+      <c r="D58" s="21"/>
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
       <c r="G58" s="5"/>
       <c r="H58" s="5"/>
-      <c r="I58" s="5"/>
+      <c r="I58" s="21"/>
       <c r="J58" s="5"/>
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
@@ -3200,15 +3428,15 @@
       <c r="Y58" s="5"/>
       <c r="Z58" s="5"/>
     </row>
-    <row r="59" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
+      <c r="D59" s="21"/>
       <c r="E59" s="5"/>
       <c r="F59" s="5"/>
       <c r="G59" s="5"/>
       <c r="H59" s="5"/>
-      <c r="I59" s="5"/>
+      <c r="I59" s="21"/>
       <c r="J59" s="5"/>
       <c r="K59" s="5"/>
       <c r="L59" s="5"/>
@@ -3227,15 +3455,15 @@
       <c r="Y59" s="5"/>
       <c r="Z59" s="5"/>
     </row>
-    <row r="60" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
+      <c r="D60" s="21"/>
       <c r="E60" s="5"/>
       <c r="F60" s="5"/>
       <c r="G60" s="5"/>
       <c r="H60" s="5"/>
-      <c r="I60" s="5"/>
+      <c r="I60" s="21"/>
       <c r="J60" s="5"/>
       <c r="K60" s="5"/>
       <c r="L60" s="5"/>
@@ -3254,15 +3482,15 @@
       <c r="Y60" s="5"/>
       <c r="Z60" s="5"/>
     </row>
-    <row r="61" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
+      <c r="D61" s="21"/>
       <c r="E61" s="5"/>
       <c r="F61" s="5"/>
       <c r="G61" s="5"/>
       <c r="H61" s="5"/>
-      <c r="I61" s="5"/>
+      <c r="I61" s="21"/>
       <c r="J61" s="5"/>
       <c r="K61" s="5"/>
       <c r="L61" s="5"/>
@@ -3281,15 +3509,15 @@
       <c r="Y61" s="5"/>
       <c r="Z61" s="5"/>
     </row>
-    <row r="62" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
+      <c r="D62" s="21"/>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
       <c r="G62" s="5"/>
       <c r="H62" s="5"/>
-      <c r="I62" s="5"/>
+      <c r="I62" s="21"/>
       <c r="J62" s="5"/>
       <c r="K62" s="5"/>
       <c r="L62" s="5"/>
@@ -3308,15 +3536,15 @@
       <c r="Y62" s="5"/>
       <c r="Z62" s="5"/>
     </row>
-    <row r="63" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
+      <c r="D63" s="21"/>
       <c r="E63" s="5"/>
       <c r="F63" s="5"/>
       <c r="G63" s="5"/>
       <c r="H63" s="5"/>
-      <c r="I63" s="5"/>
+      <c r="I63" s="21"/>
       <c r="J63" s="5"/>
       <c r="K63" s="5"/>
       <c r="L63" s="5"/>
@@ -3335,15 +3563,15 @@
       <c r="Y63" s="5"/>
       <c r="Z63" s="5"/>
     </row>
-    <row r="64" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
-      <c r="D64" s="5"/>
+      <c r="D64" s="21"/>
       <c r="E64" s="5"/>
       <c r="F64" s="5"/>
       <c r="G64" s="5"/>
       <c r="H64" s="5"/>
-      <c r="I64" s="5"/>
+      <c r="I64" s="21"/>
       <c r="J64" s="5"/>
       <c r="K64" s="5"/>
       <c r="L64" s="5"/>
@@ -3362,15 +3590,15 @@
       <c r="Y64" s="5"/>
       <c r="Z64" s="5"/>
     </row>
-    <row r="65" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
-      <c r="D65" s="5"/>
+      <c r="D65" s="21"/>
       <c r="E65" s="5"/>
       <c r="F65" s="5"/>
       <c r="G65" s="5"/>
       <c r="H65" s="5"/>
-      <c r="I65" s="5"/>
+      <c r="I65" s="21"/>
       <c r="J65" s="5"/>
       <c r="K65" s="5"/>
       <c r="L65" s="5"/>
@@ -3416,6 +3644,411 @@
       <c r="Y66" s="5"/>
       <c r="Z66" s="5"/>
     </row>
+    <row r="67" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="5"/>
+      <c r="G67" s="5"/>
+      <c r="H67" s="5"/>
+      <c r="I67" s="5"/>
+      <c r="J67" s="5"/>
+      <c r="K67" s="5"/>
+      <c r="L67" s="5"/>
+      <c r="M67" s="5"/>
+      <c r="N67" s="5"/>
+      <c r="O67" s="5"/>
+      <c r="P67" s="5"/>
+      <c r="Q67" s="5"/>
+      <c r="R67" s="5"/>
+      <c r="S67" s="5"/>
+      <c r="T67" s="5"/>
+      <c r="U67" s="5"/>
+      <c r="V67" s="5"/>
+      <c r="W67" s="5"/>
+      <c r="X67" s="5"/>
+      <c r="Y67" s="5"/>
+      <c r="Z67" s="5"/>
+    </row>
+    <row r="68" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B68" s="5"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
+      <c r="G68" s="5"/>
+      <c r="H68" s="5"/>
+      <c r="I68" s="5"/>
+      <c r="J68" s="5"/>
+      <c r="K68" s="5"/>
+      <c r="L68" s="5"/>
+      <c r="M68" s="5"/>
+      <c r="N68" s="5"/>
+      <c r="O68" s="5"/>
+      <c r="P68" s="5"/>
+      <c r="Q68" s="5"/>
+      <c r="R68" s="5"/>
+      <c r="S68" s="5"/>
+      <c r="T68" s="5"/>
+      <c r="U68" s="5"/>
+      <c r="V68" s="5"/>
+      <c r="W68" s="5"/>
+      <c r="X68" s="5"/>
+      <c r="Y68" s="5"/>
+      <c r="Z68" s="5"/>
+    </row>
+    <row r="69" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
+      <c r="G69" s="5"/>
+      <c r="H69" s="5"/>
+      <c r="I69" s="5"/>
+      <c r="J69" s="5"/>
+      <c r="K69" s="5"/>
+      <c r="L69" s="5"/>
+      <c r="M69" s="5"/>
+      <c r="N69" s="5"/>
+      <c r="O69" s="5"/>
+      <c r="P69" s="5"/>
+      <c r="Q69" s="5"/>
+      <c r="R69" s="5"/>
+      <c r="S69" s="5"/>
+      <c r="T69" s="5"/>
+      <c r="U69" s="5"/>
+      <c r="V69" s="5"/>
+      <c r="W69" s="5"/>
+      <c r="X69" s="5"/>
+      <c r="Y69" s="5"/>
+      <c r="Z69" s="5"/>
+    </row>
+    <row r="70" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5"/>
+      <c r="I70" s="5"/>
+      <c r="J70" s="5"/>
+      <c r="K70" s="5"/>
+      <c r="L70" s="5"/>
+      <c r="M70" s="5"/>
+      <c r="N70" s="5"/>
+      <c r="O70" s="5"/>
+      <c r="P70" s="5"/>
+      <c r="Q70" s="5"/>
+      <c r="R70" s="5"/>
+      <c r="S70" s="5"/>
+      <c r="T70" s="5"/>
+      <c r="U70" s="5"/>
+      <c r="V70" s="5"/>
+      <c r="W70" s="5"/>
+      <c r="X70" s="5"/>
+      <c r="Y70" s="5"/>
+      <c r="Z70" s="5"/>
+    </row>
+    <row r="71" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B71" s="5"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="5"/>
+      <c r="G71" s="5"/>
+      <c r="H71" s="5"/>
+      <c r="I71" s="5"/>
+      <c r="J71" s="5"/>
+      <c r="K71" s="5"/>
+      <c r="L71" s="5"/>
+      <c r="M71" s="5"/>
+      <c r="N71" s="5"/>
+      <c r="O71" s="5"/>
+      <c r="P71" s="5"/>
+      <c r="Q71" s="5"/>
+      <c r="R71" s="5"/>
+      <c r="S71" s="5"/>
+      <c r="T71" s="5"/>
+      <c r="U71" s="5"/>
+      <c r="V71" s="5"/>
+      <c r="W71" s="5"/>
+      <c r="X71" s="5"/>
+      <c r="Y71" s="5"/>
+      <c r="Z71" s="5"/>
+    </row>
+    <row r="72" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="5"/>
+      <c r="G72" s="5"/>
+      <c r="H72" s="5"/>
+      <c r="I72" s="5"/>
+      <c r="J72" s="5"/>
+      <c r="K72" s="5"/>
+      <c r="L72" s="5"/>
+      <c r="M72" s="5"/>
+      <c r="N72" s="5"/>
+      <c r="O72" s="5"/>
+      <c r="P72" s="5"/>
+      <c r="Q72" s="5"/>
+      <c r="R72" s="5"/>
+      <c r="S72" s="5"/>
+      <c r="T72" s="5"/>
+      <c r="U72" s="5"/>
+      <c r="V72" s="5"/>
+      <c r="W72" s="5"/>
+      <c r="X72" s="5"/>
+      <c r="Y72" s="5"/>
+      <c r="Z72" s="5"/>
+    </row>
+    <row r="73" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B73" s="5"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="5"/>
+      <c r="F73" s="5"/>
+      <c r="G73" s="5"/>
+      <c r="H73" s="5"/>
+      <c r="I73" s="5"/>
+      <c r="J73" s="5"/>
+      <c r="K73" s="5"/>
+      <c r="L73" s="5"/>
+      <c r="M73" s="5"/>
+      <c r="N73" s="5"/>
+      <c r="O73" s="5"/>
+      <c r="P73" s="5"/>
+      <c r="Q73" s="5"/>
+      <c r="R73" s="5"/>
+      <c r="S73" s="5"/>
+      <c r="T73" s="5"/>
+      <c r="U73" s="5"/>
+      <c r="V73" s="5"/>
+      <c r="W73" s="5"/>
+      <c r="X73" s="5"/>
+      <c r="Y73" s="5"/>
+      <c r="Z73" s="5"/>
+    </row>
+    <row r="74" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B74" s="5"/>
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
+      <c r="E74" s="5"/>
+      <c r="F74" s="5"/>
+      <c r="G74" s="5"/>
+      <c r="H74" s="5"/>
+      <c r="I74" s="5"/>
+      <c r="J74" s="5"/>
+      <c r="K74" s="5"/>
+      <c r="L74" s="5"/>
+      <c r="M74" s="5"/>
+      <c r="N74" s="5"/>
+      <c r="O74" s="5"/>
+      <c r="P74" s="5"/>
+      <c r="Q74" s="5"/>
+      <c r="R74" s="5"/>
+      <c r="S74" s="5"/>
+      <c r="T74" s="5"/>
+      <c r="U74" s="5"/>
+      <c r="V74" s="5"/>
+      <c r="W74" s="5"/>
+      <c r="X74" s="5"/>
+      <c r="Y74" s="5"/>
+      <c r="Z74" s="5"/>
+    </row>
+    <row r="75" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B75" s="5"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="5"/>
+      <c r="G75" s="5"/>
+      <c r="H75" s="5"/>
+      <c r="I75" s="5"/>
+      <c r="J75" s="5"/>
+      <c r="K75" s="5"/>
+      <c r="L75" s="5"/>
+      <c r="M75" s="5"/>
+      <c r="N75" s="5"/>
+      <c r="O75" s="5"/>
+      <c r="P75" s="5"/>
+      <c r="Q75" s="5"/>
+      <c r="R75" s="5"/>
+      <c r="S75" s="5"/>
+      <c r="T75" s="5"/>
+      <c r="U75" s="5"/>
+      <c r="V75" s="5"/>
+      <c r="W75" s="5"/>
+      <c r="X75" s="5"/>
+      <c r="Y75" s="5"/>
+      <c r="Z75" s="5"/>
+    </row>
+    <row r="76" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B76" s="5"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
+      <c r="E76" s="5"/>
+      <c r="F76" s="5"/>
+      <c r="G76" s="5"/>
+      <c r="H76" s="5"/>
+      <c r="I76" s="5"/>
+      <c r="J76" s="5"/>
+      <c r="K76" s="5"/>
+      <c r="L76" s="5"/>
+      <c r="M76" s="5"/>
+      <c r="N76" s="5"/>
+      <c r="O76" s="5"/>
+      <c r="P76" s="5"/>
+      <c r="Q76" s="5"/>
+      <c r="R76" s="5"/>
+      <c r="S76" s="5"/>
+      <c r="T76" s="5"/>
+      <c r="U76" s="5"/>
+      <c r="V76" s="5"/>
+      <c r="W76" s="5"/>
+      <c r="X76" s="5"/>
+      <c r="Y76" s="5"/>
+      <c r="Z76" s="5"/>
+    </row>
+    <row r="77" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B77" s="5"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
+      <c r="E77" s="5"/>
+      <c r="F77" s="5"/>
+      <c r="G77" s="5"/>
+      <c r="H77" s="5"/>
+      <c r="I77" s="5"/>
+      <c r="J77" s="5"/>
+      <c r="K77" s="5"/>
+      <c r="L77" s="5"/>
+      <c r="M77" s="5"/>
+      <c r="N77" s="5"/>
+      <c r="O77" s="5"/>
+      <c r="P77" s="5"/>
+      <c r="Q77" s="5"/>
+      <c r="R77" s="5"/>
+      <c r="S77" s="5"/>
+      <c r="T77" s="5"/>
+      <c r="U77" s="5"/>
+      <c r="V77" s="5"/>
+      <c r="W77" s="5"/>
+      <c r="X77" s="5"/>
+      <c r="Y77" s="5"/>
+      <c r="Z77" s="5"/>
+    </row>
+    <row r="78" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B78" s="5"/>
+      <c r="C78" s="5"/>
+      <c r="D78" s="5"/>
+      <c r="E78" s="5"/>
+      <c r="F78" s="5"/>
+      <c r="G78" s="5"/>
+      <c r="H78" s="5"/>
+      <c r="I78" s="5"/>
+      <c r="J78" s="5"/>
+      <c r="K78" s="5"/>
+      <c r="L78" s="5"/>
+      <c r="M78" s="5"/>
+      <c r="N78" s="5"/>
+      <c r="O78" s="5"/>
+      <c r="P78" s="5"/>
+      <c r="Q78" s="5"/>
+      <c r="R78" s="5"/>
+      <c r="S78" s="5"/>
+      <c r="T78" s="5"/>
+      <c r="U78" s="5"/>
+      <c r="V78" s="5"/>
+      <c r="W78" s="5"/>
+      <c r="X78" s="5"/>
+      <c r="Y78" s="5"/>
+      <c r="Z78" s="5"/>
+    </row>
+    <row r="79" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B79" s="5"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="5"/>
+      <c r="F79" s="5"/>
+      <c r="G79" s="5"/>
+      <c r="H79" s="5"/>
+      <c r="I79" s="5"/>
+      <c r="J79" s="5"/>
+      <c r="K79" s="5"/>
+      <c r="L79" s="5"/>
+      <c r="M79" s="5"/>
+      <c r="N79" s="5"/>
+      <c r="O79" s="5"/>
+      <c r="P79" s="5"/>
+      <c r="Q79" s="5"/>
+      <c r="R79" s="5"/>
+      <c r="S79" s="5"/>
+      <c r="T79" s="5"/>
+      <c r="U79" s="5"/>
+      <c r="V79" s="5"/>
+      <c r="W79" s="5"/>
+      <c r="X79" s="5"/>
+      <c r="Y79" s="5"/>
+      <c r="Z79" s="5"/>
+    </row>
+    <row r="80" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B80" s="5"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5"/>
+      <c r="F80" s="5"/>
+      <c r="G80" s="5"/>
+      <c r="H80" s="5"/>
+      <c r="I80" s="5"/>
+      <c r="J80" s="5"/>
+      <c r="K80" s="5"/>
+      <c r="L80" s="5"/>
+      <c r="M80" s="5"/>
+      <c r="N80" s="5"/>
+      <c r="O80" s="5"/>
+      <c r="P80" s="5"/>
+      <c r="Q80" s="5"/>
+      <c r="R80" s="5"/>
+      <c r="S80" s="5"/>
+      <c r="T80" s="5"/>
+      <c r="U80" s="5"/>
+      <c r="V80" s="5"/>
+      <c r="W80" s="5"/>
+      <c r="X80" s="5"/>
+      <c r="Y80" s="5"/>
+      <c r="Z80" s="5"/>
+    </row>
+    <row r="81" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B81" s="5"/>
+      <c r="C81" s="5"/>
+      <c r="D81" s="5"/>
+      <c r="E81" s="5"/>
+      <c r="F81" s="5"/>
+      <c r="G81" s="5"/>
+      <c r="H81" s="5"/>
+      <c r="I81" s="5"/>
+      <c r="J81" s="5"/>
+      <c r="K81" s="5"/>
+      <c r="L81" s="5"/>
+      <c r="M81" s="5"/>
+      <c r="N81" s="5"/>
+      <c r="O81" s="5"/>
+      <c r="P81" s="5"/>
+      <c r="Q81" s="5"/>
+      <c r="R81" s="5"/>
+      <c r="S81" s="5"/>
+      <c r="T81" s="5"/>
+      <c r="U81" s="5"/>
+      <c r="V81" s="5"/>
+      <c r="W81" s="5"/>
+      <c r="X81" s="5"/>
+      <c r="Y81" s="5"/>
+      <c r="Z81" s="5"/>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="9">
@@ -3427,82 +4060,82 @@
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="J11:K11"/>
     <mergeCell ref="M11:N11"/>
-    <mergeCell ref="E40:H40"/>
+    <mergeCell ref="E55:H55"/>
   </mergeCells>
-  <conditionalFormatting sqref="E35">
-    <cfRule type="cellIs" dxfId="29" priority="139" operator="lessThan">
+  <conditionalFormatting sqref="E50">
+    <cfRule type="cellIs" dxfId="47" priority="157" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="140" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="158" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="141" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="45" priority="159" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H35">
-    <cfRule type="cellIs" dxfId="26" priority="34" operator="lessThan">
+  <conditionalFormatting sqref="H50">
+    <cfRule type="cellIs" dxfId="17" priority="16" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="36" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="18" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K35">
-    <cfRule type="cellIs" dxfId="23" priority="31" operator="lessThan">
+  <conditionalFormatting sqref="K50">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="33" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N35">
-    <cfRule type="cellIs" dxfId="20" priority="28" operator="lessThan">
+  <conditionalFormatting sqref="N50">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q35">
-    <cfRule type="cellIs" dxfId="17" priority="25" operator="lessThan">
+  <conditionalFormatting sqref="Q50">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="27" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T35">
-    <cfRule type="cellIs" dxfId="11" priority="19" operator="lessThan">
+  <conditionalFormatting sqref="T50">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W35">
-    <cfRule type="cellIs" dxfId="8" priority="16" operator="lessThan">
+  <conditionalFormatting sqref="W50">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
contest 22 to 35 schedule.
</commit_message>
<xml_diff>
--- a/2022/EBE Boys 2022.xlsx
+++ b/2022/EBE Boys 2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD1B85EB-A1BE-624E-BA0C-83B44F078F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF35F956-29F7-7D44-A8FD-00AA6E927BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="520" windowWidth="35840" windowHeight="20420" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="58">
   <si>
     <t>Points</t>
   </si>
@@ -105,18 +105,36 @@
     <t>Supriser Lee</t>
   </si>
   <si>
+    <t>SRH vs KKR</t>
+  </si>
+  <si>
     <t>KKR vs MI</t>
   </si>
   <si>
     <t>RCB vs KKR</t>
   </si>
   <si>
+    <t>DC vs PBKS</t>
+  </si>
+  <si>
     <t>DC vs MI</t>
   </si>
   <si>
+    <t>PBKS vs SRH</t>
+  </si>
+  <si>
     <t>CheemsRajah</t>
   </si>
   <si>
+    <t>RR vs KKR</t>
+  </si>
+  <si>
+    <t>CSK vs RCB</t>
+  </si>
+  <si>
+    <t>DC vs RCB</t>
+  </si>
+  <si>
     <t>CSK vs SRH</t>
   </si>
   <si>
@@ -126,9 +144,15 @@
     <t>PBKS vs RCB</t>
   </si>
   <si>
+    <t>MI vs CSK</t>
+  </si>
+  <si>
     <t>JAYAGAN ARMY</t>
   </si>
   <si>
+    <t>DC vs RR</t>
+  </si>
+  <si>
     <t>CSK vs KKR</t>
   </si>
   <si>
@@ -141,6 +165,9 @@
     <t>KKR vs DC</t>
   </si>
   <si>
+    <t>MI vs PBKS</t>
+  </si>
+  <si>
     <t>RR vs RCB</t>
   </si>
   <si>
@@ -172,6 +199,21 @@
   </si>
   <si>
     <t>SRH vs GT</t>
+  </si>
+  <si>
+    <t>RR vs GT</t>
+  </si>
+  <si>
+    <t>MI vs LSG</t>
+  </si>
+  <si>
+    <t>GT vs CSK</t>
+  </si>
+  <si>
+    <t>LSG vs RCB</t>
+  </si>
+  <si>
+    <t>KKR vs GT</t>
   </si>
 </sst>
 </file>
@@ -1483,7 +1525,7 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="D11" s="18" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="E11" s="18"/>
       <c r="G11" s="16" t="s">
@@ -1495,7 +1537,7 @@
       </c>
       <c r="K11" s="17"/>
       <c r="M11" s="16" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="N11" s="17"/>
       <c r="P11" s="16" t="s">
@@ -1572,7 +1614,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="D13" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E13, ($W13,$T13,$Q13,$N13,$K13,$H13,$E13), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E13, ($W13,$T13,$Q13,$N13,$K13,$H13,$E13), 0),  $A$2:$B$10, 2, FALSE))</f>
@@ -1632,7 +1674,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D14" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E14, ($W14,$T14,$Q14,$N14,$K14,$H14,$E14), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E14, ($W14,$T14,$Q14,$N14,$K14,$H14,$E14), 0),  $A$2:$B$10, 2, FALSE))</f>
@@ -1692,7 +1734,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D15" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E15, ($W15,$T15,$Q15,$N15,$K15,$H15,$E15), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E15, ($W15,$T15,$Q15,$N15,$K15,$H15,$E15), 0),  $A$2:$B$10, 2, FALSE))</f>
@@ -1752,7 +1794,7 @@
         <v>1</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="D16" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E16, ($W16,$T16,$Q16,$N16,$K16,$H16,$E16), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E16, ($W16,$T16,$Q16,$N16,$K16,$H16,$E16), 0),  $A$2:$B$10, 2, FALSE))</f>
@@ -1812,7 +1854,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D17" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E17, ($W17,$T17,$Q17,$N17,$K17,$H17,$E17), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E17, ($W17,$T17,$Q17,$N17,$K17,$H17,$E17), 0),  $A$2:$B$10, 2, FALSE))</f>
@@ -1872,7 +1914,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D18" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E18, ($W18,$T18,$Q18,$N18,$K18,$H18,$E18), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E18, ($W18,$T18,$Q18,$N18,$K18,$H18,$E18), 0),  $A$2:$B$10, 2, FALSE))</f>
@@ -1932,7 +1974,7 @@
         <v>1</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D19" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E19, ($W19,$T19,$Q19,$N19,$K19,$H19,$E19), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E19, ($W19,$T19,$Q19,$N19,$K19,$H19,$E19), 0),  $A$2:$B$10, 2, FALSE))</f>
@@ -1992,7 +2034,7 @@
         <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D20" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E20, ($W20,$T20,$Q20,$N20,$K20,$H20,$E20), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E20, ($W20,$T20,$Q20,$N20,$K20,$H20,$E20), 0),  $A$2:$B$10, 2, FALSE))</f>
@@ -2052,7 +2094,7 @@
         <v>1</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D21" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E21, ($W21,$T21,$Q21,$N21,$K21,$H21,$E21), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E21, ($W21,$T21,$Q21,$N21,$K21,$H21,$E21), 0),  $A$2:$B$10, 2, FALSE))</f>
@@ -2112,7 +2154,7 @@
         <v>1</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="D22" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E22, ($W22,$T22,$Q22,$N22,$K22,$H22,$E22), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E22, ($W22,$T22,$Q22,$N22,$K22,$H22,$E22), 0),  $A$2:$B$10, 2, FALSE))</f>
@@ -2172,7 +2214,7 @@
         <v>1</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="D23" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E23, ($W23,$T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E23, ($W23,$T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$B$10, 2, FALSE))</f>
@@ -2232,7 +2274,7 @@
         <v>1</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="D24" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E24, ($W24,$T24,$Q24,$N24,$K24,$H24,$E24), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E24, ($W24,$T24,$Q24,$N24,$K24,$H24,$E24), 0),  $A$2:$B$10, 2, FALSE))</f>
@@ -2292,7 +2334,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="D25" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E25, ($W25,$T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E25, ($W25,$T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$B$10, 2, FALSE))</f>
@@ -2350,7 +2392,7 @@
         <v>1</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D26" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E26, ($W26,$T26,$Q26,$N26,$K26,$H26,$E26), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E26, ($W26,$T26,$Q26,$N26,$K26,$H26,$E26), 0),  $A$2:$B$10, 2, FALSE))</f>
@@ -2410,7 +2452,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D27" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E27, ($W27,$T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E27, ($W27,$T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$B$10, 2, FALSE))</f>
@@ -2470,7 +2512,7 @@
         <v>1</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D28" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E28, ($W28,$T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E28, ($W28,$T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$B$10, 2, FALSE))</f>
@@ -2530,7 +2572,7 @@
         <v>1</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D29" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E29, ($W29,$T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E29, ($W29,$T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$B$10, 2, FALSE))</f>
@@ -2590,7 +2632,7 @@
         <v>1</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D30" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E30, ($W30,$T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E30, ($W30,$T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$B$10, 2, FALSE))</f>
@@ -2650,7 +2692,7 @@
         <v>1</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D31" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E31, ($W31,$T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E31, ($W31,$T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$B$10, 2, FALSE))</f>
@@ -2710,7 +2752,7 @@
         <v>1</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="D32" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E32, ($W32,$T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E32, ($W32,$T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$B$10, 2, FALSE))</f>
@@ -2768,7 +2810,7 @@
         <v>1</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="D33" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E33, ($W33,$T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E33, ($W33,$T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$B$10, 2, FALSE))</f>
@@ -2824,294 +2866,644 @@
       <c r="A34" s="1">
         <v>22</v>
       </c>
-      <c r="B34" s="1"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="3"/>
+      <c r="B34" s="1">
+        <v>1</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E34, ($W34,$T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E34, ($W34,$T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="E34" s="1"/>
-      <c r="G34" s="3"/>
+      <c r="G34" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H34, ($W34,$T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H34, ($W34,$T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="H34" s="1"/>
-      <c r="J34" s="3"/>
+      <c r="J34" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K34, ($W34,$T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K34, ($W34,$T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="K34" s="1"/>
-      <c r="M34" s="3"/>
+      <c r="M34" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N34, ($W34,$T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N34, ($W34,$T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="N34" s="1"/>
-      <c r="P34" s="3"/>
+      <c r="P34" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q34, ($W34,$T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q34, ($W34,$T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q34" s="1"/>
-      <c r="S34" s="3"/>
+      <c r="S34" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T34, ($W34,$T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T34, ($W34,$T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="T34" s="1"/>
-      <c r="V34" s="3"/>
+      <c r="V34" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W34, ($W34,$T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W34, ($W34,$T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="W34" s="1"/>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
         <v>23</v>
       </c>
-      <c r="B35" s="1"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="3"/>
+      <c r="B35" s="1">
+        <v>1</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E35, ($W35,$T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E35, ($W35,$T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="E35" s="1"/>
-      <c r="G35" s="3"/>
+      <c r="G35" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H35, ($W35,$T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H35, ($W35,$T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="H35" s="1"/>
-      <c r="J35" s="3"/>
+      <c r="J35" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K35, ($W35,$T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K35, ($W35,$T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="K35" s="1"/>
-      <c r="M35" s="3"/>
+      <c r="M35" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N35, ($W35,$T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N35, ($W35,$T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="N35" s="1"/>
-      <c r="P35" s="3"/>
+      <c r="P35" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q35, ($W35,$T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q35, ($W35,$T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q35" s="1"/>
-      <c r="S35" s="3"/>
+      <c r="S35" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T35, ($W35,$T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T35, ($W35,$T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="T35" s="1"/>
-      <c r="V35" s="3"/>
+      <c r="V35" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W35, ($W35,$T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W35, ($W35,$T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="W35" s="1"/>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>24</v>
       </c>
-      <c r="B36" s="1"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="3"/>
+      <c r="B36" s="1">
+        <v>1</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D36" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E36, ($W36,$T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E36, ($W36,$T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="E36" s="1"/>
-      <c r="G36" s="3"/>
+      <c r="G36" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H36, ($W36,$T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H36, ($W36,$T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="H36" s="1"/>
-      <c r="J36" s="3"/>
+      <c r="J36" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K36, ($W36,$T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K36, ($W36,$T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="K36" s="1"/>
-      <c r="M36" s="3"/>
+      <c r="M36" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N36, ($W36,$T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N36, ($W36,$T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="N36" s="1"/>
-      <c r="P36" s="3"/>
+      <c r="P36" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q36, ($W36,$T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q36, ($W36,$T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q36" s="1"/>
-      <c r="S36" s="3"/>
+      <c r="S36" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T36, ($W36,$T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T36, ($W36,$T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="T36" s="1"/>
-      <c r="V36" s="3"/>
+      <c r="V36" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W36, ($W36,$T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W36, ($W36,$T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="W36" s="1"/>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
         <v>25</v>
       </c>
-      <c r="B37" s="1"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="3"/>
+      <c r="B37" s="1">
+        <v>1</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E37, ($W37,$T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E37, ($W37,$T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="E37" s="1"/>
-      <c r="G37" s="3"/>
+      <c r="G37" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H37, ($W37,$T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H37, ($W37,$T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="H37" s="1"/>
-      <c r="J37" s="3"/>
+      <c r="J37" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K37, ($W37,$T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K37, ($W37,$T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="K37" s="1"/>
-      <c r="M37" s="3"/>
+      <c r="M37" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N37, ($W37,$T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N37, ($W37,$T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="N37" s="1"/>
-      <c r="P37" s="3"/>
+      <c r="P37" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q37, ($W37,$T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q37, ($W37,$T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q37" s="1"/>
-      <c r="S37" s="3"/>
+      <c r="S37" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T37, ($W37,$T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T37, ($W37,$T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="T37" s="1"/>
-      <c r="V37" s="3"/>
+      <c r="V37" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W37, ($W37,$T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W37, ($W37,$T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="W37" s="1"/>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>26</v>
       </c>
-      <c r="B38" s="1"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="3"/>
+      <c r="B38" s="1">
+        <v>1</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D38" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E38, ($W38,$T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E38, ($W38,$T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="E38" s="1"/>
-      <c r="G38" s="3"/>
+      <c r="G38" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H38, ($W38,$T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H38, ($W38,$T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="H38" s="1"/>
-      <c r="J38" s="3"/>
+      <c r="J38" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K38, ($W38,$T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K38, ($W38,$T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="K38" s="1"/>
-      <c r="M38" s="3"/>
+      <c r="M38" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N38, ($W38,$T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N38, ($W38,$T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="N38" s="1"/>
-      <c r="P38" s="3"/>
+      <c r="P38" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q38, ($W38,$T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q38, ($W38,$T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q38" s="1"/>
-      <c r="S38" s="3"/>
+      <c r="S38" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T38, ($W38,$T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T38, ($W38,$T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="T38" s="1"/>
-      <c r="V38" s="3"/>
+      <c r="V38" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W38, ($W38,$T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W38, ($W38,$T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="W38" s="1"/>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
         <v>27</v>
       </c>
-      <c r="B39" s="1"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="3"/>
+      <c r="B39" s="1">
+        <v>1</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E39, ($W39,$T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E39, ($W39,$T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="E39" s="1"/>
-      <c r="G39" s="3"/>
+      <c r="G39" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H39, ($W39,$T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H39, ($W39,$T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="H39" s="1"/>
-      <c r="J39" s="3"/>
+      <c r="J39" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K39, ($W39,$T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K39, ($W39,$T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="K39" s="1"/>
-      <c r="M39" s="3"/>
+      <c r="M39" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N39, ($W39,$T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N39, ($W39,$T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="N39" s="1"/>
-      <c r="P39" s="3"/>
+      <c r="P39" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q39, ($W39,$T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q39, ($W39,$T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q39" s="1"/>
-      <c r="S39" s="3"/>
+      <c r="S39" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T39, ($W39,$T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T39, ($W39,$T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="T39" s="1"/>
-      <c r="V39" s="3"/>
+      <c r="V39" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W39, ($W39,$T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W39, ($W39,$T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="W39" s="1"/>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>28</v>
       </c>
-      <c r="B40" s="1"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="3"/>
+      <c r="B40" s="1">
+        <v>1</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D40" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E40, ($W40,$T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E40, ($W40,$T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="E40" s="1"/>
-      <c r="G40" s="3"/>
+      <c r="G40" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H40, ($W40,$T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H40, ($W40,$T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="H40" s="1"/>
-      <c r="J40" s="3"/>
+      <c r="J40" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K40, ($W40,$T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K40, ($W40,$T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="K40" s="1"/>
-      <c r="M40" s="3"/>
+      <c r="M40" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N40, ($W40,$T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N40, ($W40,$T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="N40" s="1"/>
-      <c r="P40" s="3"/>
+      <c r="P40" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q40, ($W40,$T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q40, ($W40,$T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q40" s="1"/>
-      <c r="S40" s="3"/>
+      <c r="S40" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T40, ($W40,$T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T40, ($W40,$T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="T40" s="1"/>
-      <c r="V40" s="3"/>
+      <c r="V40" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W40, ($W40,$T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W40, ($W40,$T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="W40" s="1"/>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A41" s="6">
         <v>29</v>
       </c>
-      <c r="B41" s="1"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="3"/>
+      <c r="B41" s="1">
+        <v>1</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D41" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E41, ($W41,$T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E41, ($W41,$T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="E41" s="1"/>
-      <c r="G41" s="3"/>
+      <c r="G41" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H41, ($W41,$T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H41, ($W41,$T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="H41" s="1"/>
-      <c r="J41" s="3"/>
+      <c r="J41" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K41, ($W41,$T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K41, ($W41,$T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="K41" s="1"/>
-      <c r="M41" s="3"/>
+      <c r="M41" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N41, ($W41,$T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N41, ($W41,$T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="N41" s="1"/>
-      <c r="P41" s="3"/>
+      <c r="P41" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q41, ($W41,$T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q41, ($W41,$T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q41" s="1"/>
-      <c r="S41" s="3"/>
+      <c r="S41" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T41, ($W41,$T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T41, ($W41,$T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="T41" s="1"/>
-      <c r="V41" s="3"/>
+      <c r="V41" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W41, ($W41,$T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W41, ($W41,$T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="W41" s="1"/>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>30</v>
       </c>
-      <c r="B42" s="1"/>
-      <c r="C42" s="15"/>
-      <c r="D42" s="3"/>
+      <c r="B42" s="1">
+        <v>1</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D42" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E42, ($W42,$T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E42, ($W42,$T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="E42" s="1"/>
-      <c r="G42" s="3"/>
+      <c r="G42" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H42, ($W42,$T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H42, ($W42,$T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="H42" s="1"/>
-      <c r="J42" s="3"/>
+      <c r="J42" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K42, ($W42,$T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K42, ($W42,$T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="K42" s="1"/>
-      <c r="M42" s="3"/>
+      <c r="M42" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N42, ($W42,$T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N42, ($W42,$T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="N42" s="1"/>
-      <c r="P42" s="3"/>
+      <c r="P42" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q42, ($W42,$T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q42, ($W42,$T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q42" s="1"/>
-      <c r="S42" s="3"/>
+      <c r="S42" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T42, ($W42,$T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T42, ($W42,$T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="T42" s="1"/>
-      <c r="V42" s="3"/>
+      <c r="V42" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W42, ($W42,$T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W42, ($W42,$T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="W42" s="1"/>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A43" s="6">
         <v>31</v>
       </c>
-      <c r="B43" s="1"/>
-      <c r="C43" s="15"/>
-      <c r="D43" s="3"/>
+      <c r="B43" s="1">
+        <v>1</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D43" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E43, ($W43,$T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E43, ($W43,$T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="E43" s="1"/>
-      <c r="G43" s="3"/>
+      <c r="G43" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H43, ($W43,$T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H43, ($W43,$T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="H43" s="1"/>
-      <c r="J43" s="3"/>
+      <c r="J43" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K43, ($W43,$T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K43, ($W43,$T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="K43" s="1"/>
-      <c r="M43" s="3"/>
+      <c r="M43" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N43, ($W43,$T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N43, ($W43,$T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="N43" s="1"/>
-      <c r="P43" s="3"/>
+      <c r="P43" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q43, ($W43,$T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q43, ($W43,$T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q43" s="1"/>
-      <c r="S43" s="3"/>
+      <c r="S43" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T43, ($W43,$T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T43, ($W43,$T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="T43" s="1"/>
-      <c r="V43" s="3"/>
+      <c r="V43" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W43, ($W43,$T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W43, ($W43,$T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="W43" s="1"/>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>32</v>
       </c>
-      <c r="B44" s="1"/>
-      <c r="C44" s="15"/>
-      <c r="D44" s="3"/>
+      <c r="B44" s="1">
+        <v>1</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D44" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E44, ($W44,$T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E44, ($W44,$T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="E44" s="1"/>
-      <c r="G44" s="3"/>
+      <c r="G44" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H44, ($W44,$T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H44, ($W44,$T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="H44" s="1"/>
-      <c r="J44" s="3"/>
+      <c r="J44" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K44, ($W44,$T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K44, ($W44,$T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="K44" s="1"/>
-      <c r="M44" s="3"/>
+      <c r="M44" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N44, ($W44,$T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N44, ($W44,$T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="N44" s="1"/>
-      <c r="P44" s="3"/>
+      <c r="P44" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q44, ($W44,$T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q44, ($W44,$T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q44" s="1"/>
-      <c r="S44" s="3"/>
+      <c r="S44" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T44, ($W44,$T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T44, ($W44,$T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="T44" s="1"/>
-      <c r="V44" s="3"/>
+      <c r="V44" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W44, ($W44,$T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W44, ($W44,$T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="W44" s="1"/>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A45" s="6">
         <v>33</v>
       </c>
-      <c r="B45" s="1"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="3"/>
+      <c r="B45" s="1">
+        <v>1</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D45" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E45, ($W45,$T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E45, ($W45,$T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="E45" s="1"/>
-      <c r="G45" s="3"/>
+      <c r="G45" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H45, ($W45,$T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H45, ($W45,$T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="H45" s="1"/>
-      <c r="J45" s="3"/>
+      <c r="J45" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K45, ($W45,$T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K45, ($W45,$T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="K45" s="1"/>
-      <c r="M45" s="3"/>
+      <c r="M45" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N45, ($W45,$T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N45, ($W45,$T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="N45" s="1"/>
-      <c r="P45" s="3"/>
+      <c r="P45" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q45, ($W45,$T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q45, ($W45,$T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q45" s="1"/>
-      <c r="S45" s="3"/>
+      <c r="S45" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T45, ($W45,$T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T45, ($W45,$T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="T45" s="1"/>
-      <c r="V45" s="3"/>
+      <c r="V45" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W45, ($W45,$T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W45, ($W45,$T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="W45" s="1"/>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>34</v>
       </c>
-      <c r="B46" s="1"/>
-      <c r="C46" s="15"/>
-      <c r="D46" s="3"/>
+      <c r="B46" s="1">
+        <v>1</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D46" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E46, ($W46,$T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E46, ($W46,$T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="E46" s="1"/>
-      <c r="G46" s="3"/>
+      <c r="G46" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H46, ($W46,$T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H46, ($W46,$T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="H46" s="1"/>
-      <c r="J46" s="3"/>
+      <c r="J46" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K46, ($W46,$T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K46, ($W46,$T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="K46" s="1"/>
-      <c r="M46" s="3"/>
+      <c r="M46" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N46, ($W46,$T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N46, ($W46,$T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="N46" s="1"/>
-      <c r="P46" s="3"/>
+      <c r="P46" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q46, ($W46,$T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q46, ($W46,$T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q46" s="1"/>
-      <c r="S46" s="3"/>
+      <c r="S46" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T46, ($W46,$T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T46, ($W46,$T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="T46" s="1"/>
-      <c r="V46" s="3"/>
+      <c r="V46" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W46, ($W46,$T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W46, ($W46,$T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="W46" s="1"/>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A47" s="6">
         <v>35</v>
       </c>
-      <c r="B47" s="1"/>
-      <c r="C47" s="15"/>
-      <c r="D47" s="3"/>
+      <c r="B47" s="1">
+        <v>1</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D47" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E47, ($W47,$T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E47, ($W47,$T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="E47" s="1"/>
-      <c r="G47" s="3"/>
+      <c r="G47" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H47, ($W47,$T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H47, ($W47,$T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="H47" s="1"/>
-      <c r="J47" s="3"/>
+      <c r="J47" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K47, ($W47,$T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K47, ($W47,$T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="K47" s="1"/>
-      <c r="M47" s="3"/>
+      <c r="M47" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N47, ($W47,$T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N47, ($W47,$T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="N47" s="1"/>
-      <c r="P47" s="3"/>
+      <c r="P47" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q47, ($W47,$T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q47, ($W47,$T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q47" s="1"/>
-      <c r="S47" s="3"/>
+      <c r="S47" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T47, ($W47,$T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T47, ($W47,$T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="T47" s="1"/>
-      <c r="V47" s="3"/>
+      <c r="V47" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W47, ($W47,$T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W47, ($W47,$T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="W47" s="1"/>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Contest 22 through 29.
</commit_message>
<xml_diff>
--- a/2022/EBE Boys 2022.xlsx
+++ b/2022/EBE Boys 2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF35F956-29F7-7D44-A8FD-00AA6E927BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2700FA1-4A9A-6A4E-97DA-E4441FBCFA00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="520" windowWidth="35840" windowHeight="20420" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20420" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -470,24 +470,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -516,283 +511,18 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent6" xfId="1" builtinId="50"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="48">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="21">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1321,7 +1051,7 @@
   <dimension ref="A1:Z81"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="11" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="X50" sqref="X50"/>
     </sheetView>
   </sheetViews>
@@ -1355,23 +1085,23 @@
         <v>50</v>
       </c>
       <c r="C2" s="5"/>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
-      <c r="U2" s="25"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="24"/>
     </row>
     <row r="3" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
@@ -1381,21 +1111,21 @@
         <v>20</v>
       </c>
       <c r="C3" s="5"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27"/>
-      <c r="Q3" s="27"/>
-      <c r="R3" s="27"/>
-      <c r="S3" s="27"/>
-      <c r="T3" s="27"/>
-      <c r="U3" s="28"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="26"/>
+      <c r="R3" s="26"/>
+      <c r="S3" s="26"/>
+      <c r="T3" s="26"/>
+      <c r="U3" s="27"/>
     </row>
     <row r="4" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
@@ -1405,21 +1135,21 @@
         <v>0</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
-      <c r="O4" s="27"/>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="27"/>
-      <c r="R4" s="27"/>
-      <c r="S4" s="27"/>
-      <c r="T4" s="27"/>
-      <c r="U4" s="28"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="26"/>
+      <c r="U4" s="27"/>
     </row>
     <row r="5" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
@@ -1429,21 +1159,21 @@
         <v>-10</v>
       </c>
       <c r="C5" s="5"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="27"/>
-      <c r="L5" s="27"/>
-      <c r="M5" s="27"/>
-      <c r="N5" s="27"/>
-      <c r="O5" s="27"/>
-      <c r="P5" s="27"/>
-      <c r="Q5" s="27"/>
-      <c r="R5" s="27"/>
-      <c r="S5" s="27"/>
-      <c r="T5" s="27"/>
-      <c r="U5" s="28"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="27"/>
     </row>
     <row r="6" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
@@ -1453,21 +1183,21 @@
         <v>-15</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="27"/>
-      <c r="N6" s="27"/>
-      <c r="O6" s="27"/>
-      <c r="P6" s="27"/>
-      <c r="Q6" s="27"/>
-      <c r="R6" s="27"/>
-      <c r="S6" s="27"/>
-      <c r="T6" s="27"/>
-      <c r="U6" s="28"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="26"/>
+      <c r="R6" s="26"/>
+      <c r="S6" s="26"/>
+      <c r="T6" s="26"/>
+      <c r="U6" s="27"/>
     </row>
     <row r="7" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
@@ -1477,45 +1207,45 @@
         <v>-20</v>
       </c>
       <c r="C7" s="5"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="27"/>
-      <c r="N7" s="27"/>
-      <c r="O7" s="27"/>
-      <c r="P7" s="27"/>
-      <c r="Q7" s="27"/>
-      <c r="R7" s="27"/>
-      <c r="S7" s="27"/>
-      <c r="T7" s="27"/>
-      <c r="U7" s="28"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="26"/>
+      <c r="O7" s="26"/>
+      <c r="P7" s="26"/>
+      <c r="Q7" s="26"/>
+      <c r="R7" s="26"/>
+      <c r="S7" s="26"/>
+      <c r="T7" s="26"/>
+      <c r="U7" s="27"/>
     </row>
     <row r="8" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>7</v>
       </c>
-      <c r="B8" s="32">
+      <c r="B8" s="19">
         <v>-25</v>
       </c>
       <c r="C8" s="5"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="30"/>
-      <c r="N8" s="30"/>
-      <c r="O8" s="30"/>
-      <c r="P8" s="30"/>
-      <c r="Q8" s="30"/>
-      <c r="R8" s="30"/>
-      <c r="S8" s="30"/>
-      <c r="T8" s="30"/>
-      <c r="U8" s="31"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="29"/>
+      <c r="Q8" s="29"/>
+      <c r="R8" s="29"/>
+      <c r="S8" s="29"/>
+      <c r="T8" s="29"/>
+      <c r="U8" s="30"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C9" s="5"/>
@@ -1524,34 +1254,34 @@
       <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="18"/>
-      <c r="G11" s="16" t="s">
+      <c r="E11" s="31"/>
+      <c r="G11" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="17"/>
-      <c r="J11" s="16" t="s">
+      <c r="H11" s="21"/>
+      <c r="J11" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="K11" s="17"/>
-      <c r="M11" s="16" t="s">
+      <c r="K11" s="21"/>
+      <c r="M11" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="N11" s="17"/>
-      <c r="P11" s="16" t="s">
+      <c r="N11" s="21"/>
+      <c r="P11" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="Q11" s="17"/>
-      <c r="S11" s="16" t="s">
+      <c r="Q11" s="21"/>
+      <c r="S11" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="T11" s="17"/>
-      <c r="V11" s="16" t="s">
+      <c r="T11" s="21"/>
+      <c r="V11" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="W11" s="17"/>
+      <c r="W11" s="21"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
@@ -2872,41 +2602,55 @@
       <c r="C34" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D34" s="3" t="str">
+      <c r="D34" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E34, ($W34,$T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E34, ($W34,$T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E34" s="1"/>
-      <c r="G34" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="E34" s="1">
+        <v>70</v>
+      </c>
+      <c r="G34" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H34, ($W34,$T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H34, ($W34,$T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H34" s="1"/>
-      <c r="J34" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="H34" s="1">
+        <v>40</v>
+      </c>
+      <c r="J34" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K34, ($W34,$T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K34, ($W34,$T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K34" s="1"/>
-      <c r="M34" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="K34" s="1">
+        <v>50</v>
+      </c>
+      <c r="M34" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N34, ($W34,$T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N34, ($W34,$T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N34" s="1"/>
-      <c r="P34" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="N34" s="1">
+        <v>80</v>
+      </c>
+      <c r="P34" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q34, ($W34,$T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q34, ($W34,$T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q34" s="1"/>
-      <c r="S34" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="Q34" s="1">
+        <v>100</v>
+      </c>
+      <c r="S34" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T34, ($W34,$T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T34, ($W34,$T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T34" s="1"/>
-      <c r="V34" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="T34" s="1">
+        <v>0</v>
+      </c>
+      <c r="V34" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W34, ($W34,$T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W34, ($W34,$T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W34" s="1"/>
+        <v>-10</v>
+      </c>
+      <c r="W34" s="1">
+        <v>60</v>
+      </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
@@ -2918,41 +2662,55 @@
       <c r="C35" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D35" s="3" t="str">
+      <c r="D35" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E35, ($W35,$T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E35, ($W35,$T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E35" s="1"/>
-      <c r="G35" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="E35" s="1">
+        <v>80</v>
+      </c>
+      <c r="G35" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H35, ($W35,$T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H35, ($W35,$T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H35" s="1"/>
-      <c r="J35" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="H35" s="1">
+        <v>50</v>
+      </c>
+      <c r="J35" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K35, ($W35,$T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K35, ($W35,$T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K35" s="1"/>
-      <c r="M35" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K35" s="1">
+        <v>60</v>
+      </c>
+      <c r="M35" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N35, ($W35,$T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N35, ($W35,$T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N35" s="1"/>
-      <c r="P35" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="N35" s="1">
+        <v>100</v>
+      </c>
+      <c r="P35" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q35, ($W35,$T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q35, ($W35,$T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q35" s="1"/>
-      <c r="S35" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="1">
+        <v>70</v>
+      </c>
+      <c r="S35" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T35, ($W35,$T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T35, ($W35,$T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T35" s="1"/>
-      <c r="V35" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="T35" s="1">
+        <v>0</v>
+      </c>
+      <c r="V35" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W35, ($W35,$T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W35, ($W35,$T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W35" s="1"/>
+        <v>-20</v>
+      </c>
+      <c r="W35" s="1">
+        <v>40</v>
+      </c>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
@@ -2964,41 +2722,55 @@
       <c r="C36" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D36" s="3" t="str">
+      <c r="D36" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E36, ($W36,$T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E36, ($W36,$T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E36" s="1"/>
-      <c r="G36" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="E36" s="1">
+        <v>60</v>
+      </c>
+      <c r="G36" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H36, ($W36,$T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H36, ($W36,$T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H36" s="1"/>
-      <c r="J36" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="H36" s="1">
+        <v>50</v>
+      </c>
+      <c r="J36" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K36, ($W36,$T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K36, ($W36,$T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K36" s="1"/>
-      <c r="M36" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="K36" s="1">
+        <v>80</v>
+      </c>
+      <c r="M36" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N36, ($W36,$T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N36, ($W36,$T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N36" s="1"/>
-      <c r="P36" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="N36" s="1">
+        <v>70</v>
+      </c>
+      <c r="P36" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q36, ($W36,$T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q36, ($W36,$T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q36" s="1"/>
-      <c r="S36" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="Q36" s="1">
+        <v>100</v>
+      </c>
+      <c r="S36" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T36, ($W36,$T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T36, ($W36,$T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T36" s="1"/>
-      <c r="V36" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="T36" s="1">
+        <v>40</v>
+      </c>
+      <c r="V36" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W36, ($W36,$T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W36, ($W36,$T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W36" s="1"/>
+        <v>-25</v>
+      </c>
+      <c r="W36" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
@@ -3010,41 +2782,55 @@
       <c r="C37" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D37" s="3" t="str">
+      <c r="D37" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E37, ($W37,$T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E37, ($W37,$T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E37" s="1"/>
-      <c r="G37" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="E37" s="1">
+        <v>80</v>
+      </c>
+      <c r="G37" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H37, ($W37,$T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H37, ($W37,$T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H37" s="1"/>
-      <c r="J37" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="H37" s="1">
+        <v>50</v>
+      </c>
+      <c r="J37" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K37, ($W37,$T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K37, ($W37,$T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K37" s="1"/>
-      <c r="M37" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="K37" s="1">
+        <v>40</v>
+      </c>
+      <c r="M37" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N37, ($W37,$T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N37, ($W37,$T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N37" s="1"/>
-      <c r="P37" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="N37" s="1">
+        <v>100</v>
+      </c>
+      <c r="P37" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q37, ($W37,$T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q37, ($W37,$T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q37" s="1"/>
-      <c r="S37" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="Q37" s="1">
+        <v>0</v>
+      </c>
+      <c r="S37" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T37, ($W37,$T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T37, ($W37,$T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T37" s="1"/>
-      <c r="V37" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="T37" s="1">
+        <v>60</v>
+      </c>
+      <c r="V37" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W37, ($W37,$T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W37, ($W37,$T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W37" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="W37" s="1">
+        <v>70</v>
+      </c>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
@@ -3056,41 +2842,53 @@
       <c r="C38" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D38" s="3" t="str">
+      <c r="D38" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E38, ($W38,$T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E38, ($W38,$T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E38" s="1"/>
-      <c r="G38" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="E38" s="1">
+        <v>60</v>
+      </c>
+      <c r="G38" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H38, ($W38,$T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H38, ($W38,$T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H38" s="1"/>
-      <c r="J38" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="H38" s="1">
+        <v>80</v>
+      </c>
+      <c r="J38" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K38, ($W38,$T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K38, ($W38,$T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K38" s="1"/>
-      <c r="M38" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(N38, ($W38,$T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N38, ($W38,$T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N38" s="1"/>
-      <c r="P38" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="K38" s="1">
+        <v>70</v>
+      </c>
+      <c r="M38" s="3">
+        <v>-22.5</v>
+      </c>
+      <c r="N38" s="1">
+        <v>40</v>
+      </c>
+      <c r="P38" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q38, ($W38,$T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q38, ($W38,$T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q38" s="1"/>
-      <c r="S38" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(T38, ($W38,$T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T38, ($W38,$T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T38" s="1"/>
-      <c r="V38" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="Q38" s="1">
+        <v>100</v>
+      </c>
+      <c r="S38" s="3">
+        <v>-22.5</v>
+      </c>
+      <c r="T38" s="1">
+        <v>40</v>
+      </c>
+      <c r="V38" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W38, ($W38,$T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W38, ($W38,$T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W38" s="1"/>
+        <v>-15</v>
+      </c>
+      <c r="W38" s="1">
+        <v>50</v>
+      </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
@@ -3102,41 +2900,55 @@
       <c r="C39" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D39" s="3" t="str">
+      <c r="D39" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E39, ($W39,$T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E39, ($W39,$T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E39" s="1"/>
-      <c r="G39" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="E39" s="1">
+        <v>70</v>
+      </c>
+      <c r="G39" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H39, ($W39,$T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H39, ($W39,$T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H39" s="1"/>
-      <c r="J39" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="H39" s="1">
+        <v>80</v>
+      </c>
+      <c r="J39" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K39, ($W39,$T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K39, ($W39,$T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K39" s="1"/>
-      <c r="M39" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="K39" s="1">
+        <v>40</v>
+      </c>
+      <c r="M39" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N39, ($W39,$T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N39, ($W39,$T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N39" s="1"/>
-      <c r="P39" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="N39" s="1">
+        <v>100</v>
+      </c>
+      <c r="P39" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q39, ($W39,$T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q39, ($W39,$T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q39" s="1"/>
-      <c r="S39" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="Q39" s="1">
+        <v>0</v>
+      </c>
+      <c r="S39" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T39, ($W39,$T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T39, ($W39,$T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T39" s="1"/>
-      <c r="V39" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="T39" s="1">
+        <v>60</v>
+      </c>
+      <c r="V39" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W39, ($W39,$T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W39, ($W39,$T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W39" s="1"/>
+        <v>-15</v>
+      </c>
+      <c r="W39" s="1">
+        <v>50</v>
+      </c>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
@@ -3148,41 +2960,55 @@
       <c r="C40" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D40" s="3" t="str">
+      <c r="D40" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E40, ($W40,$T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E40, ($W40,$T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E40" s="1"/>
-      <c r="G40" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="E40" s="1">
+        <v>60</v>
+      </c>
+      <c r="G40" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H40, ($W40,$T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H40, ($W40,$T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H40" s="1"/>
-      <c r="J40" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="H40" s="1">
+        <v>100</v>
+      </c>
+      <c r="J40" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K40, ($W40,$T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K40, ($W40,$T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K40" s="1"/>
-      <c r="M40" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="K40" s="1">
+        <v>70</v>
+      </c>
+      <c r="M40" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N40, ($W40,$T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N40, ($W40,$T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N40" s="1"/>
-      <c r="P40" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="N40" s="1">
+        <v>50</v>
+      </c>
+      <c r="P40" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q40, ($W40,$T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q40, ($W40,$T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q40" s="1"/>
-      <c r="S40" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="Q40" s="1">
+        <v>80</v>
+      </c>
+      <c r="S40" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T40, ($W40,$T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T40, ($W40,$T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T40" s="1"/>
-      <c r="V40" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="T40" s="1">
+        <v>40</v>
+      </c>
+      <c r="V40" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W40, ($W40,$T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W40, ($W40,$T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W40" s="1"/>
+        <v>-25</v>
+      </c>
+      <c r="W40" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A41" s="6">
@@ -3194,41 +3020,55 @@
       <c r="C41" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="D41" s="3" t="str">
+      <c r="D41" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E41, ($W41,$T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E41, ($W41,$T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E41" s="1"/>
-      <c r="G41" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="E41" s="1">
+        <v>0</v>
+      </c>
+      <c r="G41" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H41, ($W41,$T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H41, ($W41,$T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H41" s="1"/>
-      <c r="J41" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="H41" s="1">
+        <v>70</v>
+      </c>
+      <c r="J41" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K41, ($W41,$T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K41, ($W41,$T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K41" s="1"/>
-      <c r="M41" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="K41" s="1">
+        <v>80</v>
+      </c>
+      <c r="M41" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N41, ($W41,$T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N41, ($W41,$T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N41" s="1"/>
-      <c r="P41" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="N41" s="1">
+        <v>60</v>
+      </c>
+      <c r="P41" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q41, ($W41,$T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q41, ($W41,$T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q41" s="1"/>
-      <c r="S41" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="Q41" s="1">
+        <v>40</v>
+      </c>
+      <c r="S41" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T41, ($W41,$T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T41, ($W41,$T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T41" s="1"/>
-      <c r="V41" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="T41" s="1">
+        <v>100</v>
+      </c>
+      <c r="V41" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W41, ($W41,$T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W41, ($W41,$T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W41" s="1"/>
+        <v>-15</v>
+      </c>
+      <c r="W41" s="1">
+        <v>50</v>
+      </c>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
@@ -3590,49 +3430,49 @@
       </c>
       <c r="E50" s="12">
         <f>SUM(D13:D47)</f>
-        <v>-20</v>
+        <v>-35</v>
       </c>
       <c r="G50" s="7" t="s">
         <v>7</v>
       </c>
       <c r="H50" s="12">
         <f>SUM(G13:G47)</f>
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="J50" s="7" t="s">
         <v>7</v>
       </c>
       <c r="K50" s="12">
         <f>SUM(J13:J47)</f>
-        <v>-97.5</v>
+        <v>-122.5</v>
       </c>
       <c r="M50" s="7" t="s">
         <v>7</v>
       </c>
       <c r="N50" s="12">
         <f>SUM(M13:M47)</f>
-        <v>200</v>
+        <v>322.5</v>
       </c>
       <c r="P50" s="7" t="s">
         <v>7</v>
       </c>
       <c r="Q50" s="12">
         <f>SUM(P13:P47)</f>
-        <v>-55</v>
+        <v>45</v>
       </c>
       <c r="S50" s="7" t="s">
         <v>7</v>
       </c>
       <c r="T50" s="12">
         <f>SUM(S13:S47)</f>
-        <v>-35</v>
+        <v>-117.5</v>
       </c>
       <c r="V50" s="7" t="s">
         <v>7</v>
       </c>
       <c r="W50" s="12">
         <f>SUM(V13:V47)</f>
-        <v>-2.5</v>
+        <v>-127.5</v>
       </c>
       <c r="X50" s="1">
         <f>SUM(E50,H50,K50,N50,Q50,T50,W50)</f>
@@ -3716,11 +3556,11 @@
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
-      <c r="E55" s="19"/>
-      <c r="F55" s="19"/>
-      <c r="G55" s="19"/>
-      <c r="H55" s="19"/>
-      <c r="I55" s="20"/>
+      <c r="E55" s="32"/>
+      <c r="F55" s="32"/>
+      <c r="G55" s="32"/>
+      <c r="H55" s="32"/>
+      <c r="I55" s="16"/>
       <c r="J55" s="5"/>
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
@@ -3743,11 +3583,11 @@
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
-      <c r="E56" s="21"/>
-      <c r="F56" s="21"/>
-      <c r="G56" s="21"/>
-      <c r="H56" s="21"/>
-      <c r="I56" s="22"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
+      <c r="H56" s="17"/>
+      <c r="I56" s="18"/>
       <c r="J56" s="5"/>
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
@@ -3769,12 +3609,12 @@
     <row r="57" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
-      <c r="D57" s="21"/>
+      <c r="D57" s="17"/>
       <c r="E57" s="5"/>
       <c r="F57" s="5"/>
       <c r="G57" s="5"/>
       <c r="H57" s="5"/>
-      <c r="I57" s="21"/>
+      <c r="I57" s="17"/>
       <c r="J57" s="5"/>
       <c r="K57" s="5"/>
       <c r="L57" s="5"/>
@@ -3796,12 +3636,12 @@
     <row r="58" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
-      <c r="D58" s="21"/>
+      <c r="D58" s="17"/>
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
       <c r="G58" s="5"/>
       <c r="H58" s="5"/>
-      <c r="I58" s="21"/>
+      <c r="I58" s="17"/>
       <c r="J58" s="5"/>
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
@@ -3823,12 +3663,12 @@
     <row r="59" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
-      <c r="D59" s="21"/>
+      <c r="D59" s="17"/>
       <c r="E59" s="5"/>
       <c r="F59" s="5"/>
       <c r="G59" s="5"/>
       <c r="H59" s="5"/>
-      <c r="I59" s="21"/>
+      <c r="I59" s="17"/>
       <c r="J59" s="5"/>
       <c r="K59" s="5"/>
       <c r="L59" s="5"/>
@@ -3850,12 +3690,12 @@
     <row r="60" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
-      <c r="D60" s="21"/>
+      <c r="D60" s="17"/>
       <c r="E60" s="5"/>
       <c r="F60" s="5"/>
       <c r="G60" s="5"/>
       <c r="H60" s="5"/>
-      <c r="I60" s="21"/>
+      <c r="I60" s="17"/>
       <c r="J60" s="5"/>
       <c r="K60" s="5"/>
       <c r="L60" s="5"/>
@@ -3877,12 +3717,12 @@
     <row r="61" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
-      <c r="D61" s="21"/>
+      <c r="D61" s="17"/>
       <c r="E61" s="5"/>
       <c r="F61" s="5"/>
       <c r="G61" s="5"/>
       <c r="H61" s="5"/>
-      <c r="I61" s="21"/>
+      <c r="I61" s="17"/>
       <c r="J61" s="5"/>
       <c r="K61" s="5"/>
       <c r="L61" s="5"/>
@@ -3904,12 +3744,12 @@
     <row r="62" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
-      <c r="D62" s="21"/>
+      <c r="D62" s="17"/>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
       <c r="G62" s="5"/>
       <c r="H62" s="5"/>
-      <c r="I62" s="21"/>
+      <c r="I62" s="17"/>
       <c r="J62" s="5"/>
       <c r="K62" s="5"/>
       <c r="L62" s="5"/>
@@ -3931,12 +3771,12 @@
     <row r="63" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
-      <c r="D63" s="21"/>
+      <c r="D63" s="17"/>
       <c r="E63" s="5"/>
       <c r="F63" s="5"/>
       <c r="G63" s="5"/>
       <c r="H63" s="5"/>
-      <c r="I63" s="21"/>
+      <c r="I63" s="17"/>
       <c r="J63" s="5"/>
       <c r="K63" s="5"/>
       <c r="L63" s="5"/>
@@ -3958,12 +3798,12 @@
     <row r="64" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
-      <c r="D64" s="21"/>
+      <c r="D64" s="17"/>
       <c r="E64" s="5"/>
       <c r="F64" s="5"/>
       <c r="G64" s="5"/>
       <c r="H64" s="5"/>
-      <c r="I64" s="21"/>
+      <c r="I64" s="17"/>
       <c r="J64" s="5"/>
       <c r="K64" s="5"/>
       <c r="L64" s="5"/>
@@ -3985,12 +3825,12 @@
     <row r="65" spans="2:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
-      <c r="D65" s="21"/>
+      <c r="D65" s="17"/>
       <c r="E65" s="5"/>
       <c r="F65" s="5"/>
       <c r="G65" s="5"/>
       <c r="H65" s="5"/>
-      <c r="I65" s="21"/>
+      <c r="I65" s="17"/>
       <c r="J65" s="5"/>
       <c r="K65" s="5"/>
       <c r="L65" s="5"/>
@@ -4444,6 +4284,7 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="9">
+    <mergeCell ref="E55:H55"/>
     <mergeCell ref="P11:Q11"/>
     <mergeCell ref="S11:T11"/>
     <mergeCell ref="V11:W11"/>
@@ -4452,16 +4293,15 @@
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="J11:K11"/>
     <mergeCell ref="M11:N11"/>
-    <mergeCell ref="E55:H55"/>
   </mergeCells>
   <conditionalFormatting sqref="E50">
-    <cfRule type="cellIs" dxfId="47" priority="157" operator="lessThan">
+    <cfRule type="cellIs" dxfId="20" priority="157" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="158" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="158" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="159" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="159" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Results 30 through 37. Fill contest details 53.
</commit_message>
<xml_diff>
--- a/2022/EBE Boys 2022.xlsx
+++ b/2022/EBE Boys 2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2700FA1-4A9A-6A4E-97DA-E4441FBCFA00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B4DA4AC-38C6-5D41-B876-5018269C7760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20420" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="76">
   <si>
     <t>Points</t>
   </si>
@@ -214,6 +214,60 @@
   </si>
   <si>
     <t>KKR vs GT</t>
+  </si>
+  <si>
+    <t>RCB vs SRH</t>
+  </si>
+  <si>
+    <t>LSG vs MI</t>
+  </si>
+  <si>
+    <t>PBKS vs CSK</t>
+  </si>
+  <si>
+    <t>RCB vs RR</t>
+  </si>
+  <si>
+    <t>GT vs SRH</t>
+  </si>
+  <si>
+    <t>DC vs KKR</t>
+  </si>
+  <si>
+    <t>PBKS vs LSG</t>
+  </si>
+  <si>
+    <t>GT vs RCB</t>
+  </si>
+  <si>
+    <t>RR vs MI</t>
+  </si>
+  <si>
+    <t>DC vs LSG</t>
+  </si>
+  <si>
+    <t>SRH vs CSK</t>
+  </si>
+  <si>
+    <t>KKR vs RR</t>
+  </si>
+  <si>
+    <t>GT vs PBKS</t>
+  </si>
+  <si>
+    <t>RCB vs CSK</t>
+  </si>
+  <si>
+    <t>DC vs SRH</t>
+  </si>
+  <si>
+    <t>GT vs MI</t>
+  </si>
+  <si>
+    <t>PBKS vs RR</t>
+  </si>
+  <si>
+    <t>LSG vs KKR</t>
   </si>
 </sst>
 </file>
@@ -522,7 +576,367 @@
     <cellStyle name="20% - Accent6" xfId="1" builtinId="50"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="57">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1048,11 +1462,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
-  <dimension ref="A1:Z81"/>
+  <dimension ref="A1:Z99"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X50" sqref="X50"/>
+      <pane ySplit="11" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X68" sqref="X68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3080,41 +3494,55 @@
       <c r="C42" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D42" s="3" t="str">
+      <c r="D42" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E42, ($W42,$T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E42, ($W42,$T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E42" s="1"/>
-      <c r="G42" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="E42" s="1">
+        <v>70</v>
+      </c>
+      <c r="G42" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H42, ($W42,$T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H42, ($W42,$T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H42" s="1"/>
-      <c r="J42" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="H42" s="1">
+        <v>40</v>
+      </c>
+      <c r="J42" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K42, ($W42,$T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K42, ($W42,$T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K42" s="1"/>
-      <c r="M42" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="K42" s="1">
+        <v>100</v>
+      </c>
+      <c r="M42" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N42, ($W42,$T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N42, ($W42,$T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N42" s="1"/>
-      <c r="P42" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="N42" s="1">
+        <v>0</v>
+      </c>
+      <c r="P42" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q42, ($W42,$T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q42, ($W42,$T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q42" s="1"/>
-      <c r="S42" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="Q42" s="1">
+        <v>60</v>
+      </c>
+      <c r="S42" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T42, ($W42,$T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T42, ($W42,$T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T42" s="1"/>
-      <c r="V42" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="T42" s="1">
+        <v>80</v>
+      </c>
+      <c r="V42" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W42, ($W42,$T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W42, ($W42,$T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W42" s="1"/>
+        <v>-15</v>
+      </c>
+      <c r="W42" s="1">
+        <v>50</v>
+      </c>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A43" s="6">
@@ -3126,41 +3554,55 @@
       <c r="C43" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="D43" s="3" t="str">
+      <c r="D43" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E43, ($W43,$T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E43, ($W43,$T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E43" s="1"/>
-      <c r="G43" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="E43" s="1">
+        <v>0</v>
+      </c>
+      <c r="G43" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H43, ($W43,$T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H43, ($W43,$T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H43" s="1"/>
-      <c r="J43" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="H43" s="1">
+        <v>80</v>
+      </c>
+      <c r="J43" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K43, ($W43,$T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K43, ($W43,$T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K43" s="1"/>
-      <c r="M43" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K43" s="1">
+        <v>60</v>
+      </c>
+      <c r="M43" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N43, ($W43,$T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N43, ($W43,$T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N43" s="1"/>
-      <c r="P43" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="N43" s="1">
+        <v>40</v>
+      </c>
+      <c r="P43" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q43, ($W43,$T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q43, ($W43,$T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q43" s="1"/>
-      <c r="S43" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="1">
+        <v>70</v>
+      </c>
+      <c r="S43" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T43, ($W43,$T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T43, ($W43,$T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T43" s="1"/>
-      <c r="V43" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="T43" s="1">
+        <v>50</v>
+      </c>
+      <c r="V43" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W43, ($W43,$T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W43, ($W43,$T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W43" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="W43" s="1">
+        <v>100</v>
+      </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
@@ -3172,41 +3614,55 @@
       <c r="C44" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D44" s="3" t="str">
+      <c r="D44" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E44, ($W44,$T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E44, ($W44,$T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E44" s="1"/>
-      <c r="G44" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="E44" s="1">
+        <v>40</v>
+      </c>
+      <c r="G44" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H44, ($W44,$T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H44, ($W44,$T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H44" s="1"/>
-      <c r="J44" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="H44" s="1">
+        <v>70</v>
+      </c>
+      <c r="J44" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K44, ($W44,$T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K44, ($W44,$T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K44" s="1"/>
-      <c r="M44" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="K44" s="1">
+        <v>80</v>
+      </c>
+      <c r="M44" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N44, ($W44,$T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N44, ($W44,$T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N44" s="1"/>
-      <c r="P44" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="N44" s="1">
+        <v>60</v>
+      </c>
+      <c r="P44" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q44, ($W44,$T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q44, ($W44,$T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q44" s="1"/>
-      <c r="S44" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="Q44" s="1">
+        <v>0</v>
+      </c>
+      <c r="S44" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T44, ($W44,$T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T44, ($W44,$T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T44" s="1"/>
-      <c r="V44" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="T44" s="1">
+        <v>50</v>
+      </c>
+      <c r="V44" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W44, ($W44,$T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W44, ($W44,$T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W44" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="W44" s="1">
+        <v>100</v>
+      </c>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A45" s="6">
@@ -3218,41 +3674,55 @@
       <c r="C45" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D45" s="3" t="str">
+      <c r="D45" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E45, ($W45,$T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E45, ($W45,$T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E45" s="1"/>
-      <c r="G45" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="E45" s="1">
+        <v>60</v>
+      </c>
+      <c r="G45" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H45, ($W45,$T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H45, ($W45,$T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H45" s="1"/>
-      <c r="J45" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="H45" s="1">
+        <v>40</v>
+      </c>
+      <c r="J45" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K45, ($W45,$T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K45, ($W45,$T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K45" s="1"/>
-      <c r="M45" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="K45" s="1">
+        <v>50</v>
+      </c>
+      <c r="M45" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N45, ($W45,$T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N45, ($W45,$T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N45" s="1"/>
-      <c r="P45" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="N45" s="1">
+        <v>100</v>
+      </c>
+      <c r="P45" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q45, ($W45,$T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q45, ($W45,$T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q45" s="1"/>
-      <c r="S45" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="Q45" s="1">
+        <v>0</v>
+      </c>
+      <c r="S45" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T45, ($W45,$T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T45, ($W45,$T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T45" s="1"/>
-      <c r="V45" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="T45" s="1">
+        <v>70</v>
+      </c>
+      <c r="V45" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W45, ($W45,$T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W45, ($W45,$T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W45" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="W45" s="1">
+        <v>80</v>
+      </c>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
@@ -3264,41 +3734,53 @@
       <c r="C46" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D46" s="3" t="str">
+      <c r="D46" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E46, ($W46,$T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E46, ($W46,$T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E46" s="1"/>
-      <c r="G46" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="E46" s="1">
+        <v>40</v>
+      </c>
+      <c r="G46" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H46, ($W46,$T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H46, ($W46,$T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H46" s="1"/>
-      <c r="J46" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="H46" s="1">
+        <v>80</v>
+      </c>
+      <c r="J46" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K46, ($W46,$T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K46, ($W46,$T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K46" s="1"/>
-      <c r="M46" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(N46, ($W46,$T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N46, ($W46,$T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N46" s="1"/>
-      <c r="P46" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="K46" s="1">
+        <v>0</v>
+      </c>
+      <c r="M46" s="3">
+        <v>-5</v>
+      </c>
+      <c r="N46" s="1">
+        <v>70</v>
+      </c>
+      <c r="P46" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q46, ($W46,$T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q46, ($W46,$T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q46" s="1"/>
-      <c r="S46" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="Q46" s="1">
+        <v>100</v>
+      </c>
+      <c r="S46" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T46, ($W46,$T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T46, ($W46,$T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T46" s="1"/>
-      <c r="V46" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(W46, ($W46,$T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W46, ($W46,$T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W46" s="1"/>
+        <v>-15</v>
+      </c>
+      <c r="T46" s="1">
+        <v>50</v>
+      </c>
+      <c r="V46" s="3">
+        <v>-5</v>
+      </c>
+      <c r="W46" s="1">
+        <v>70</v>
+      </c>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A47" s="6">
@@ -3310,681 +3792,1065 @@
       <c r="C47" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="D47" s="3" t="str">
+      <c r="D47" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E47, ($W47,$T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E47, ($W47,$T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E47" s="1"/>
-      <c r="G47" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="E47" s="1">
+        <v>40</v>
+      </c>
+      <c r="G47" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H47, ($W47,$T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H47, ($W47,$T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H47" s="1"/>
-      <c r="J47" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="H47" s="1">
+        <v>80</v>
+      </c>
+      <c r="J47" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K47, ($W47,$T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K47, ($W47,$T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K47" s="1"/>
-      <c r="M47" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="K47" s="1">
+        <v>50</v>
+      </c>
+      <c r="M47" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N47, ($W47,$T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N47, ($W47,$T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N47" s="1"/>
-      <c r="P47" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="N47" s="1">
+        <v>70</v>
+      </c>
+      <c r="P47" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q47, ($W47,$T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q47, ($W47,$T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q47" s="1"/>
-      <c r="S47" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="Q47" s="1">
+        <v>100</v>
+      </c>
+      <c r="S47" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T47, ($W47,$T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T47, ($W47,$T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T47" s="1"/>
-      <c r="V47" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="T47" s="1">
+        <v>60</v>
+      </c>
+      <c r="V47" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W47, ($W47,$T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W47, ($W47,$T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W47" s="1"/>
+        <v>-25</v>
+      </c>
+      <c r="W47" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A48" s="6"/>
-      <c r="B48" s="1" t="s">
+      <c r="A48" s="6">
+        <v>36</v>
+      </c>
+      <c r="B48" s="1">
+        <v>1</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D48" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(E48, ($W48,$T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E48, ($W48,$T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-25</v>
+      </c>
+      <c r="E48" s="1">
+        <v>0</v>
+      </c>
+      <c r="G48" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(H48, ($W48,$T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H48, ($W48,$T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>50</v>
+      </c>
+      <c r="H48" s="1">
+        <v>100</v>
+      </c>
+      <c r="J48" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(K48, ($W48,$T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K48, ($W48,$T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-20</v>
+      </c>
+      <c r="K48" s="1">
+        <v>40</v>
+      </c>
+      <c r="M48" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(N48, ($W48,$T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N48, ($W48,$T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>20</v>
+      </c>
+      <c r="N48" s="1">
+        <v>80</v>
+      </c>
+      <c r="P48" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q48, ($W48,$T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q48, ($W48,$T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="Q48" s="1">
+        <v>70</v>
+      </c>
+      <c r="S48" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(T48, ($W48,$T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T48, ($W48,$T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-10</v>
+      </c>
+      <c r="T48" s="1">
+        <v>60</v>
+      </c>
+      <c r="V48" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(W48, ($W48,$T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W48, ($W48,$T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-15</v>
+      </c>
+      <c r="W48" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A49" s="6">
+        <v>37</v>
+      </c>
+      <c r="B49" s="1">
+        <v>1</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D49" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(E49, ($W49,$T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E49, ($W49,$T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>50</v>
+      </c>
+      <c r="E49" s="1">
+        <v>100</v>
+      </c>
+      <c r="G49" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(H49, ($W49,$T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H49, ($W49,$T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-20</v>
+      </c>
+      <c r="H49" s="1">
+        <v>40</v>
+      </c>
+      <c r="J49" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(K49, ($W49,$T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K49, ($W49,$T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-15</v>
+      </c>
+      <c r="K49" s="1">
+        <v>50</v>
+      </c>
+      <c r="M49" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(N49, ($W49,$T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N49, ($W49,$T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="N49" s="1">
+        <v>70</v>
+      </c>
+      <c r="P49" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q49, ($W49,$T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q49, ($W49,$T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>20</v>
+      </c>
+      <c r="Q49" s="1">
+        <v>80</v>
+      </c>
+      <c r="S49" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(T49, ($W49,$T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T49, ($W49,$T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-25</v>
+      </c>
+      <c r="T49" s="1">
+        <v>0</v>
+      </c>
+      <c r="V49" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(W49, ($W49,$T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W49, ($W49,$T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-10</v>
+      </c>
+      <c r="W49" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A50" s="6">
+        <v>38</v>
+      </c>
+      <c r="B50" s="1">
+        <v>1</v>
+      </c>
+      <c r="C50" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D50" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E50, ($W50,$T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E50, ($W50,$T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E50" s="1"/>
+      <c r="G50" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H50, ($W50,$T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H50, ($W50,$T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H50" s="1"/>
+      <c r="J50" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K50, ($W50,$T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K50, ($W50,$T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K50" s="1"/>
+      <c r="M50" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N50, ($W50,$T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N50, ($W50,$T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N50" s="1"/>
+      <c r="P50" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q50, ($W50,$T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q50, ($W50,$T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q50" s="1"/>
+      <c r="S50" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T50, ($W50,$T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T50, ($W50,$T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T50" s="1"/>
+      <c r="V50" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W50, ($W50,$T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W50, ($W50,$T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="W50" s="1"/>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A51" s="6">
+        <v>39</v>
+      </c>
+      <c r="B51" s="1">
+        <v>1</v>
+      </c>
+      <c r="C51" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D51" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E51, ($W51,$T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E51, ($W51,$T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E51" s="1"/>
+      <c r="G51" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H51, ($W51,$T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H51, ($W51,$T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H51" s="1"/>
+      <c r="J51" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K51, ($W51,$T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K51, ($W51,$T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K51" s="1"/>
+      <c r="M51" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N51, ($W51,$T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N51, ($W51,$T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N51" s="1"/>
+      <c r="P51" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q51, ($W51,$T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q51, ($W51,$T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q51" s="1"/>
+      <c r="S51" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T51, ($W51,$T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T51, ($W51,$T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T51" s="1"/>
+      <c r="V51" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W51, ($W51,$T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W51, ($W51,$T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="W51" s="1"/>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A52" s="6">
+        <v>40</v>
+      </c>
+      <c r="B52" s="1">
+        <v>1</v>
+      </c>
+      <c r="C52" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D52" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E52, ($W52,$T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E52, ($W52,$T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E52" s="1"/>
+      <c r="G52" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H52, ($W52,$T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H52, ($W52,$T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H52" s="1"/>
+      <c r="J52" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K52, ($W52,$T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K52, ($W52,$T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K52" s="1"/>
+      <c r="M52" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N52, ($W52,$T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N52, ($W52,$T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N52" s="1"/>
+      <c r="P52" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q52, ($W52,$T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q52, ($W52,$T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q52" s="1"/>
+      <c r="S52" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T52, ($W52,$T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T52, ($W52,$T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T52" s="1"/>
+      <c r="V52" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W52, ($W52,$T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W52, ($W52,$T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="W52" s="1"/>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A53" s="6">
+        <v>41</v>
+      </c>
+      <c r="B53" s="1">
+        <v>1</v>
+      </c>
+      <c r="C53" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D53" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E53, ($W53,$T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E53, ($W53,$T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E53" s="1"/>
+      <c r="G53" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H53, ($W53,$T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H53, ($W53,$T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H53" s="1"/>
+      <c r="J53" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K53, ($W53,$T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K53, ($W53,$T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K53" s="1"/>
+      <c r="M53" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N53, ($W53,$T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N53, ($W53,$T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N53" s="1"/>
+      <c r="P53" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q53, ($W53,$T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q53, ($W53,$T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q53" s="1"/>
+      <c r="S53" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T53, ($W53,$T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T53, ($W53,$T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T53" s="1"/>
+      <c r="V53" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W53, ($W53,$T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W53, ($W53,$T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="W53" s="1"/>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A54" s="6">
+        <v>42</v>
+      </c>
+      <c r="B54" s="1">
+        <v>1</v>
+      </c>
+      <c r="C54" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D54" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E54, ($W54,$T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E54, ($W54,$T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E54" s="1"/>
+      <c r="G54" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H54, ($W54,$T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H54, ($W54,$T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H54" s="1"/>
+      <c r="J54" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K54, ($W54,$T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K54, ($W54,$T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K54" s="1"/>
+      <c r="M54" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N54, ($W54,$T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N54, ($W54,$T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N54" s="1"/>
+      <c r="P54" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q54, ($W54,$T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q54, ($W54,$T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q54" s="1"/>
+      <c r="S54" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T54, ($W54,$T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T54, ($W54,$T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T54" s="1"/>
+      <c r="V54" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W54, ($W54,$T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W54, ($W54,$T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="W54" s="1"/>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A55" s="6">
+        <v>43</v>
+      </c>
+      <c r="B55" s="1">
+        <v>1</v>
+      </c>
+      <c r="C55" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="D55" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E55, ($W55,$T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E55, ($W55,$T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E55" s="1"/>
+      <c r="G55" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H55, ($W55,$T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H55, ($W55,$T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H55" s="1"/>
+      <c r="J55" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K55, ($W55,$T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K55, ($W55,$T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K55" s="1"/>
+      <c r="M55" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N55, ($W55,$T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N55, ($W55,$T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N55" s="1"/>
+      <c r="P55" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q55, ($W55,$T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q55, ($W55,$T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q55" s="1"/>
+      <c r="S55" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T55, ($W55,$T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T55, ($W55,$T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T55" s="1"/>
+      <c r="V55" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W55, ($W55,$T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W55, ($W55,$T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="W55" s="1"/>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A56" s="6">
+        <v>44</v>
+      </c>
+      <c r="B56" s="1">
+        <v>1</v>
+      </c>
+      <c r="C56" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D56" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E56, ($W56,$T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E56, ($W56,$T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E56" s="1"/>
+      <c r="G56" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H56, ($W56,$T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H56, ($W56,$T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H56" s="1"/>
+      <c r="J56" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K56, ($W56,$T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K56, ($W56,$T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K56" s="1"/>
+      <c r="M56" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N56, ($W56,$T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N56, ($W56,$T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N56" s="1"/>
+      <c r="P56" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q56, ($W56,$T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q56, ($W56,$T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q56" s="1"/>
+      <c r="S56" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T56, ($W56,$T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T56, ($W56,$T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T56" s="1"/>
+      <c r="V56" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W56, ($W56,$T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W56, ($W56,$T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="W56" s="1"/>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A57" s="6">
+        <v>45</v>
+      </c>
+      <c r="B57" s="1">
+        <v>1</v>
+      </c>
+      <c r="C57" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D57" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E57, ($W57,$T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E57, ($W57,$T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E57" s="1"/>
+      <c r="G57" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H57, ($W57,$T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H57, ($W57,$T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H57" s="1"/>
+      <c r="J57" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K57, ($W57,$T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K57, ($W57,$T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K57" s="1"/>
+      <c r="M57" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N57, ($W57,$T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N57, ($W57,$T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N57" s="1"/>
+      <c r="P57" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q57, ($W57,$T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q57, ($W57,$T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q57" s="1"/>
+      <c r="S57" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T57, ($W57,$T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T57, ($W57,$T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T57" s="1"/>
+      <c r="V57" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W57, ($W57,$T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W57, ($W57,$T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="W57" s="1"/>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A58" s="6">
+        <v>46</v>
+      </c>
+      <c r="B58" s="1">
+        <v>1</v>
+      </c>
+      <c r="C58" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D58" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E58, ($W58,$T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E58, ($W58,$T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E58" s="1"/>
+      <c r="G58" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H58, ($W58,$T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H58, ($W58,$T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H58" s="1"/>
+      <c r="J58" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K58, ($W58,$T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K58, ($W58,$T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K58" s="1"/>
+      <c r="M58" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N58, ($W58,$T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N58, ($W58,$T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N58" s="1"/>
+      <c r="P58" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q58, ($W58,$T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q58, ($W58,$T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q58" s="1"/>
+      <c r="S58" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T58, ($W58,$T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T58, ($W58,$T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T58" s="1"/>
+      <c r="V58" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W58, ($W58,$T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W58, ($W58,$T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="W58" s="1"/>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A59" s="6">
+        <v>47</v>
+      </c>
+      <c r="B59" s="1">
+        <v>1</v>
+      </c>
+      <c r="C59" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D59" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E59, ($W59,$T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E59, ($W59,$T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E59" s="1"/>
+      <c r="G59" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H59, ($W59,$T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H59, ($W59,$T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H59" s="1"/>
+      <c r="J59" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K59, ($W59,$T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K59, ($W59,$T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K59" s="1"/>
+      <c r="M59" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N59, ($W59,$T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N59, ($W59,$T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N59" s="1"/>
+      <c r="P59" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q59, ($W59,$T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q59, ($W59,$T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q59" s="1"/>
+      <c r="S59" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T59, ($W59,$T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T59, ($W59,$T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T59" s="1"/>
+      <c r="V59" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W59, ($W59,$T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W59, ($W59,$T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="W59" s="1"/>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A60" s="6">
+        <v>48</v>
+      </c>
+      <c r="B60" s="1">
+        <v>1</v>
+      </c>
+      <c r="C60" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D60" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E60, ($W60,$T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E60, ($W60,$T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E60" s="1"/>
+      <c r="G60" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H60, ($W60,$T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H60, ($W60,$T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H60" s="1"/>
+      <c r="J60" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K60, ($W60,$T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K60, ($W60,$T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K60" s="1"/>
+      <c r="M60" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N60, ($W60,$T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N60, ($W60,$T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N60" s="1"/>
+      <c r="P60" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q60, ($W60,$T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q60, ($W60,$T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q60" s="1"/>
+      <c r="S60" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T60, ($W60,$T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T60, ($W60,$T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T60" s="1"/>
+      <c r="V60" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W60, ($W60,$T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W60, ($W60,$T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="W60" s="1"/>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A61" s="6">
+        <v>49</v>
+      </c>
+      <c r="B61" s="1">
+        <v>1</v>
+      </c>
+      <c r="C61" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D61" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E61, ($W61,$T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E61, ($W61,$T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E61" s="1"/>
+      <c r="G61" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H61, ($W61,$T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H61, ($W61,$T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H61" s="1"/>
+      <c r="J61" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K61, ($W61,$T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K61, ($W61,$T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K61" s="1"/>
+      <c r="M61" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N61, ($W61,$T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N61, ($W61,$T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N61" s="1"/>
+      <c r="P61" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q61, ($W61,$T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q61, ($W61,$T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q61" s="1"/>
+      <c r="S61" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T61, ($W61,$T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T61, ($W61,$T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T61" s="1"/>
+      <c r="V61" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W61, ($W61,$T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W61, ($W61,$T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="W61" s="1"/>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A62" s="6">
+        <v>50</v>
+      </c>
+      <c r="B62" s="1">
+        <v>1</v>
+      </c>
+      <c r="C62" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="D62" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E62, ($W62,$T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E62, ($W62,$T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E62" s="1"/>
+      <c r="G62" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H62, ($W62,$T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H62, ($W62,$T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H62" s="1"/>
+      <c r="J62" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K62, ($W62,$T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K62, ($W62,$T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K62" s="1"/>
+      <c r="M62" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N62, ($W62,$T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N62, ($W62,$T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N62" s="1"/>
+      <c r="P62" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q62, ($W62,$T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q62, ($W62,$T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q62" s="1"/>
+      <c r="S62" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T62, ($W62,$T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T62, ($W62,$T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T62" s="1"/>
+      <c r="V62" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W62, ($W62,$T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W62, ($W62,$T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="W62" s="1"/>
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A63" s="6">
+        <v>51</v>
+      </c>
+      <c r="B63" s="1">
+        <v>1</v>
+      </c>
+      <c r="C63" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D63" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E63, ($W63,$T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E63, ($W63,$T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E63" s="1"/>
+      <c r="G63" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H63, ($W63,$T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H63, ($W63,$T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H63" s="1"/>
+      <c r="J63" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K63, ($W63,$T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K63, ($W63,$T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K63" s="1"/>
+      <c r="M63" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N63, ($W63,$T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N63, ($W63,$T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N63" s="1"/>
+      <c r="P63" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q63, ($W63,$T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q63, ($W63,$T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q63" s="1"/>
+      <c r="S63" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T63, ($W63,$T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T63, ($W63,$T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T63" s="1"/>
+      <c r="V63" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W63, ($W63,$T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W63, ($W63,$T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="W63" s="1"/>
+    </row>
+    <row r="64" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A64" s="6">
+        <v>52</v>
+      </c>
+      <c r="B64" s="1">
+        <v>1</v>
+      </c>
+      <c r="C64" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D64" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E64, ($W64,$T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E64, ($W64,$T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E64" s="1"/>
+      <c r="G64" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H64, ($W64,$T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H64, ($W64,$T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H64" s="1"/>
+      <c r="J64" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K64, ($W64,$T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K64, ($W64,$T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K64" s="1"/>
+      <c r="M64" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N64, ($W64,$T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N64, ($W64,$T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N64" s="1"/>
+      <c r="P64" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q64, ($W64,$T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q64, ($W64,$T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q64" s="1"/>
+      <c r="S64" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T64, ($W64,$T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T64, ($W64,$T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T64" s="1"/>
+      <c r="V64" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W64, ($W64,$T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W64, ($W64,$T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="W64" s="1"/>
+    </row>
+    <row r="65" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A65" s="6">
+        <v>53</v>
+      </c>
+      <c r="B65" s="1">
+        <v>1</v>
+      </c>
+      <c r="C65" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="D65" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E65" s="1"/>
+      <c r="G65" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H65" s="1"/>
+      <c r="J65" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K65" s="1"/>
+      <c r="M65" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N65" s="1"/>
+      <c r="P65" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q65" s="1"/>
+      <c r="S65" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T65" s="1"/>
+      <c r="V65" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="W65" s="1"/>
+    </row>
+    <row r="66" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A66" s="6"/>
+      <c r="B66" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C48" s="10"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="9" t="s">
+      <c r="C66" s="10"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G48" s="1"/>
-      <c r="H48" s="9" t="s">
+      <c r="G66" s="1"/>
+      <c r="H66" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J48" s="1"/>
-      <c r="K48" s="9" t="s">
+      <c r="J66" s="1"/>
+      <c r="K66" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="M48" s="1"/>
-      <c r="N48" s="9" t="s">
+      <c r="M66" s="1"/>
+      <c r="N66" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="P48" s="1"/>
-      <c r="Q48" s="9" t="s">
+      <c r="P66" s="1"/>
+      <c r="Q66" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="S48" s="1"/>
-      <c r="T48" s="9" t="s">
+      <c r="S66" s="1"/>
+      <c r="T66" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="V48" s="1"/>
-      <c r="W48" s="9" t="s">
+      <c r="V66" s="1"/>
+      <c r="W66" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A49" s="5"/>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="11" t="str">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A67" s="5"/>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="11" t="str">
         <f>D12</f>
         <v>Jaya</v>
       </c>
-      <c r="G49" s="1"/>
-      <c r="H49" s="11" t="str">
+      <c r="G67" s="1"/>
+      <c r="H67" s="11" t="str">
         <f>G12</f>
         <v>Justin</v>
       </c>
-      <c r="J49" s="1"/>
-      <c r="K49" s="11" t="str">
+      <c r="J67" s="1"/>
+      <c r="K67" s="11" t="str">
         <f>J12</f>
         <v>Ram</v>
       </c>
-      <c r="M49" s="1"/>
-      <c r="N49" s="11" t="str">
+      <c r="M67" s="1"/>
+      <c r="N67" s="11" t="str">
         <f>M12</f>
         <v>Sibi</v>
       </c>
-      <c r="P49" s="1"/>
-      <c r="Q49" s="11" t="str">
+      <c r="P67" s="1"/>
+      <c r="Q67" s="11" t="str">
         <f>P12</f>
         <v>Sundar</v>
       </c>
-      <c r="S49" s="1"/>
-      <c r="T49" s="11" t="str">
+      <c r="S67" s="1"/>
+      <c r="T67" s="11" t="str">
         <f>S12</f>
         <v>Upili</v>
       </c>
-      <c r="V49" s="1"/>
-      <c r="W49" s="11" t="str">
+      <c r="V67" s="1"/>
+      <c r="W67" s="11" t="str">
         <f>V12</f>
         <v>Vicky</v>
       </c>
     </row>
-    <row r="50" spans="1:26" ht="21" x14ac:dyDescent="0.25">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E50" s="12">
-        <f>SUM(D13:D47)</f>
-        <v>-35</v>
-      </c>
-      <c r="G50" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H50" s="12">
-        <f>SUM(G13:G47)</f>
-        <v>35</v>
-      </c>
-      <c r="J50" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="K50" s="12">
-        <f>SUM(J13:J47)</f>
-        <v>-122.5</v>
-      </c>
-      <c r="M50" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="N50" s="12">
-        <f>SUM(M13:M47)</f>
-        <v>322.5</v>
-      </c>
-      <c r="P50" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q50" s="12">
-        <f>SUM(P13:P47)</f>
-        <v>45</v>
-      </c>
-      <c r="S50" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="T50" s="12">
-        <f>SUM(S13:S47)</f>
-        <v>-117.5</v>
-      </c>
-      <c r="V50" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="W50" s="12">
-        <f>SUM(V13:V47)</f>
-        <v>-127.5</v>
-      </c>
-      <c r="X50" s="1">
-        <f>SUM(E50,H50,K50,N50,Q50,T50,W50)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A51" s="5"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
-      <c r="S51" s="5"/>
-      <c r="T51" s="5"/>
-    </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A52" s="5"/>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
-      <c r="S52" s="5"/>
-      <c r="T52" s="5"/>
-    </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A53" s="5"/>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5"/>
-      <c r="H53" s="5"/>
-      <c r="I53" s="5"/>
-      <c r="J53" s="5"/>
-      <c r="K53" s="5"/>
-      <c r="L53" s="5"/>
-      <c r="M53" s="5"/>
-      <c r="N53" s="5"/>
-      <c r="O53" s="5"/>
-      <c r="P53" s="5"/>
-      <c r="Q53" s="5"/>
-      <c r="R53" s="5"/>
-      <c r="S53" s="5"/>
-      <c r="T53" s="5"/>
-      <c r="U53" s="5"/>
-      <c r="V53" s="5"/>
-      <c r="W53" s="5"/>
-      <c r="X53" s="5"/>
-      <c r="Y53" s="5"/>
-      <c r="Z53" s="5"/>
-    </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
-      <c r="G54" s="5"/>
-      <c r="H54" s="5"/>
-      <c r="I54" s="5"/>
-      <c r="J54" s="5"/>
-      <c r="K54" s="5"/>
-      <c r="L54" s="5"/>
-      <c r="M54" s="5"/>
-      <c r="N54" s="5"/>
-      <c r="O54" s="5"/>
-      <c r="P54" s="5"/>
-      <c r="Q54" s="5"/>
-      <c r="R54" s="5"/>
-      <c r="S54" s="5"/>
-      <c r="T54" s="5"/>
-      <c r="U54" s="5"/>
-      <c r="V54" s="5"/>
-      <c r="W54" s="5"/>
-      <c r="X54" s="5"/>
-      <c r="Y54" s="5"/>
-      <c r="Z54" s="5"/>
-    </row>
-    <row r="55" spans="1:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="32"/>
-      <c r="F55" s="32"/>
-      <c r="G55" s="32"/>
-      <c r="H55" s="32"/>
-      <c r="I55" s="16"/>
-      <c r="J55" s="5"/>
-      <c r="K55" s="5"/>
-      <c r="L55" s="5"/>
-      <c r="M55" s="5"/>
-      <c r="N55" s="5"/>
-      <c r="O55" s="5"/>
-      <c r="P55" s="5"/>
-      <c r="Q55" s="5"/>
-      <c r="R55" s="5"/>
-      <c r="S55" s="5"/>
-      <c r="T55" s="5"/>
-      <c r="U55" s="5"/>
-      <c r="V55" s="5"/>
-      <c r="W55" s="5"/>
-      <c r="X55" s="5"/>
-      <c r="Y55" s="5"/>
-      <c r="Z55" s="5"/>
-    </row>
-    <row r="56" spans="1:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
-      <c r="E56" s="17"/>
-      <c r="F56" s="17"/>
-      <c r="G56" s="17"/>
-      <c r="H56" s="17"/>
-      <c r="I56" s="18"/>
-      <c r="J56" s="5"/>
-      <c r="K56" s="5"/>
-      <c r="L56" s="5"/>
-      <c r="M56" s="5"/>
-      <c r="N56" s="5"/>
-      <c r="O56" s="5"/>
-      <c r="P56" s="5"/>
-      <c r="Q56" s="5"/>
-      <c r="R56" s="5"/>
-      <c r="S56" s="5"/>
-      <c r="T56" s="5"/>
-      <c r="U56" s="5"/>
-      <c r="V56" s="5"/>
-      <c r="W56" s="5"/>
-      <c r="X56" s="5"/>
-      <c r="Y56" s="5"/>
-      <c r="Z56" s="5"/>
-    </row>
-    <row r="57" spans="1:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="17"/>
-      <c r="E57" s="5"/>
-      <c r="F57" s="5"/>
-      <c r="G57" s="5"/>
-      <c r="H57" s="5"/>
-      <c r="I57" s="17"/>
-      <c r="J57" s="5"/>
-      <c r="K57" s="5"/>
-      <c r="L57" s="5"/>
-      <c r="M57" s="5"/>
-      <c r="N57" s="5"/>
-      <c r="O57" s="5"/>
-      <c r="P57" s="5"/>
-      <c r="Q57" s="5"/>
-      <c r="R57" s="5"/>
-      <c r="S57" s="5"/>
-      <c r="T57" s="5"/>
-      <c r="U57" s="5"/>
-      <c r="V57" s="5"/>
-      <c r="W57" s="5"/>
-      <c r="X57" s="5"/>
-      <c r="Y57" s="5"/>
-      <c r="Z57" s="5"/>
-    </row>
-    <row r="58" spans="1:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="17"/>
-      <c r="E58" s="5"/>
-      <c r="F58" s="5"/>
-      <c r="G58" s="5"/>
-      <c r="H58" s="5"/>
-      <c r="I58" s="17"/>
-      <c r="J58" s="5"/>
-      <c r="K58" s="5"/>
-      <c r="L58" s="5"/>
-      <c r="M58" s="5"/>
-      <c r="N58" s="5"/>
-      <c r="O58" s="5"/>
-      <c r="P58" s="5"/>
-      <c r="Q58" s="5"/>
-      <c r="R58" s="5"/>
-      <c r="S58" s="5"/>
-      <c r="T58" s="5"/>
-      <c r="U58" s="5"/>
-      <c r="V58" s="5"/>
-      <c r="W58" s="5"/>
-      <c r="X58" s="5"/>
-      <c r="Y58" s="5"/>
-      <c r="Z58" s="5"/>
-    </row>
-    <row r="59" spans="1:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="17"/>
-      <c r="E59" s="5"/>
-      <c r="F59" s="5"/>
-      <c r="G59" s="5"/>
-      <c r="H59" s="5"/>
-      <c r="I59" s="17"/>
-      <c r="J59" s="5"/>
-      <c r="K59" s="5"/>
-      <c r="L59" s="5"/>
-      <c r="M59" s="5"/>
-      <c r="N59" s="5"/>
-      <c r="O59" s="5"/>
-      <c r="P59" s="5"/>
-      <c r="Q59" s="5"/>
-      <c r="R59" s="5"/>
-      <c r="S59" s="5"/>
-      <c r="T59" s="5"/>
-      <c r="U59" s="5"/>
-      <c r="V59" s="5"/>
-      <c r="W59" s="5"/>
-      <c r="X59" s="5"/>
-      <c r="Y59" s="5"/>
-      <c r="Z59" s="5"/>
-    </row>
-    <row r="60" spans="1:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="17"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="5"/>
-      <c r="G60" s="5"/>
-      <c r="H60" s="5"/>
-      <c r="I60" s="17"/>
-      <c r="J60" s="5"/>
-      <c r="K60" s="5"/>
-      <c r="L60" s="5"/>
-      <c r="M60" s="5"/>
-      <c r="N60" s="5"/>
-      <c r="O60" s="5"/>
-      <c r="P60" s="5"/>
-      <c r="Q60" s="5"/>
-      <c r="R60" s="5"/>
-      <c r="S60" s="5"/>
-      <c r="T60" s="5"/>
-      <c r="U60" s="5"/>
-      <c r="V60" s="5"/>
-      <c r="W60" s="5"/>
-      <c r="X60" s="5"/>
-      <c r="Y60" s="5"/>
-      <c r="Z60" s="5"/>
-    </row>
-    <row r="61" spans="1:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="B61" s="5"/>
-      <c r="C61" s="5"/>
-      <c r="D61" s="17"/>
-      <c r="E61" s="5"/>
-      <c r="F61" s="5"/>
-      <c r="G61" s="5"/>
-      <c r="H61" s="5"/>
-      <c r="I61" s="17"/>
-      <c r="J61" s="5"/>
-      <c r="K61" s="5"/>
-      <c r="L61" s="5"/>
-      <c r="M61" s="5"/>
-      <c r="N61" s="5"/>
-      <c r="O61" s="5"/>
-      <c r="P61" s="5"/>
-      <c r="Q61" s="5"/>
-      <c r="R61" s="5"/>
-      <c r="S61" s="5"/>
-      <c r="T61" s="5"/>
-      <c r="U61" s="5"/>
-      <c r="V61" s="5"/>
-      <c r="W61" s="5"/>
-      <c r="X61" s="5"/>
-      <c r="Y61" s="5"/>
-      <c r="Z61" s="5"/>
-    </row>
-    <row r="62" spans="1:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="B62" s="5"/>
-      <c r="C62" s="5"/>
-      <c r="D62" s="17"/>
-      <c r="E62" s="5"/>
-      <c r="F62" s="5"/>
-      <c r="G62" s="5"/>
-      <c r="H62" s="5"/>
-      <c r="I62" s="17"/>
-      <c r="J62" s="5"/>
-      <c r="K62" s="5"/>
-      <c r="L62" s="5"/>
-      <c r="M62" s="5"/>
-      <c r="N62" s="5"/>
-      <c r="O62" s="5"/>
-      <c r="P62" s="5"/>
-      <c r="Q62" s="5"/>
-      <c r="R62" s="5"/>
-      <c r="S62" s="5"/>
-      <c r="T62" s="5"/>
-      <c r="U62" s="5"/>
-      <c r="V62" s="5"/>
-      <c r="W62" s="5"/>
-      <c r="X62" s="5"/>
-      <c r="Y62" s="5"/>
-      <c r="Z62" s="5"/>
-    </row>
-    <row r="63" spans="1:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="17"/>
-      <c r="E63" s="5"/>
-      <c r="F63" s="5"/>
-      <c r="G63" s="5"/>
-      <c r="H63" s="5"/>
-      <c r="I63" s="17"/>
-      <c r="J63" s="5"/>
-      <c r="K63" s="5"/>
-      <c r="L63" s="5"/>
-      <c r="M63" s="5"/>
-      <c r="N63" s="5"/>
-      <c r="O63" s="5"/>
-      <c r="P63" s="5"/>
-      <c r="Q63" s="5"/>
-      <c r="R63" s="5"/>
-      <c r="S63" s="5"/>
-      <c r="T63" s="5"/>
-      <c r="U63" s="5"/>
-      <c r="V63" s="5"/>
-      <c r="W63" s="5"/>
-      <c r="X63" s="5"/>
-      <c r="Y63" s="5"/>
-      <c r="Z63" s="5"/>
-    </row>
-    <row r="64" spans="1:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="17"/>
-      <c r="E64" s="5"/>
-      <c r="F64" s="5"/>
-      <c r="G64" s="5"/>
-      <c r="H64" s="5"/>
-      <c r="I64" s="17"/>
-      <c r="J64" s="5"/>
-      <c r="K64" s="5"/>
-      <c r="L64" s="5"/>
-      <c r="M64" s="5"/>
-      <c r="N64" s="5"/>
-      <c r="O64" s="5"/>
-      <c r="P64" s="5"/>
-      <c r="Q64" s="5"/>
-      <c r="R64" s="5"/>
-      <c r="S64" s="5"/>
-      <c r="T64" s="5"/>
-      <c r="U64" s="5"/>
-      <c r="V64" s="5"/>
-      <c r="W64" s="5"/>
-      <c r="X64" s="5"/>
-      <c r="Y64" s="5"/>
-      <c r="Z64" s="5"/>
-    </row>
-    <row r="65" spans="2:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="B65" s="5"/>
-      <c r="C65" s="5"/>
-      <c r="D65" s="17"/>
-      <c r="E65" s="5"/>
-      <c r="F65" s="5"/>
-      <c r="G65" s="5"/>
-      <c r="H65" s="5"/>
-      <c r="I65" s="17"/>
-      <c r="J65" s="5"/>
-      <c r="K65" s="5"/>
-      <c r="L65" s="5"/>
-      <c r="M65" s="5"/>
-      <c r="N65" s="5"/>
-      <c r="O65" s="5"/>
-      <c r="P65" s="5"/>
-      <c r="Q65" s="5"/>
-      <c r="R65" s="5"/>
-      <c r="S65" s="5"/>
-      <c r="T65" s="5"/>
-      <c r="U65" s="5"/>
-      <c r="V65" s="5"/>
-      <c r="W65" s="5"/>
-      <c r="X65" s="5"/>
-      <c r="Y65" s="5"/>
-      <c r="Z65" s="5"/>
-    </row>
-    <row r="66" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="B66" s="5"/>
-      <c r="C66" s="5"/>
-      <c r="D66" s="5"/>
-      <c r="E66" s="5"/>
-      <c r="F66" s="5"/>
-      <c r="G66" s="5"/>
-      <c r="H66" s="5"/>
-      <c r="I66" s="5"/>
-      <c r="J66" s="5"/>
-      <c r="K66" s="5"/>
-      <c r="L66" s="5"/>
-      <c r="M66" s="5"/>
-      <c r="N66" s="5"/>
-      <c r="O66" s="5"/>
-      <c r="P66" s="5"/>
-      <c r="Q66" s="5"/>
-      <c r="R66" s="5"/>
-      <c r="S66" s="5"/>
-      <c r="T66" s="5"/>
-      <c r="U66" s="5"/>
-      <c r="V66" s="5"/>
-      <c r="W66" s="5"/>
-      <c r="X66" s="5"/>
-      <c r="Y66" s="5"/>
-      <c r="Z66" s="5"/>
-    </row>
-    <row r="67" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
-      <c r="E67" s="5"/>
-      <c r="F67" s="5"/>
-      <c r="G67" s="5"/>
-      <c r="H67" s="5"/>
-      <c r="I67" s="5"/>
-      <c r="J67" s="5"/>
-      <c r="K67" s="5"/>
-      <c r="L67" s="5"/>
-      <c r="M67" s="5"/>
-      <c r="N67" s="5"/>
-      <c r="O67" s="5"/>
-      <c r="P67" s="5"/>
-      <c r="Q67" s="5"/>
-      <c r="R67" s="5"/>
-      <c r="S67" s="5"/>
-      <c r="T67" s="5"/>
-      <c r="U67" s="5"/>
-      <c r="V67" s="5"/>
-      <c r="W67" s="5"/>
-      <c r="X67" s="5"/>
-      <c r="Y67" s="5"/>
-      <c r="Z67" s="5"/>
-    </row>
-    <row r="68" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:26" ht="21" x14ac:dyDescent="0.25">
+      <c r="A68" s="5"/>
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
-      <c r="D68" s="5"/>
-      <c r="E68" s="5"/>
-      <c r="F68" s="5"/>
-      <c r="G68" s="5"/>
-      <c r="H68" s="5"/>
-      <c r="I68" s="5"/>
-      <c r="J68" s="5"/>
-      <c r="K68" s="5"/>
-      <c r="L68" s="5"/>
-      <c r="M68" s="5"/>
-      <c r="N68" s="5"/>
-      <c r="O68" s="5"/>
-      <c r="P68" s="5"/>
-      <c r="Q68" s="5"/>
-      <c r="R68" s="5"/>
-      <c r="S68" s="5"/>
-      <c r="T68" s="5"/>
-      <c r="U68" s="5"/>
-      <c r="V68" s="5"/>
-      <c r="W68" s="5"/>
-      <c r="X68" s="5"/>
-      <c r="Y68" s="5"/>
-      <c r="Z68" s="5"/>
-    </row>
-    <row r="69" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="D68" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E68" s="12">
+        <f>SUM(D13:D65)</f>
+        <v>-105</v>
+      </c>
+      <c r="G68" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H68" s="12">
+        <f>SUM(G13:G65)</f>
+        <v>85</v>
+      </c>
+      <c r="J68" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K68" s="12">
+        <f>SUM(J13:J65)</f>
+        <v>-152.5</v>
+      </c>
+      <c r="M68" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="N68" s="12">
+        <f>SUM(M13:M65)</f>
+        <v>332.5</v>
+      </c>
+      <c r="P68" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q68" s="12">
+        <f>SUM(P13:P65)</f>
+        <v>105</v>
+      </c>
+      <c r="S68" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="T68" s="12">
+        <f>SUM(S13:S65)</f>
+        <v>-187.5</v>
+      </c>
+      <c r="V68" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="W68" s="12">
+        <f>SUM(V13:V65)</f>
+        <v>-77.5</v>
+      </c>
+      <c r="X68" s="1">
+        <f>SUM(E68,H68,K68,N68,Q68,T68,W68)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A69" s="5"/>
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
       <c r="E69" s="5"/>
-      <c r="F69" s="5"/>
-      <c r="G69" s="5"/>
-      <c r="H69" s="5"/>
-      <c r="I69" s="5"/>
-      <c r="J69" s="5"/>
-      <c r="K69" s="5"/>
-      <c r="L69" s="5"/>
-      <c r="M69" s="5"/>
-      <c r="N69" s="5"/>
-      <c r="O69" s="5"/>
-      <c r="P69" s="5"/>
-      <c r="Q69" s="5"/>
-      <c r="R69" s="5"/>
       <c r="S69" s="5"/>
       <c r="T69" s="5"/>
-      <c r="U69" s="5"/>
-      <c r="V69" s="5"/>
-      <c r="W69" s="5"/>
-      <c r="X69" s="5"/>
-      <c r="Y69" s="5"/>
-      <c r="Z69" s="5"/>
-    </row>
-    <row r="70" spans="2:26" x14ac:dyDescent="0.2">
+    </row>
+    <row r="70" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A70" s="5"/>
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
       <c r="E70" s="5"/>
-      <c r="F70" s="5"/>
-      <c r="G70" s="5"/>
-      <c r="H70" s="5"/>
-      <c r="I70" s="5"/>
-      <c r="J70" s="5"/>
-      <c r="K70" s="5"/>
-      <c r="L70" s="5"/>
-      <c r="M70" s="5"/>
-      <c r="N70" s="5"/>
-      <c r="O70" s="5"/>
-      <c r="P70" s="5"/>
-      <c r="Q70" s="5"/>
-      <c r="R70" s="5"/>
       <c r="S70" s="5"/>
       <c r="T70" s="5"/>
-      <c r="U70" s="5"/>
-      <c r="V70" s="5"/>
-      <c r="W70" s="5"/>
-      <c r="X70" s="5"/>
-      <c r="Y70" s="5"/>
-      <c r="Z70" s="5"/>
-    </row>
-    <row r="71" spans="2:26" x14ac:dyDescent="0.2">
+    </row>
+    <row r="71" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A71" s="5"/>
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
@@ -4011,7 +4877,7 @@
       <c r="Y71" s="5"/>
       <c r="Z71" s="5"/>
     </row>
-    <row r="72" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
@@ -4038,15 +4904,15 @@
       <c r="Y72" s="5"/>
       <c r="Z72" s="5"/>
     </row>
-    <row r="73" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
-      <c r="E73" s="5"/>
-      <c r="F73" s="5"/>
-      <c r="G73" s="5"/>
-      <c r="H73" s="5"/>
-      <c r="I73" s="5"/>
+      <c r="E73" s="32"/>
+      <c r="F73" s="32"/>
+      <c r="G73" s="32"/>
+      <c r="H73" s="32"/>
+      <c r="I73" s="16"/>
       <c r="J73" s="5"/>
       <c r="K73" s="5"/>
       <c r="L73" s="5"/>
@@ -4065,15 +4931,15 @@
       <c r="Y73" s="5"/>
       <c r="Z73" s="5"/>
     </row>
-    <row r="74" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
-      <c r="E74" s="5"/>
-      <c r="F74" s="5"/>
-      <c r="G74" s="5"/>
-      <c r="H74" s="5"/>
-      <c r="I74" s="5"/>
+      <c r="E74" s="17"/>
+      <c r="F74" s="17"/>
+      <c r="G74" s="17"/>
+      <c r="H74" s="17"/>
+      <c r="I74" s="18"/>
       <c r="J74" s="5"/>
       <c r="K74" s="5"/>
       <c r="L74" s="5"/>
@@ -4092,15 +4958,15 @@
       <c r="Y74" s="5"/>
       <c r="Z74" s="5"/>
     </row>
-    <row r="75" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
-      <c r="D75" s="5"/>
+      <c r="D75" s="17"/>
       <c r="E75" s="5"/>
       <c r="F75" s="5"/>
       <c r="G75" s="5"/>
       <c r="H75" s="5"/>
-      <c r="I75" s="5"/>
+      <c r="I75" s="17"/>
       <c r="J75" s="5"/>
       <c r="K75" s="5"/>
       <c r="L75" s="5"/>
@@ -4119,15 +4985,15 @@
       <c r="Y75" s="5"/>
       <c r="Z75" s="5"/>
     </row>
-    <row r="76" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
-      <c r="D76" s="5"/>
+      <c r="D76" s="17"/>
       <c r="E76" s="5"/>
       <c r="F76" s="5"/>
       <c r="G76" s="5"/>
       <c r="H76" s="5"/>
-      <c r="I76" s="5"/>
+      <c r="I76" s="17"/>
       <c r="J76" s="5"/>
       <c r="K76" s="5"/>
       <c r="L76" s="5"/>
@@ -4146,15 +5012,15 @@
       <c r="Y76" s="5"/>
       <c r="Z76" s="5"/>
     </row>
-    <row r="77" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
-      <c r="D77" s="5"/>
+      <c r="D77" s="17"/>
       <c r="E77" s="5"/>
       <c r="F77" s="5"/>
       <c r="G77" s="5"/>
       <c r="H77" s="5"/>
-      <c r="I77" s="5"/>
+      <c r="I77" s="17"/>
       <c r="J77" s="5"/>
       <c r="K77" s="5"/>
       <c r="L77" s="5"/>
@@ -4173,15 +5039,15 @@
       <c r="Y77" s="5"/>
       <c r="Z77" s="5"/>
     </row>
-    <row r="78" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B78" s="5"/>
       <c r="C78" s="5"/>
-      <c r="D78" s="5"/>
+      <c r="D78" s="17"/>
       <c r="E78" s="5"/>
       <c r="F78" s="5"/>
       <c r="G78" s="5"/>
       <c r="H78" s="5"/>
-      <c r="I78" s="5"/>
+      <c r="I78" s="17"/>
       <c r="J78" s="5"/>
       <c r="K78" s="5"/>
       <c r="L78" s="5"/>
@@ -4200,15 +5066,15 @@
       <c r="Y78" s="5"/>
       <c r="Z78" s="5"/>
     </row>
-    <row r="79" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
-      <c r="D79" s="5"/>
+      <c r="D79" s="17"/>
       <c r="E79" s="5"/>
       <c r="F79" s="5"/>
       <c r="G79" s="5"/>
       <c r="H79" s="5"/>
-      <c r="I79" s="5"/>
+      <c r="I79" s="17"/>
       <c r="J79" s="5"/>
       <c r="K79" s="5"/>
       <c r="L79" s="5"/>
@@ -4227,15 +5093,15 @@
       <c r="Y79" s="5"/>
       <c r="Z79" s="5"/>
     </row>
-    <row r="80" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
-      <c r="D80" s="5"/>
+      <c r="D80" s="17"/>
       <c r="E80" s="5"/>
       <c r="F80" s="5"/>
       <c r="G80" s="5"/>
       <c r="H80" s="5"/>
-      <c r="I80" s="5"/>
+      <c r="I80" s="17"/>
       <c r="J80" s="5"/>
       <c r="K80" s="5"/>
       <c r="L80" s="5"/>
@@ -4254,15 +5120,15 @@
       <c r="Y80" s="5"/>
       <c r="Z80" s="5"/>
     </row>
-    <row r="81" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B81" s="5"/>
       <c r="C81" s="5"/>
-      <c r="D81" s="5"/>
+      <c r="D81" s="17"/>
       <c r="E81" s="5"/>
       <c r="F81" s="5"/>
       <c r="G81" s="5"/>
       <c r="H81" s="5"/>
-      <c r="I81" s="5"/>
+      <c r="I81" s="17"/>
       <c r="J81" s="5"/>
       <c r="K81" s="5"/>
       <c r="L81" s="5"/>
@@ -4281,10 +5147,496 @@
       <c r="Y81" s="5"/>
       <c r="Z81" s="5"/>
     </row>
+    <row r="82" spans="2:26" ht="19" x14ac:dyDescent="0.25">
+      <c r="B82" s="5"/>
+      <c r="C82" s="5"/>
+      <c r="D82" s="17"/>
+      <c r="E82" s="5"/>
+      <c r="F82" s="5"/>
+      <c r="G82" s="5"/>
+      <c r="H82" s="5"/>
+      <c r="I82" s="17"/>
+      <c r="J82" s="5"/>
+      <c r="K82" s="5"/>
+      <c r="L82" s="5"/>
+      <c r="M82" s="5"/>
+      <c r="N82" s="5"/>
+      <c r="O82" s="5"/>
+      <c r="P82" s="5"/>
+      <c r="Q82" s="5"/>
+      <c r="R82" s="5"/>
+      <c r="S82" s="5"/>
+      <c r="T82" s="5"/>
+      <c r="U82" s="5"/>
+      <c r="V82" s="5"/>
+      <c r="W82" s="5"/>
+      <c r="X82" s="5"/>
+      <c r="Y82" s="5"/>
+      <c r="Z82" s="5"/>
+    </row>
+    <row r="83" spans="2:26" ht="19" x14ac:dyDescent="0.25">
+      <c r="B83" s="5"/>
+      <c r="C83" s="5"/>
+      <c r="D83" s="17"/>
+      <c r="E83" s="5"/>
+      <c r="F83" s="5"/>
+      <c r="G83" s="5"/>
+      <c r="H83" s="5"/>
+      <c r="I83" s="17"/>
+      <c r="J83" s="5"/>
+      <c r="K83" s="5"/>
+      <c r="L83" s="5"/>
+      <c r="M83" s="5"/>
+      <c r="N83" s="5"/>
+      <c r="O83" s="5"/>
+      <c r="P83" s="5"/>
+      <c r="Q83" s="5"/>
+      <c r="R83" s="5"/>
+      <c r="S83" s="5"/>
+      <c r="T83" s="5"/>
+      <c r="U83" s="5"/>
+      <c r="V83" s="5"/>
+      <c r="W83" s="5"/>
+      <c r="X83" s="5"/>
+      <c r="Y83" s="5"/>
+      <c r="Z83" s="5"/>
+    </row>
+    <row r="84" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B84" s="5"/>
+      <c r="C84" s="5"/>
+      <c r="D84" s="5"/>
+      <c r="E84" s="5"/>
+      <c r="F84" s="5"/>
+      <c r="G84" s="5"/>
+      <c r="H84" s="5"/>
+      <c r="I84" s="5"/>
+      <c r="J84" s="5"/>
+      <c r="K84" s="5"/>
+      <c r="L84" s="5"/>
+      <c r="M84" s="5"/>
+      <c r="N84" s="5"/>
+      <c r="O84" s="5"/>
+      <c r="P84" s="5"/>
+      <c r="Q84" s="5"/>
+      <c r="R84" s="5"/>
+      <c r="S84" s="5"/>
+      <c r="T84" s="5"/>
+      <c r="U84" s="5"/>
+      <c r="V84" s="5"/>
+      <c r="W84" s="5"/>
+      <c r="X84" s="5"/>
+      <c r="Y84" s="5"/>
+      <c r="Z84" s="5"/>
+    </row>
+    <row r="85" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B85" s="5"/>
+      <c r="C85" s="5"/>
+      <c r="D85" s="5"/>
+      <c r="E85" s="5"/>
+      <c r="F85" s="5"/>
+      <c r="G85" s="5"/>
+      <c r="H85" s="5"/>
+      <c r="I85" s="5"/>
+      <c r="J85" s="5"/>
+      <c r="K85" s="5"/>
+      <c r="L85" s="5"/>
+      <c r="M85" s="5"/>
+      <c r="N85" s="5"/>
+      <c r="O85" s="5"/>
+      <c r="P85" s="5"/>
+      <c r="Q85" s="5"/>
+      <c r="R85" s="5"/>
+      <c r="S85" s="5"/>
+      <c r="T85" s="5"/>
+      <c r="U85" s="5"/>
+      <c r="V85" s="5"/>
+      <c r="W85" s="5"/>
+      <c r="X85" s="5"/>
+      <c r="Y85" s="5"/>
+      <c r="Z85" s="5"/>
+    </row>
+    <row r="86" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B86" s="5"/>
+      <c r="C86" s="5"/>
+      <c r="D86" s="5"/>
+      <c r="E86" s="5"/>
+      <c r="F86" s="5"/>
+      <c r="G86" s="5"/>
+      <c r="H86" s="5"/>
+      <c r="I86" s="5"/>
+      <c r="J86" s="5"/>
+      <c r="K86" s="5"/>
+      <c r="L86" s="5"/>
+      <c r="M86" s="5"/>
+      <c r="N86" s="5"/>
+      <c r="O86" s="5"/>
+      <c r="P86" s="5"/>
+      <c r="Q86" s="5"/>
+      <c r="R86" s="5"/>
+      <c r="S86" s="5"/>
+      <c r="T86" s="5"/>
+      <c r="U86" s="5"/>
+      <c r="V86" s="5"/>
+      <c r="W86" s="5"/>
+      <c r="X86" s="5"/>
+      <c r="Y86" s="5"/>
+      <c r="Z86" s="5"/>
+    </row>
+    <row r="87" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B87" s="5"/>
+      <c r="C87" s="5"/>
+      <c r="D87" s="5"/>
+      <c r="E87" s="5"/>
+      <c r="F87" s="5"/>
+      <c r="G87" s="5"/>
+      <c r="H87" s="5"/>
+      <c r="I87" s="5"/>
+      <c r="J87" s="5"/>
+      <c r="K87" s="5"/>
+      <c r="L87" s="5"/>
+      <c r="M87" s="5"/>
+      <c r="N87" s="5"/>
+      <c r="O87" s="5"/>
+      <c r="P87" s="5"/>
+      <c r="Q87" s="5"/>
+      <c r="R87" s="5"/>
+      <c r="S87" s="5"/>
+      <c r="T87" s="5"/>
+      <c r="U87" s="5"/>
+      <c r="V87" s="5"/>
+      <c r="W87" s="5"/>
+      <c r="X87" s="5"/>
+      <c r="Y87" s="5"/>
+      <c r="Z87" s="5"/>
+    </row>
+    <row r="88" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B88" s="5"/>
+      <c r="C88" s="5"/>
+      <c r="D88" s="5"/>
+      <c r="E88" s="5"/>
+      <c r="F88" s="5"/>
+      <c r="G88" s="5"/>
+      <c r="H88" s="5"/>
+      <c r="I88" s="5"/>
+      <c r="J88" s="5"/>
+      <c r="K88" s="5"/>
+      <c r="L88" s="5"/>
+      <c r="M88" s="5"/>
+      <c r="N88" s="5"/>
+      <c r="O88" s="5"/>
+      <c r="P88" s="5"/>
+      <c r="Q88" s="5"/>
+      <c r="R88" s="5"/>
+      <c r="S88" s="5"/>
+      <c r="T88" s="5"/>
+      <c r="U88" s="5"/>
+      <c r="V88" s="5"/>
+      <c r="W88" s="5"/>
+      <c r="X88" s="5"/>
+      <c r="Y88" s="5"/>
+      <c r="Z88" s="5"/>
+    </row>
+    <row r="89" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B89" s="5"/>
+      <c r="C89" s="5"/>
+      <c r="D89" s="5"/>
+      <c r="E89" s="5"/>
+      <c r="F89" s="5"/>
+      <c r="G89" s="5"/>
+      <c r="H89" s="5"/>
+      <c r="I89" s="5"/>
+      <c r="J89" s="5"/>
+      <c r="K89" s="5"/>
+      <c r="L89" s="5"/>
+      <c r="M89" s="5"/>
+      <c r="N89" s="5"/>
+      <c r="O89" s="5"/>
+      <c r="P89" s="5"/>
+      <c r="Q89" s="5"/>
+      <c r="R89" s="5"/>
+      <c r="S89" s="5"/>
+      <c r="T89" s="5"/>
+      <c r="U89" s="5"/>
+      <c r="V89" s="5"/>
+      <c r="W89" s="5"/>
+      <c r="X89" s="5"/>
+      <c r="Y89" s="5"/>
+      <c r="Z89" s="5"/>
+    </row>
+    <row r="90" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B90" s="5"/>
+      <c r="C90" s="5"/>
+      <c r="D90" s="5"/>
+      <c r="E90" s="5"/>
+      <c r="F90" s="5"/>
+      <c r="G90" s="5"/>
+      <c r="H90" s="5"/>
+      <c r="I90" s="5"/>
+      <c r="J90" s="5"/>
+      <c r="K90" s="5"/>
+      <c r="L90" s="5"/>
+      <c r="M90" s="5"/>
+      <c r="N90" s="5"/>
+      <c r="O90" s="5"/>
+      <c r="P90" s="5"/>
+      <c r="Q90" s="5"/>
+      <c r="R90" s="5"/>
+      <c r="S90" s="5"/>
+      <c r="T90" s="5"/>
+      <c r="U90" s="5"/>
+      <c r="V90" s="5"/>
+      <c r="W90" s="5"/>
+      <c r="X90" s="5"/>
+      <c r="Y90" s="5"/>
+      <c r="Z90" s="5"/>
+    </row>
+    <row r="91" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B91" s="5"/>
+      <c r="C91" s="5"/>
+      <c r="D91" s="5"/>
+      <c r="E91" s="5"/>
+      <c r="F91" s="5"/>
+      <c r="G91" s="5"/>
+      <c r="H91" s="5"/>
+      <c r="I91" s="5"/>
+      <c r="J91" s="5"/>
+      <c r="K91" s="5"/>
+      <c r="L91" s="5"/>
+      <c r="M91" s="5"/>
+      <c r="N91" s="5"/>
+      <c r="O91" s="5"/>
+      <c r="P91" s="5"/>
+      <c r="Q91" s="5"/>
+      <c r="R91" s="5"/>
+      <c r="S91" s="5"/>
+      <c r="T91" s="5"/>
+      <c r="U91" s="5"/>
+      <c r="V91" s="5"/>
+      <c r="W91" s="5"/>
+      <c r="X91" s="5"/>
+      <c r="Y91" s="5"/>
+      <c r="Z91" s="5"/>
+    </row>
+    <row r="92" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B92" s="5"/>
+      <c r="C92" s="5"/>
+      <c r="D92" s="5"/>
+      <c r="E92" s="5"/>
+      <c r="F92" s="5"/>
+      <c r="G92" s="5"/>
+      <c r="H92" s="5"/>
+      <c r="I92" s="5"/>
+      <c r="J92" s="5"/>
+      <c r="K92" s="5"/>
+      <c r="L92" s="5"/>
+      <c r="M92" s="5"/>
+      <c r="N92" s="5"/>
+      <c r="O92" s="5"/>
+      <c r="P92" s="5"/>
+      <c r="Q92" s="5"/>
+      <c r="R92" s="5"/>
+      <c r="S92" s="5"/>
+      <c r="T92" s="5"/>
+      <c r="U92" s="5"/>
+      <c r="V92" s="5"/>
+      <c r="W92" s="5"/>
+      <c r="X92" s="5"/>
+      <c r="Y92" s="5"/>
+      <c r="Z92" s="5"/>
+    </row>
+    <row r="93" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B93" s="5"/>
+      <c r="C93" s="5"/>
+      <c r="D93" s="5"/>
+      <c r="E93" s="5"/>
+      <c r="F93" s="5"/>
+      <c r="G93" s="5"/>
+      <c r="H93" s="5"/>
+      <c r="I93" s="5"/>
+      <c r="J93" s="5"/>
+      <c r="K93" s="5"/>
+      <c r="L93" s="5"/>
+      <c r="M93" s="5"/>
+      <c r="N93" s="5"/>
+      <c r="O93" s="5"/>
+      <c r="P93" s="5"/>
+      <c r="Q93" s="5"/>
+      <c r="R93" s="5"/>
+      <c r="S93" s="5"/>
+      <c r="T93" s="5"/>
+      <c r="U93" s="5"/>
+      <c r="V93" s="5"/>
+      <c r="W93" s="5"/>
+      <c r="X93" s="5"/>
+      <c r="Y93" s="5"/>
+      <c r="Z93" s="5"/>
+    </row>
+    <row r="94" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B94" s="5"/>
+      <c r="C94" s="5"/>
+      <c r="D94" s="5"/>
+      <c r="E94" s="5"/>
+      <c r="F94" s="5"/>
+      <c r="G94" s="5"/>
+      <c r="H94" s="5"/>
+      <c r="I94" s="5"/>
+      <c r="J94" s="5"/>
+      <c r="K94" s="5"/>
+      <c r="L94" s="5"/>
+      <c r="M94" s="5"/>
+      <c r="N94" s="5"/>
+      <c r="O94" s="5"/>
+      <c r="P94" s="5"/>
+      <c r="Q94" s="5"/>
+      <c r="R94" s="5"/>
+      <c r="S94" s="5"/>
+      <c r="T94" s="5"/>
+      <c r="U94" s="5"/>
+      <c r="V94" s="5"/>
+      <c r="W94" s="5"/>
+      <c r="X94" s="5"/>
+      <c r="Y94" s="5"/>
+      <c r="Z94" s="5"/>
+    </row>
+    <row r="95" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B95" s="5"/>
+      <c r="C95" s="5"/>
+      <c r="D95" s="5"/>
+      <c r="E95" s="5"/>
+      <c r="F95" s="5"/>
+      <c r="G95" s="5"/>
+      <c r="H95" s="5"/>
+      <c r="I95" s="5"/>
+      <c r="J95" s="5"/>
+      <c r="K95" s="5"/>
+      <c r="L95" s="5"/>
+      <c r="M95" s="5"/>
+      <c r="N95" s="5"/>
+      <c r="O95" s="5"/>
+      <c r="P95" s="5"/>
+      <c r="Q95" s="5"/>
+      <c r="R95" s="5"/>
+      <c r="S95" s="5"/>
+      <c r="T95" s="5"/>
+      <c r="U95" s="5"/>
+      <c r="V95" s="5"/>
+      <c r="W95" s="5"/>
+      <c r="X95" s="5"/>
+      <c r="Y95" s="5"/>
+      <c r="Z95" s="5"/>
+    </row>
+    <row r="96" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B96" s="5"/>
+      <c r="C96" s="5"/>
+      <c r="D96" s="5"/>
+      <c r="E96" s="5"/>
+      <c r="F96" s="5"/>
+      <c r="G96" s="5"/>
+      <c r="H96" s="5"/>
+      <c r="I96" s="5"/>
+      <c r="J96" s="5"/>
+      <c r="K96" s="5"/>
+      <c r="L96" s="5"/>
+      <c r="M96" s="5"/>
+      <c r="N96" s="5"/>
+      <c r="O96" s="5"/>
+      <c r="P96" s="5"/>
+      <c r="Q96" s="5"/>
+      <c r="R96" s="5"/>
+      <c r="S96" s="5"/>
+      <c r="T96" s="5"/>
+      <c r="U96" s="5"/>
+      <c r="V96" s="5"/>
+      <c r="W96" s="5"/>
+      <c r="X96" s="5"/>
+      <c r="Y96" s="5"/>
+      <c r="Z96" s="5"/>
+    </row>
+    <row r="97" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B97" s="5"/>
+      <c r="C97" s="5"/>
+      <c r="D97" s="5"/>
+      <c r="E97" s="5"/>
+      <c r="F97" s="5"/>
+      <c r="G97" s="5"/>
+      <c r="H97" s="5"/>
+      <c r="I97" s="5"/>
+      <c r="J97" s="5"/>
+      <c r="K97" s="5"/>
+      <c r="L97" s="5"/>
+      <c r="M97" s="5"/>
+      <c r="N97" s="5"/>
+      <c r="O97" s="5"/>
+      <c r="P97" s="5"/>
+      <c r="Q97" s="5"/>
+      <c r="R97" s="5"/>
+      <c r="S97" s="5"/>
+      <c r="T97" s="5"/>
+      <c r="U97" s="5"/>
+      <c r="V97" s="5"/>
+      <c r="W97" s="5"/>
+      <c r="X97" s="5"/>
+      <c r="Y97" s="5"/>
+      <c r="Z97" s="5"/>
+    </row>
+    <row r="98" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B98" s="5"/>
+      <c r="C98" s="5"/>
+      <c r="D98" s="5"/>
+      <c r="E98" s="5"/>
+      <c r="F98" s="5"/>
+      <c r="G98" s="5"/>
+      <c r="H98" s="5"/>
+      <c r="I98" s="5"/>
+      <c r="J98" s="5"/>
+      <c r="K98" s="5"/>
+      <c r="L98" s="5"/>
+      <c r="M98" s="5"/>
+      <c r="N98" s="5"/>
+      <c r="O98" s="5"/>
+      <c r="P98" s="5"/>
+      <c r="Q98" s="5"/>
+      <c r="R98" s="5"/>
+      <c r="S98" s="5"/>
+      <c r="T98" s="5"/>
+      <c r="U98" s="5"/>
+      <c r="V98" s="5"/>
+      <c r="W98" s="5"/>
+      <c r="X98" s="5"/>
+      <c r="Y98" s="5"/>
+      <c r="Z98" s="5"/>
+    </row>
+    <row r="99" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B99" s="5"/>
+      <c r="C99" s="5"/>
+      <c r="D99" s="5"/>
+      <c r="E99" s="5"/>
+      <c r="F99" s="5"/>
+      <c r="G99" s="5"/>
+      <c r="H99" s="5"/>
+      <c r="I99" s="5"/>
+      <c r="J99" s="5"/>
+      <c r="K99" s="5"/>
+      <c r="L99" s="5"/>
+      <c r="M99" s="5"/>
+      <c r="N99" s="5"/>
+      <c r="O99" s="5"/>
+      <c r="P99" s="5"/>
+      <c r="Q99" s="5"/>
+      <c r="R99" s="5"/>
+      <c r="S99" s="5"/>
+      <c r="T99" s="5"/>
+      <c r="U99" s="5"/>
+      <c r="V99" s="5"/>
+      <c r="W99" s="5"/>
+      <c r="X99" s="5"/>
+      <c r="Y99" s="5"/>
+      <c r="Z99" s="5"/>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="9">
-    <mergeCell ref="E55:H55"/>
+    <mergeCell ref="E73:H73"/>
     <mergeCell ref="P11:Q11"/>
     <mergeCell ref="S11:T11"/>
     <mergeCell ref="V11:W11"/>
@@ -4294,18 +5646,18 @@
     <mergeCell ref="J11:K11"/>
     <mergeCell ref="M11:N11"/>
   </mergeCells>
-  <conditionalFormatting sqref="E50">
-    <cfRule type="cellIs" dxfId="20" priority="157" operator="lessThan">
+  <conditionalFormatting sqref="E68">
+    <cfRule type="cellIs" dxfId="56" priority="193" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="158" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="194" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="159" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="54" priority="195" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H50">
+  <conditionalFormatting sqref="H68">
     <cfRule type="cellIs" dxfId="17" priority="16" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -4316,7 +5668,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K50">
+  <conditionalFormatting sqref="K68">
     <cfRule type="cellIs" dxfId="14" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -4327,7 +5679,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N50">
+  <conditionalFormatting sqref="N68">
     <cfRule type="cellIs" dxfId="11" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -4338,7 +5690,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q50">
+  <conditionalFormatting sqref="Q68">
     <cfRule type="cellIs" dxfId="8" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -4349,7 +5701,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T50">
+  <conditionalFormatting sqref="T68">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -4360,7 +5712,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W50">
+  <conditionalFormatting sqref="W68">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -4380,7 +5732,7 @@
   <dimension ref="A18:A23"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G86" sqref="G86"/>
+      <selection activeCell="C1" sqref="A1:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Results contest 38 through 46.
</commit_message>
<xml_diff>
--- a/2022/EBE Boys 2022.xlsx
+++ b/2022/EBE Boys 2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B4DA4AC-38C6-5D41-B876-5018269C7760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9BE37BC-E907-4747-AEE4-014A6F66582A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20420" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -3972,41 +3972,55 @@
       <c r="C50" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="D50" s="3" t="str">
+      <c r="D50" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E50, ($W50,$T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E50, ($W50,$T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E50" s="1"/>
-      <c r="G50" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="E50" s="1">
+        <v>70</v>
+      </c>
+      <c r="G50" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H50, ($W50,$T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H50, ($W50,$T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H50" s="1"/>
-      <c r="J50" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="H50" s="1">
+        <v>80</v>
+      </c>
+      <c r="J50" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K50, ($W50,$T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K50, ($W50,$T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K50" s="1"/>
-      <c r="M50" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K50" s="1">
+        <v>60</v>
+      </c>
+      <c r="M50" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N50, ($W50,$T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N50, ($W50,$T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N50" s="1"/>
-      <c r="P50" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="N50" s="1">
+        <v>100</v>
+      </c>
+      <c r="P50" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q50, ($W50,$T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q50, ($W50,$T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q50" s="1"/>
-      <c r="S50" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="Q50" s="1">
+        <v>50</v>
+      </c>
+      <c r="S50" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T50, ($W50,$T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T50, ($W50,$T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T50" s="1"/>
-      <c r="V50" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="T50" s="1">
+        <v>40</v>
+      </c>
+      <c r="V50" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W50, ($W50,$T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W50, ($W50,$T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W50" s="1"/>
+        <v>-25</v>
+      </c>
+      <c r="W50" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A51" s="6">
@@ -4018,41 +4032,55 @@
       <c r="C51" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="D51" s="3" t="str">
+      <c r="D51" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E51, ($W51,$T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E51, ($W51,$T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E51" s="1"/>
-      <c r="G51" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="E51" s="1">
+        <v>0</v>
+      </c>
+      <c r="G51" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H51, ($W51,$T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H51, ($W51,$T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H51" s="1"/>
-      <c r="J51" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="H51" s="1">
+        <v>80</v>
+      </c>
+      <c r="J51" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K51, ($W51,$T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K51, ($W51,$T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K51" s="1"/>
-      <c r="M51" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="K51" s="1">
+        <v>50</v>
+      </c>
+      <c r="M51" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N51, ($W51,$T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N51, ($W51,$T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N51" s="1"/>
-      <c r="P51" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="N51" s="1">
+        <v>60</v>
+      </c>
+      <c r="P51" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q51, ($W51,$T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q51, ($W51,$T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q51" s="1"/>
-      <c r="S51" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q51" s="1">
+        <v>70</v>
+      </c>
+      <c r="S51" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T51, ($W51,$T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T51, ($W51,$T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T51" s="1"/>
-      <c r="V51" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="T51" s="1">
+        <v>100</v>
+      </c>
+      <c r="V51" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W51, ($W51,$T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W51, ($W51,$T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W51" s="1"/>
+        <v>-20</v>
+      </c>
+      <c r="W51" s="1">
+        <v>40</v>
+      </c>
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A52" s="6">
@@ -4064,41 +4092,55 @@
       <c r="C52" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="D52" s="3" t="str">
+      <c r="D52" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E52, ($W52,$T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E52, ($W52,$T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E52" s="1"/>
-      <c r="G52" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="E52" s="1">
+        <v>0</v>
+      </c>
+      <c r="G52" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H52, ($W52,$T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H52, ($W52,$T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H52" s="1"/>
-      <c r="J52" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="H52" s="1">
+        <v>100</v>
+      </c>
+      <c r="J52" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K52, ($W52,$T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K52, ($W52,$T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K52" s="1"/>
-      <c r="M52" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K52" s="1">
+        <v>60</v>
+      </c>
+      <c r="M52" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N52, ($W52,$T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N52, ($W52,$T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N52" s="1"/>
-      <c r="P52" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="N52" s="1">
+        <v>80</v>
+      </c>
+      <c r="P52" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q52, ($W52,$T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q52, ($W52,$T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q52" s="1"/>
-      <c r="S52" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q52" s="1">
+        <v>70</v>
+      </c>
+      <c r="S52" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T52, ($W52,$T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T52, ($W52,$T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T52" s="1"/>
-      <c r="V52" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="T52" s="1">
+        <v>40</v>
+      </c>
+      <c r="V52" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W52, ($W52,$T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W52, ($W52,$T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W52" s="1"/>
+        <v>-15</v>
+      </c>
+      <c r="W52" s="1">
+        <v>50</v>
+      </c>
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A53" s="6">
@@ -4110,41 +4152,55 @@
       <c r="C53" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="D53" s="3" t="str">
+      <c r="D53" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E53, ($W53,$T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E53, ($W53,$T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E53" s="1"/>
-      <c r="G53" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="E53" s="1">
+        <v>100</v>
+      </c>
+      <c r="G53" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H53, ($W53,$T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H53, ($W53,$T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H53" s="1"/>
-      <c r="J53" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="H53" s="1">
+        <v>50</v>
+      </c>
+      <c r="J53" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K53, ($W53,$T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K53, ($W53,$T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K53" s="1"/>
-      <c r="M53" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K53" s="1">
+        <v>60</v>
+      </c>
+      <c r="M53" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N53, ($W53,$T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N53, ($W53,$T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N53" s="1"/>
-      <c r="P53" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="N53" s="1">
+        <v>0</v>
+      </c>
+      <c r="P53" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q53, ($W53,$T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q53, ($W53,$T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q53" s="1"/>
-      <c r="S53" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q53" s="1">
+        <v>70</v>
+      </c>
+      <c r="S53" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T53, ($W53,$T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T53, ($W53,$T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T53" s="1"/>
-      <c r="V53" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="T53" s="1">
+        <v>40</v>
+      </c>
+      <c r="V53" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W53, ($W53,$T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W53, ($W53,$T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W53" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="W53" s="1">
+        <v>80</v>
+      </c>
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A54" s="6">
@@ -4156,41 +4212,53 @@
       <c r="C54" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="D54" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(E54, ($W54,$T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E54, ($W54,$T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E54" s="1"/>
-      <c r="G54" s="3" t="str">
+      <c r="D54" s="3">
+        <v>-17.5</v>
+      </c>
+      <c r="E54" s="1">
+        <v>50</v>
+      </c>
+      <c r="G54" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H54, ($W54,$T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H54, ($W54,$T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H54" s="1"/>
-      <c r="J54" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(K54, ($W54,$T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K54, ($W54,$T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K54" s="1"/>
-      <c r="M54" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="H54" s="1">
+        <v>100</v>
+      </c>
+      <c r="J54" s="3">
+        <v>-17.5</v>
+      </c>
+      <c r="K54" s="1">
+        <v>50</v>
+      </c>
+      <c r="M54" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N54, ($W54,$T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N54, ($W54,$T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N54" s="1"/>
-      <c r="P54" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="N54" s="1">
+        <v>60</v>
+      </c>
+      <c r="P54" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q54, ($W54,$T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q54, ($W54,$T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q54" s="1"/>
-      <c r="S54" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q54" s="1">
+        <v>70</v>
+      </c>
+      <c r="S54" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T54, ($W54,$T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T54, ($W54,$T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T54" s="1"/>
-      <c r="V54" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="T54" s="1">
+        <v>0</v>
+      </c>
+      <c r="V54" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W54, ($W54,$T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W54, ($W54,$T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W54" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="W54" s="1">
+        <v>80</v>
+      </c>
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A55" s="6">
@@ -4202,41 +4270,55 @@
       <c r="C55" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="D55" s="3" t="str">
+      <c r="D55" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E55, ($W55,$T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E55, ($W55,$T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E55" s="1"/>
-      <c r="G55" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="E55" s="1">
+        <v>60</v>
+      </c>
+      <c r="G55" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H55, ($W55,$T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H55, ($W55,$T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H55" s="1"/>
-      <c r="J55" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="H55" s="1">
+        <v>40</v>
+      </c>
+      <c r="J55" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K55, ($W55,$T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K55, ($W55,$T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K55" s="1"/>
-      <c r="M55" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="K55" s="1">
+        <v>50</v>
+      </c>
+      <c r="M55" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N55, ($W55,$T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N55, ($W55,$T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N55" s="1"/>
-      <c r="P55" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="N55" s="1">
+        <v>0</v>
+      </c>
+      <c r="P55" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q55, ($W55,$T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q55, ($W55,$T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q55" s="1"/>
-      <c r="S55" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q55" s="1">
+        <v>70</v>
+      </c>
+      <c r="S55" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T55, ($W55,$T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T55, ($W55,$T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T55" s="1"/>
-      <c r="V55" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="T55" s="1">
+        <v>100</v>
+      </c>
+      <c r="V55" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W55, ($W55,$T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W55, ($W55,$T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W55" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="W55" s="1">
+        <v>80</v>
+      </c>
     </row>
     <row r="56" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A56" s="6">
@@ -4248,41 +4330,55 @@
       <c r="C56" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="D56" s="3" t="str">
+      <c r="D56" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E56, ($W56,$T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E56, ($W56,$T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E56" s="1"/>
-      <c r="G56" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="E56" s="1">
+        <v>40</v>
+      </c>
+      <c r="G56" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H56, ($W56,$T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H56, ($W56,$T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H56" s="1"/>
-      <c r="J56" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="H56" s="1">
+        <v>60</v>
+      </c>
+      <c r="J56" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K56, ($W56,$T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K56, ($W56,$T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K56" s="1"/>
-      <c r="M56" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="K56" s="1">
+        <v>100</v>
+      </c>
+      <c r="M56" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N56, ($W56,$T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N56, ($W56,$T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N56" s="1"/>
-      <c r="P56" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="N56" s="1">
+        <v>70</v>
+      </c>
+      <c r="P56" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q56, ($W56,$T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q56, ($W56,$T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q56" s="1"/>
-      <c r="S56" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="Q56" s="1">
+        <v>80</v>
+      </c>
+      <c r="S56" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T56, ($W56,$T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T56, ($W56,$T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T56" s="1"/>
-      <c r="V56" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="T56" s="1">
+        <v>0</v>
+      </c>
+      <c r="V56" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W56, ($W56,$T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W56, ($W56,$T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W56" s="1"/>
+        <v>-15</v>
+      </c>
+      <c r="W56" s="1">
+        <v>50</v>
+      </c>
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A57" s="6">
@@ -4294,41 +4390,55 @@
       <c r="C57" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="D57" s="3" t="str">
+      <c r="D57" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E57, ($W57,$T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E57, ($W57,$T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E57" s="1"/>
-      <c r="G57" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="E57" s="1">
+        <v>40</v>
+      </c>
+      <c r="G57" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H57, ($W57,$T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H57, ($W57,$T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H57" s="1"/>
-      <c r="J57" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="H57" s="1">
+        <v>0</v>
+      </c>
+      <c r="J57" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K57, ($W57,$T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K57, ($W57,$T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K57" s="1"/>
-      <c r="M57" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K57" s="1">
+        <v>60</v>
+      </c>
+      <c r="M57" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N57, ($W57,$T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N57, ($W57,$T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N57" s="1"/>
-      <c r="P57" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="N57" s="1">
+        <v>70</v>
+      </c>
+      <c r="P57" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q57, ($W57,$T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q57, ($W57,$T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q57" s="1"/>
-      <c r="S57" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="Q57" s="1">
+        <v>100</v>
+      </c>
+      <c r="S57" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T57, ($W57,$T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T57, ($W57,$T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T57" s="1"/>
-      <c r="V57" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="T57" s="1">
+        <v>80</v>
+      </c>
+      <c r="V57" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W57, ($W57,$T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W57, ($W57,$T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W57" s="1"/>
+        <v>-15</v>
+      </c>
+      <c r="W57" s="1">
+        <v>50</v>
+      </c>
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A58" s="6">
@@ -4340,41 +4450,55 @@
       <c r="C58" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="D58" s="3" t="str">
+      <c r="D58" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E58, ($W58,$T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E58, ($W58,$T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E58" s="1"/>
-      <c r="G58" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="E58" s="1">
+        <v>80</v>
+      </c>
+      <c r="G58" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H58, ($W58,$T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H58, ($W58,$T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H58" s="1"/>
-      <c r="J58" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="H58" s="1">
+        <v>70</v>
+      </c>
+      <c r="J58" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K58, ($W58,$T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K58, ($W58,$T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K58" s="1"/>
-      <c r="M58" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="K58" s="1">
+        <v>50</v>
+      </c>
+      <c r="M58" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N58, ($W58,$T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N58, ($W58,$T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N58" s="1"/>
-      <c r="P58" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="N58" s="1">
+        <v>0</v>
+      </c>
+      <c r="P58" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q58, ($W58,$T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q58, ($W58,$T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q58" s="1"/>
-      <c r="S58" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="Q58" s="1">
+        <v>100</v>
+      </c>
+      <c r="S58" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T58, ($W58,$T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T58, ($W58,$T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T58" s="1"/>
-      <c r="V58" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="T58" s="1">
+        <v>60</v>
+      </c>
+      <c r="V58" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W58, ($W58,$T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W58, ($W58,$T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W58" s="1"/>
+        <v>-20</v>
+      </c>
+      <c r="W58" s="1">
+        <v>40</v>
+      </c>
     </row>
     <row r="59" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A59" s="6">
@@ -4782,35 +4906,35 @@
       </c>
       <c r="E68" s="12">
         <f>SUM(D13:D65)</f>
-        <v>-105</v>
+        <v>-152.5</v>
       </c>
       <c r="G68" s="7" t="s">
         <v>7</v>
       </c>
       <c r="H68" s="12">
         <f>SUM(G13:G65)</f>
-        <v>85</v>
+        <v>155</v>
       </c>
       <c r="J68" s="7" t="s">
         <v>7</v>
       </c>
       <c r="K68" s="12">
         <f>SUM(J13:J65)</f>
-        <v>-152.5</v>
+        <v>-205</v>
       </c>
       <c r="M68" s="7" t="s">
         <v>7</v>
       </c>
       <c r="N68" s="12">
         <f>SUM(M13:M65)</f>
-        <v>332.5</v>
+        <v>307.5</v>
       </c>
       <c r="P68" s="7" t="s">
         <v>7</v>
       </c>
       <c r="Q68" s="12">
         <f>SUM(P13:P65)</f>
-        <v>105</v>
+        <v>210</v>
       </c>
       <c r="S68" s="7" t="s">
         <v>7</v>
@@ -4824,7 +4948,7 @@
       </c>
       <c r="W68" s="12">
         <f>SUM(V13:V65)</f>
-        <v>-77.5</v>
+        <v>-127.5</v>
       </c>
       <c r="X68" s="1">
         <f>SUM(E68,H68,K68,N68,Q68,T68,W68)</f>

</xml_diff>

<commit_message>
Contest 47 through 54
</commit_message>
<xml_diff>
--- a/2022/EBE Boys 2022.xlsx
+++ b/2022/EBE Boys 2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9BE37BC-E907-4747-AEE4-014A6F66582A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2F10BF-BBE3-044E-88D8-13CC84127A74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20420" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="82">
   <si>
     <t>Points</t>
   </si>
@@ -268,6 +268,24 @@
   </si>
   <si>
     <t>LSG vs KKR</t>
+  </si>
+  <si>
+    <t>CSK vs DC</t>
+  </si>
+  <si>
+    <t>MI vs KKR</t>
+  </si>
+  <si>
+    <t>LSG vs GT</t>
+  </si>
+  <si>
+    <t>RR vs DC</t>
+  </si>
+  <si>
+    <t>CSK vs MI</t>
+  </si>
+  <si>
+    <t>RCB vs PBKS</t>
   </si>
 </sst>
 </file>
@@ -532,6 +550,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -568,195 +589,12 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent6" xfId="1" builtinId="50"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="57">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="39">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1462,11 +1300,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
-  <dimension ref="A1:Z99"/>
+  <dimension ref="A1:Z106"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X68" sqref="X68"/>
+      <pane ySplit="11" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X75" sqref="X75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1499,23 +1337,23 @@
         <v>50</v>
       </c>
       <c r="C2" s="5"/>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
-      <c r="S2" s="23"/>
-      <c r="T2" s="23"/>
-      <c r="U2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="24"/>
+      <c r="S2" s="24"/>
+      <c r="T2" s="24"/>
+      <c r="U2" s="25"/>
     </row>
     <row r="3" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
@@ -1525,21 +1363,21 @@
         <v>20</v>
       </c>
       <c r="C3" s="5"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="26"/>
-      <c r="R3" s="26"/>
-      <c r="S3" s="26"/>
-      <c r="T3" s="26"/>
-      <c r="U3" s="27"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
+      <c r="Q3" s="27"/>
+      <c r="R3" s="27"/>
+      <c r="S3" s="27"/>
+      <c r="T3" s="27"/>
+      <c r="U3" s="28"/>
     </row>
     <row r="4" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
@@ -1549,21 +1387,21 @@
         <v>0</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="26"/>
-      <c r="O4" s="26"/>
-      <c r="P4" s="26"/>
-      <c r="Q4" s="26"/>
-      <c r="R4" s="26"/>
-      <c r="S4" s="26"/>
-      <c r="T4" s="26"/>
-      <c r="U4" s="27"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="27"/>
+      <c r="R4" s="27"/>
+      <c r="S4" s="27"/>
+      <c r="T4" s="27"/>
+      <c r="U4" s="28"/>
     </row>
     <row r="5" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
@@ -1573,21 +1411,21 @@
         <v>-10</v>
       </c>
       <c r="C5" s="5"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="26"/>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="26"/>
-      <c r="R5" s="26"/>
-      <c r="S5" s="26"/>
-      <c r="T5" s="26"/>
-      <c r="U5" s="27"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="27"/>
+      <c r="Q5" s="27"/>
+      <c r="R5" s="27"/>
+      <c r="S5" s="27"/>
+      <c r="T5" s="27"/>
+      <c r="U5" s="28"/>
     </row>
     <row r="6" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
@@ -1597,21 +1435,21 @@
         <v>-15</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="26"/>
-      <c r="O6" s="26"/>
-      <c r="P6" s="26"/>
-      <c r="Q6" s="26"/>
-      <c r="R6" s="26"/>
-      <c r="S6" s="26"/>
-      <c r="T6" s="26"/>
-      <c r="U6" s="27"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="27"/>
+      <c r="R6" s="27"/>
+      <c r="S6" s="27"/>
+      <c r="T6" s="27"/>
+      <c r="U6" s="28"/>
     </row>
     <row r="7" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
@@ -1621,21 +1459,21 @@
         <v>-20</v>
       </c>
       <c r="C7" s="5"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="26"/>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="26"/>
-      <c r="R7" s="26"/>
-      <c r="S7" s="26"/>
-      <c r="T7" s="26"/>
-      <c r="U7" s="27"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="27"/>
+      <c r="Q7" s="27"/>
+      <c r="R7" s="27"/>
+      <c r="S7" s="27"/>
+      <c r="T7" s="27"/>
+      <c r="U7" s="28"/>
     </row>
     <row r="8" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
@@ -1645,21 +1483,21 @@
         <v>-25</v>
       </c>
       <c r="C8" s="5"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="29"/>
-      <c r="R8" s="29"/>
-      <c r="S8" s="29"/>
-      <c r="T8" s="29"/>
-      <c r="U8" s="30"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="30"/>
+      <c r="O8" s="30"/>
+      <c r="P8" s="30"/>
+      <c r="Q8" s="30"/>
+      <c r="R8" s="30"/>
+      <c r="S8" s="30"/>
+      <c r="T8" s="30"/>
+      <c r="U8" s="31"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C9" s="5"/>
@@ -1668,34 +1506,34 @@
       <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="31"/>
-      <c r="G11" s="20" t="s">
+      <c r="E11" s="32"/>
+      <c r="G11" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="21"/>
-      <c r="J11" s="20" t="s">
+      <c r="H11" s="22"/>
+      <c r="J11" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="K11" s="21"/>
-      <c r="M11" s="20" t="s">
+      <c r="K11" s="22"/>
+      <c r="M11" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="N11" s="21"/>
-      <c r="P11" s="20" t="s">
+      <c r="N11" s="22"/>
+      <c r="P11" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="Q11" s="21"/>
-      <c r="S11" s="20" t="s">
+      <c r="Q11" s="22"/>
+      <c r="S11" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="T11" s="21"/>
-      <c r="V11" s="20" t="s">
+      <c r="T11" s="22"/>
+      <c r="V11" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="W11" s="21"/>
+      <c r="W11" s="22"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
@@ -4510,41 +4348,55 @@
       <c r="C59" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="D59" s="3" t="str">
+      <c r="D59" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E59, ($W59,$T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E59, ($W59,$T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E59" s="1"/>
-      <c r="G59" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="E59" s="1">
+        <v>80</v>
+      </c>
+      <c r="G59" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H59, ($W59,$T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H59, ($W59,$T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H59" s="1"/>
-      <c r="J59" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="H59" s="1">
+        <v>70</v>
+      </c>
+      <c r="J59" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K59, ($W59,$T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K59, ($W59,$T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K59" s="1"/>
-      <c r="M59" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="K59" s="1">
+        <v>50</v>
+      </c>
+      <c r="M59" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N59, ($W59,$T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N59, ($W59,$T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N59" s="1"/>
-      <c r="P59" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="N59" s="1">
+        <v>100</v>
+      </c>
+      <c r="P59" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q59, ($W59,$T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q59, ($W59,$T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q59" s="1"/>
-      <c r="S59" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="Q59" s="1">
+        <v>60</v>
+      </c>
+      <c r="S59" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T59, ($W59,$T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T59, ($W59,$T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T59" s="1"/>
-      <c r="V59" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="T59" s="1">
+        <v>0</v>
+      </c>
+      <c r="V59" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W59, ($W59,$T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W59, ($W59,$T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W59" s="1"/>
+        <v>-20</v>
+      </c>
+      <c r="W59" s="1">
+        <v>40</v>
+      </c>
     </row>
     <row r="60" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A60" s="6">
@@ -4556,41 +4408,55 @@
       <c r="C60" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="D60" s="3" t="str">
+      <c r="D60" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E60, ($W60,$T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E60, ($W60,$T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E60" s="1"/>
-      <c r="G60" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="E60" s="1">
+        <v>0</v>
+      </c>
+      <c r="G60" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H60, ($W60,$T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H60, ($W60,$T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H60" s="1"/>
-      <c r="J60" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="H60" s="1">
+        <v>60</v>
+      </c>
+      <c r="J60" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K60, ($W60,$T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K60, ($W60,$T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K60" s="1"/>
-      <c r="M60" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="K60" s="1">
+        <v>40</v>
+      </c>
+      <c r="M60" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N60, ($W60,$T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N60, ($W60,$T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N60" s="1"/>
-      <c r="P60" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="N60" s="1">
+        <v>100</v>
+      </c>
+      <c r="P60" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q60, ($W60,$T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q60, ($W60,$T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q60" s="1"/>
-      <c r="S60" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="Q60" s="1">
+        <v>80</v>
+      </c>
+      <c r="S60" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T60, ($W60,$T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T60, ($W60,$T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T60" s="1"/>
-      <c r="V60" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="T60" s="1">
+        <v>50</v>
+      </c>
+      <c r="V60" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W60, ($W60,$T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W60, ($W60,$T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W60" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="W60" s="1">
+        <v>70</v>
+      </c>
     </row>
     <row r="61" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A61" s="6">
@@ -4602,41 +4468,55 @@
       <c r="C61" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="D61" s="3" t="str">
+      <c r="D61" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E61, ($W61,$T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E61, ($W61,$T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E61" s="1"/>
-      <c r="G61" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="E61" s="1">
+        <v>40</v>
+      </c>
+      <c r="G61" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H61, ($W61,$T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H61, ($W61,$T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H61" s="1"/>
-      <c r="J61" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="H61" s="1">
+        <v>100</v>
+      </c>
+      <c r="J61" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K61, ($W61,$T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K61, ($W61,$T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K61" s="1"/>
-      <c r="M61" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K61" s="1">
+        <v>60</v>
+      </c>
+      <c r="M61" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N61, ($W61,$T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N61, ($W61,$T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N61" s="1"/>
-      <c r="P61" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="N61" s="1">
+        <v>50</v>
+      </c>
+      <c r="P61" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q61, ($W61,$T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q61, ($W61,$T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q61" s="1"/>
-      <c r="S61" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="Q61" s="1">
+        <v>80</v>
+      </c>
+      <c r="S61" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T61, ($W61,$T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T61, ($W61,$T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T61" s="1"/>
-      <c r="V61" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="T61" s="1">
+        <v>70</v>
+      </c>
+      <c r="V61" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W61, ($W61,$T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W61, ($W61,$T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W61" s="1"/>
+        <v>-25</v>
+      </c>
+      <c r="W61" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="62" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A62" s="6">
@@ -4648,41 +4528,55 @@
       <c r="C62" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="D62" s="3" t="str">
+      <c r="D62" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E62, ($W62,$T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E62, ($W62,$T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E62" s="1"/>
-      <c r="G62" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="E62" s="1">
+        <v>0</v>
+      </c>
+      <c r="G62" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H62, ($W62,$T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H62, ($W62,$T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H62" s="1"/>
-      <c r="J62" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="H62" s="1">
+        <v>100</v>
+      </c>
+      <c r="J62" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K62, ($W62,$T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K62, ($W62,$T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K62" s="1"/>
-      <c r="M62" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="K62" s="1">
+        <v>40</v>
+      </c>
+      <c r="M62" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N62, ($W62,$T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N62, ($W62,$T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N62" s="1"/>
-      <c r="P62" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="N62" s="1">
+        <v>80</v>
+      </c>
+      <c r="P62" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q62, ($W62,$T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q62, ($W62,$T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q62" s="1"/>
-      <c r="S62" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="Q62" s="1">
+        <v>60</v>
+      </c>
+      <c r="S62" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T62, ($W62,$T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T62, ($W62,$T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T62" s="1"/>
-      <c r="V62" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="T62" s="1">
+        <v>50</v>
+      </c>
+      <c r="V62" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W62, ($W62,$T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W62, ($W62,$T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W62" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="W62" s="1">
+        <v>70</v>
+      </c>
     </row>
     <row r="63" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A63" s="6">
@@ -4694,41 +4588,55 @@
       <c r="C63" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="D63" s="3" t="str">
+      <c r="D63" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E63, ($W63,$T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E63, ($W63,$T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E63" s="1"/>
-      <c r="G63" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="E63" s="1">
+        <v>50</v>
+      </c>
+      <c r="G63" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H63, ($W63,$T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H63, ($W63,$T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H63" s="1"/>
-      <c r="J63" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="H63" s="1">
+        <v>100</v>
+      </c>
+      <c r="J63" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K63, ($W63,$T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K63, ($W63,$T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K63" s="1"/>
-      <c r="M63" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K63" s="1">
+        <v>60</v>
+      </c>
+      <c r="M63" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N63, ($W63,$T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N63, ($W63,$T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N63" s="1"/>
-      <c r="P63" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="N63" s="1">
+        <v>80</v>
+      </c>
+      <c r="P63" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q63, ($W63,$T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q63, ($W63,$T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q63" s="1"/>
-      <c r="S63" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="Q63" s="1">
+        <v>0</v>
+      </c>
+      <c r="S63" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T63, ($W63,$T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T63, ($W63,$T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T63" s="1"/>
-      <c r="V63" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="T63" s="1">
+        <v>70</v>
+      </c>
+      <c r="V63" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W63, ($W63,$T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W63, ($W63,$T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W63" s="1"/>
+        <v>-20</v>
+      </c>
+      <c r="W63" s="1">
+        <v>40</v>
+      </c>
     </row>
     <row r="64" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A64" s="6">
@@ -4740,41 +4648,55 @@
       <c r="C64" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="D64" s="3" t="str">
+      <c r="D64" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E64, ($W64,$T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E64, ($W64,$T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E64" s="1"/>
-      <c r="G64" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="E64" s="1">
+        <v>40</v>
+      </c>
+      <c r="G64" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H64, ($W64,$T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H64, ($W64,$T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H64" s="1"/>
-      <c r="J64" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="H64" s="1">
+        <v>50</v>
+      </c>
+      <c r="J64" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K64, ($W64,$T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K64, ($W64,$T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K64" s="1"/>
-      <c r="M64" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="K64" s="1">
+        <v>100</v>
+      </c>
+      <c r="M64" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N64, ($W64,$T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N64, ($W64,$T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N64" s="1"/>
-      <c r="P64" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="N64" s="1">
+        <v>80</v>
+      </c>
+      <c r="P64" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q64, ($W64,$T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q64, ($W64,$T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q64" s="1"/>
-      <c r="S64" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="Q64" s="1">
+        <v>60</v>
+      </c>
+      <c r="S64" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T64, ($W64,$T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T64, ($W64,$T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T64" s="1"/>
-      <c r="V64" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="T64" s="1">
+        <v>0</v>
+      </c>
+      <c r="V64" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W64, ($W64,$T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W64, ($W64,$T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W64" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="W64" s="1">
+        <v>70</v>
+      </c>
     </row>
     <row r="65" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A65" s="6">
@@ -4786,392 +4708,553 @@
       <c r="C65" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="D65" s="3" t="str">
+      <c r="D65" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="E65" s="1">
+        <v>70</v>
+      </c>
+      <c r="G65" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(H65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>20</v>
+      </c>
+      <c r="H65" s="1">
+        <v>80</v>
+      </c>
+      <c r="J65" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(K65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-20</v>
+      </c>
+      <c r="K65" s="1">
+        <v>40</v>
+      </c>
+      <c r="M65" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(N65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-10</v>
+      </c>
+      <c r="N65" s="1">
+        <v>60</v>
+      </c>
+      <c r="P65" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-15</v>
+      </c>
+      <c r="Q65" s="1">
+        <v>50</v>
+      </c>
+      <c r="S65" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(T65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>50</v>
+      </c>
+      <c r="T65" s="1">
+        <v>100</v>
+      </c>
+      <c r="V65" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(W65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-25</v>
+      </c>
+      <c r="W65" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A66" s="6">
+        <v>54</v>
+      </c>
+      <c r="B66" s="1">
+        <v>1</v>
+      </c>
+      <c r="C66" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D66" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(E66, ($W66,$T66,$Q66,$N66,$K66,$H66,$E66), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E66, ($W66,$T66,$Q66,$N66,$K66,$H66,$E66), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>20</v>
+      </c>
+      <c r="E66" s="1">
+        <v>80</v>
+      </c>
+      <c r="G66" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(H66, ($W66,$T66,$Q66,$N66,$K66,$H66,$E66), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H66, ($W66,$T66,$Q66,$N66,$K66,$H66,$E66), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>50</v>
+      </c>
+      <c r="H66" s="1">
+        <v>100</v>
+      </c>
+      <c r="J66" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(K66, ($W66,$T66,$Q66,$N66,$K66,$H66,$E66), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K66, ($W66,$T66,$Q66,$N66,$K66,$H66,$E66), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-20</v>
+      </c>
+      <c r="K66" s="1">
+        <v>40</v>
+      </c>
+      <c r="M66" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(N66, ($W66,$T66,$Q66,$N66,$K66,$H66,$E66), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N66, ($W66,$T66,$Q66,$N66,$K66,$H66,$E66), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-15</v>
+      </c>
+      <c r="N66" s="1">
+        <v>50</v>
+      </c>
+      <c r="P66" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q66, ($W66,$T66,$Q66,$N66,$K66,$H66,$E66), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q66, ($W66,$T66,$Q66,$N66,$K66,$H66,$E66), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-25</v>
+      </c>
+      <c r="Q66" s="1">
+        <v>0</v>
+      </c>
+      <c r="S66" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(T66, ($W66,$T66,$Q66,$N66,$K66,$H66,$E66), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T66, ($W66,$T66,$Q66,$N66,$K66,$H66,$E66), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="T66" s="1">
+        <v>70</v>
+      </c>
+      <c r="V66" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(W66, ($W66,$T66,$Q66,$N66,$K66,$H66,$E66), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W66, ($W66,$T66,$Q66,$N66,$K66,$H66,$E66), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-10</v>
+      </c>
+      <c r="W66" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A67" s="6">
+        <v>55</v>
+      </c>
+      <c r="B67" s="1">
+        <v>1</v>
+      </c>
+      <c r="C67" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D67" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E67, ($W67,$T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E67, ($W67,$T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$B$10, 2, FALSE))</f>
         <v/>
       </c>
-      <c r="E65" s="1"/>
-      <c r="G65" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(H65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE))</f>
+      <c r="E67" s="1"/>
+      <c r="G67" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H67, ($W67,$T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H67, ($W67,$T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$B$10, 2, FALSE))</f>
         <v/>
       </c>
-      <c r="H65" s="1"/>
-      <c r="J65" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(K65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE))</f>
+      <c r="H67" s="1"/>
+      <c r="J67" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K67, ($W67,$T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K67, ($W67,$T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$B$10, 2, FALSE))</f>
         <v/>
       </c>
-      <c r="K65" s="1"/>
-      <c r="M65" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(N65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE))</f>
+      <c r="K67" s="1"/>
+      <c r="M67" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N67, ($W67,$T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N67, ($W67,$T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$B$10, 2, FALSE))</f>
         <v/>
       </c>
-      <c r="N65" s="1"/>
-      <c r="P65" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(Q65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE))</f>
+      <c r="N67" s="1"/>
+      <c r="P67" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q67, ($W67,$T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q67, ($W67,$T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$B$10, 2, FALSE))</f>
         <v/>
       </c>
-      <c r="Q65" s="1"/>
-      <c r="S65" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(T65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE))</f>
+      <c r="Q67" s="1"/>
+      <c r="S67" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T67, ($W67,$T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T67, ($W67,$T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$B$10, 2, FALSE))</f>
         <v/>
       </c>
-      <c r="T65" s="1"/>
-      <c r="V65" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(W65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W65, ($W65,$T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$B$10, 2, FALSE))</f>
+      <c r="T67" s="1"/>
+      <c r="V67" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W67, ($W67,$T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W67, ($W67,$T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$B$10, 2, FALSE))</f>
         <v/>
       </c>
-      <c r="W65" s="1"/>
-    </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A66" s="6"/>
-      <c r="B66" s="1" t="s">
+      <c r="W67" s="1"/>
+    </row>
+    <row r="68" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A68" s="6">
+        <v>56</v>
+      </c>
+      <c r="B68" s="1">
+        <v>1</v>
+      </c>
+      <c r="C68" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D68" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E68, ($W68,$T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E68, ($W68,$T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E68" s="1"/>
+      <c r="G68" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H68, ($W68,$T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H68, ($W68,$T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H68" s="1"/>
+      <c r="J68" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K68, ($W68,$T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K68, ($W68,$T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K68" s="1"/>
+      <c r="M68" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N68, ($W68,$T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N68, ($W68,$T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N68" s="1"/>
+      <c r="P68" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q68, ($W68,$T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q68, ($W68,$T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q68" s="1"/>
+      <c r="S68" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T68, ($W68,$T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T68, ($W68,$T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T68" s="1"/>
+      <c r="V68" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W68, ($W68,$T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W68, ($W68,$T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="W68" s="1"/>
+    </row>
+    <row r="69" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A69" s="6">
+        <v>57</v>
+      </c>
+      <c r="B69" s="1">
+        <v>1</v>
+      </c>
+      <c r="C69" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D69" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E69, ($W69,$T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E69, ($W69,$T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E69" s="1"/>
+      <c r="G69" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H69, ($W69,$T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H69, ($W69,$T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H69" s="1"/>
+      <c r="J69" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K69, ($W69,$T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K69, ($W69,$T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K69" s="1"/>
+      <c r="M69" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N69, ($W69,$T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N69, ($W69,$T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N69" s="1"/>
+      <c r="P69" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q69, ($W69,$T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q69, ($W69,$T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q69" s="1"/>
+      <c r="S69" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T69, ($W69,$T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T69, ($W69,$T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T69" s="1"/>
+      <c r="V69" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W69, ($W69,$T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W69, ($W69,$T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="W69" s="1"/>
+    </row>
+    <row r="70" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A70" s="6">
+        <v>58</v>
+      </c>
+      <c r="B70" s="1">
+        <v>1</v>
+      </c>
+      <c r="C70" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D70" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E70, ($W70,$T70,$Q70,$N70,$K70,$H70,$E70), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E70, ($W70,$T70,$Q70,$N70,$K70,$H70,$E70), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E70" s="1"/>
+      <c r="G70" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H70, ($W70,$T70,$Q70,$N70,$K70,$H70,$E70), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H70, ($W70,$T70,$Q70,$N70,$K70,$H70,$E70), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H70" s="1"/>
+      <c r="J70" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K70, ($W70,$T70,$Q70,$N70,$K70,$H70,$E70), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K70, ($W70,$T70,$Q70,$N70,$K70,$H70,$E70), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K70" s="1"/>
+      <c r="M70" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N70, ($W70,$T70,$Q70,$N70,$K70,$H70,$E70), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N70, ($W70,$T70,$Q70,$N70,$K70,$H70,$E70), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N70" s="1"/>
+      <c r="P70" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q70, ($W70,$T70,$Q70,$N70,$K70,$H70,$E70), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q70, ($W70,$T70,$Q70,$N70,$K70,$H70,$E70), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q70" s="1"/>
+      <c r="S70" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T70, ($W70,$T70,$Q70,$N70,$K70,$H70,$E70), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T70, ($W70,$T70,$Q70,$N70,$K70,$H70,$E70), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T70" s="1"/>
+      <c r="V70" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W70, ($W70,$T70,$Q70,$N70,$K70,$H70,$E70), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W70, ($W70,$T70,$Q70,$N70,$K70,$H70,$E70), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="W70" s="1"/>
+    </row>
+    <row r="71" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A71" s="6">
+        <v>59</v>
+      </c>
+      <c r="B71" s="1">
+        <v>1</v>
+      </c>
+      <c r="C71" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D71" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E71, ($W71,$T71,$Q71,$N71,$K71,$H71,$E71), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E71, ($W71,$T71,$Q71,$N71,$K71,$H71,$E71), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E71" s="1"/>
+      <c r="G71" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H71, ($W71,$T71,$Q71,$N71,$K71,$H71,$E71), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H71, ($W71,$T71,$Q71,$N71,$K71,$H71,$E71), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H71" s="1"/>
+      <c r="J71" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K71, ($W71,$T71,$Q71,$N71,$K71,$H71,$E71), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K71, ($W71,$T71,$Q71,$N71,$K71,$H71,$E71), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K71" s="1"/>
+      <c r="M71" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N71, ($W71,$T71,$Q71,$N71,$K71,$H71,$E71), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N71, ($W71,$T71,$Q71,$N71,$K71,$H71,$E71), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N71" s="1"/>
+      <c r="P71" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q71, ($W71,$T71,$Q71,$N71,$K71,$H71,$E71), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q71, ($W71,$T71,$Q71,$N71,$K71,$H71,$E71), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q71" s="1"/>
+      <c r="S71" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T71, ($W71,$T71,$Q71,$N71,$K71,$H71,$E71), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T71, ($W71,$T71,$Q71,$N71,$K71,$H71,$E71), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T71" s="1"/>
+      <c r="V71" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W71, ($W71,$T71,$Q71,$N71,$K71,$H71,$E71), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W71, ($W71,$T71,$Q71,$N71,$K71,$H71,$E71), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="W71" s="1"/>
+    </row>
+    <row r="72" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A72" s="6">
+        <v>60</v>
+      </c>
+      <c r="B72" s="1">
+        <v>1</v>
+      </c>
+      <c r="C72" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D72" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E72" s="1"/>
+      <c r="G72" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H72" s="1"/>
+      <c r="J72" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K72" s="1"/>
+      <c r="M72" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N72" s="1"/>
+      <c r="P72" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q72" s="1"/>
+      <c r="S72" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T72" s="1"/>
+      <c r="V72" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="W72" s="1"/>
+    </row>
+    <row r="73" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A73" s="6"/>
+      <c r="B73" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C66" s="10"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="9" t="s">
+      <c r="C73" s="10"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G66" s="1"/>
-      <c r="H66" s="9" t="s">
+      <c r="G73" s="1"/>
+      <c r="H73" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J66" s="1"/>
-      <c r="K66" s="9" t="s">
+      <c r="J73" s="1"/>
+      <c r="K73" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="M66" s="1"/>
-      <c r="N66" s="9" t="s">
+      <c r="M73" s="1"/>
+      <c r="N73" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="P66" s="1"/>
-      <c r="Q66" s="9" t="s">
+      <c r="P73" s="1"/>
+      <c r="Q73" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="S66" s="1"/>
-      <c r="T66" s="9" t="s">
+      <c r="S73" s="1"/>
+      <c r="T73" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="V66" s="1"/>
-      <c r="W66" s="9" t="s">
+      <c r="V73" s="1"/>
+      <c r="W73" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A67" s="5"/>
-      <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="1"/>
-      <c r="E67" s="11" t="str">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A74" s="5"/>
+      <c r="B74" s="5"/>
+      <c r="C74" s="5"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="11" t="str">
         <f>D12</f>
         <v>Jaya</v>
       </c>
-      <c r="G67" s="1"/>
-      <c r="H67" s="11" t="str">
+      <c r="G74" s="1"/>
+      <c r="H74" s="11" t="str">
         <f>G12</f>
         <v>Justin</v>
       </c>
-      <c r="J67" s="1"/>
-      <c r="K67" s="11" t="str">
+      <c r="J74" s="1"/>
+      <c r="K74" s="11" t="str">
         <f>J12</f>
         <v>Ram</v>
       </c>
-      <c r="M67" s="1"/>
-      <c r="N67" s="11" t="str">
+      <c r="M74" s="1"/>
+      <c r="N74" s="11" t="str">
         <f>M12</f>
         <v>Sibi</v>
       </c>
-      <c r="P67" s="1"/>
-      <c r="Q67" s="11" t="str">
+      <c r="P74" s="1"/>
+      <c r="Q74" s="11" t="str">
         <f>P12</f>
         <v>Sundar</v>
       </c>
-      <c r="S67" s="1"/>
-      <c r="T67" s="11" t="str">
+      <c r="S74" s="1"/>
+      <c r="T74" s="11" t="str">
         <f>S12</f>
         <v>Upili</v>
       </c>
-      <c r="V67" s="1"/>
-      <c r="W67" s="11" t="str">
+      <c r="V74" s="1"/>
+      <c r="W74" s="11" t="str">
         <f>V12</f>
         <v>Vicky</v>
       </c>
     </row>
-    <row r="68" spans="1:26" ht="21" x14ac:dyDescent="0.25">
-      <c r="A68" s="5"/>
-      <c r="B68" s="5"/>
-      <c r="C68" s="5"/>
-      <c r="D68" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E68" s="12">
-        <f>SUM(D13:D65)</f>
-        <v>-152.5</v>
-      </c>
-      <c r="G68" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H68" s="12">
-        <f>SUM(G13:G65)</f>
-        <v>155</v>
-      </c>
-      <c r="J68" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="K68" s="12">
-        <f>SUM(J13:J65)</f>
-        <v>-205</v>
-      </c>
-      <c r="M68" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="N68" s="12">
-        <f>SUM(M13:M65)</f>
-        <v>307.5</v>
-      </c>
-      <c r="P68" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q68" s="12">
-        <f>SUM(P13:P65)</f>
-        <v>210</v>
-      </c>
-      <c r="S68" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="T68" s="12">
-        <f>SUM(S13:S65)</f>
-        <v>-187.5</v>
-      </c>
-      <c r="V68" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="W68" s="12">
-        <f>SUM(V13:V65)</f>
-        <v>-127.5</v>
-      </c>
-      <c r="X68" s="1">
-        <f>SUM(E68,H68,K68,N68,Q68,T68,W68)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A69" s="5"/>
-      <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
-      <c r="E69" s="5"/>
-      <c r="S69" s="5"/>
-      <c r="T69" s="5"/>
-    </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A70" s="5"/>
-      <c r="B70" s="5"/>
-      <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
-      <c r="E70" s="5"/>
-      <c r="S70" s="5"/>
-      <c r="T70" s="5"/>
-    </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A71" s="5"/>
-      <c r="B71" s="5"/>
-      <c r="C71" s="5"/>
-      <c r="D71" s="5"/>
-      <c r="E71" s="5"/>
-      <c r="F71" s="5"/>
-      <c r="G71" s="5"/>
-      <c r="H71" s="5"/>
-      <c r="I71" s="5"/>
-      <c r="J71" s="5"/>
-      <c r="K71" s="5"/>
-      <c r="L71" s="5"/>
-      <c r="M71" s="5"/>
-      <c r="N71" s="5"/>
-      <c r="O71" s="5"/>
-      <c r="P71" s="5"/>
-      <c r="Q71" s="5"/>
-      <c r="R71" s="5"/>
-      <c r="S71" s="5"/>
-      <c r="T71" s="5"/>
-      <c r="U71" s="5"/>
-      <c r="V71" s="5"/>
-      <c r="W71" s="5"/>
-      <c r="X71" s="5"/>
-      <c r="Y71" s="5"/>
-      <c r="Z71" s="5"/>
-    </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="B72" s="5"/>
-      <c r="C72" s="5"/>
-      <c r="D72" s="5"/>
-      <c r="E72" s="5"/>
-      <c r="F72" s="5"/>
-      <c r="G72" s="5"/>
-      <c r="H72" s="5"/>
-      <c r="I72" s="5"/>
-      <c r="J72" s="5"/>
-      <c r="K72" s="5"/>
-      <c r="L72" s="5"/>
-      <c r="M72" s="5"/>
-      <c r="N72" s="5"/>
-      <c r="O72" s="5"/>
-      <c r="P72" s="5"/>
-      <c r="Q72" s="5"/>
-      <c r="R72" s="5"/>
-      <c r="S72" s="5"/>
-      <c r="T72" s="5"/>
-      <c r="U72" s="5"/>
-      <c r="V72" s="5"/>
-      <c r="W72" s="5"/>
-      <c r="X72" s="5"/>
-      <c r="Y72" s="5"/>
-      <c r="Z72" s="5"/>
-    </row>
-    <row r="73" spans="1:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="B73" s="5"/>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
-      <c r="E73" s="32"/>
-      <c r="F73" s="32"/>
-      <c r="G73" s="32"/>
-      <c r="H73" s="32"/>
-      <c r="I73" s="16"/>
-      <c r="J73" s="5"/>
-      <c r="K73" s="5"/>
-      <c r="L73" s="5"/>
-      <c r="M73" s="5"/>
-      <c r="N73" s="5"/>
-      <c r="O73" s="5"/>
-      <c r="P73" s="5"/>
-      <c r="Q73" s="5"/>
-      <c r="R73" s="5"/>
-      <c r="S73" s="5"/>
-      <c r="T73" s="5"/>
-      <c r="U73" s="5"/>
-      <c r="V73" s="5"/>
-      <c r="W73" s="5"/>
-      <c r="X73" s="5"/>
-      <c r="Y73" s="5"/>
-      <c r="Z73" s="5"/>
-    </row>
-    <row r="74" spans="1:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="B74" s="5"/>
-      <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
-      <c r="E74" s="17"/>
-      <c r="F74" s="17"/>
-      <c r="G74" s="17"/>
-      <c r="H74" s="17"/>
-      <c r="I74" s="18"/>
-      <c r="J74" s="5"/>
-      <c r="K74" s="5"/>
-      <c r="L74" s="5"/>
-      <c r="M74" s="5"/>
-      <c r="N74" s="5"/>
-      <c r="O74" s="5"/>
-      <c r="P74" s="5"/>
-      <c r="Q74" s="5"/>
-      <c r="R74" s="5"/>
-      <c r="S74" s="5"/>
-      <c r="T74" s="5"/>
-      <c r="U74" s="5"/>
-      <c r="V74" s="5"/>
-      <c r="W74" s="5"/>
-      <c r="X74" s="5"/>
-      <c r="Y74" s="5"/>
-      <c r="Z74" s="5"/>
-    </row>
-    <row r="75" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:26" ht="21" x14ac:dyDescent="0.25">
+      <c r="A75" s="5"/>
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
-      <c r="D75" s="17"/>
-      <c r="E75" s="5"/>
-      <c r="F75" s="5"/>
-      <c r="G75" s="5"/>
-      <c r="H75" s="5"/>
-      <c r="I75" s="17"/>
-      <c r="J75" s="5"/>
-      <c r="K75" s="5"/>
-      <c r="L75" s="5"/>
-      <c r="M75" s="5"/>
-      <c r="N75" s="5"/>
-      <c r="O75" s="5"/>
-      <c r="P75" s="5"/>
-      <c r="Q75" s="5"/>
-      <c r="R75" s="5"/>
-      <c r="S75" s="5"/>
-      <c r="T75" s="5"/>
-      <c r="U75" s="5"/>
-      <c r="V75" s="5"/>
-      <c r="W75" s="5"/>
-      <c r="X75" s="5"/>
-      <c r="Y75" s="5"/>
-      <c r="Z75" s="5"/>
-    </row>
-    <row r="76" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+      <c r="D75" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E75" s="12">
+        <f>SUM(D13:D72)</f>
+        <v>-217.5</v>
+      </c>
+      <c r="G75" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H75" s="12">
+        <f>SUM(G13:G72)</f>
+        <v>350</v>
+      </c>
+      <c r="J75" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K75" s="12">
+        <f>SUM(J13:J72)</f>
+        <v>-270</v>
+      </c>
+      <c r="M75" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="N75" s="12">
+        <f>SUM(M13:M72)</f>
+        <v>427.5</v>
+      </c>
+      <c r="P75" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q75" s="12">
+        <f>SUM(P13:P72)</f>
+        <v>155</v>
+      </c>
+      <c r="S75" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="T75" s="12">
+        <f>SUM(S13:S72)</f>
+        <v>-217.5</v>
+      </c>
+      <c r="V75" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="W75" s="12">
+        <f>SUM(V13:V72)</f>
+        <v>-227.5</v>
+      </c>
+      <c r="X75" s="1">
+        <f>SUM(E75,H75,K75,N75,Q75,T75,W75)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A76" s="5"/>
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
-      <c r="D76" s="17"/>
+      <c r="D76" s="5"/>
       <c r="E76" s="5"/>
-      <c r="F76" s="5"/>
-      <c r="G76" s="5"/>
-      <c r="H76" s="5"/>
-      <c r="I76" s="17"/>
-      <c r="J76" s="5"/>
-      <c r="K76" s="5"/>
-      <c r="L76" s="5"/>
-      <c r="M76" s="5"/>
-      <c r="N76" s="5"/>
-      <c r="O76" s="5"/>
-      <c r="P76" s="5"/>
-      <c r="Q76" s="5"/>
-      <c r="R76" s="5"/>
       <c r="S76" s="5"/>
       <c r="T76" s="5"/>
-      <c r="U76" s="5"/>
-      <c r="V76" s="5"/>
-      <c r="W76" s="5"/>
-      <c r="X76" s="5"/>
-      <c r="Y76" s="5"/>
-      <c r="Z76" s="5"/>
-    </row>
-    <row r="77" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A77" s="5"/>
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
-      <c r="D77" s="17"/>
+      <c r="D77" s="5"/>
       <c r="E77" s="5"/>
-      <c r="F77" s="5"/>
-      <c r="G77" s="5"/>
-      <c r="H77" s="5"/>
-      <c r="I77" s="17"/>
-      <c r="J77" s="5"/>
-      <c r="K77" s="5"/>
-      <c r="L77" s="5"/>
-      <c r="M77" s="5"/>
-      <c r="N77" s="5"/>
-      <c r="O77" s="5"/>
-      <c r="P77" s="5"/>
-      <c r="Q77" s="5"/>
-      <c r="R77" s="5"/>
       <c r="S77" s="5"/>
       <c r="T77" s="5"/>
-      <c r="U77" s="5"/>
-      <c r="V77" s="5"/>
-      <c r="W77" s="5"/>
-      <c r="X77" s="5"/>
-      <c r="Y77" s="5"/>
-      <c r="Z77" s="5"/>
-    </row>
-    <row r="78" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A78" s="5"/>
       <c r="B78" s="5"/>
       <c r="C78" s="5"/>
-      <c r="D78" s="17"/>
+      <c r="D78" s="5"/>
       <c r="E78" s="5"/>
       <c r="F78" s="5"/>
       <c r="G78" s="5"/>
       <c r="H78" s="5"/>
-      <c r="I78" s="17"/>
+      <c r="I78" s="5"/>
       <c r="J78" s="5"/>
       <c r="K78" s="5"/>
       <c r="L78" s="5"/>
@@ -5190,15 +5273,15 @@
       <c r="Y78" s="5"/>
       <c r="Z78" s="5"/>
     </row>
-    <row r="79" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
-      <c r="D79" s="17"/>
+      <c r="D79" s="5"/>
       <c r="E79" s="5"/>
       <c r="F79" s="5"/>
       <c r="G79" s="5"/>
       <c r="H79" s="5"/>
-      <c r="I79" s="17"/>
+      <c r="I79" s="5"/>
       <c r="J79" s="5"/>
       <c r="K79" s="5"/>
       <c r="L79" s="5"/>
@@ -5220,12 +5303,12 @@
     <row r="80" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
-      <c r="D80" s="17"/>
-      <c r="E80" s="5"/>
-      <c r="F80" s="5"/>
-      <c r="G80" s="5"/>
-      <c r="H80" s="5"/>
-      <c r="I80" s="17"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="20"/>
+      <c r="F80" s="20"/>
+      <c r="G80" s="20"/>
+      <c r="H80" s="20"/>
+      <c r="I80" s="16"/>
       <c r="J80" s="5"/>
       <c r="K80" s="5"/>
       <c r="L80" s="5"/>
@@ -5247,12 +5330,12 @@
     <row r="81" spans="2:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B81" s="5"/>
       <c r="C81" s="5"/>
-      <c r="D81" s="17"/>
-      <c r="E81" s="5"/>
-      <c r="F81" s="5"/>
-      <c r="G81" s="5"/>
-      <c r="H81" s="5"/>
-      <c r="I81" s="17"/>
+      <c r="D81" s="5"/>
+      <c r="E81" s="17"/>
+      <c r="F81" s="17"/>
+      <c r="G81" s="17"/>
+      <c r="H81" s="17"/>
+      <c r="I81" s="18"/>
       <c r="J81" s="5"/>
       <c r="K81" s="5"/>
       <c r="L81" s="5"/>
@@ -5325,15 +5408,15 @@
       <c r="Y83" s="5"/>
       <c r="Z83" s="5"/>
     </row>
-    <row r="84" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B84" s="5"/>
       <c r="C84" s="5"/>
-      <c r="D84" s="5"/>
+      <c r="D84" s="17"/>
       <c r="E84" s="5"/>
       <c r="F84" s="5"/>
       <c r="G84" s="5"/>
       <c r="H84" s="5"/>
-      <c r="I84" s="5"/>
+      <c r="I84" s="17"/>
       <c r="J84" s="5"/>
       <c r="K84" s="5"/>
       <c r="L84" s="5"/>
@@ -5352,15 +5435,15 @@
       <c r="Y84" s="5"/>
       <c r="Z84" s="5"/>
     </row>
-    <row r="85" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
-      <c r="D85" s="5"/>
+      <c r="D85" s="17"/>
       <c r="E85" s="5"/>
       <c r="F85" s="5"/>
       <c r="G85" s="5"/>
       <c r="H85" s="5"/>
-      <c r="I85" s="5"/>
+      <c r="I85" s="17"/>
       <c r="J85" s="5"/>
       <c r="K85" s="5"/>
       <c r="L85" s="5"/>
@@ -5379,15 +5462,15 @@
       <c r="Y85" s="5"/>
       <c r="Z85" s="5"/>
     </row>
-    <row r="86" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
-      <c r="D86" s="5"/>
+      <c r="D86" s="17"/>
       <c r="E86" s="5"/>
       <c r="F86" s="5"/>
       <c r="G86" s="5"/>
       <c r="H86" s="5"/>
-      <c r="I86" s="5"/>
+      <c r="I86" s="17"/>
       <c r="J86" s="5"/>
       <c r="K86" s="5"/>
       <c r="L86" s="5"/>
@@ -5406,15 +5489,15 @@
       <c r="Y86" s="5"/>
       <c r="Z86" s="5"/>
     </row>
-    <row r="87" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
-      <c r="D87" s="5"/>
+      <c r="D87" s="17"/>
       <c r="E87" s="5"/>
       <c r="F87" s="5"/>
       <c r="G87" s="5"/>
       <c r="H87" s="5"/>
-      <c r="I87" s="5"/>
+      <c r="I87" s="17"/>
       <c r="J87" s="5"/>
       <c r="K87" s="5"/>
       <c r="L87" s="5"/>
@@ -5433,15 +5516,15 @@
       <c r="Y87" s="5"/>
       <c r="Z87" s="5"/>
     </row>
-    <row r="88" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
-      <c r="D88" s="5"/>
+      <c r="D88" s="17"/>
       <c r="E88" s="5"/>
       <c r="F88" s="5"/>
       <c r="G88" s="5"/>
       <c r="H88" s="5"/>
-      <c r="I88" s="5"/>
+      <c r="I88" s="17"/>
       <c r="J88" s="5"/>
       <c r="K88" s="5"/>
       <c r="L88" s="5"/>
@@ -5460,15 +5543,15 @@
       <c r="Y88" s="5"/>
       <c r="Z88" s="5"/>
     </row>
-    <row r="89" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
-      <c r="D89" s="5"/>
+      <c r="D89" s="17"/>
       <c r="E89" s="5"/>
       <c r="F89" s="5"/>
       <c r="G89" s="5"/>
       <c r="H89" s="5"/>
-      <c r="I89" s="5"/>
+      <c r="I89" s="17"/>
       <c r="J89" s="5"/>
       <c r="K89" s="5"/>
       <c r="L89" s="5"/>
@@ -5487,15 +5570,15 @@
       <c r="Y89" s="5"/>
       <c r="Z89" s="5"/>
     </row>
-    <row r="90" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
-      <c r="D90" s="5"/>
+      <c r="D90" s="17"/>
       <c r="E90" s="5"/>
       <c r="F90" s="5"/>
       <c r="G90" s="5"/>
       <c r="H90" s="5"/>
-      <c r="I90" s="5"/>
+      <c r="I90" s="17"/>
       <c r="J90" s="5"/>
       <c r="K90" s="5"/>
       <c r="L90" s="5"/>
@@ -5757,10 +5840,199 @@
       <c r="Y99" s="5"/>
       <c r="Z99" s="5"/>
     </row>
+    <row r="100" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B100" s="5"/>
+      <c r="C100" s="5"/>
+      <c r="D100" s="5"/>
+      <c r="E100" s="5"/>
+      <c r="F100" s="5"/>
+      <c r="G100" s="5"/>
+      <c r="H100" s="5"/>
+      <c r="I100" s="5"/>
+      <c r="J100" s="5"/>
+      <c r="K100" s="5"/>
+      <c r="L100" s="5"/>
+      <c r="M100" s="5"/>
+      <c r="N100" s="5"/>
+      <c r="O100" s="5"/>
+      <c r="P100" s="5"/>
+      <c r="Q100" s="5"/>
+      <c r="R100" s="5"/>
+      <c r="S100" s="5"/>
+      <c r="T100" s="5"/>
+      <c r="U100" s="5"/>
+      <c r="V100" s="5"/>
+      <c r="W100" s="5"/>
+      <c r="X100" s="5"/>
+      <c r="Y100" s="5"/>
+      <c r="Z100" s="5"/>
+    </row>
+    <row r="101" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B101" s="5"/>
+      <c r="C101" s="5"/>
+      <c r="D101" s="5"/>
+      <c r="E101" s="5"/>
+      <c r="F101" s="5"/>
+      <c r="G101" s="5"/>
+      <c r="H101" s="5"/>
+      <c r="I101" s="5"/>
+      <c r="J101" s="5"/>
+      <c r="K101" s="5"/>
+      <c r="L101" s="5"/>
+      <c r="M101" s="5"/>
+      <c r="N101" s="5"/>
+      <c r="O101" s="5"/>
+      <c r="P101" s="5"/>
+      <c r="Q101" s="5"/>
+      <c r="R101" s="5"/>
+      <c r="S101" s="5"/>
+      <c r="T101" s="5"/>
+      <c r="U101" s="5"/>
+      <c r="V101" s="5"/>
+      <c r="W101" s="5"/>
+      <c r="X101" s="5"/>
+      <c r="Y101" s="5"/>
+      <c r="Z101" s="5"/>
+    </row>
+    <row r="102" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B102" s="5"/>
+      <c r="C102" s="5"/>
+      <c r="D102" s="5"/>
+      <c r="E102" s="5"/>
+      <c r="F102" s="5"/>
+      <c r="G102" s="5"/>
+      <c r="H102" s="5"/>
+      <c r="I102" s="5"/>
+      <c r="J102" s="5"/>
+      <c r="K102" s="5"/>
+      <c r="L102" s="5"/>
+      <c r="M102" s="5"/>
+      <c r="N102" s="5"/>
+      <c r="O102" s="5"/>
+      <c r="P102" s="5"/>
+      <c r="Q102" s="5"/>
+      <c r="R102" s="5"/>
+      <c r="S102" s="5"/>
+      <c r="T102" s="5"/>
+      <c r="U102" s="5"/>
+      <c r="V102" s="5"/>
+      <c r="W102" s="5"/>
+      <c r="X102" s="5"/>
+      <c r="Y102" s="5"/>
+      <c r="Z102" s="5"/>
+    </row>
+    <row r="103" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B103" s="5"/>
+      <c r="C103" s="5"/>
+      <c r="D103" s="5"/>
+      <c r="E103" s="5"/>
+      <c r="F103" s="5"/>
+      <c r="G103" s="5"/>
+      <c r="H103" s="5"/>
+      <c r="I103" s="5"/>
+      <c r="J103" s="5"/>
+      <c r="K103" s="5"/>
+      <c r="L103" s="5"/>
+      <c r="M103" s="5"/>
+      <c r="N103" s="5"/>
+      <c r="O103" s="5"/>
+      <c r="P103" s="5"/>
+      <c r="Q103" s="5"/>
+      <c r="R103" s="5"/>
+      <c r="S103" s="5"/>
+      <c r="T103" s="5"/>
+      <c r="U103" s="5"/>
+      <c r="V103" s="5"/>
+      <c r="W103" s="5"/>
+      <c r="X103" s="5"/>
+      <c r="Y103" s="5"/>
+      <c r="Z103" s="5"/>
+    </row>
+    <row r="104" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B104" s="5"/>
+      <c r="C104" s="5"/>
+      <c r="D104" s="5"/>
+      <c r="E104" s="5"/>
+      <c r="F104" s="5"/>
+      <c r="G104" s="5"/>
+      <c r="H104" s="5"/>
+      <c r="I104" s="5"/>
+      <c r="J104" s="5"/>
+      <c r="K104" s="5"/>
+      <c r="L104" s="5"/>
+      <c r="M104" s="5"/>
+      <c r="N104" s="5"/>
+      <c r="O104" s="5"/>
+      <c r="P104" s="5"/>
+      <c r="Q104" s="5"/>
+      <c r="R104" s="5"/>
+      <c r="S104" s="5"/>
+      <c r="T104" s="5"/>
+      <c r="U104" s="5"/>
+      <c r="V104" s="5"/>
+      <c r="W104" s="5"/>
+      <c r="X104" s="5"/>
+      <c r="Y104" s="5"/>
+      <c r="Z104" s="5"/>
+    </row>
+    <row r="105" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B105" s="5"/>
+      <c r="C105" s="5"/>
+      <c r="D105" s="5"/>
+      <c r="E105" s="5"/>
+      <c r="F105" s="5"/>
+      <c r="G105" s="5"/>
+      <c r="H105" s="5"/>
+      <c r="I105" s="5"/>
+      <c r="J105" s="5"/>
+      <c r="K105" s="5"/>
+      <c r="L105" s="5"/>
+      <c r="M105" s="5"/>
+      <c r="N105" s="5"/>
+      <c r="O105" s="5"/>
+      <c r="P105" s="5"/>
+      <c r="Q105" s="5"/>
+      <c r="R105" s="5"/>
+      <c r="S105" s="5"/>
+      <c r="T105" s="5"/>
+      <c r="U105" s="5"/>
+      <c r="V105" s="5"/>
+      <c r="W105" s="5"/>
+      <c r="X105" s="5"/>
+      <c r="Y105" s="5"/>
+      <c r="Z105" s="5"/>
+    </row>
+    <row r="106" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B106" s="5"/>
+      <c r="C106" s="5"/>
+      <c r="D106" s="5"/>
+      <c r="E106" s="5"/>
+      <c r="F106" s="5"/>
+      <c r="G106" s="5"/>
+      <c r="H106" s="5"/>
+      <c r="I106" s="5"/>
+      <c r="J106" s="5"/>
+      <c r="K106" s="5"/>
+      <c r="L106" s="5"/>
+      <c r="M106" s="5"/>
+      <c r="N106" s="5"/>
+      <c r="O106" s="5"/>
+      <c r="P106" s="5"/>
+      <c r="Q106" s="5"/>
+      <c r="R106" s="5"/>
+      <c r="S106" s="5"/>
+      <c r="T106" s="5"/>
+      <c r="U106" s="5"/>
+      <c r="V106" s="5"/>
+      <c r="W106" s="5"/>
+      <c r="X106" s="5"/>
+      <c r="Y106" s="5"/>
+      <c r="Z106" s="5"/>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="9">
-    <mergeCell ref="E73:H73"/>
+    <mergeCell ref="E80:H80"/>
     <mergeCell ref="P11:Q11"/>
     <mergeCell ref="S11:T11"/>
     <mergeCell ref="V11:W11"/>
@@ -5770,18 +6042,18 @@
     <mergeCell ref="J11:K11"/>
     <mergeCell ref="M11:N11"/>
   </mergeCells>
-  <conditionalFormatting sqref="E68">
-    <cfRule type="cellIs" dxfId="56" priority="193" operator="lessThan">
+  <conditionalFormatting sqref="E75">
+    <cfRule type="cellIs" dxfId="38" priority="211" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="194" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="212" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="195" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="36" priority="213" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H68">
+  <conditionalFormatting sqref="H75">
     <cfRule type="cellIs" dxfId="17" priority="16" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -5792,7 +6064,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K68">
+  <conditionalFormatting sqref="K75">
     <cfRule type="cellIs" dxfId="14" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -5803,7 +6075,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N68">
+  <conditionalFormatting sqref="N75">
     <cfRule type="cellIs" dxfId="11" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -5814,7 +6086,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q68">
+  <conditionalFormatting sqref="Q75">
     <cfRule type="cellIs" dxfId="8" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -5825,7 +6097,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T68">
+  <conditionalFormatting sqref="T75">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -5836,7 +6108,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W68">
+  <conditionalFormatting sqref="W75">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Const 55 CSK vs DC
</commit_message>
<xml_diff>
--- a/2022/EBE Boys 2022.xlsx
+++ b/2022/EBE Boys 2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2F10BF-BBE3-044E-88D8-13CC84127A74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9429F9-8168-9A41-BCD0-D41588804321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20420" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -4828,41 +4828,55 @@
       <c r="C67" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="D67" s="3" t="str">
+      <c r="D67" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E67, ($W67,$T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E67, ($W67,$T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E67" s="1"/>
-      <c r="G67" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="E67" s="1">
+        <v>50</v>
+      </c>
+      <c r="G67" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H67, ($W67,$T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H67, ($W67,$T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H67" s="1"/>
-      <c r="J67" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="H67" s="1">
+        <v>100</v>
+      </c>
+      <c r="J67" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K67, ($W67,$T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K67, ($W67,$T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K67" s="1"/>
-      <c r="M67" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="K67" s="1">
+        <v>0</v>
+      </c>
+      <c r="M67" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N67, ($W67,$T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N67, ($W67,$T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N67" s="1"/>
-      <c r="P67" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="N67" s="1">
+        <v>70</v>
+      </c>
+      <c r="P67" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q67, ($W67,$T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q67, ($W67,$T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q67" s="1"/>
-      <c r="S67" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="Q67" s="1">
+        <v>80</v>
+      </c>
+      <c r="S67" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T67, ($W67,$T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T67, ($W67,$T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T67" s="1"/>
-      <c r="V67" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="T67" s="1">
+        <v>60</v>
+      </c>
+      <c r="V67" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W67, ($W67,$T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W67, ($W67,$T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W67" s="1"/>
+        <v>-20</v>
+      </c>
+      <c r="W67" s="1">
+        <v>40</v>
+      </c>
     </row>
     <row r="68" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A68" s="6">
@@ -5178,21 +5192,21 @@
       </c>
       <c r="E75" s="12">
         <f>SUM(D13:D72)</f>
-        <v>-217.5</v>
+        <v>-232.5</v>
       </c>
       <c r="G75" s="7" t="s">
         <v>7</v>
       </c>
       <c r="H75" s="12">
         <f>SUM(G13:G72)</f>
-        <v>350</v>
+        <v>400</v>
       </c>
       <c r="J75" s="7" t="s">
         <v>7</v>
       </c>
       <c r="K75" s="12">
         <f>SUM(J13:J72)</f>
-        <v>-270</v>
+        <v>-295</v>
       </c>
       <c r="M75" s="7" t="s">
         <v>7</v>
@@ -5206,21 +5220,21 @@
       </c>
       <c r="Q75" s="12">
         <f>SUM(P13:P72)</f>
-        <v>155</v>
+        <v>175</v>
       </c>
       <c r="S75" s="7" t="s">
         <v>7</v>
       </c>
       <c r="T75" s="12">
         <f>SUM(S13:S72)</f>
-        <v>-217.5</v>
+        <v>-227.5</v>
       </c>
       <c r="V75" s="7" t="s">
         <v>7</v>
       </c>
       <c r="W75" s="12">
         <f>SUM(V13:V72)</f>
-        <v>-227.5</v>
+        <v>-247.5</v>
       </c>
       <c r="X75" s="1">
         <f>SUM(E75,H75,K75,N75,Q75,T75,W75)</f>

</xml_diff>

<commit_message>
Contest 56 MI vs KKR
</commit_message>
<xml_diff>
--- a/2022/EBE Boys 2022.xlsx
+++ b/2022/EBE Boys 2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9429F9-8168-9A41-BCD0-D41588804321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE1F4A1-71B9-584A-A793-287D92138DD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20420" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -4888,41 +4888,55 @@
       <c r="C68" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="D68" s="3" t="str">
+      <c r="D68" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E68, ($W68,$T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E68, ($W68,$T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E68" s="1"/>
-      <c r="G68" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="E68" s="1">
+        <v>0</v>
+      </c>
+      <c r="G68" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H68, ($W68,$T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H68, ($W68,$T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H68" s="1"/>
-      <c r="J68" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="H68" s="1">
+        <v>100</v>
+      </c>
+      <c r="J68" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K68, ($W68,$T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K68, ($W68,$T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K68" s="1"/>
-      <c r="M68" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="K68" s="1">
+        <v>50</v>
+      </c>
+      <c r="M68" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N68, ($W68,$T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N68, ($W68,$T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N68" s="1"/>
-      <c r="P68" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="N68" s="1">
+        <v>70</v>
+      </c>
+      <c r="P68" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q68, ($W68,$T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q68, ($W68,$T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q68" s="1"/>
-      <c r="S68" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="Q68" s="1">
+        <v>40</v>
+      </c>
+      <c r="S68" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T68, ($W68,$T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T68, ($W68,$T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T68" s="1"/>
-      <c r="V68" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="T68" s="1">
+        <v>80</v>
+      </c>
+      <c r="V68" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W68, ($W68,$T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W68, ($W68,$T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W68" s="1"/>
+        <v>-10</v>
+      </c>
+      <c r="W68" s="1">
+        <v>60</v>
+      </c>
     </row>
     <row r="69" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A69" s="6">
@@ -5192,21 +5206,21 @@
       </c>
       <c r="E75" s="12">
         <f>SUM(D13:D72)</f>
-        <v>-232.5</v>
+        <v>-257.5</v>
       </c>
       <c r="G75" s="7" t="s">
         <v>7</v>
       </c>
       <c r="H75" s="12">
         <f>SUM(G13:G72)</f>
-        <v>400</v>
+        <v>450</v>
       </c>
       <c r="J75" s="7" t="s">
         <v>7</v>
       </c>
       <c r="K75" s="12">
         <f>SUM(J13:J72)</f>
-        <v>-295</v>
+        <v>-310</v>
       </c>
       <c r="M75" s="7" t="s">
         <v>7</v>
@@ -5220,21 +5234,21 @@
       </c>
       <c r="Q75" s="12">
         <f>SUM(P13:P72)</f>
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="S75" s="7" t="s">
         <v>7</v>
       </c>
       <c r="T75" s="12">
         <f>SUM(S13:S72)</f>
-        <v>-227.5</v>
+        <v>-207.5</v>
       </c>
       <c r="V75" s="7" t="s">
         <v>7</v>
       </c>
       <c r="W75" s="12">
         <f>SUM(V13:V72)</f>
-        <v>-247.5</v>
+        <v>-257.5</v>
       </c>
       <c r="X75" s="1">
         <f>SUM(E75,H75,K75,N75,Q75,T75,W75)</f>

</xml_diff>

<commit_message>
Results contest 64 through 70.
</commit_message>
<xml_diff>
--- a/2022/EBE Boys 2022.xlsx
+++ b/2022/EBE Boys 2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE1F4A1-71B9-584A-A793-287D92138DD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D211A2D0-A1DF-4242-9A3C-6F1EA6A230C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20420" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="95">
   <si>
     <t>Points</t>
   </si>
@@ -286,6 +286,45 @@
   </si>
   <si>
     <t>RCB vs PBKS</t>
+  </si>
+  <si>
+    <t>KKR vs SRH</t>
+  </si>
+  <si>
+    <t>CSK vs GT</t>
+  </si>
+  <si>
+    <t>LSG vs RR</t>
+  </si>
+  <si>
+    <t>PBKS vs DC</t>
+  </si>
+  <si>
+    <t>MI vs SRH</t>
+  </si>
+  <si>
+    <t>KKR vs LSG</t>
+  </si>
+  <si>
+    <t>Qualifier 1</t>
+  </si>
+  <si>
+    <t>Eliminator</t>
+  </si>
+  <si>
+    <t>Qualifier 2</t>
+  </si>
+  <si>
+    <t>Finals</t>
+  </si>
+  <si>
+    <t>CSK vs RR</t>
+  </si>
+  <si>
+    <t>SRH vs PBKS</t>
+  </si>
+  <si>
+    <t>GT vs RR</t>
   </si>
 </sst>
 </file>
@@ -594,7 +633,367 @@
     <cellStyle name="20% - Accent6" xfId="1" builtinId="50"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="39">
+  <dxfs count="75">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1300,11 +1699,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
-  <dimension ref="A1:Z106"/>
+  <dimension ref="A1:Z120"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X75" sqref="X75"/>
+      <pane ySplit="11" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X89" sqref="X89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4698,7 +5097,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A65" s="6">
         <v>53</v>
       </c>
@@ -4758,7 +5157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A66" s="6">
         <v>54</v>
       </c>
@@ -4818,7 +5217,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A67" s="6">
         <v>55</v>
       </c>
@@ -4878,7 +5277,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A68" s="6">
         <v>56</v>
       </c>
@@ -4938,7 +5337,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A69" s="6">
         <v>57</v>
       </c>
@@ -4948,43 +5347,57 @@
       <c r="C69" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="D69" s="3" t="str">
+      <c r="D69" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E69, ($W69,$T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E69, ($W69,$T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E69" s="1"/>
-      <c r="G69" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="E69" s="1">
+        <v>50</v>
+      </c>
+      <c r="G69" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H69, ($W69,$T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H69, ($W69,$T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H69" s="1"/>
-      <c r="J69" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="H69" s="1">
+        <v>70</v>
+      </c>
+      <c r="J69" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K69, ($W69,$T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K69, ($W69,$T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K69" s="1"/>
-      <c r="M69" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="K69" s="1">
+        <v>100</v>
+      </c>
+      <c r="M69" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N69, ($W69,$T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N69, ($W69,$T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N69" s="1"/>
-      <c r="P69" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="N69" s="1">
+        <v>40</v>
+      </c>
+      <c r="P69" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q69, ($W69,$T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q69, ($W69,$T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q69" s="1"/>
-      <c r="S69" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="Q69" s="1">
+        <v>80</v>
+      </c>
+      <c r="S69" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T69, ($W69,$T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T69, ($W69,$T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T69" s="1"/>
-      <c r="V69" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="T69" s="1">
+        <v>0</v>
+      </c>
+      <c r="V69" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W69, ($W69,$T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W69, ($W69,$T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W69" s="1"/>
-    </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.2">
+        <v>-10</v>
+      </c>
+      <c r="W69" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="70" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A70" s="6">
         <v>58</v>
       </c>
@@ -4994,43 +5407,57 @@
       <c r="C70" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="D70" s="3" t="str">
+      <c r="D70" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E70, ($W70,$T70,$Q70,$N70,$K70,$H70,$E70), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E70, ($W70,$T70,$Q70,$N70,$K70,$H70,$E70), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E70" s="1"/>
-      <c r="G70" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="E70" s="1">
+        <v>80</v>
+      </c>
+      <c r="G70" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H70, ($W70,$T70,$Q70,$N70,$K70,$H70,$E70), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H70, ($W70,$T70,$Q70,$N70,$K70,$H70,$E70), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H70" s="1"/>
-      <c r="J70" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="H70" s="1">
+        <v>60</v>
+      </c>
+      <c r="J70" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K70, ($W70,$T70,$Q70,$N70,$K70,$H70,$E70), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K70, ($W70,$T70,$Q70,$N70,$K70,$H70,$E70), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K70" s="1"/>
-      <c r="M70" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="K70" s="1">
+        <v>50</v>
+      </c>
+      <c r="M70" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N70, ($W70,$T70,$Q70,$N70,$K70,$H70,$E70), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N70, ($W70,$T70,$Q70,$N70,$K70,$H70,$E70), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N70" s="1"/>
-      <c r="P70" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="N70" s="1">
+        <v>70</v>
+      </c>
+      <c r="P70" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q70, ($W70,$T70,$Q70,$N70,$K70,$H70,$E70), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q70, ($W70,$T70,$Q70,$N70,$K70,$H70,$E70), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q70" s="1"/>
-      <c r="S70" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="Q70" s="1">
+        <v>40</v>
+      </c>
+      <c r="S70" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T70, ($W70,$T70,$Q70,$N70,$K70,$H70,$E70), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T70, ($W70,$T70,$Q70,$N70,$K70,$H70,$E70), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T70" s="1"/>
-      <c r="V70" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="T70" s="1">
+        <v>100</v>
+      </c>
+      <c r="V70" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W70, ($W70,$T70,$Q70,$N70,$K70,$H70,$E70), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W70, ($W70,$T70,$Q70,$N70,$K70,$H70,$E70), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W70" s="1"/>
-    </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.2">
+        <v>-25</v>
+      </c>
+      <c r="W70" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A71" s="6">
         <v>59</v>
       </c>
@@ -5040,43 +5467,57 @@
       <c r="C71" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="D71" s="3" t="str">
+      <c r="D71" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E71, ($W71,$T71,$Q71,$N71,$K71,$H71,$E71), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E71, ($W71,$T71,$Q71,$N71,$K71,$H71,$E71), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E71" s="1"/>
-      <c r="G71" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="E71" s="1">
+        <v>80</v>
+      </c>
+      <c r="G71" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H71, ($W71,$T71,$Q71,$N71,$K71,$H71,$E71), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H71, ($W71,$T71,$Q71,$N71,$K71,$H71,$E71), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H71" s="1"/>
-      <c r="J71" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="H71" s="1">
+        <v>100</v>
+      </c>
+      <c r="J71" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K71, ($W71,$T71,$Q71,$N71,$K71,$H71,$E71), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K71, ($W71,$T71,$Q71,$N71,$K71,$H71,$E71), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K71" s="1"/>
-      <c r="M71" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K71" s="1">
+        <v>60</v>
+      </c>
+      <c r="M71" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N71, ($W71,$T71,$Q71,$N71,$K71,$H71,$E71), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N71, ($W71,$T71,$Q71,$N71,$K71,$H71,$E71), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N71" s="1"/>
-      <c r="P71" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="N71" s="1">
+        <v>0</v>
+      </c>
+      <c r="P71" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q71, ($W71,$T71,$Q71,$N71,$K71,$H71,$E71), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q71, ($W71,$T71,$Q71,$N71,$K71,$H71,$E71), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q71" s="1"/>
-      <c r="S71" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="Q71" s="1">
+        <v>50</v>
+      </c>
+      <c r="S71" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T71, ($W71,$T71,$Q71,$N71,$K71,$H71,$E71), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T71, ($W71,$T71,$Q71,$N71,$K71,$H71,$E71), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T71" s="1"/>
-      <c r="V71" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="T71" s="1">
+        <v>40</v>
+      </c>
+      <c r="V71" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W71, ($W71,$T71,$Q71,$N71,$K71,$H71,$E71), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W71, ($W71,$T71,$Q71,$N71,$K71,$H71,$E71), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W71" s="1"/>
-    </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="W71" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A72" s="6">
         <v>60</v>
       </c>
@@ -5086,573 +5527,986 @@
       <c r="C72" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="D72" s="3" t="str">
+      <c r="D72" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-10</v>
+      </c>
+      <c r="E72" s="1">
+        <v>60</v>
+      </c>
+      <c r="G72" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(H72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="H72" s="1">
+        <v>70</v>
+      </c>
+      <c r="J72" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(K72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-25</v>
+      </c>
+      <c r="K72" s="1">
+        <v>0</v>
+      </c>
+      <c r="M72" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(N72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>50</v>
+      </c>
+      <c r="N72" s="1">
+        <v>100</v>
+      </c>
+      <c r="P72" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>20</v>
+      </c>
+      <c r="Q72" s="1">
+        <v>80</v>
+      </c>
+      <c r="S72" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(T72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-15</v>
+      </c>
+      <c r="T72" s="1">
+        <v>50</v>
+      </c>
+      <c r="V72" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(W72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-20</v>
+      </c>
+      <c r="W72" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="73" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A73" s="6">
+        <v>61</v>
+      </c>
+      <c r="B73" s="1">
+        <v>1</v>
+      </c>
+      <c r="C73" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="D73" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(E73, ($W73,$T73,$Q73,$N73,$K73,$H73,$E73), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E73, ($W73,$T73,$Q73,$N73,$K73,$H73,$E73), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="E73" s="1">
+        <v>70</v>
+      </c>
+      <c r="G73" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(H73, ($W73,$T73,$Q73,$N73,$K73,$H73,$E73), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H73, ($W73,$T73,$Q73,$N73,$K73,$H73,$E73), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>20</v>
+      </c>
+      <c r="H73" s="1">
+        <v>80</v>
+      </c>
+      <c r="J73" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(K73, ($W73,$T73,$Q73,$N73,$K73,$H73,$E73), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K73, ($W73,$T73,$Q73,$N73,$K73,$H73,$E73), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-10</v>
+      </c>
+      <c r="K73" s="1">
+        <v>60</v>
+      </c>
+      <c r="M73" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(N73, ($W73,$T73,$Q73,$N73,$K73,$H73,$E73), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N73, ($W73,$T73,$Q73,$N73,$K73,$H73,$E73), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-25</v>
+      </c>
+      <c r="N73" s="1">
+        <v>0</v>
+      </c>
+      <c r="P73" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q73, ($W73,$T73,$Q73,$N73,$K73,$H73,$E73), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q73, ($W73,$T73,$Q73,$N73,$K73,$H73,$E73), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>50</v>
+      </c>
+      <c r="Q73" s="1">
+        <v>100</v>
+      </c>
+      <c r="S73" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(T73, ($W73,$T73,$Q73,$N73,$K73,$H73,$E73), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T73, ($W73,$T73,$Q73,$N73,$K73,$H73,$E73), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-20</v>
+      </c>
+      <c r="T73" s="1">
+        <v>40</v>
+      </c>
+      <c r="V73" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(W73, ($W73,$T73,$Q73,$N73,$K73,$H73,$E73), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W73, ($W73,$T73,$Q73,$N73,$K73,$H73,$E73), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-15</v>
+      </c>
+      <c r="W73" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="74" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A74" s="6">
+        <v>62</v>
+      </c>
+      <c r="B74" s="1">
+        <v>1</v>
+      </c>
+      <c r="C74" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D74" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(E74, ($W74,$T74,$Q74,$N74,$K74,$H74,$E74), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E74, ($W74,$T74,$Q74,$N74,$K74,$H74,$E74), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-25</v>
+      </c>
+      <c r="E74" s="1">
+        <v>0</v>
+      </c>
+      <c r="G74" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(H74, ($W74,$T74,$Q74,$N74,$K74,$H74,$E74), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H74, ($W74,$T74,$Q74,$N74,$K74,$H74,$E74), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-10</v>
+      </c>
+      <c r="H74" s="1">
+        <v>60</v>
+      </c>
+      <c r="J74" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(K74, ($W74,$T74,$Q74,$N74,$K74,$H74,$E74), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K74, ($W74,$T74,$Q74,$N74,$K74,$H74,$E74), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>50</v>
+      </c>
+      <c r="K74" s="1">
+        <v>100</v>
+      </c>
+      <c r="M74" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(N74, ($W74,$T74,$Q74,$N74,$K74,$H74,$E74), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N74, ($W74,$T74,$Q74,$N74,$K74,$H74,$E74), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="N74" s="1">
+        <v>70</v>
+      </c>
+      <c r="P74" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q74, ($W74,$T74,$Q74,$N74,$K74,$H74,$E74), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q74, ($W74,$T74,$Q74,$N74,$K74,$H74,$E74), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-15</v>
+      </c>
+      <c r="Q74" s="1">
+        <v>50</v>
+      </c>
+      <c r="S74" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(T74, ($W74,$T74,$Q74,$N74,$K74,$H74,$E74), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T74, ($W74,$T74,$Q74,$N74,$K74,$H74,$E74), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>20</v>
+      </c>
+      <c r="T74" s="1">
+        <v>80</v>
+      </c>
+      <c r="V74" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(W74, ($W74,$T74,$Q74,$N74,$K74,$H74,$E74), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W74, ($W74,$T74,$Q74,$N74,$K74,$H74,$E74), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-20</v>
+      </c>
+      <c r="W74" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="75" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A75" s="6">
+        <v>63</v>
+      </c>
+      <c r="B75" s="1">
+        <v>1</v>
+      </c>
+      <c r="C75" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D75" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(E75, ($W75,$T75,$Q75,$N75,$K75,$H75,$E75), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E75, ($W75,$T75,$Q75,$N75,$K75,$H75,$E75), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>50</v>
+      </c>
+      <c r="E75" s="1">
+        <v>100</v>
+      </c>
+      <c r="G75" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(H75, ($W75,$T75,$Q75,$N75,$K75,$H75,$E75), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H75, ($W75,$T75,$Q75,$N75,$K75,$H75,$E75), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-10</v>
+      </c>
+      <c r="H75" s="1">
+        <v>60</v>
+      </c>
+      <c r="J75" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(K75, ($W75,$T75,$Q75,$N75,$K75,$H75,$E75), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K75, ($W75,$T75,$Q75,$N75,$K75,$H75,$E75), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="K75" s="1">
+        <v>70</v>
+      </c>
+      <c r="M75" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(N75, ($W75,$T75,$Q75,$N75,$K75,$H75,$E75), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N75, ($W75,$T75,$Q75,$N75,$K75,$H75,$E75), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-25</v>
+      </c>
+      <c r="N75" s="1">
+        <v>0</v>
+      </c>
+      <c r="P75" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q75, ($W75,$T75,$Q75,$N75,$K75,$H75,$E75), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q75, ($W75,$T75,$Q75,$N75,$K75,$H75,$E75), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-20</v>
+      </c>
+      <c r="Q75" s="1">
+        <v>40</v>
+      </c>
+      <c r="S75" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(T75, ($W75,$T75,$Q75,$N75,$K75,$H75,$E75), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T75, ($W75,$T75,$Q75,$N75,$K75,$H75,$E75), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>20</v>
+      </c>
+      <c r="T75" s="1">
+        <v>80</v>
+      </c>
+      <c r="V75" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(W75, ($W75,$T75,$Q75,$N75,$K75,$H75,$E75), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W75, ($W75,$T75,$Q75,$N75,$K75,$H75,$E75), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-15</v>
+      </c>
+      <c r="W75" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="76" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A76" s="6">
+        <v>64</v>
+      </c>
+      <c r="B76" s="1">
+        <v>1</v>
+      </c>
+      <c r="C76" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D76" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(E76, ($W76,$T76,$Q76,$N76,$K76,$H76,$E76), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E76, ($W76,$T76,$Q76,$N76,$K76,$H76,$E76), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-15</v>
+      </c>
+      <c r="E76" s="1">
+        <v>50</v>
+      </c>
+      <c r="G76" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(H76, ($W76,$T76,$Q76,$N76,$K76,$H76,$E76), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H76, ($W76,$T76,$Q76,$N76,$K76,$H76,$E76), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-20</v>
+      </c>
+      <c r="H76" s="1">
+        <v>40</v>
+      </c>
+      <c r="J76" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(K76, ($W76,$T76,$Q76,$N76,$K76,$H76,$E76), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K76, ($W76,$T76,$Q76,$N76,$K76,$H76,$E76), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="K76" s="1">
+        <v>70</v>
+      </c>
+      <c r="M76" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(N76, ($W76,$T76,$Q76,$N76,$K76,$H76,$E76), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N76, ($W76,$T76,$Q76,$N76,$K76,$H76,$E76), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-25</v>
+      </c>
+      <c r="N76" s="1">
+        <v>0</v>
+      </c>
+      <c r="P76" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q76, ($W76,$T76,$Q76,$N76,$K76,$H76,$E76), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q76, ($W76,$T76,$Q76,$N76,$K76,$H76,$E76), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>20</v>
+      </c>
+      <c r="Q76" s="1">
+        <v>80</v>
+      </c>
+      <c r="S76" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(T76, ($W76,$T76,$Q76,$N76,$K76,$H76,$E76), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T76, ($W76,$T76,$Q76,$N76,$K76,$H76,$E76), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>50</v>
+      </c>
+      <c r="T76" s="1">
+        <v>100</v>
+      </c>
+      <c r="V76" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(W76, ($W76,$T76,$Q76,$N76,$K76,$H76,$E76), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W76, ($W76,$T76,$Q76,$N76,$K76,$H76,$E76), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-10</v>
+      </c>
+      <c r="W76" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="77" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A77" s="6">
+        <v>65</v>
+      </c>
+      <c r="B77" s="1">
+        <v>1</v>
+      </c>
+      <c r="C77" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D77" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(E77, ($W77,$T77,$Q77,$N77,$K77,$H77,$E77), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E77, ($W77,$T77,$Q77,$N77,$K77,$H77,$E77), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-15</v>
+      </c>
+      <c r="E77" s="1">
+        <v>50</v>
+      </c>
+      <c r="G77" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(H77, ($W77,$T77,$Q77,$N77,$K77,$H77,$E77), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H77, ($W77,$T77,$Q77,$N77,$K77,$H77,$E77), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="H77" s="1">
+        <v>70</v>
+      </c>
+      <c r="J77" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(K77, ($W77,$T77,$Q77,$N77,$K77,$H77,$E77), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K77, ($W77,$T77,$Q77,$N77,$K77,$H77,$E77), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-20</v>
+      </c>
+      <c r="K77" s="1">
+        <v>40</v>
+      </c>
+      <c r="M77" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(N77, ($W77,$T77,$Q77,$N77,$K77,$H77,$E77), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N77, ($W77,$T77,$Q77,$N77,$K77,$H77,$E77), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>50</v>
+      </c>
+      <c r="N77" s="1">
+        <v>100</v>
+      </c>
+      <c r="P77" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q77, ($W77,$T77,$Q77,$N77,$K77,$H77,$E77), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q77, ($W77,$T77,$Q77,$N77,$K77,$H77,$E77), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-25</v>
+      </c>
+      <c r="Q77" s="1">
+        <v>0</v>
+      </c>
+      <c r="S77" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(T77, ($W77,$T77,$Q77,$N77,$K77,$H77,$E77), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T77, ($W77,$T77,$Q77,$N77,$K77,$H77,$E77), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>20</v>
+      </c>
+      <c r="T77" s="1">
+        <v>80</v>
+      </c>
+      <c r="V77" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(W77, ($W77,$T77,$Q77,$N77,$K77,$H77,$E77), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W77, ($W77,$T77,$Q77,$N77,$K77,$H77,$E77), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-10</v>
+      </c>
+      <c r="W77" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="78" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A78" s="6">
+        <v>66</v>
+      </c>
+      <c r="B78" s="1">
+        <v>1</v>
+      </c>
+      <c r="C78" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D78" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(E78, ($W78,$T78,$Q78,$N78,$K78,$H78,$E78), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E78, ($W78,$T78,$Q78,$N78,$K78,$H78,$E78), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-15</v>
+      </c>
+      <c r="E78" s="1">
+        <v>50</v>
+      </c>
+      <c r="G78" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(H78, ($W78,$T78,$Q78,$N78,$K78,$H78,$E78), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H78, ($W78,$T78,$Q78,$N78,$K78,$H78,$E78), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="H78" s="1">
+        <v>70</v>
+      </c>
+      <c r="J78" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(K78, ($W78,$T78,$Q78,$N78,$K78,$H78,$E78), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K78, ($W78,$T78,$Q78,$N78,$K78,$H78,$E78), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>50</v>
+      </c>
+      <c r="K78" s="1">
+        <v>100</v>
+      </c>
+      <c r="M78" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(N78, ($W78,$T78,$Q78,$N78,$K78,$H78,$E78), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N78, ($W78,$T78,$Q78,$N78,$K78,$H78,$E78), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>20</v>
+      </c>
+      <c r="N78" s="1">
+        <v>80</v>
+      </c>
+      <c r="P78" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q78, ($W78,$T78,$Q78,$N78,$K78,$H78,$E78), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q78, ($W78,$T78,$Q78,$N78,$K78,$H78,$E78), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-20</v>
+      </c>
+      <c r="Q78" s="1">
+        <v>40</v>
+      </c>
+      <c r="S78" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(T78, ($W78,$T78,$Q78,$N78,$K78,$H78,$E78), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T78, ($W78,$T78,$Q78,$N78,$K78,$H78,$E78), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-10</v>
+      </c>
+      <c r="T78" s="1">
+        <v>60</v>
+      </c>
+      <c r="V78" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(W78, ($W78,$T78,$Q78,$N78,$K78,$H78,$E78), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W78, ($W78,$T78,$Q78,$N78,$K78,$H78,$E78), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-25</v>
+      </c>
+      <c r="W78" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A79" s="6">
+        <v>67</v>
+      </c>
+      <c r="B79" s="1">
+        <v>1</v>
+      </c>
+      <c r="C79" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="D79" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(E79, ($W79,$T79,$Q79,$N79,$K79,$H79,$E79), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E79, ($W79,$T79,$Q79,$N79,$K79,$H79,$E79), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>20</v>
+      </c>
+      <c r="E79" s="1">
+        <v>80</v>
+      </c>
+      <c r="G79" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(H79, ($W79,$T79,$Q79,$N79,$K79,$H79,$E79), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H79, ($W79,$T79,$Q79,$N79,$K79,$H79,$E79), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="H79" s="1">
+        <v>70</v>
+      </c>
+      <c r="J79" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(K79, ($W79,$T79,$Q79,$N79,$K79,$H79,$E79), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K79, ($W79,$T79,$Q79,$N79,$K79,$H79,$E79), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>50</v>
+      </c>
+      <c r="K79" s="1">
+        <v>100</v>
+      </c>
+      <c r="M79" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(N79, ($W79,$T79,$Q79,$N79,$K79,$H79,$E79), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N79, ($W79,$T79,$Q79,$N79,$K79,$H79,$E79), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-25</v>
+      </c>
+      <c r="N79" s="1">
+        <v>0</v>
+      </c>
+      <c r="P79" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q79, ($W79,$T79,$Q79,$N79,$K79,$H79,$E79), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q79, ($W79,$T79,$Q79,$N79,$K79,$H79,$E79), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-10</v>
+      </c>
+      <c r="Q79" s="1">
+        <v>60</v>
+      </c>
+      <c r="S79" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(T79, ($W79,$T79,$Q79,$N79,$K79,$H79,$E79), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T79, ($W79,$T79,$Q79,$N79,$K79,$H79,$E79), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-20</v>
+      </c>
+      <c r="T79" s="1">
+        <v>40</v>
+      </c>
+      <c r="V79" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(W79, ($W79,$T79,$Q79,$N79,$K79,$H79,$E79), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W79, ($W79,$T79,$Q79,$N79,$K79,$H79,$E79), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-15</v>
+      </c>
+      <c r="W79" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="80" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A80" s="6">
+        <v>68</v>
+      </c>
+      <c r="B80" s="1">
+        <v>1</v>
+      </c>
+      <c r="C80" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="D80" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(E80, ($W80,$T80,$Q80,$N80,$K80,$H80,$E80), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E80, ($W80,$T80,$Q80,$N80,$K80,$H80,$E80), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-15</v>
+      </c>
+      <c r="E80" s="1">
+        <v>50</v>
+      </c>
+      <c r="G80" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(H80, ($W80,$T80,$Q80,$N80,$K80,$H80,$E80), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H80, ($W80,$T80,$Q80,$N80,$K80,$H80,$E80), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>20</v>
+      </c>
+      <c r="H80" s="1">
+        <v>80</v>
+      </c>
+      <c r="J80" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(K80, ($W80,$T80,$Q80,$N80,$K80,$H80,$E80), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K80, ($W80,$T80,$Q80,$N80,$K80,$H80,$E80), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="K80" s="1">
+        <v>70</v>
+      </c>
+      <c r="M80" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(N80, ($W80,$T80,$Q80,$N80,$K80,$H80,$E80), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N80, ($W80,$T80,$Q80,$N80,$K80,$H80,$E80), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-25</v>
+      </c>
+      <c r="N80" s="1">
+        <v>0</v>
+      </c>
+      <c r="P80" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q80, ($W80,$T80,$Q80,$N80,$K80,$H80,$E80), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q80, ($W80,$T80,$Q80,$N80,$K80,$H80,$E80), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-10</v>
+      </c>
+      <c r="Q80" s="1">
+        <v>60</v>
+      </c>
+      <c r="S80" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(T80, ($W80,$T80,$Q80,$N80,$K80,$H80,$E80), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T80, ($W80,$T80,$Q80,$N80,$K80,$H80,$E80), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-20</v>
+      </c>
+      <c r="T80" s="1">
+        <v>40</v>
+      </c>
+      <c r="V80" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(W80, ($W80,$T80,$Q80,$N80,$K80,$H80,$E80), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W80, ($W80,$T80,$Q80,$N80,$K80,$H80,$E80), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>50</v>
+      </c>
+      <c r="W80" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="81" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A81" s="6">
+        <v>69</v>
+      </c>
+      <c r="B81" s="1">
+        <v>1</v>
+      </c>
+      <c r="C81" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D81" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(E81, ($W81,$T81,$Q81,$N81,$K81,$H81,$E81), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E81, ($W81,$T81,$Q81,$N81,$K81,$H81,$E81), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-20</v>
+      </c>
+      <c r="E81" s="1">
+        <v>40</v>
+      </c>
+      <c r="G81" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(H81, ($W81,$T81,$Q81,$N81,$K81,$H81,$E81), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H81, ($W81,$T81,$Q81,$N81,$K81,$H81,$E81), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-25</v>
+      </c>
+      <c r="H81" s="1">
+        <v>0</v>
+      </c>
+      <c r="J81" s="3">
+        <v>23.34</v>
+      </c>
+      <c r="K81" s="1">
+        <v>100</v>
+      </c>
+      <c r="M81" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(N81, ($W81,$T81,$Q81,$N81,$K81,$H81,$E81), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N81, ($W81,$T81,$Q81,$N81,$K81,$H81,$E81), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-10</v>
+      </c>
+      <c r="N81" s="1">
+        <v>60</v>
+      </c>
+      <c r="P81" s="3">
+        <v>23.33</v>
+      </c>
+      <c r="Q81" s="1">
+        <v>100</v>
+      </c>
+      <c r="S81" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(T81, ($W81,$T81,$Q81,$N81,$K81,$H81,$E81), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T81, ($W81,$T81,$Q81,$N81,$K81,$H81,$E81), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-15</v>
+      </c>
+      <c r="T81" s="1">
+        <v>50</v>
+      </c>
+      <c r="V81" s="3">
+        <v>23.33</v>
+      </c>
+      <c r="W81" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="82" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A82" s="6">
+        <v>70</v>
+      </c>
+      <c r="B82" s="1">
+        <v>1</v>
+      </c>
+      <c r="C82" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D82" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(E82, ($W82,$T82,$Q82,$N82,$K82,$H82,$E82), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E82, ($W82,$T82,$Q82,$N82,$K82,$H82,$E82), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>50</v>
+      </c>
+      <c r="E82" s="1">
+        <v>100</v>
+      </c>
+      <c r="G82" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(H82, ($W82,$T82,$Q82,$N82,$K82,$H82,$E82), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H82, ($W82,$T82,$Q82,$N82,$K82,$H82,$E82), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>20</v>
+      </c>
+      <c r="H82" s="1">
+        <v>80</v>
+      </c>
+      <c r="J82" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(K82, ($W82,$T82,$Q82,$N82,$K82,$H82,$E82), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K82, ($W82,$T82,$Q82,$N82,$K82,$H82,$E82), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-15</v>
+      </c>
+      <c r="K82" s="1">
+        <v>50</v>
+      </c>
+      <c r="M82" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(N82, ($W82,$T82,$Q82,$N82,$K82,$H82,$E82), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N82, ($W82,$T82,$Q82,$N82,$K82,$H82,$E82), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-10</v>
+      </c>
+      <c r="N82" s="1">
+        <v>60</v>
+      </c>
+      <c r="P82" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q82, ($W82,$T82,$Q82,$N82,$K82,$H82,$E82), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q82, ($W82,$T82,$Q82,$N82,$K82,$H82,$E82), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-25</v>
+      </c>
+      <c r="Q82" s="1">
+        <v>0</v>
+      </c>
+      <c r="S82" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(T82, ($W82,$T82,$Q82,$N82,$K82,$H82,$E82), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T82, ($W82,$T82,$Q82,$N82,$K82,$H82,$E82), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="T82" s="1">
+        <v>70</v>
+      </c>
+      <c r="V82" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(W82, ($W82,$T82,$Q82,$N82,$K82,$H82,$E82), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W82, ($W82,$T82,$Q82,$N82,$K82,$H82,$E82), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v>-20</v>
+      </c>
+      <c r="W82" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="83" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A83" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B83" s="1">
+        <v>1</v>
+      </c>
+      <c r="C83" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="D83" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E83, ($W83,$T83,$Q83,$N83,$K83,$H83,$E83), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E83, ($W83,$T83,$Q83,$N83,$K83,$H83,$E83), 0),  $A$2:$B$10, 2, FALSE))</f>
         <v/>
       </c>
-      <c r="E72" s="1"/>
-      <c r="G72" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(H72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE))</f>
+      <c r="E83" s="1"/>
+      <c r="G83" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H83, ($W83,$T83,$Q83,$N83,$K83,$H83,$E83), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H83, ($W83,$T83,$Q83,$N83,$K83,$H83,$E83), 0),  $A$2:$B$10, 2, FALSE))</f>
         <v/>
       </c>
-      <c r="H72" s="1"/>
-      <c r="J72" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(K72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE))</f>
+      <c r="H83" s="1"/>
+      <c r="J83" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K83, ($W83,$T83,$Q83,$N83,$K83,$H83,$E83), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K83, ($W83,$T83,$Q83,$N83,$K83,$H83,$E83), 0),  $A$2:$B$10, 2, FALSE))</f>
         <v/>
       </c>
-      <c r="K72" s="1"/>
-      <c r="M72" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(N72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE))</f>
+      <c r="K83" s="1"/>
+      <c r="M83" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N83, ($W83,$T83,$Q83,$N83,$K83,$H83,$E83), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N83, ($W83,$T83,$Q83,$N83,$K83,$H83,$E83), 0),  $A$2:$B$10, 2, FALSE))</f>
         <v/>
       </c>
-      <c r="N72" s="1"/>
-      <c r="P72" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(Q72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE))</f>
+      <c r="N83" s="1"/>
+      <c r="P83" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q83, ($W83,$T83,$Q83,$N83,$K83,$H83,$E83), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q83, ($W83,$T83,$Q83,$N83,$K83,$H83,$E83), 0),  $A$2:$B$10, 2, FALSE))</f>
         <v/>
       </c>
-      <c r="Q72" s="1"/>
-      <c r="S72" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(T72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE))</f>
+      <c r="Q83" s="1"/>
+      <c r="S83" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T83, ($W83,$T83,$Q83,$N83,$K83,$H83,$E83), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T83, ($W83,$T83,$Q83,$N83,$K83,$H83,$E83), 0),  $A$2:$B$10, 2, FALSE))</f>
         <v/>
       </c>
-      <c r="T72" s="1"/>
-      <c r="V72" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(W72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W72, ($W72,$T72,$Q72,$N72,$K72,$H72,$E72), 0),  $A$2:$B$10, 2, FALSE))</f>
+      <c r="T83" s="1"/>
+      <c r="V83" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W83, ($W83,$T83,$Q83,$N83,$K83,$H83,$E83), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W83, ($W83,$T83,$Q83,$N83,$K83,$H83,$E83), 0),  $A$2:$B$10, 2, FALSE))</f>
         <v/>
       </c>
-      <c r="W72" s="1"/>
-    </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A73" s="6"/>
-      <c r="B73" s="1" t="s">
+      <c r="W83" s="1"/>
+    </row>
+    <row r="84" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A84" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B84" s="1">
+        <v>1</v>
+      </c>
+      <c r="C84" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D84" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E84, ($W84,$T84,$Q84,$N84,$K84,$H84,$E84), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E84, ($W84,$T84,$Q84,$N84,$K84,$H84,$E84), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E84" s="1"/>
+      <c r="G84" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H84, ($W84,$T84,$Q84,$N84,$K84,$H84,$E84), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H84, ($W84,$T84,$Q84,$N84,$K84,$H84,$E84), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H84" s="1"/>
+      <c r="J84" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K84, ($W84,$T84,$Q84,$N84,$K84,$H84,$E84), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K84, ($W84,$T84,$Q84,$N84,$K84,$H84,$E84), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K84" s="1"/>
+      <c r="M84" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N84, ($W84,$T84,$Q84,$N84,$K84,$H84,$E84), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N84, ($W84,$T84,$Q84,$N84,$K84,$H84,$E84), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N84" s="1"/>
+      <c r="P84" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q84, ($W84,$T84,$Q84,$N84,$K84,$H84,$E84), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q84, ($W84,$T84,$Q84,$N84,$K84,$H84,$E84), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q84" s="1"/>
+      <c r="S84" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T84, ($W84,$T84,$Q84,$N84,$K84,$H84,$E84), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T84, ($W84,$T84,$Q84,$N84,$K84,$H84,$E84), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T84" s="1"/>
+      <c r="V84" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W84, ($W84,$T84,$Q84,$N84,$K84,$H84,$E84), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W84, ($W84,$T84,$Q84,$N84,$K84,$H84,$E84), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="W84" s="1"/>
+    </row>
+    <row r="85" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A85" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B85" s="1">
+        <v>1</v>
+      </c>
+      <c r="C85" s="15"/>
+      <c r="D85" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E85, ($W85,$T85,$Q85,$N85,$K85,$H85,$E85), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E85, ($W85,$T85,$Q85,$N85,$K85,$H85,$E85), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E85" s="1"/>
+      <c r="G85" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H85, ($W85,$T85,$Q85,$N85,$K85,$H85,$E85), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H85, ($W85,$T85,$Q85,$N85,$K85,$H85,$E85), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H85" s="1"/>
+      <c r="J85" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K85, ($W85,$T85,$Q85,$N85,$K85,$H85,$E85), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K85, ($W85,$T85,$Q85,$N85,$K85,$H85,$E85), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K85" s="1"/>
+      <c r="M85" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N85, ($W85,$T85,$Q85,$N85,$K85,$H85,$E85), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N85, ($W85,$T85,$Q85,$N85,$K85,$H85,$E85), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N85" s="1"/>
+      <c r="P85" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q85, ($W85,$T85,$Q85,$N85,$K85,$H85,$E85), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q85, ($W85,$T85,$Q85,$N85,$K85,$H85,$E85), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q85" s="1"/>
+      <c r="S85" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T85, ($W85,$T85,$Q85,$N85,$K85,$H85,$E85), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T85, ($W85,$T85,$Q85,$N85,$K85,$H85,$E85), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T85" s="1"/>
+      <c r="V85" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W85, ($W85,$T85,$Q85,$N85,$K85,$H85,$E85), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W85, ($W85,$T85,$Q85,$N85,$K85,$H85,$E85), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="W85" s="1"/>
+    </row>
+    <row r="86" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A86" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B86" s="1">
+        <v>1</v>
+      </c>
+      <c r="C86" s="15"/>
+      <c r="D86" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E86, ($W86,$T86,$Q86,$N86,$K86,$H86,$E86), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E86, ($W86,$T86,$Q86,$N86,$K86,$H86,$E86), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E86" s="1"/>
+      <c r="G86" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H86, ($W86,$T86,$Q86,$N86,$K86,$H86,$E86), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H86, ($W86,$T86,$Q86,$N86,$K86,$H86,$E86), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H86" s="1"/>
+      <c r="J86" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K86, ($W86,$T86,$Q86,$N86,$K86,$H86,$E86), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K86, ($W86,$T86,$Q86,$N86,$K86,$H86,$E86), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K86" s="1"/>
+      <c r="M86" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N86, ($W86,$T86,$Q86,$N86,$K86,$H86,$E86), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N86, ($W86,$T86,$Q86,$N86,$K86,$H86,$E86), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N86" s="1"/>
+      <c r="P86" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q86, ($W86,$T86,$Q86,$N86,$K86,$H86,$E86), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q86, ($W86,$T86,$Q86,$N86,$K86,$H86,$E86), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q86" s="1"/>
+      <c r="S86" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T86, ($W86,$T86,$Q86,$N86,$K86,$H86,$E86), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T86, ($W86,$T86,$Q86,$N86,$K86,$H86,$E86), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T86" s="1"/>
+      <c r="V86" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(W86, ($W86,$T86,$Q86,$N86,$K86,$H86,$E86), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W86, ($W86,$T86,$Q86,$N86,$K86,$H86,$E86), 0),  $A$2:$B$10, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="W86" s="1"/>
+    </row>
+    <row r="87" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A87" s="6"/>
+      <c r="B87" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C73" s="10"/>
-      <c r="D73" s="1"/>
-      <c r="E73" s="9" t="s">
+      <c r="C87" s="10"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G73" s="1"/>
-      <c r="H73" s="9" t="s">
+      <c r="G87" s="1"/>
+      <c r="H87" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J73" s="1"/>
-      <c r="K73" s="9" t="s">
+      <c r="J87" s="1"/>
+      <c r="K87" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="M73" s="1"/>
-      <c r="N73" s="9" t="s">
+      <c r="M87" s="1"/>
+      <c r="N87" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="P73" s="1"/>
-      <c r="Q73" s="9" t="s">
+      <c r="P87" s="1"/>
+      <c r="Q87" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="S73" s="1"/>
-      <c r="T73" s="9" t="s">
+      <c r="S87" s="1"/>
+      <c r="T87" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="V73" s="1"/>
-      <c r="W73" s="9" t="s">
+      <c r="V87" s="1"/>
+      <c r="W87" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A74" s="5"/>
-      <c r="B74" s="5"/>
-      <c r="C74" s="5"/>
-      <c r="D74" s="1"/>
-      <c r="E74" s="11" t="str">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A88" s="5"/>
+      <c r="B88" s="5"/>
+      <c r="C88" s="5"/>
+      <c r="D88" s="1"/>
+      <c r="E88" s="11" t="str">
         <f>D12</f>
         <v>Jaya</v>
       </c>
-      <c r="G74" s="1"/>
-      <c r="H74" s="11" t="str">
+      <c r="G88" s="1"/>
+      <c r="H88" s="11" t="str">
         <f>G12</f>
         <v>Justin</v>
       </c>
-      <c r="J74" s="1"/>
-      <c r="K74" s="11" t="str">
+      <c r="J88" s="1"/>
+      <c r="K88" s="11" t="str">
         <f>J12</f>
         <v>Ram</v>
       </c>
-      <c r="M74" s="1"/>
-      <c r="N74" s="11" t="str">
+      <c r="M88" s="1"/>
+      <c r="N88" s="11" t="str">
         <f>M12</f>
         <v>Sibi</v>
       </c>
-      <c r="P74" s="1"/>
-      <c r="Q74" s="11" t="str">
+      <c r="P88" s="1"/>
+      <c r="Q88" s="11" t="str">
         <f>P12</f>
         <v>Sundar</v>
       </c>
-      <c r="S74" s="1"/>
-      <c r="T74" s="11" t="str">
+      <c r="S88" s="1"/>
+      <c r="T88" s="11" t="str">
         <f>S12</f>
         <v>Upili</v>
       </c>
-      <c r="V74" s="1"/>
-      <c r="W74" s="11" t="str">
+      <c r="V88" s="1"/>
+      <c r="W88" s="11" t="str">
         <f>V12</f>
         <v>Vicky</v>
       </c>
     </row>
-    <row r="75" spans="1:26" ht="21" x14ac:dyDescent="0.25">
-      <c r="A75" s="5"/>
-      <c r="B75" s="5"/>
-      <c r="C75" s="5"/>
-      <c r="D75" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E75" s="12">
-        <f>SUM(D13:D72)</f>
-        <v>-257.5</v>
-      </c>
-      <c r="G75" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H75" s="12">
-        <f>SUM(G13:G72)</f>
-        <v>450</v>
-      </c>
-      <c r="J75" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="K75" s="12">
-        <f>SUM(J13:J72)</f>
-        <v>-310</v>
-      </c>
-      <c r="M75" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="N75" s="12">
-        <f>SUM(M13:M72)</f>
-        <v>427.5</v>
-      </c>
-      <c r="P75" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q75" s="12">
-        <f>SUM(P13:P72)</f>
-        <v>155</v>
-      </c>
-      <c r="S75" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="T75" s="12">
-        <f>SUM(S13:S72)</f>
-        <v>-207.5</v>
-      </c>
-      <c r="V75" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="W75" s="12">
-        <f>SUM(V13:V72)</f>
-        <v>-257.5</v>
-      </c>
-      <c r="X75" s="1">
-        <f>SUM(E75,H75,K75,N75,Q75,T75,W75)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A76" s="5"/>
-      <c r="B76" s="5"/>
-      <c r="C76" s="5"/>
-      <c r="D76" s="5"/>
-      <c r="E76" s="5"/>
-      <c r="S76" s="5"/>
-      <c r="T76" s="5"/>
-    </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A77" s="5"/>
-      <c r="B77" s="5"/>
-      <c r="C77" s="5"/>
-      <c r="D77" s="5"/>
-      <c r="E77" s="5"/>
-      <c r="S77" s="5"/>
-      <c r="T77" s="5"/>
-    </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A78" s="5"/>
-      <c r="B78" s="5"/>
-      <c r="C78" s="5"/>
-      <c r="D78" s="5"/>
-      <c r="E78" s="5"/>
-      <c r="F78" s="5"/>
-      <c r="G78" s="5"/>
-      <c r="H78" s="5"/>
-      <c r="I78" s="5"/>
-      <c r="J78" s="5"/>
-      <c r="K78" s="5"/>
-      <c r="L78" s="5"/>
-      <c r="M78" s="5"/>
-      <c r="N78" s="5"/>
-      <c r="O78" s="5"/>
-      <c r="P78" s="5"/>
-      <c r="Q78" s="5"/>
-      <c r="R78" s="5"/>
-      <c r="S78" s="5"/>
-      <c r="T78" s="5"/>
-      <c r="U78" s="5"/>
-      <c r="V78" s="5"/>
-      <c r="W78" s="5"/>
-      <c r="X78" s="5"/>
-      <c r="Y78" s="5"/>
-      <c r="Z78" s="5"/>
-    </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="B79" s="5"/>
-      <c r="C79" s="5"/>
-      <c r="D79" s="5"/>
-      <c r="E79" s="5"/>
-      <c r="F79" s="5"/>
-      <c r="G79" s="5"/>
-      <c r="H79" s="5"/>
-      <c r="I79" s="5"/>
-      <c r="J79" s="5"/>
-      <c r="K79" s="5"/>
-      <c r="L79" s="5"/>
-      <c r="M79" s="5"/>
-      <c r="N79" s="5"/>
-      <c r="O79" s="5"/>
-      <c r="P79" s="5"/>
-      <c r="Q79" s="5"/>
-      <c r="R79" s="5"/>
-      <c r="S79" s="5"/>
-      <c r="T79" s="5"/>
-      <c r="U79" s="5"/>
-      <c r="V79" s="5"/>
-      <c r="W79" s="5"/>
-      <c r="X79" s="5"/>
-      <c r="Y79" s="5"/>
-      <c r="Z79" s="5"/>
-    </row>
-    <row r="80" spans="1:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="B80" s="5"/>
-      <c r="C80" s="5"/>
-      <c r="D80" s="5"/>
-      <c r="E80" s="20"/>
-      <c r="F80" s="20"/>
-      <c r="G80" s="20"/>
-      <c r="H80" s="20"/>
-      <c r="I80" s="16"/>
-      <c r="J80" s="5"/>
-      <c r="K80" s="5"/>
-      <c r="L80" s="5"/>
-      <c r="M80" s="5"/>
-      <c r="N80" s="5"/>
-      <c r="O80" s="5"/>
-      <c r="P80" s="5"/>
-      <c r="Q80" s="5"/>
-      <c r="R80" s="5"/>
-      <c r="S80" s="5"/>
-      <c r="T80" s="5"/>
-      <c r="U80" s="5"/>
-      <c r="V80" s="5"/>
-      <c r="W80" s="5"/>
-      <c r="X80" s="5"/>
-      <c r="Y80" s="5"/>
-      <c r="Z80" s="5"/>
-    </row>
-    <row r="81" spans="2:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="B81" s="5"/>
-      <c r="C81" s="5"/>
-      <c r="D81" s="5"/>
-      <c r="E81" s="17"/>
-      <c r="F81" s="17"/>
-      <c r="G81" s="17"/>
-      <c r="H81" s="17"/>
-      <c r="I81" s="18"/>
-      <c r="J81" s="5"/>
-      <c r="K81" s="5"/>
-      <c r="L81" s="5"/>
-      <c r="M81" s="5"/>
-      <c r="N81" s="5"/>
-      <c r="O81" s="5"/>
-      <c r="P81" s="5"/>
-      <c r="Q81" s="5"/>
-      <c r="R81" s="5"/>
-      <c r="S81" s="5"/>
-      <c r="T81" s="5"/>
-      <c r="U81" s="5"/>
-      <c r="V81" s="5"/>
-      <c r="W81" s="5"/>
-      <c r="X81" s="5"/>
-      <c r="Y81" s="5"/>
-      <c r="Z81" s="5"/>
-    </row>
-    <row r="82" spans="2:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="B82" s="5"/>
-      <c r="C82" s="5"/>
-      <c r="D82" s="17"/>
-      <c r="E82" s="5"/>
-      <c r="F82" s="5"/>
-      <c r="G82" s="5"/>
-      <c r="H82" s="5"/>
-      <c r="I82" s="17"/>
-      <c r="J82" s="5"/>
-      <c r="K82" s="5"/>
-      <c r="L82" s="5"/>
-      <c r="M82" s="5"/>
-      <c r="N82" s="5"/>
-      <c r="O82" s="5"/>
-      <c r="P82" s="5"/>
-      <c r="Q82" s="5"/>
-      <c r="R82" s="5"/>
-      <c r="S82" s="5"/>
-      <c r="T82" s="5"/>
-      <c r="U82" s="5"/>
-      <c r="V82" s="5"/>
-      <c r="W82" s="5"/>
-      <c r="X82" s="5"/>
-      <c r="Y82" s="5"/>
-      <c r="Z82" s="5"/>
-    </row>
-    <row r="83" spans="2:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="B83" s="5"/>
-      <c r="C83" s="5"/>
-      <c r="D83" s="17"/>
-      <c r="E83" s="5"/>
-      <c r="F83" s="5"/>
-      <c r="G83" s="5"/>
-      <c r="H83" s="5"/>
-      <c r="I83" s="17"/>
-      <c r="J83" s="5"/>
-      <c r="K83" s="5"/>
-      <c r="L83" s="5"/>
-      <c r="M83" s="5"/>
-      <c r="N83" s="5"/>
-      <c r="O83" s="5"/>
-      <c r="P83" s="5"/>
-      <c r="Q83" s="5"/>
-      <c r="R83" s="5"/>
-      <c r="S83" s="5"/>
-      <c r="T83" s="5"/>
-      <c r="U83" s="5"/>
-      <c r="V83" s="5"/>
-      <c r="W83" s="5"/>
-      <c r="X83" s="5"/>
-      <c r="Y83" s="5"/>
-      <c r="Z83" s="5"/>
-    </row>
-    <row r="84" spans="2:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="B84" s="5"/>
-      <c r="C84" s="5"/>
-      <c r="D84" s="17"/>
-      <c r="E84" s="5"/>
-      <c r="F84" s="5"/>
-      <c r="G84" s="5"/>
-      <c r="H84" s="5"/>
-      <c r="I84" s="17"/>
-      <c r="J84" s="5"/>
-      <c r="K84" s="5"/>
-      <c r="L84" s="5"/>
-      <c r="M84" s="5"/>
-      <c r="N84" s="5"/>
-      <c r="O84" s="5"/>
-      <c r="P84" s="5"/>
-      <c r="Q84" s="5"/>
-      <c r="R84" s="5"/>
-      <c r="S84" s="5"/>
-      <c r="T84" s="5"/>
-      <c r="U84" s="5"/>
-      <c r="V84" s="5"/>
-      <c r="W84" s="5"/>
-      <c r="X84" s="5"/>
-      <c r="Y84" s="5"/>
-      <c r="Z84" s="5"/>
-    </row>
-    <row r="85" spans="2:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="B85" s="5"/>
-      <c r="C85" s="5"/>
-      <c r="D85" s="17"/>
-      <c r="E85" s="5"/>
-      <c r="F85" s="5"/>
-      <c r="G85" s="5"/>
-      <c r="H85" s="5"/>
-      <c r="I85" s="17"/>
-      <c r="J85" s="5"/>
-      <c r="K85" s="5"/>
-      <c r="L85" s="5"/>
-      <c r="M85" s="5"/>
-      <c r="N85" s="5"/>
-      <c r="O85" s="5"/>
-      <c r="P85" s="5"/>
-      <c r="Q85" s="5"/>
-      <c r="R85" s="5"/>
-      <c r="S85" s="5"/>
-      <c r="T85" s="5"/>
-      <c r="U85" s="5"/>
-      <c r="V85" s="5"/>
-      <c r="W85" s="5"/>
-      <c r="X85" s="5"/>
-      <c r="Y85" s="5"/>
-      <c r="Z85" s="5"/>
-    </row>
-    <row r="86" spans="2:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="B86" s="5"/>
-      <c r="C86" s="5"/>
-      <c r="D86" s="17"/>
-      <c r="E86" s="5"/>
-      <c r="F86" s="5"/>
-      <c r="G86" s="5"/>
-      <c r="H86" s="5"/>
-      <c r="I86" s="17"/>
-      <c r="J86" s="5"/>
-      <c r="K86" s="5"/>
-      <c r="L86" s="5"/>
-      <c r="M86" s="5"/>
-      <c r="N86" s="5"/>
-      <c r="O86" s="5"/>
-      <c r="P86" s="5"/>
-      <c r="Q86" s="5"/>
-      <c r="R86" s="5"/>
-      <c r="S86" s="5"/>
-      <c r="T86" s="5"/>
-      <c r="U86" s="5"/>
-      <c r="V86" s="5"/>
-      <c r="W86" s="5"/>
-      <c r="X86" s="5"/>
-      <c r="Y86" s="5"/>
-      <c r="Z86" s="5"/>
-    </row>
-    <row r="87" spans="2:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="B87" s="5"/>
-      <c r="C87" s="5"/>
-      <c r="D87" s="17"/>
-      <c r="E87" s="5"/>
-      <c r="F87" s="5"/>
-      <c r="G87" s="5"/>
-      <c r="H87" s="5"/>
-      <c r="I87" s="17"/>
-      <c r="J87" s="5"/>
-      <c r="K87" s="5"/>
-      <c r="L87" s="5"/>
-      <c r="M87" s="5"/>
-      <c r="N87" s="5"/>
-      <c r="O87" s="5"/>
-      <c r="P87" s="5"/>
-      <c r="Q87" s="5"/>
-      <c r="R87" s="5"/>
-      <c r="S87" s="5"/>
-      <c r="T87" s="5"/>
-      <c r="U87" s="5"/>
-      <c r="V87" s="5"/>
-      <c r="W87" s="5"/>
-      <c r="X87" s="5"/>
-      <c r="Y87" s="5"/>
-      <c r="Z87" s="5"/>
-    </row>
-    <row r="88" spans="2:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="B88" s="5"/>
-      <c r="C88" s="5"/>
-      <c r="D88" s="17"/>
-      <c r="E88" s="5"/>
-      <c r="F88" s="5"/>
-      <c r="G88" s="5"/>
-      <c r="H88" s="5"/>
-      <c r="I88" s="17"/>
-      <c r="J88" s="5"/>
-      <c r="K88" s="5"/>
-      <c r="L88" s="5"/>
-      <c r="M88" s="5"/>
-      <c r="N88" s="5"/>
-      <c r="O88" s="5"/>
-      <c r="P88" s="5"/>
-      <c r="Q88" s="5"/>
-      <c r="R88" s="5"/>
-      <c r="S88" s="5"/>
-      <c r="T88" s="5"/>
-      <c r="U88" s="5"/>
-      <c r="V88" s="5"/>
-      <c r="W88" s="5"/>
-      <c r="X88" s="5"/>
-      <c r="Y88" s="5"/>
-      <c r="Z88" s="5"/>
-    </row>
-    <row r="89" spans="2:26" ht="19" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:26" ht="21" x14ac:dyDescent="0.25">
+      <c r="A89" s="5"/>
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
-      <c r="D89" s="17"/>
-      <c r="E89" s="5"/>
-      <c r="F89" s="5"/>
-      <c r="G89" s="5"/>
-      <c r="H89" s="5"/>
-      <c r="I89" s="17"/>
-      <c r="J89" s="5"/>
-      <c r="K89" s="5"/>
-      <c r="L89" s="5"/>
-      <c r="M89" s="5"/>
-      <c r="N89" s="5"/>
-      <c r="O89" s="5"/>
-      <c r="P89" s="5"/>
-      <c r="Q89" s="5"/>
-      <c r="R89" s="5"/>
-      <c r="S89" s="5"/>
-      <c r="T89" s="5"/>
-      <c r="U89" s="5"/>
-      <c r="V89" s="5"/>
-      <c r="W89" s="5"/>
-      <c r="X89" s="5"/>
-      <c r="Y89" s="5"/>
-      <c r="Z89" s="5"/>
-    </row>
-    <row r="90" spans="2:26" ht="19" x14ac:dyDescent="0.25">
+      <c r="D89" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E89" s="12">
+        <f>SUM(D13:D86)</f>
+        <v>-227.5</v>
+      </c>
+      <c r="G89" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H89" s="12">
+        <f>SUM(G13:G86)</f>
+        <v>485</v>
+      </c>
+      <c r="J89" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K89" s="12">
+        <f>SUM(J13:J86)</f>
+        <v>-181.66</v>
+      </c>
+      <c r="M89" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="N89" s="12">
+        <f>SUM(M13:M86)</f>
+        <v>357.5</v>
+      </c>
+      <c r="P89" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q89" s="12">
+        <f>SUM(P13:P86)</f>
+        <v>128.32999999999998</v>
+      </c>
+      <c r="S89" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="T89" s="12">
+        <f>SUM(S13:S86)</f>
+        <v>-192.5</v>
+      </c>
+      <c r="V89" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="W89" s="12">
+        <f>SUM(V13:V86)</f>
+        <v>-369.17</v>
+      </c>
+      <c r="X89" s="1">
+        <f>SUM(E89,H89,K89,N89,Q89,T89,W89)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A90" s="5"/>
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
-      <c r="D90" s="17"/>
+      <c r="D90" s="5"/>
       <c r="E90" s="5"/>
-      <c r="F90" s="5"/>
-      <c r="G90" s="5"/>
-      <c r="H90" s="5"/>
-      <c r="I90" s="17"/>
-      <c r="J90" s="5"/>
-      <c r="K90" s="5"/>
-      <c r="L90" s="5"/>
-      <c r="M90" s="5"/>
-      <c r="N90" s="5"/>
-      <c r="O90" s="5"/>
-      <c r="P90" s="5"/>
-      <c r="Q90" s="5"/>
-      <c r="R90" s="5"/>
       <c r="S90" s="5"/>
       <c r="T90" s="5"/>
-      <c r="U90" s="5"/>
-      <c r="V90" s="5"/>
-      <c r="W90" s="5"/>
-      <c r="X90" s="5"/>
-      <c r="Y90" s="5"/>
-      <c r="Z90" s="5"/>
-    </row>
-    <row r="91" spans="2:26" x14ac:dyDescent="0.2">
+    </row>
+    <row r="91" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A91" s="5"/>
       <c r="B91" s="5"/>
       <c r="C91" s="5"/>
       <c r="D91" s="5"/>
       <c r="E91" s="5"/>
-      <c r="F91" s="5"/>
-      <c r="G91" s="5"/>
-      <c r="H91" s="5"/>
-      <c r="I91" s="5"/>
-      <c r="J91" s="5"/>
-      <c r="K91" s="5"/>
-      <c r="L91" s="5"/>
-      <c r="M91" s="5"/>
-      <c r="N91" s="5"/>
-      <c r="O91" s="5"/>
-      <c r="P91" s="5"/>
-      <c r="Q91" s="5"/>
-      <c r="R91" s="5"/>
       <c r="S91" s="5"/>
       <c r="T91" s="5"/>
-      <c r="U91" s="5"/>
-      <c r="V91" s="5"/>
-      <c r="W91" s="5"/>
-      <c r="X91" s="5"/>
-      <c r="Y91" s="5"/>
-      <c r="Z91" s="5"/>
-    </row>
-    <row r="92" spans="2:26" x14ac:dyDescent="0.2">
+    </row>
+    <row r="92" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A92" s="5"/>
       <c r="B92" s="5"/>
       <c r="C92" s="5"/>
       <c r="D92" s="5"/>
@@ -5679,7 +6533,7 @@
       <c r="Y92" s="5"/>
       <c r="Z92" s="5"/>
     </row>
-    <row r="93" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
       <c r="D93" s="5"/>
@@ -5706,15 +6560,15 @@
       <c r="Y93" s="5"/>
       <c r="Z93" s="5"/>
     </row>
-    <row r="94" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
       <c r="D94" s="5"/>
-      <c r="E94" s="5"/>
-      <c r="F94" s="5"/>
-      <c r="G94" s="5"/>
-      <c r="H94" s="5"/>
-      <c r="I94" s="5"/>
+      <c r="E94" s="20"/>
+      <c r="F94" s="20"/>
+      <c r="G94" s="20"/>
+      <c r="H94" s="20"/>
+      <c r="I94" s="16"/>
       <c r="J94" s="5"/>
       <c r="K94" s="5"/>
       <c r="L94" s="5"/>
@@ -5733,15 +6587,15 @@
       <c r="Y94" s="5"/>
       <c r="Z94" s="5"/>
     </row>
-    <row r="95" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B95" s="5"/>
       <c r="C95" s="5"/>
       <c r="D95" s="5"/>
-      <c r="E95" s="5"/>
-      <c r="F95" s="5"/>
-      <c r="G95" s="5"/>
-      <c r="H95" s="5"/>
-      <c r="I95" s="5"/>
+      <c r="E95" s="17"/>
+      <c r="F95" s="17"/>
+      <c r="G95" s="17"/>
+      <c r="H95" s="17"/>
+      <c r="I95" s="18"/>
       <c r="J95" s="5"/>
       <c r="K95" s="5"/>
       <c r="L95" s="5"/>
@@ -5760,15 +6614,15 @@
       <c r="Y95" s="5"/>
       <c r="Z95" s="5"/>
     </row>
-    <row r="96" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B96" s="5"/>
       <c r="C96" s="5"/>
-      <c r="D96" s="5"/>
+      <c r="D96" s="17"/>
       <c r="E96" s="5"/>
       <c r="F96" s="5"/>
       <c r="G96" s="5"/>
       <c r="H96" s="5"/>
-      <c r="I96" s="5"/>
+      <c r="I96" s="17"/>
       <c r="J96" s="5"/>
       <c r="K96" s="5"/>
       <c r="L96" s="5"/>
@@ -5787,15 +6641,15 @@
       <c r="Y96" s="5"/>
       <c r="Z96" s="5"/>
     </row>
-    <row r="97" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B97" s="5"/>
       <c r="C97" s="5"/>
-      <c r="D97" s="5"/>
+      <c r="D97" s="17"/>
       <c r="E97" s="5"/>
       <c r="F97" s="5"/>
       <c r="G97" s="5"/>
       <c r="H97" s="5"/>
-      <c r="I97" s="5"/>
+      <c r="I97" s="17"/>
       <c r="J97" s="5"/>
       <c r="K97" s="5"/>
       <c r="L97" s="5"/>
@@ -5814,15 +6668,15 @@
       <c r="Y97" s="5"/>
       <c r="Z97" s="5"/>
     </row>
-    <row r="98" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B98" s="5"/>
       <c r="C98" s="5"/>
-      <c r="D98" s="5"/>
+      <c r="D98" s="17"/>
       <c r="E98" s="5"/>
       <c r="F98" s="5"/>
       <c r="G98" s="5"/>
       <c r="H98" s="5"/>
-      <c r="I98" s="5"/>
+      <c r="I98" s="17"/>
       <c r="J98" s="5"/>
       <c r="K98" s="5"/>
       <c r="L98" s="5"/>
@@ -5841,15 +6695,15 @@
       <c r="Y98" s="5"/>
       <c r="Z98" s="5"/>
     </row>
-    <row r="99" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B99" s="5"/>
       <c r="C99" s="5"/>
-      <c r="D99" s="5"/>
+      <c r="D99" s="17"/>
       <c r="E99" s="5"/>
       <c r="F99" s="5"/>
       <c r="G99" s="5"/>
       <c r="H99" s="5"/>
-      <c r="I99" s="5"/>
+      <c r="I99" s="17"/>
       <c r="J99" s="5"/>
       <c r="K99" s="5"/>
       <c r="L99" s="5"/>
@@ -5868,15 +6722,15 @@
       <c r="Y99" s="5"/>
       <c r="Z99" s="5"/>
     </row>
-    <row r="100" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B100" s="5"/>
       <c r="C100" s="5"/>
-      <c r="D100" s="5"/>
+      <c r="D100" s="17"/>
       <c r="E100" s="5"/>
       <c r="F100" s="5"/>
       <c r="G100" s="5"/>
       <c r="H100" s="5"/>
-      <c r="I100" s="5"/>
+      <c r="I100" s="17"/>
       <c r="J100" s="5"/>
       <c r="K100" s="5"/>
       <c r="L100" s="5"/>
@@ -5895,15 +6749,15 @@
       <c r="Y100" s="5"/>
       <c r="Z100" s="5"/>
     </row>
-    <row r="101" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B101" s="5"/>
       <c r="C101" s="5"/>
-      <c r="D101" s="5"/>
+      <c r="D101" s="17"/>
       <c r="E101" s="5"/>
       <c r="F101" s="5"/>
       <c r="G101" s="5"/>
       <c r="H101" s="5"/>
-      <c r="I101" s="5"/>
+      <c r="I101" s="17"/>
       <c r="J101" s="5"/>
       <c r="K101" s="5"/>
       <c r="L101" s="5"/>
@@ -5922,15 +6776,15 @@
       <c r="Y101" s="5"/>
       <c r="Z101" s="5"/>
     </row>
-    <row r="102" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B102" s="5"/>
       <c r="C102" s="5"/>
-      <c r="D102" s="5"/>
+      <c r="D102" s="17"/>
       <c r="E102" s="5"/>
       <c r="F102" s="5"/>
       <c r="G102" s="5"/>
       <c r="H102" s="5"/>
-      <c r="I102" s="5"/>
+      <c r="I102" s="17"/>
       <c r="J102" s="5"/>
       <c r="K102" s="5"/>
       <c r="L102" s="5"/>
@@ -5949,15 +6803,15 @@
       <c r="Y102" s="5"/>
       <c r="Z102" s="5"/>
     </row>
-    <row r="103" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B103" s="5"/>
       <c r="C103" s="5"/>
-      <c r="D103" s="5"/>
+      <c r="D103" s="17"/>
       <c r="E103" s="5"/>
       <c r="F103" s="5"/>
       <c r="G103" s="5"/>
       <c r="H103" s="5"/>
-      <c r="I103" s="5"/>
+      <c r="I103" s="17"/>
       <c r="J103" s="5"/>
       <c r="K103" s="5"/>
       <c r="L103" s="5"/>
@@ -5976,15 +6830,15 @@
       <c r="Y103" s="5"/>
       <c r="Z103" s="5"/>
     </row>
-    <row r="104" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B104" s="5"/>
       <c r="C104" s="5"/>
-      <c r="D104" s="5"/>
+      <c r="D104" s="17"/>
       <c r="E104" s="5"/>
       <c r="F104" s="5"/>
       <c r="G104" s="5"/>
       <c r="H104" s="5"/>
-      <c r="I104" s="5"/>
+      <c r="I104" s="17"/>
       <c r="J104" s="5"/>
       <c r="K104" s="5"/>
       <c r="L104" s="5"/>
@@ -6057,10 +6911,388 @@
       <c r="Y106" s="5"/>
       <c r="Z106" s="5"/>
     </row>
+    <row r="107" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B107" s="5"/>
+      <c r="C107" s="5"/>
+      <c r="D107" s="5"/>
+      <c r="E107" s="5"/>
+      <c r="F107" s="5"/>
+      <c r="G107" s="5"/>
+      <c r="H107" s="5"/>
+      <c r="I107" s="5"/>
+      <c r="J107" s="5"/>
+      <c r="K107" s="5"/>
+      <c r="L107" s="5"/>
+      <c r="M107" s="5"/>
+      <c r="N107" s="5"/>
+      <c r="O107" s="5"/>
+      <c r="P107" s="5"/>
+      <c r="Q107" s="5"/>
+      <c r="R107" s="5"/>
+      <c r="S107" s="5"/>
+      <c r="T107" s="5"/>
+      <c r="U107" s="5"/>
+      <c r="V107" s="5"/>
+      <c r="W107" s="5"/>
+      <c r="X107" s="5"/>
+      <c r="Y107" s="5"/>
+      <c r="Z107" s="5"/>
+    </row>
+    <row r="108" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B108" s="5"/>
+      <c r="C108" s="5"/>
+      <c r="D108" s="5"/>
+      <c r="E108" s="5"/>
+      <c r="F108" s="5"/>
+      <c r="G108" s="5"/>
+      <c r="H108" s="5"/>
+      <c r="I108" s="5"/>
+      <c r="J108" s="5"/>
+      <c r="K108" s="5"/>
+      <c r="L108" s="5"/>
+      <c r="M108" s="5"/>
+      <c r="N108" s="5"/>
+      <c r="O108" s="5"/>
+      <c r="P108" s="5"/>
+      <c r="Q108" s="5"/>
+      <c r="R108" s="5"/>
+      <c r="S108" s="5"/>
+      <c r="T108" s="5"/>
+      <c r="U108" s="5"/>
+      <c r="V108" s="5"/>
+      <c r="W108" s="5"/>
+      <c r="X108" s="5"/>
+      <c r="Y108" s="5"/>
+      <c r="Z108" s="5"/>
+    </row>
+    <row r="109" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B109" s="5"/>
+      <c r="C109" s="5"/>
+      <c r="D109" s="5"/>
+      <c r="E109" s="5"/>
+      <c r="F109" s="5"/>
+      <c r="G109" s="5"/>
+      <c r="H109" s="5"/>
+      <c r="I109" s="5"/>
+      <c r="J109" s="5"/>
+      <c r="K109" s="5"/>
+      <c r="L109" s="5"/>
+      <c r="M109" s="5"/>
+      <c r="N109" s="5"/>
+      <c r="O109" s="5"/>
+      <c r="P109" s="5"/>
+      <c r="Q109" s="5"/>
+      <c r="R109" s="5"/>
+      <c r="S109" s="5"/>
+      <c r="T109" s="5"/>
+      <c r="U109" s="5"/>
+      <c r="V109" s="5"/>
+      <c r="W109" s="5"/>
+      <c r="X109" s="5"/>
+      <c r="Y109" s="5"/>
+      <c r="Z109" s="5"/>
+    </row>
+    <row r="110" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B110" s="5"/>
+      <c r="C110" s="5"/>
+      <c r="D110" s="5"/>
+      <c r="E110" s="5"/>
+      <c r="F110" s="5"/>
+      <c r="G110" s="5"/>
+      <c r="H110" s="5"/>
+      <c r="I110" s="5"/>
+      <c r="J110" s="5"/>
+      <c r="K110" s="5"/>
+      <c r="L110" s="5"/>
+      <c r="M110" s="5"/>
+      <c r="N110" s="5"/>
+      <c r="O110" s="5"/>
+      <c r="P110" s="5"/>
+      <c r="Q110" s="5"/>
+      <c r="R110" s="5"/>
+      <c r="S110" s="5"/>
+      <c r="T110" s="5"/>
+      <c r="U110" s="5"/>
+      <c r="V110" s="5"/>
+      <c r="W110" s="5"/>
+      <c r="X110" s="5"/>
+      <c r="Y110" s="5"/>
+      <c r="Z110" s="5"/>
+    </row>
+    <row r="111" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B111" s="5"/>
+      <c r="C111" s="5"/>
+      <c r="D111" s="5"/>
+      <c r="E111" s="5"/>
+      <c r="F111" s="5"/>
+      <c r="G111" s="5"/>
+      <c r="H111" s="5"/>
+      <c r="I111" s="5"/>
+      <c r="J111" s="5"/>
+      <c r="K111" s="5"/>
+      <c r="L111" s="5"/>
+      <c r="M111" s="5"/>
+      <c r="N111" s="5"/>
+      <c r="O111" s="5"/>
+      <c r="P111" s="5"/>
+      <c r="Q111" s="5"/>
+      <c r="R111" s="5"/>
+      <c r="S111" s="5"/>
+      <c r="T111" s="5"/>
+      <c r="U111" s="5"/>
+      <c r="V111" s="5"/>
+      <c r="W111" s="5"/>
+      <c r="X111" s="5"/>
+      <c r="Y111" s="5"/>
+      <c r="Z111" s="5"/>
+    </row>
+    <row r="112" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B112" s="5"/>
+      <c r="C112" s="5"/>
+      <c r="D112" s="5"/>
+      <c r="E112" s="5"/>
+      <c r="F112" s="5"/>
+      <c r="G112" s="5"/>
+      <c r="H112" s="5"/>
+      <c r="I112" s="5"/>
+      <c r="J112" s="5"/>
+      <c r="K112" s="5"/>
+      <c r="L112" s="5"/>
+      <c r="M112" s="5"/>
+      <c r="N112" s="5"/>
+      <c r="O112" s="5"/>
+      <c r="P112" s="5"/>
+      <c r="Q112" s="5"/>
+      <c r="R112" s="5"/>
+      <c r="S112" s="5"/>
+      <c r="T112" s="5"/>
+      <c r="U112" s="5"/>
+      <c r="V112" s="5"/>
+      <c r="W112" s="5"/>
+      <c r="X112" s="5"/>
+      <c r="Y112" s="5"/>
+      <c r="Z112" s="5"/>
+    </row>
+    <row r="113" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B113" s="5"/>
+      <c r="C113" s="5"/>
+      <c r="D113" s="5"/>
+      <c r="E113" s="5"/>
+      <c r="F113" s="5"/>
+      <c r="G113" s="5"/>
+      <c r="H113" s="5"/>
+      <c r="I113" s="5"/>
+      <c r="J113" s="5"/>
+      <c r="K113" s="5"/>
+      <c r="L113" s="5"/>
+      <c r="M113" s="5"/>
+      <c r="N113" s="5"/>
+      <c r="O113" s="5"/>
+      <c r="P113" s="5"/>
+      <c r="Q113" s="5"/>
+      <c r="R113" s="5"/>
+      <c r="S113" s="5"/>
+      <c r="T113" s="5"/>
+      <c r="U113" s="5"/>
+      <c r="V113" s="5"/>
+      <c r="W113" s="5"/>
+      <c r="X113" s="5"/>
+      <c r="Y113" s="5"/>
+      <c r="Z113" s="5"/>
+    </row>
+    <row r="114" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B114" s="5"/>
+      <c r="C114" s="5"/>
+      <c r="D114" s="5"/>
+      <c r="E114" s="5"/>
+      <c r="F114" s="5"/>
+      <c r="G114" s="5"/>
+      <c r="H114" s="5"/>
+      <c r="I114" s="5"/>
+      <c r="J114" s="5"/>
+      <c r="K114" s="5"/>
+      <c r="L114" s="5"/>
+      <c r="M114" s="5"/>
+      <c r="N114" s="5"/>
+      <c r="O114" s="5"/>
+      <c r="P114" s="5"/>
+      <c r="Q114" s="5"/>
+      <c r="R114" s="5"/>
+      <c r="S114" s="5"/>
+      <c r="T114" s="5"/>
+      <c r="U114" s="5"/>
+      <c r="V114" s="5"/>
+      <c r="W114" s="5"/>
+      <c r="X114" s="5"/>
+      <c r="Y114" s="5"/>
+      <c r="Z114" s="5"/>
+    </row>
+    <row r="115" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B115" s="5"/>
+      <c r="C115" s="5"/>
+      <c r="D115" s="5"/>
+      <c r="E115" s="5"/>
+      <c r="F115" s="5"/>
+      <c r="G115" s="5"/>
+      <c r="H115" s="5"/>
+      <c r="I115" s="5"/>
+      <c r="J115" s="5"/>
+      <c r="K115" s="5"/>
+      <c r="L115" s="5"/>
+      <c r="M115" s="5"/>
+      <c r="N115" s="5"/>
+      <c r="O115" s="5"/>
+      <c r="P115" s="5"/>
+      <c r="Q115" s="5"/>
+      <c r="R115" s="5"/>
+      <c r="S115" s="5"/>
+      <c r="T115" s="5"/>
+      <c r="U115" s="5"/>
+      <c r="V115" s="5"/>
+      <c r="W115" s="5"/>
+      <c r="X115" s="5"/>
+      <c r="Y115" s="5"/>
+      <c r="Z115" s="5"/>
+    </row>
+    <row r="116" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B116" s="5"/>
+      <c r="C116" s="5"/>
+      <c r="D116" s="5"/>
+      <c r="E116" s="5"/>
+      <c r="F116" s="5"/>
+      <c r="G116" s="5"/>
+      <c r="H116" s="5"/>
+      <c r="I116" s="5"/>
+      <c r="J116" s="5"/>
+      <c r="K116" s="5"/>
+      <c r="L116" s="5"/>
+      <c r="M116" s="5"/>
+      <c r="N116" s="5"/>
+      <c r="O116" s="5"/>
+      <c r="P116" s="5"/>
+      <c r="Q116" s="5"/>
+      <c r="R116" s="5"/>
+      <c r="S116" s="5"/>
+      <c r="T116" s="5"/>
+      <c r="U116" s="5"/>
+      <c r="V116" s="5"/>
+      <c r="W116" s="5"/>
+      <c r="X116" s="5"/>
+      <c r="Y116" s="5"/>
+      <c r="Z116" s="5"/>
+    </row>
+    <row r="117" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B117" s="5"/>
+      <c r="C117" s="5"/>
+      <c r="D117" s="5"/>
+      <c r="E117" s="5"/>
+      <c r="F117" s="5"/>
+      <c r="G117" s="5"/>
+      <c r="H117" s="5"/>
+      <c r="I117" s="5"/>
+      <c r="J117" s="5"/>
+      <c r="K117" s="5"/>
+      <c r="L117" s="5"/>
+      <c r="M117" s="5"/>
+      <c r="N117" s="5"/>
+      <c r="O117" s="5"/>
+      <c r="P117" s="5"/>
+      <c r="Q117" s="5"/>
+      <c r="R117" s="5"/>
+      <c r="S117" s="5"/>
+      <c r="T117" s="5"/>
+      <c r="U117" s="5"/>
+      <c r="V117" s="5"/>
+      <c r="W117" s="5"/>
+      <c r="X117" s="5"/>
+      <c r="Y117" s="5"/>
+      <c r="Z117" s="5"/>
+    </row>
+    <row r="118" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B118" s="5"/>
+      <c r="C118" s="5"/>
+      <c r="D118" s="5"/>
+      <c r="E118" s="5"/>
+      <c r="F118" s="5"/>
+      <c r="G118" s="5"/>
+      <c r="H118" s="5"/>
+      <c r="I118" s="5"/>
+      <c r="J118" s="5"/>
+      <c r="K118" s="5"/>
+      <c r="L118" s="5"/>
+      <c r="M118" s="5"/>
+      <c r="N118" s="5"/>
+      <c r="O118" s="5"/>
+      <c r="P118" s="5"/>
+      <c r="Q118" s="5"/>
+      <c r="R118" s="5"/>
+      <c r="S118" s="5"/>
+      <c r="T118" s="5"/>
+      <c r="U118" s="5"/>
+      <c r="V118" s="5"/>
+      <c r="W118" s="5"/>
+      <c r="X118" s="5"/>
+      <c r="Y118" s="5"/>
+      <c r="Z118" s="5"/>
+    </row>
+    <row r="119" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B119" s="5"/>
+      <c r="C119" s="5"/>
+      <c r="D119" s="5"/>
+      <c r="E119" s="5"/>
+      <c r="F119" s="5"/>
+      <c r="G119" s="5"/>
+      <c r="H119" s="5"/>
+      <c r="I119" s="5"/>
+      <c r="J119" s="5"/>
+      <c r="K119" s="5"/>
+      <c r="L119" s="5"/>
+      <c r="M119" s="5"/>
+      <c r="N119" s="5"/>
+      <c r="O119" s="5"/>
+      <c r="P119" s="5"/>
+      <c r="Q119" s="5"/>
+      <c r="R119" s="5"/>
+      <c r="S119" s="5"/>
+      <c r="T119" s="5"/>
+      <c r="U119" s="5"/>
+      <c r="V119" s="5"/>
+      <c r="W119" s="5"/>
+      <c r="X119" s="5"/>
+      <c r="Y119" s="5"/>
+      <c r="Z119" s="5"/>
+    </row>
+    <row r="120" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B120" s="5"/>
+      <c r="C120" s="5"/>
+      <c r="D120" s="5"/>
+      <c r="E120" s="5"/>
+      <c r="F120" s="5"/>
+      <c r="G120" s="5"/>
+      <c r="H120" s="5"/>
+      <c r="I120" s="5"/>
+      <c r="J120" s="5"/>
+      <c r="K120" s="5"/>
+      <c r="L120" s="5"/>
+      <c r="M120" s="5"/>
+      <c r="N120" s="5"/>
+      <c r="O120" s="5"/>
+      <c r="P120" s="5"/>
+      <c r="Q120" s="5"/>
+      <c r="R120" s="5"/>
+      <c r="S120" s="5"/>
+      <c r="T120" s="5"/>
+      <c r="U120" s="5"/>
+      <c r="V120" s="5"/>
+      <c r="W120" s="5"/>
+      <c r="X120" s="5"/>
+      <c r="Y120" s="5"/>
+      <c r="Z120" s="5"/>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="9">
-    <mergeCell ref="E80:H80"/>
+    <mergeCell ref="E94:H94"/>
     <mergeCell ref="P11:Q11"/>
     <mergeCell ref="S11:T11"/>
     <mergeCell ref="V11:W11"/>
@@ -6070,18 +7302,18 @@
     <mergeCell ref="J11:K11"/>
     <mergeCell ref="M11:N11"/>
   </mergeCells>
-  <conditionalFormatting sqref="E75">
-    <cfRule type="cellIs" dxfId="38" priority="211" operator="lessThan">
+  <conditionalFormatting sqref="E89">
+    <cfRule type="cellIs" dxfId="74" priority="247" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="212" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="248" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="213" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="72" priority="249" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H75">
+  <conditionalFormatting sqref="H89">
     <cfRule type="cellIs" dxfId="17" priority="16" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -6092,7 +7324,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K75">
+  <conditionalFormatting sqref="K89">
     <cfRule type="cellIs" dxfId="14" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -6103,7 +7335,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N75">
+  <conditionalFormatting sqref="N89">
     <cfRule type="cellIs" dxfId="11" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -6114,7 +7346,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q75">
+  <conditionalFormatting sqref="Q89">
     <cfRule type="cellIs" dxfId="8" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -6125,7 +7357,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T75">
+  <conditionalFormatting sqref="T89">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -6136,7 +7368,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W75">
+  <conditionalFormatting sqref="W89">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
eliminator LSG vs RCB.
</commit_message>
<xml_diff>
--- a/2022/EBE Boys 2022.xlsx
+++ b/2022/EBE Boys 2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D211A2D0-A1DF-4242-9A3C-6F1EA6A230C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07318F5C-48BC-8D49-A25A-99B962DCCA22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20420" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="112">
   <si>
     <t>Points</t>
   </si>
@@ -325,13 +325,64 @@
   </si>
   <si>
     <t>GT vs RR</t>
+  </si>
+  <si>
+    <t>Predictions Rank 1</t>
+  </si>
+  <si>
+    <t>Predictions Rank 2</t>
+  </si>
+  <si>
+    <t>Vikcy</t>
+  </si>
+  <si>
+    <t>Qualifier 1 GT vs RR</t>
+  </si>
+  <si>
+    <t>Rank 1</t>
+  </si>
+  <si>
+    <t>Rank 2</t>
+  </si>
+  <si>
+    <t>Winner Prediction - Coins</t>
+  </si>
+  <si>
+    <t>Scorecard</t>
+  </si>
+  <si>
+    <t>Format 1</t>
+  </si>
+  <si>
+    <t>Format 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final score </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finals </t>
+  </si>
+  <si>
+    <t>Total coins</t>
+  </si>
+  <si>
+    <t>Outgoing</t>
+  </si>
+  <si>
+    <t>Coins</t>
+  </si>
+  <si>
+    <t>Incoming</t>
+  </si>
+  <si>
+    <t>Eliminator LSG vs RCB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -378,8 +429,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -416,8 +482,19 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -559,12 +636,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -581,17 +683,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -628,522 +720,46 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="20% - Accent6" xfId="1" builtinId="50"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="75">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="24">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1699,23 +1315,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
-  <dimension ref="A1:Z120"/>
+  <dimension ref="A1:Z118"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X89" sqref="X89"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="11" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U103" sqref="U103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5" customWidth="1"/>
-    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.1640625" customWidth="1"/>
+    <col min="6" max="7" width="11.33203125" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" customWidth="1"/>
     <col min="12" max="12" width="4.33203125" customWidth="1"/>
     <col min="15" max="15" width="4.5" customWidth="1"/>
-    <col min="18" max="18" width="4.5" customWidth="1"/>
-    <col min="21" max="21" width="5" customWidth="1"/>
+    <col min="18" max="18" width="10.33203125" customWidth="1"/>
+    <col min="21" max="21" width="13.5" customWidth="1"/>
     <col min="24" max="24" width="6.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1736,23 +1352,23 @@
         <v>50</v>
       </c>
       <c r="C2" s="5"/>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
-      <c r="U2" s="25"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="21"/>
     </row>
     <row r="3" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
@@ -1762,21 +1378,21 @@
         <v>20</v>
       </c>
       <c r="C3" s="5"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27"/>
-      <c r="Q3" s="27"/>
-      <c r="R3" s="27"/>
-      <c r="S3" s="27"/>
-      <c r="T3" s="27"/>
-      <c r="U3" s="28"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="23"/>
+      <c r="U3" s="24"/>
     </row>
     <row r="4" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
@@ -1786,21 +1402,21 @@
         <v>0</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
-      <c r="O4" s="27"/>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="27"/>
-      <c r="R4" s="27"/>
-      <c r="S4" s="27"/>
-      <c r="T4" s="27"/>
-      <c r="U4" s="28"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="23"/>
+      <c r="U4" s="24"/>
     </row>
     <row r="5" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
@@ -1810,21 +1426,21 @@
         <v>-10</v>
       </c>
       <c r="C5" s="5"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="27"/>
-      <c r="L5" s="27"/>
-      <c r="M5" s="27"/>
-      <c r="N5" s="27"/>
-      <c r="O5" s="27"/>
-      <c r="P5" s="27"/>
-      <c r="Q5" s="27"/>
-      <c r="R5" s="27"/>
-      <c r="S5" s="27"/>
-      <c r="T5" s="27"/>
-      <c r="U5" s="28"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
+      <c r="U5" s="24"/>
     </row>
     <row r="6" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
@@ -1834,21 +1450,21 @@
         <v>-15</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="27"/>
-      <c r="N6" s="27"/>
-      <c r="O6" s="27"/>
-      <c r="P6" s="27"/>
-      <c r="Q6" s="27"/>
-      <c r="R6" s="27"/>
-      <c r="S6" s="27"/>
-      <c r="T6" s="27"/>
-      <c r="U6" s="28"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="23"/>
+      <c r="T6" s="23"/>
+      <c r="U6" s="24"/>
     </row>
     <row r="7" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
@@ -1858,45 +1474,45 @@
         <v>-20</v>
       </c>
       <c r="C7" s="5"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="27"/>
-      <c r="N7" s="27"/>
-      <c r="O7" s="27"/>
-      <c r="P7" s="27"/>
-      <c r="Q7" s="27"/>
-      <c r="R7" s="27"/>
-      <c r="S7" s="27"/>
-      <c r="T7" s="27"/>
-      <c r="U7" s="28"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="23"/>
+      <c r="U7" s="24"/>
     </row>
     <row r="8" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>7</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="16">
         <v>-25</v>
       </c>
       <c r="C8" s="5"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="30"/>
-      <c r="N8" s="30"/>
-      <c r="O8" s="30"/>
-      <c r="P8" s="30"/>
-      <c r="Q8" s="30"/>
-      <c r="R8" s="30"/>
-      <c r="S8" s="30"/>
-      <c r="T8" s="30"/>
-      <c r="U8" s="31"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="26"/>
+      <c r="P8" s="26"/>
+      <c r="Q8" s="26"/>
+      <c r="R8" s="26"/>
+      <c r="S8" s="26"/>
+      <c r="T8" s="26"/>
+      <c r="U8" s="27"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C9" s="5"/>
@@ -1905,34 +1521,34 @@
       <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="D11" s="32" t="s">
+      <c r="D11" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="32"/>
-      <c r="G11" s="21" t="s">
+      <c r="E11" s="28"/>
+      <c r="G11" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="22"/>
-      <c r="J11" s="21" t="s">
+      <c r="H11" s="18"/>
+      <c r="J11" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="K11" s="22"/>
-      <c r="M11" s="21" t="s">
+      <c r="K11" s="18"/>
+      <c r="M11" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="N11" s="22"/>
-      <c r="P11" s="21" t="s">
+      <c r="N11" s="18"/>
+      <c r="P11" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="Q11" s="22"/>
-      <c r="S11" s="21" t="s">
+      <c r="Q11" s="18"/>
+      <c r="S11" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="T11" s="22"/>
-      <c r="V11" s="21" t="s">
+      <c r="T11" s="18"/>
+      <c r="V11" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="W11" s="22"/>
+      <c r="W11" s="18"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
@@ -6184,41 +5800,55 @@
       <c r="C83" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="D83" s="3" t="str">
+      <c r="D83" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E83, ($W83,$T83,$Q83,$N83,$K83,$H83,$E83), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E83, ($W83,$T83,$Q83,$N83,$K83,$H83,$E83), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E83" s="1"/>
-      <c r="G83" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="E83" s="1">
+        <v>50</v>
+      </c>
+      <c r="G83" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H83, ($W83,$T83,$Q83,$N83,$K83,$H83,$E83), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H83, ($W83,$T83,$Q83,$N83,$K83,$H83,$E83), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H83" s="1"/>
-      <c r="J83" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="H83" s="1">
+        <v>70</v>
+      </c>
+      <c r="J83" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K83, ($W83,$T83,$Q83,$N83,$K83,$H83,$E83), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K83, ($W83,$T83,$Q83,$N83,$K83,$H83,$E83), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K83" s="1"/>
-      <c r="M83" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K83" s="1">
+        <v>60</v>
+      </c>
+      <c r="M83" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N83, ($W83,$T83,$Q83,$N83,$K83,$H83,$E83), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N83, ($W83,$T83,$Q83,$N83,$K83,$H83,$E83), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N83" s="1"/>
-      <c r="P83" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="N83" s="1">
+        <v>100</v>
+      </c>
+      <c r="P83" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q83, ($W83,$T83,$Q83,$N83,$K83,$H83,$E83), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q83, ($W83,$T83,$Q83,$N83,$K83,$H83,$E83), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q83" s="1"/>
-      <c r="S83" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="Q83" s="1">
+        <v>40</v>
+      </c>
+      <c r="S83" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T83, ($W83,$T83,$Q83,$N83,$K83,$H83,$E83), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T83, ($W83,$T83,$Q83,$N83,$K83,$H83,$E83), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T83" s="1"/>
-      <c r="V83" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="T83" s="1">
+        <v>0</v>
+      </c>
+      <c r="V83" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W83, ($W83,$T83,$Q83,$N83,$K83,$H83,$E83), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W83, ($W83,$T83,$Q83,$N83,$K83,$H83,$E83), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W83" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="W83" s="1">
+        <v>80</v>
+      </c>
     </row>
     <row r="84" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A84" s="6" t="s">
@@ -6230,41 +5860,55 @@
       <c r="C84" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="D84" s="3" t="str">
+      <c r="D84" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E84, ($W84,$T84,$Q84,$N84,$K84,$H84,$E84), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E84, ($W84,$T84,$Q84,$N84,$K84,$H84,$E84), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E84" s="1"/>
-      <c r="G84" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="E84" s="1">
+        <v>40</v>
+      </c>
+      <c r="G84" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H84, ($W84,$T84,$Q84,$N84,$K84,$H84,$E84), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H84, ($W84,$T84,$Q84,$N84,$K84,$H84,$E84), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H84" s="1"/>
-      <c r="J84" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="H84" s="1">
+        <v>50</v>
+      </c>
+      <c r="J84" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K84, ($W84,$T84,$Q84,$N84,$K84,$H84,$E84), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K84, ($W84,$T84,$Q84,$N84,$K84,$H84,$E84), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K84" s="1"/>
-      <c r="M84" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="K84" s="1">
+        <v>80</v>
+      </c>
+      <c r="M84" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N84, ($W84,$T84,$Q84,$N84,$K84,$H84,$E84), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N84, ($W84,$T84,$Q84,$N84,$K84,$H84,$E84), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N84" s="1"/>
-      <c r="P84" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="N84" s="1">
+        <v>60</v>
+      </c>
+      <c r="P84" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q84, ($W84,$T84,$Q84,$N84,$K84,$H84,$E84), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q84, ($W84,$T84,$Q84,$N84,$K84,$H84,$E84), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q84" s="1"/>
-      <c r="S84" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q84" s="1">
+        <v>70</v>
+      </c>
+      <c r="S84" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T84, ($W84,$T84,$Q84,$N84,$K84,$H84,$E84), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T84, ($W84,$T84,$Q84,$N84,$K84,$H84,$E84), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T84" s="1"/>
-      <c r="V84" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="T84" s="1">
+        <v>0</v>
+      </c>
+      <c r="V84" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W84, ($W84,$T84,$Q84,$N84,$K84,$H84,$E84), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W84, ($W84,$T84,$Q84,$N84,$K84,$H84,$E84), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W84" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="W84" s="1">
+        <v>100</v>
+      </c>
     </row>
     <row r="85" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A85" s="6" t="s">
@@ -6273,7 +5917,9 @@
       <c r="B85" s="1">
         <v>1</v>
       </c>
-      <c r="C85" s="15"/>
+      <c r="C85" s="15" t="s">
+        <v>42</v>
+      </c>
       <c r="D85" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E85, ($W85,$T85,$Q85,$N85,$K85,$H85,$E85), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E85, ($W85,$T85,$Q85,$N85,$K85,$H85,$E85), 0),  $A$2:$B$10, 2, FALSE))</f>
         <v/>
@@ -6438,49 +6084,49 @@
       </c>
       <c r="E89" s="12">
         <f>SUM(D13:D86)</f>
-        <v>-227.5</v>
+        <v>-262.5</v>
       </c>
       <c r="G89" s="7" t="s">
         <v>7</v>
       </c>
       <c r="H89" s="12">
         <f>SUM(G13:G86)</f>
-        <v>485</v>
+        <v>470</v>
       </c>
       <c r="J89" s="7" t="s">
         <v>7</v>
       </c>
       <c r="K89" s="12">
         <f>SUM(J13:J86)</f>
-        <v>-181.66</v>
+        <v>-171.66</v>
       </c>
       <c r="M89" s="7" t="s">
         <v>7</v>
       </c>
       <c r="N89" s="12">
         <f>SUM(M13:M86)</f>
-        <v>357.5</v>
+        <v>397.5</v>
       </c>
       <c r="P89" s="7" t="s">
         <v>7</v>
       </c>
       <c r="Q89" s="12">
         <f>SUM(P13:P86)</f>
-        <v>128.32999999999998</v>
+        <v>108.32999999999998</v>
       </c>
       <c r="S89" s="7" t="s">
         <v>7</v>
       </c>
       <c r="T89" s="12">
         <f>SUM(S13:S86)</f>
-        <v>-192.5</v>
+        <v>-242.5</v>
       </c>
       <c r="V89" s="7" t="s">
         <v>7</v>
       </c>
       <c r="W89" s="12">
         <f>SUM(V13:V86)</f>
-        <v>-369.17</v>
+        <v>-299.17</v>
       </c>
       <c r="X89" s="1">
         <f>SUM(E89,H89,K89,N89,Q89,T89,W89)</f>
@@ -6563,298 +6209,388 @@
     <row r="94" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
-      <c r="D94" s="5"/>
-      <c r="E94" s="20"/>
-      <c r="F94" s="20"/>
-      <c r="G94" s="20"/>
-      <c r="H94" s="20"/>
-      <c r="I94" s="16"/>
-      <c r="J94" s="5"/>
-      <c r="K94" s="5"/>
-      <c r="L94" s="5"/>
-      <c r="M94" s="5"/>
-      <c r="N94" s="5"/>
-      <c r="O94" s="5"/>
-      <c r="P94" s="5"/>
-      <c r="Q94" s="5"/>
-      <c r="R94" s="5"/>
-      <c r="S94" s="5"/>
-      <c r="T94" s="5"/>
-      <c r="U94" s="5"/>
-      <c r="V94" s="5"/>
-      <c r="W94" s="5"/>
-      <c r="X94" s="5"/>
-      <c r="Y94" s="5"/>
+      <c r="E94" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="F94" s="31"/>
+      <c r="G94" s="31"/>
+      <c r="H94" s="31"/>
+      <c r="I94" s="32"/>
+      <c r="P94" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q94" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="R94" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="S94" s="36"/>
+      <c r="T94" s="37"/>
+      <c r="U94" s="34" t="s">
+        <v>105</v>
+      </c>
       <c r="Z94" s="5"/>
     </row>
     <row r="95" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="B95" s="5"/>
       <c r="C95" s="5"/>
-      <c r="D95" s="5"/>
-      <c r="E95" s="17"/>
-      <c r="F95" s="17"/>
-      <c r="G95" s="17"/>
-      <c r="H95" s="17"/>
-      <c r="I95" s="18"/>
-      <c r="J95" s="5"/>
-      <c r="K95" s="5"/>
-      <c r="L95" s="5"/>
-      <c r="M95" s="5"/>
-      <c r="N95" s="5"/>
-      <c r="O95" s="5"/>
-      <c r="P95" s="5"/>
-      <c r="Q95" s="5"/>
-      <c r="R95" s="5"/>
-      <c r="S95" s="5"/>
-      <c r="T95" s="5"/>
-      <c r="U95" s="5"/>
-      <c r="V95" s="5"/>
-      <c r="W95" s="5"/>
-      <c r="X95" s="5"/>
-      <c r="Y95" s="5"/>
+      <c r="E95" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="F95" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="G95" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="H95" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="I95" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="P95" s="39"/>
+      <c r="Q95" s="34"/>
+      <c r="R95" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="S95" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="T95" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="U95" s="34"/>
       <c r="Z95" s="5"/>
     </row>
-    <row r="96" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:26" ht="21" x14ac:dyDescent="0.25">
       <c r="B96" s="5"/>
       <c r="C96" s="5"/>
-      <c r="D96" s="17"/>
-      <c r="E96" s="5"/>
-      <c r="F96" s="5"/>
-      <c r="G96" s="5"/>
-      <c r="H96" s="5"/>
-      <c r="I96" s="17"/>
-      <c r="J96" s="5"/>
-      <c r="K96" s="5"/>
-      <c r="L96" s="5"/>
-      <c r="M96" s="5"/>
-      <c r="N96" s="5"/>
-      <c r="O96" s="5"/>
-      <c r="P96" s="5"/>
-      <c r="Q96" s="5"/>
-      <c r="R96" s="5"/>
-      <c r="S96" s="5"/>
-      <c r="T96" s="5"/>
-      <c r="U96" s="5"/>
-      <c r="V96" s="5"/>
-      <c r="W96" s="5"/>
-      <c r="X96" s="5"/>
-      <c r="Y96" s="5"/>
+      <c r="D96" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E96" s="1">
+        <v>0</v>
+      </c>
+      <c r="F96" s="1">
+        <v>0</v>
+      </c>
+      <c r="G96" s="1"/>
+      <c r="H96" s="1"/>
+      <c r="I96" s="29">
+        <f>SUM(E96:H96)</f>
+        <v>0</v>
+      </c>
+      <c r="P96" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q96" s="12">
+        <f>E89</f>
+        <v>-262.5</v>
+      </c>
+      <c r="R96" s="40">
+        <v>-200</v>
+      </c>
+      <c r="S96" s="12">
+        <f>I96</f>
+        <v>0</v>
+      </c>
+      <c r="T96" s="12">
+        <f>IFERROR((-SUM($R$96:$R$102)/SUM($S$96:$S$102))*$S96, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U96" s="12">
+        <f>SUM(Q96,R96,T96)</f>
+        <v>-462.5</v>
+      </c>
+      <c r="V96" s="29" t="s">
+        <v>8</v>
+      </c>
       <c r="Z96" s="5"/>
     </row>
-    <row r="97" spans="2:26" ht="19" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:26" ht="21" x14ac:dyDescent="0.25">
       <c r="B97" s="5"/>
       <c r="C97" s="5"/>
-      <c r="D97" s="17"/>
-      <c r="E97" s="5"/>
-      <c r="F97" s="5"/>
-      <c r="G97" s="5"/>
-      <c r="H97" s="5"/>
-      <c r="I97" s="17"/>
-      <c r="J97" s="5"/>
-      <c r="K97" s="5"/>
-      <c r="L97" s="5"/>
-      <c r="M97" s="5"/>
-      <c r="N97" s="5"/>
-      <c r="O97" s="5"/>
-      <c r="P97" s="5"/>
-      <c r="Q97" s="5"/>
-      <c r="R97" s="5"/>
-      <c r="S97" s="5"/>
-      <c r="T97" s="5"/>
-      <c r="U97" s="5"/>
-      <c r="V97" s="5"/>
-      <c r="W97" s="5"/>
-      <c r="X97" s="5"/>
-      <c r="Y97" s="5"/>
+      <c r="D97" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="E97" s="1">
+        <v>3</v>
+      </c>
+      <c r="F97" s="1">
+        <v>0</v>
+      </c>
+      <c r="G97" s="1"/>
+      <c r="H97" s="1"/>
+      <c r="I97" s="29">
+        <f t="shared" ref="I97:I102" si="0">SUM(E97:H97)</f>
+        <v>3</v>
+      </c>
+      <c r="P97" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q97" s="12">
+        <f>H89</f>
+        <v>470</v>
+      </c>
+      <c r="R97" s="40">
+        <v>-200</v>
+      </c>
+      <c r="S97" s="12">
+        <f t="shared" ref="S97:S102" si="1">I97</f>
+        <v>3</v>
+      </c>
+      <c r="T97" s="12">
+        <f t="shared" ref="T97:T102" si="2">IFERROR((-SUM($R$96:$R$102)/SUM($S$96:$S$102))*$S97, 0)</f>
+        <v>105</v>
+      </c>
+      <c r="U97" s="12">
+        <f t="shared" ref="U97:U102" si="3">SUM(Q97,R97,T97)</f>
+        <v>375</v>
+      </c>
+      <c r="V97" s="29" t="s">
+        <v>5</v>
+      </c>
       <c r="Z97" s="5"/>
     </row>
-    <row r="98" spans="2:26" ht="19" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:26" ht="21" x14ac:dyDescent="0.25">
       <c r="B98" s="5"/>
       <c r="C98" s="5"/>
-      <c r="D98" s="17"/>
-      <c r="E98" s="5"/>
-      <c r="F98" s="5"/>
-      <c r="G98" s="5"/>
-      <c r="H98" s="5"/>
-      <c r="I98" s="17"/>
-      <c r="J98" s="5"/>
-      <c r="K98" s="5"/>
-      <c r="L98" s="5"/>
-      <c r="M98" s="5"/>
-      <c r="N98" s="5"/>
-      <c r="O98" s="5"/>
-      <c r="P98" s="5"/>
-      <c r="Q98" s="5"/>
-      <c r="R98" s="5"/>
-      <c r="S98" s="5"/>
-      <c r="T98" s="5"/>
-      <c r="U98" s="5"/>
-      <c r="V98" s="5"/>
-      <c r="W98" s="5"/>
-      <c r="X98" s="5"/>
-      <c r="Y98" s="5"/>
+      <c r="D98" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E98" s="1">
+        <v>11</v>
+      </c>
+      <c r="F98" s="1">
+        <v>5</v>
+      </c>
+      <c r="G98" s="1"/>
+      <c r="H98" s="1"/>
+      <c r="I98" s="29">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="P98" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q98" s="12">
+        <f>K89</f>
+        <v>-171.66</v>
+      </c>
+      <c r="R98" s="40">
+        <v>-200</v>
+      </c>
+      <c r="S98" s="12">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="T98" s="12">
+        <f t="shared" si="2"/>
+        <v>560</v>
+      </c>
+      <c r="U98" s="12">
+        <f t="shared" si="3"/>
+        <v>188.34000000000003</v>
+      </c>
+      <c r="V98" s="29" t="s">
+        <v>9</v>
+      </c>
       <c r="Z98" s="5"/>
     </row>
-    <row r="99" spans="2:26" ht="19" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:26" ht="21" x14ac:dyDescent="0.25">
       <c r="B99" s="5"/>
       <c r="C99" s="5"/>
-      <c r="D99" s="17"/>
-      <c r="E99" s="5"/>
-      <c r="F99" s="5"/>
-      <c r="G99" s="5"/>
-      <c r="H99" s="5"/>
-      <c r="I99" s="17"/>
-      <c r="J99" s="5"/>
-      <c r="K99" s="5"/>
-      <c r="L99" s="5"/>
-      <c r="M99" s="5"/>
-      <c r="N99" s="5"/>
-      <c r="O99" s="5"/>
-      <c r="P99" s="5"/>
-      <c r="Q99" s="5"/>
-      <c r="R99" s="5"/>
-      <c r="S99" s="5"/>
-      <c r="T99" s="5"/>
-      <c r="U99" s="5"/>
-      <c r="V99" s="5"/>
-      <c r="W99" s="5"/>
-      <c r="X99" s="5"/>
-      <c r="Y99" s="5"/>
+      <c r="D99" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E99" s="1">
+        <v>11</v>
+      </c>
+      <c r="F99" s="1">
+        <v>0</v>
+      </c>
+      <c r="G99" s="1"/>
+      <c r="H99" s="1"/>
+      <c r="I99" s="29">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="P99" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q99" s="12">
+        <f>N89</f>
+        <v>397.5</v>
+      </c>
+      <c r="R99" s="40">
+        <v>-200</v>
+      </c>
+      <c r="S99" s="12">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="T99" s="12">
+        <f t="shared" si="2"/>
+        <v>385</v>
+      </c>
+      <c r="U99" s="12">
+        <f t="shared" si="3"/>
+        <v>582.5</v>
+      </c>
+      <c r="V99" s="29" t="s">
+        <v>12</v>
+      </c>
       <c r="Z99" s="5"/>
     </row>
-    <row r="100" spans="2:26" ht="19" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:26" ht="21" x14ac:dyDescent="0.25">
       <c r="B100" s="5"/>
       <c r="C100" s="5"/>
-      <c r="D100" s="17"/>
-      <c r="E100" s="5"/>
-      <c r="F100" s="5"/>
-      <c r="G100" s="5"/>
-      <c r="H100" s="5"/>
-      <c r="I100" s="17"/>
-      <c r="J100" s="5"/>
-      <c r="K100" s="5"/>
-      <c r="L100" s="5"/>
-      <c r="M100" s="5"/>
-      <c r="N100" s="5"/>
-      <c r="O100" s="5"/>
-      <c r="P100" s="5"/>
-      <c r="Q100" s="5"/>
-      <c r="R100" s="5"/>
-      <c r="S100" s="5"/>
-      <c r="T100" s="5"/>
-      <c r="U100" s="5"/>
-      <c r="V100" s="5"/>
-      <c r="W100" s="5"/>
-      <c r="X100" s="5"/>
-      <c r="Y100" s="5"/>
+      <c r="D100" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E100" s="1">
+        <v>0</v>
+      </c>
+      <c r="F100" s="1">
+        <v>0</v>
+      </c>
+      <c r="G100" s="1"/>
+      <c r="H100" s="1"/>
+      <c r="I100" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P100" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q100" s="12">
+        <f>Q89</f>
+        <v>108.32999999999998</v>
+      </c>
+      <c r="R100" s="40">
+        <v>-200</v>
+      </c>
+      <c r="S100" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T100" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U100" s="12">
+        <f t="shared" si="3"/>
+        <v>-91.670000000000016</v>
+      </c>
+      <c r="V100" s="29" t="s">
+        <v>10</v>
+      </c>
       <c r="Z100" s="5"/>
     </row>
-    <row r="101" spans="2:26" ht="19" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:26" ht="21" x14ac:dyDescent="0.25">
       <c r="B101" s="5"/>
       <c r="C101" s="5"/>
-      <c r="D101" s="17"/>
-      <c r="E101" s="5"/>
-      <c r="F101" s="5"/>
-      <c r="G101" s="5"/>
-      <c r="H101" s="5"/>
-      <c r="I101" s="17"/>
-      <c r="J101" s="5"/>
-      <c r="K101" s="5"/>
-      <c r="L101" s="5"/>
-      <c r="M101" s="5"/>
-      <c r="N101" s="5"/>
-      <c r="O101" s="5"/>
-      <c r="P101" s="5"/>
-      <c r="Q101" s="5"/>
-      <c r="R101" s="5"/>
-      <c r="S101" s="5"/>
-      <c r="T101" s="5"/>
-      <c r="U101" s="5"/>
-      <c r="V101" s="5"/>
-      <c r="W101" s="5"/>
-      <c r="X101" s="5"/>
-      <c r="Y101" s="5"/>
+      <c r="D101" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E101" s="1">
+        <v>0</v>
+      </c>
+      <c r="F101" s="1">
+        <v>0</v>
+      </c>
+      <c r="G101" s="1"/>
+      <c r="H101" s="1"/>
+      <c r="I101" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P101" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q101" s="12">
+        <f>T89</f>
+        <v>-242.5</v>
+      </c>
+      <c r="R101" s="40">
+        <v>-200</v>
+      </c>
+      <c r="S101" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T101" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U101" s="12">
+        <f t="shared" si="3"/>
+        <v>-442.5</v>
+      </c>
+      <c r="V101" s="29" t="s">
+        <v>17</v>
+      </c>
       <c r="Z101" s="5"/>
     </row>
-    <row r="102" spans="2:26" ht="19" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:26" ht="21" x14ac:dyDescent="0.25">
       <c r="B102" s="5"/>
       <c r="C102" s="5"/>
-      <c r="D102" s="17"/>
-      <c r="E102" s="5"/>
-      <c r="F102" s="5"/>
-      <c r="G102" s="5"/>
-      <c r="H102" s="5"/>
-      <c r="I102" s="17"/>
-      <c r="J102" s="5"/>
-      <c r="K102" s="5"/>
-      <c r="L102" s="5"/>
-      <c r="M102" s="5"/>
-      <c r="N102" s="5"/>
-      <c r="O102" s="5"/>
-      <c r="P102" s="5"/>
-      <c r="Q102" s="5"/>
-      <c r="R102" s="5"/>
-      <c r="S102" s="5"/>
-      <c r="T102" s="5"/>
-      <c r="U102" s="5"/>
-      <c r="V102" s="5"/>
-      <c r="W102" s="5"/>
-      <c r="X102" s="5"/>
-      <c r="Y102" s="5"/>
+      <c r="D102" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="E102" s="1">
+        <v>3</v>
+      </c>
+      <c r="F102" s="1">
+        <v>7</v>
+      </c>
+      <c r="G102" s="1"/>
+      <c r="H102" s="1"/>
+      <c r="I102" s="29">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="P102" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q102" s="12">
+        <f>W89</f>
+        <v>-299.17</v>
+      </c>
+      <c r="R102" s="40">
+        <v>-200</v>
+      </c>
+      <c r="S102" s="12">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="T102" s="12">
+        <f t="shared" si="2"/>
+        <v>350</v>
+      </c>
+      <c r="U102" s="12">
+        <f t="shared" si="3"/>
+        <v>-149.17000000000002</v>
+      </c>
+      <c r="V102" s="29" t="s">
+        <v>97</v>
+      </c>
       <c r="Z102" s="5"/>
     </row>
-    <row r="103" spans="2:26" ht="19" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:26" ht="21" x14ac:dyDescent="0.25">
       <c r="B103" s="5"/>
       <c r="C103" s="5"/>
-      <c r="D103" s="17"/>
-      <c r="E103" s="5"/>
-      <c r="F103" s="5"/>
-      <c r="G103" s="5"/>
-      <c r="H103" s="5"/>
-      <c r="I103" s="17"/>
-      <c r="J103" s="5"/>
-      <c r="K103" s="5"/>
-      <c r="L103" s="5"/>
-      <c r="M103" s="5"/>
-      <c r="N103" s="5"/>
-      <c r="O103" s="5"/>
-      <c r="P103" s="5"/>
-      <c r="Q103" s="5"/>
-      <c r="R103" s="5"/>
-      <c r="S103" s="5"/>
-      <c r="T103" s="5"/>
-      <c r="U103" s="5"/>
-      <c r="V103" s="5"/>
-      <c r="W103" s="5"/>
-      <c r="X103" s="5"/>
-      <c r="Y103" s="5"/>
+      <c r="U103" s="41">
+        <f>SUM(U96:U102)</f>
+        <v>0</v>
+      </c>
       <c r="Z103" s="5"/>
     </row>
-    <row r="104" spans="2:26" ht="19" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B104" s="5"/>
       <c r="C104" s="5"/>
-      <c r="D104" s="17"/>
-      <c r="E104" s="5"/>
-      <c r="F104" s="5"/>
-      <c r="G104" s="5"/>
-      <c r="H104" s="5"/>
-      <c r="I104" s="17"/>
-      <c r="J104" s="5"/>
-      <c r="K104" s="5"/>
-      <c r="L104" s="5"/>
-      <c r="M104" s="5"/>
-      <c r="N104" s="5"/>
-      <c r="O104" s="5"/>
-      <c r="P104" s="5"/>
-      <c r="Q104" s="5"/>
-      <c r="R104" s="5"/>
-      <c r="S104" s="5"/>
-      <c r="T104" s="5"/>
-      <c r="U104" s="5"/>
-      <c r="V104" s="5"/>
-      <c r="W104" s="5"/>
-      <c r="X104" s="5"/>
-      <c r="Y104" s="5"/>
       <c r="Z104" s="5"/>
     </row>
     <row r="105" spans="2:26" x14ac:dyDescent="0.2">
@@ -7235,63 +6971,9 @@
       <c r="Y118" s="5"/>
       <c r="Z118" s="5"/>
     </row>
-    <row r="119" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="B119" s="5"/>
-      <c r="C119" s="5"/>
-      <c r="D119" s="5"/>
-      <c r="E119" s="5"/>
-      <c r="F119" s="5"/>
-      <c r="G119" s="5"/>
-      <c r="H119" s="5"/>
-      <c r="I119" s="5"/>
-      <c r="J119" s="5"/>
-      <c r="K119" s="5"/>
-      <c r="L119" s="5"/>
-      <c r="M119" s="5"/>
-      <c r="N119" s="5"/>
-      <c r="O119" s="5"/>
-      <c r="P119" s="5"/>
-      <c r="Q119" s="5"/>
-      <c r="R119" s="5"/>
-      <c r="S119" s="5"/>
-      <c r="T119" s="5"/>
-      <c r="U119" s="5"/>
-      <c r="V119" s="5"/>
-      <c r="W119" s="5"/>
-      <c r="X119" s="5"/>
-      <c r="Y119" s="5"/>
-      <c r="Z119" s="5"/>
-    </row>
-    <row r="120" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="B120" s="5"/>
-      <c r="C120" s="5"/>
-      <c r="D120" s="5"/>
-      <c r="E120" s="5"/>
-      <c r="F120" s="5"/>
-      <c r="G120" s="5"/>
-      <c r="H120" s="5"/>
-      <c r="I120" s="5"/>
-      <c r="J120" s="5"/>
-      <c r="K120" s="5"/>
-      <c r="L120" s="5"/>
-      <c r="M120" s="5"/>
-      <c r="N120" s="5"/>
-      <c r="O120" s="5"/>
-      <c r="P120" s="5"/>
-      <c r="Q120" s="5"/>
-      <c r="R120" s="5"/>
-      <c r="S120" s="5"/>
-      <c r="T120" s="5"/>
-      <c r="U120" s="5"/>
-      <c r="V120" s="5"/>
-      <c r="W120" s="5"/>
-      <c r="X120" s="5"/>
-      <c r="Y120" s="5"/>
-      <c r="Z120" s="5"/>
-    </row>
   </sheetData>
   <dataConsolidate/>
-  <mergeCells count="9">
+  <mergeCells count="13">
     <mergeCell ref="E94:H94"/>
     <mergeCell ref="P11:Q11"/>
     <mergeCell ref="S11:T11"/>
@@ -7301,81 +6983,96 @@
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="J11:K11"/>
     <mergeCell ref="M11:N11"/>
+    <mergeCell ref="P94:P95"/>
+    <mergeCell ref="Q94:Q95"/>
+    <mergeCell ref="R94:T94"/>
+    <mergeCell ref="U94:U95"/>
   </mergeCells>
-  <conditionalFormatting sqref="E89">
-    <cfRule type="cellIs" dxfId="74" priority="247" operator="lessThan">
+  <conditionalFormatting sqref="E89 U101:U102 Q96:Q102">
+    <cfRule type="cellIs" dxfId="23" priority="256" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="248" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="257" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="249" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="258" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H89">
-    <cfRule type="cellIs" dxfId="17" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="20" priority="25" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="26" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="27" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K89">
-    <cfRule type="cellIs" dxfId="14" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="17" priority="22" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="23" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="24" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N89">
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="19" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="20" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="21" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q89">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="16" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="17" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="18" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T89">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="14" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="15" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W89">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="12" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U96:U100">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7385,10 +7082,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25E9A583-41BF-8143-84DF-F8B494A614D1}">
-  <dimension ref="A18:A23"/>
+  <dimension ref="E6:J24"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:XFD8"/>
+    <sheetView showGridLines="0" topLeftCell="C6" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7400,15 +7097,210 @@
     <col min="11" max="11" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="18" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="E6" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="5:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="E7" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="5:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="E8" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="5:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="E9" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="5:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="E10" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="5:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="E11" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="5:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="E12" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="5:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="E13" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="F13" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="5:10" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="5:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E17" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="5:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E18" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="5:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E19" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="5:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E20" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="5:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E21" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="5:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="E22" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="5:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="E23" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" s="30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="5:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="E24" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="F24" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" s="30" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I73:K81">
-    <sortCondition descending="1" ref="K73:K81"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I71:K79">
+    <sortCondition descending="1" ref="K71:K79"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Results qualifier 2 RR vs RCB
</commit_message>
<xml_diff>
--- a/2022/EBE Boys 2022.xlsx
+++ b/2022/EBE Boys 2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07318F5C-48BC-8D49-A25A-99B962DCCA22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348A3893-5081-AA48-86F3-603312F22A3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20420" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20420" activeTab="1" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="114">
   <si>
     <t>Points</t>
   </si>
@@ -376,6 +376,12 @@
   </si>
   <si>
     <t>Eliminator LSG vs RCB</t>
+  </si>
+  <si>
+    <t>Qualifier 2 RR vs RCB</t>
+  </si>
+  <si>
+    <t>Finals GT vs RR</t>
   </si>
 </sst>
 </file>
@@ -1317,7 +1323,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
   <dimension ref="A1:Z118"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="11" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="U103" sqref="U103"/>
     </sheetView>
@@ -1331,7 +1337,7 @@
     <col min="12" max="12" width="4.33203125" customWidth="1"/>
     <col min="15" max="15" width="4.5" customWidth="1"/>
     <col min="18" max="18" width="10.33203125" customWidth="1"/>
-    <col min="21" max="21" width="13.5" customWidth="1"/>
+    <col min="21" max="21" width="13.1640625" customWidth="1"/>
     <col min="24" max="24" width="6.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5920,41 +5926,55 @@
       <c r="C85" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D85" s="3" t="str">
+      <c r="D85" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E85, ($W85,$T85,$Q85,$N85,$K85,$H85,$E85), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E85, ($W85,$T85,$Q85,$N85,$K85,$H85,$E85), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E85" s="1"/>
-      <c r="G85" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="E85" s="1">
+        <v>50</v>
+      </c>
+      <c r="G85" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H85, ($W85,$T85,$Q85,$N85,$K85,$H85,$E85), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H85, ($W85,$T85,$Q85,$N85,$K85,$H85,$E85), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H85" s="1"/>
-      <c r="J85" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="H85" s="1">
+        <v>70</v>
+      </c>
+      <c r="J85" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K85, ($W85,$T85,$Q85,$N85,$K85,$H85,$E85), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K85, ($W85,$T85,$Q85,$N85,$K85,$H85,$E85), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K85" s="1"/>
-      <c r="M85" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K85" s="1">
+        <v>60</v>
+      </c>
+      <c r="M85" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N85, ($W85,$T85,$Q85,$N85,$K85,$H85,$E85), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N85, ($W85,$T85,$Q85,$N85,$K85,$H85,$E85), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N85" s="1"/>
-      <c r="P85" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="N85" s="1">
+        <v>40</v>
+      </c>
+      <c r="P85" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q85, ($W85,$T85,$Q85,$N85,$K85,$H85,$E85), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q85, ($W85,$T85,$Q85,$N85,$K85,$H85,$E85), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q85" s="1"/>
-      <c r="S85" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="Q85" s="1">
+        <v>100</v>
+      </c>
+      <c r="S85" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T85, ($W85,$T85,$Q85,$N85,$K85,$H85,$E85), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T85, ($W85,$T85,$Q85,$N85,$K85,$H85,$E85), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T85" s="1"/>
-      <c r="V85" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="T85" s="1">
+        <v>0</v>
+      </c>
+      <c r="V85" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W85, ($W85,$T85,$Q85,$N85,$K85,$H85,$E85), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W85, ($W85,$T85,$Q85,$N85,$K85,$H85,$E85), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W85" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="W85" s="1">
+        <v>80</v>
+      </c>
     </row>
     <row r="86" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A86" s="6" t="s">
@@ -6084,7 +6104,7 @@
       </c>
       <c r="E89" s="12">
         <f>SUM(D13:D86)</f>
-        <v>-262.5</v>
+        <v>-277.5</v>
       </c>
       <c r="G89" s="7" t="s">
         <v>7</v>
@@ -6098,35 +6118,35 @@
       </c>
       <c r="K89" s="12">
         <f>SUM(J13:J86)</f>
-        <v>-171.66</v>
+        <v>-181.66</v>
       </c>
       <c r="M89" s="7" t="s">
         <v>7</v>
       </c>
       <c r="N89" s="12">
         <f>SUM(M13:M86)</f>
-        <v>397.5</v>
+        <v>377.5</v>
       </c>
       <c r="P89" s="7" t="s">
         <v>7</v>
       </c>
       <c r="Q89" s="12">
         <f>SUM(P13:P86)</f>
-        <v>108.32999999999998</v>
+        <v>158.32999999999998</v>
       </c>
       <c r="S89" s="7" t="s">
         <v>7</v>
       </c>
       <c r="T89" s="12">
         <f>SUM(S13:S86)</f>
-        <v>-242.5</v>
+        <v>-267.5</v>
       </c>
       <c r="V89" s="7" t="s">
         <v>7</v>
       </c>
       <c r="W89" s="12">
         <f>SUM(V13:V86)</f>
-        <v>-299.17</v>
+        <v>-279.17</v>
       </c>
       <c r="X89" s="1">
         <f>SUM(E89,H89,K89,N89,Q89,T89,W89)</f>
@@ -6276,33 +6296,35 @@
       <c r="F96" s="1">
         <v>0</v>
       </c>
-      <c r="G96" s="1"/>
+      <c r="G96" s="1">
+        <v>3</v>
+      </c>
       <c r="H96" s="1"/>
       <c r="I96" s="29">
         <f>SUM(E96:H96)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P96" s="29" t="s">
         <v>8</v>
       </c>
       <c r="Q96" s="12">
         <f>E89</f>
-        <v>-262.5</v>
+        <v>-277.5</v>
       </c>
       <c r="R96" s="40">
         <v>-200</v>
       </c>
       <c r="S96" s="12">
         <f>I96</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T96" s="12">
         <f>IFERROR((-SUM($R$96:$R$102)/SUM($S$96:$S$102))*$S96, 0)</f>
-        <v>0</v>
+        <v>51.219512195121951</v>
       </c>
       <c r="U96" s="12">
         <f>SUM(Q96,R96,T96)</f>
-        <v>-462.5</v>
+        <v>-426.28048780487802</v>
       </c>
       <c r="V96" s="29" t="s">
         <v>8</v>
@@ -6321,7 +6343,9 @@
       <c r="F97" s="1">
         <v>0</v>
       </c>
-      <c r="G97" s="1"/>
+      <c r="G97" s="1">
+        <v>0</v>
+      </c>
       <c r="H97" s="1"/>
       <c r="I97" s="29">
         <f t="shared" ref="I97:I102" si="0">SUM(E97:H97)</f>
@@ -6343,11 +6367,11 @@
       </c>
       <c r="T97" s="12">
         <f t="shared" ref="T97:T102" si="2">IFERROR((-SUM($R$96:$R$102)/SUM($S$96:$S$102))*$S97, 0)</f>
-        <v>105</v>
+        <v>51.219512195121951</v>
       </c>
       <c r="U97" s="12">
         <f t="shared" ref="U97:U102" si="3">SUM(Q97,R97,T97)</f>
-        <v>375</v>
+        <v>321.21951219512198</v>
       </c>
       <c r="V97" s="29" t="s">
         <v>5</v>
@@ -6366,7 +6390,9 @@
       <c r="F98" s="1">
         <v>5</v>
       </c>
-      <c r="G98" s="1"/>
+      <c r="G98" s="1">
+        <v>0</v>
+      </c>
       <c r="H98" s="1"/>
       <c r="I98" s="29">
         <f t="shared" si="0"/>
@@ -6377,7 +6403,7 @@
       </c>
       <c r="Q98" s="12">
         <f>K89</f>
-        <v>-171.66</v>
+        <v>-181.66</v>
       </c>
       <c r="R98" s="40">
         <v>-200</v>
@@ -6388,11 +6414,11 @@
       </c>
       <c r="T98" s="12">
         <f t="shared" si="2"/>
-        <v>560</v>
+        <v>273.17073170731709</v>
       </c>
       <c r="U98" s="12">
         <f t="shared" si="3"/>
-        <v>188.34000000000003</v>
+        <v>-108.48926829268288</v>
       </c>
       <c r="V98" s="29" t="s">
         <v>9</v>
@@ -6411,33 +6437,35 @@
       <c r="F99" s="1">
         <v>0</v>
       </c>
-      <c r="G99" s="1"/>
+      <c r="G99" s="1">
+        <v>3</v>
+      </c>
       <c r="H99" s="1"/>
       <c r="I99" s="29">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="P99" s="29" t="s">
         <v>12</v>
       </c>
       <c r="Q99" s="12">
         <f>N89</f>
-        <v>397.5</v>
+        <v>377.5</v>
       </c>
       <c r="R99" s="40">
         <v>-200</v>
       </c>
       <c r="S99" s="12">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="T99" s="12">
         <f t="shared" si="2"/>
-        <v>385</v>
+        <v>239.02439024390245</v>
       </c>
       <c r="U99" s="12">
         <f t="shared" si="3"/>
-        <v>582.5</v>
+        <v>416.52439024390242</v>
       </c>
       <c r="V99" s="29" t="s">
         <v>12</v>
@@ -6456,33 +6484,35 @@
       <c r="F100" s="1">
         <v>0</v>
       </c>
-      <c r="G100" s="1"/>
+      <c r="G100" s="1">
+        <v>11</v>
+      </c>
       <c r="H100" s="1"/>
       <c r="I100" s="29">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="P100" s="29" t="s">
         <v>10</v>
       </c>
       <c r="Q100" s="12">
         <f>Q89</f>
-        <v>108.32999999999998</v>
+        <v>158.32999999999998</v>
       </c>
       <c r="R100" s="40">
         <v>-200</v>
       </c>
       <c r="S100" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="T100" s="12">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>187.80487804878049</v>
       </c>
       <c r="U100" s="12">
         <f t="shared" si="3"/>
-        <v>-91.670000000000016</v>
+        <v>146.13487804878048</v>
       </c>
       <c r="V100" s="29" t="s">
         <v>10</v>
@@ -6501,7 +6531,9 @@
       <c r="F101" s="1">
         <v>0</v>
       </c>
-      <c r="G101" s="1"/>
+      <c r="G101" s="1">
+        <v>0</v>
+      </c>
       <c r="H101" s="1"/>
       <c r="I101" s="29">
         <f t="shared" si="0"/>
@@ -6512,7 +6544,7 @@
       </c>
       <c r="Q101" s="12">
         <f>T89</f>
-        <v>-242.5</v>
+        <v>-267.5</v>
       </c>
       <c r="R101" s="40">
         <v>-200</v>
@@ -6527,7 +6559,7 @@
       </c>
       <c r="U101" s="12">
         <f t="shared" si="3"/>
-        <v>-442.5</v>
+        <v>-467.5</v>
       </c>
       <c r="V101" s="29" t="s">
         <v>17</v>
@@ -6546,33 +6578,35 @@
       <c r="F102" s="1">
         <v>7</v>
       </c>
-      <c r="G102" s="1"/>
+      <c r="G102" s="1">
+        <v>25</v>
+      </c>
       <c r="H102" s="1"/>
       <c r="I102" s="29">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="P102" s="29" t="s">
         <v>97</v>
       </c>
       <c r="Q102" s="12">
         <f>W89</f>
-        <v>-299.17</v>
+        <v>-279.17</v>
       </c>
       <c r="R102" s="40">
         <v>-200</v>
       </c>
       <c r="S102" s="12">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="T102" s="12">
         <f t="shared" si="2"/>
-        <v>350</v>
+        <v>597.56097560975616</v>
       </c>
       <c r="U102" s="12">
         <f t="shared" si="3"/>
-        <v>-149.17000000000002</v>
+        <v>118.39097560975614</v>
       </c>
       <c r="V102" s="29" t="s">
         <v>97</v>
@@ -6584,7 +6618,7 @@
       <c r="C103" s="5"/>
       <c r="U103" s="41">
         <f>SUM(U96:U102)</f>
-        <v>0</v>
+        <v>1.1368683772161603E-13</v>
       </c>
       <c r="Z103" s="5"/>
     </row>
@@ -7082,10 +7116,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25E9A583-41BF-8143-84DF-F8B494A614D1}">
-  <dimension ref="E6:J24"/>
+  <dimension ref="E6:J47"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C6" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7298,6 +7332,202 @@
         <v>18</v>
       </c>
     </row>
+    <row r="29" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="E29" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="5:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="E30" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="F30" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="J30" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="5:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="E31" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="G31" s="30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="5:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="E32" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" s="30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="5:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="E33" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33" s="30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="5:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="E34" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="G34" s="30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="5:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="E35" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F35" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="G35" s="30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="5:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="E36" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="F36" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" s="30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="E40" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="J40" s="7"/>
+    </row>
+    <row r="41" spans="5:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="E41" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="F41" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="G41" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="I41" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="J41" s="7"/>
+    </row>
+    <row r="42" spans="5:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="E42" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="F42" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="G42" s="30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="5:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="E43" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="G43" s="30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="5:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="E44" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="G44" s="30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="5:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="E45" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F45" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="G45" s="30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="5:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="E46" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F46" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="G46" s="30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="5:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="E47" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="F47" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="G47" s="30" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I71:K79">
     <sortCondition descending="1" ref="K71:K79"/>

</xml_diff>

<commit_message>
Finals GT vs RR
</commit_message>
<xml_diff>
--- a/2022/EBE Boys 2022.xlsx
+++ b/2022/EBE Boys 2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348A3893-5081-AA48-86F3-603312F22A3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7450A2F2-17FD-7641-BFCD-9B9415C6FA93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20420" activeTab="1" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20420" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="114">
   <si>
     <t>Points</t>
   </si>
@@ -388,6 +388,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.000000"/>
+  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -672,7 +675,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -759,6 +762,7 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent6" xfId="1" builtinId="50"/>
@@ -1323,7 +1327,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
   <dimension ref="A1:Z118"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="11" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="U103" sqref="U103"/>
     </sheetView>
@@ -5984,41 +5988,55 @@
         <v>1</v>
       </c>
       <c r="C86" s="15"/>
-      <c r="D86" s="3" t="str">
+      <c r="D86" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E86, ($W86,$T86,$Q86,$N86,$K86,$H86,$E86), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E86, ($W86,$T86,$Q86,$N86,$K86,$H86,$E86), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E86" s="1"/>
-      <c r="G86" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="E86" s="1">
+        <v>40</v>
+      </c>
+      <c r="G86" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H86, ($W86,$T86,$Q86,$N86,$K86,$H86,$E86), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H86, ($W86,$T86,$Q86,$N86,$K86,$H86,$E86), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H86" s="1"/>
-      <c r="J86" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="H86" s="1">
+        <v>80</v>
+      </c>
+      <c r="J86" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K86, ($W86,$T86,$Q86,$N86,$K86,$H86,$E86), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K86, ($W86,$T86,$Q86,$N86,$K86,$H86,$E86), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K86" s="1"/>
-      <c r="M86" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K86" s="1">
+        <v>60</v>
+      </c>
+      <c r="M86" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N86, ($W86,$T86,$Q86,$N86,$K86,$H86,$E86), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N86, ($W86,$T86,$Q86,$N86,$K86,$H86,$E86), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N86" s="1"/>
-      <c r="P86" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="N86" s="1">
+        <v>100</v>
+      </c>
+      <c r="P86" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q86, ($W86,$T86,$Q86,$N86,$K86,$H86,$E86), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q86, ($W86,$T86,$Q86,$N86,$K86,$H86,$E86), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q86" s="1"/>
-      <c r="S86" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q86" s="1">
+        <v>70</v>
+      </c>
+      <c r="S86" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T86, ($W86,$T86,$Q86,$N86,$K86,$H86,$E86), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T86, ($W86,$T86,$Q86,$N86,$K86,$H86,$E86), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T86" s="1"/>
-      <c r="V86" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="T86" s="1">
+        <v>50</v>
+      </c>
+      <c r="V86" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W86, ($W86,$T86,$Q86,$N86,$K86,$H86,$E86), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W86, ($W86,$T86,$Q86,$N86,$K86,$H86,$E86), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W86" s="1"/>
+        <v>-25</v>
+      </c>
+      <c r="W86" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="87" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A87" s="6"/>
@@ -6104,28 +6122,28 @@
       </c>
       <c r="E89" s="12">
         <f>SUM(D13:D86)</f>
-        <v>-277.5</v>
+        <v>-297.5</v>
       </c>
       <c r="G89" s="7" t="s">
         <v>7</v>
       </c>
       <c r="H89" s="12">
         <f>SUM(G13:G86)</f>
-        <v>470</v>
+        <v>490</v>
       </c>
       <c r="J89" s="7" t="s">
         <v>7</v>
       </c>
       <c r="K89" s="12">
         <f>SUM(J13:J86)</f>
-        <v>-181.66</v>
+        <v>-191.66</v>
       </c>
       <c r="M89" s="7" t="s">
         <v>7</v>
       </c>
       <c r="N89" s="12">
         <f>SUM(M13:M86)</f>
-        <v>377.5</v>
+        <v>427.5</v>
       </c>
       <c r="P89" s="7" t="s">
         <v>7</v>
@@ -6139,14 +6157,14 @@
       </c>
       <c r="T89" s="12">
         <f>SUM(S13:S86)</f>
-        <v>-267.5</v>
+        <v>-282.5</v>
       </c>
       <c r="V89" s="7" t="s">
         <v>7</v>
       </c>
       <c r="W89" s="12">
         <f>SUM(V13:V86)</f>
-        <v>-279.17</v>
+        <v>-304.17</v>
       </c>
       <c r="X89" s="1">
         <f>SUM(E89,H89,K89,N89,Q89,T89,W89)</f>
@@ -6299,7 +6317,9 @@
       <c r="G96" s="1">
         <v>3</v>
       </c>
-      <c r="H96" s="1"/>
+      <c r="H96" s="1">
+        <v>0</v>
+      </c>
       <c r="I96" s="29">
         <f>SUM(E96:H96)</f>
         <v>3</v>
@@ -6309,7 +6329,7 @@
       </c>
       <c r="Q96" s="12">
         <f>E89</f>
-        <v>-277.5</v>
+        <v>-297.5</v>
       </c>
       <c r="R96" s="40">
         <v>-200</v>
@@ -6320,11 +6340,11 @@
       </c>
       <c r="T96" s="12">
         <f>IFERROR((-SUM($R$96:$R$102)/SUM($S$96:$S$102))*$S96, 0)</f>
-        <v>51.219512195121951</v>
+        <v>42.424242424242422</v>
       </c>
       <c r="U96" s="12">
         <f>SUM(Q96,R96,T96)</f>
-        <v>-426.28048780487802</v>
+        <v>-455.07575757575756</v>
       </c>
       <c r="V96" s="29" t="s">
         <v>8</v>
@@ -6346,32 +6366,34 @@
       <c r="G97" s="1">
         <v>0</v>
       </c>
-      <c r="H97" s="1"/>
+      <c r="H97" s="1">
+        <v>3</v>
+      </c>
       <c r="I97" s="29">
         <f t="shared" ref="I97:I102" si="0">SUM(E97:H97)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="P97" s="29" t="s">
         <v>5</v>
       </c>
       <c r="Q97" s="12">
         <f>H89</f>
-        <v>470</v>
+        <v>490</v>
       </c>
       <c r="R97" s="40">
         <v>-200</v>
       </c>
       <c r="S97" s="12">
         <f t="shared" ref="S97:S102" si="1">I97</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="T97" s="12">
         <f t="shared" ref="T97:T102" si="2">IFERROR((-SUM($R$96:$R$102)/SUM($S$96:$S$102))*$S97, 0)</f>
-        <v>51.219512195121951</v>
+        <v>84.848484848484844</v>
       </c>
       <c r="U97" s="12">
         <f t="shared" ref="U97:U102" si="3">SUM(Q97,R97,T97)</f>
-        <v>321.21951219512198</v>
+        <v>374.84848484848487</v>
       </c>
       <c r="V97" s="29" t="s">
         <v>5</v>
@@ -6393,32 +6415,34 @@
       <c r="G98" s="1">
         <v>0</v>
       </c>
-      <c r="H98" s="1"/>
+      <c r="H98" s="1">
+        <v>3</v>
+      </c>
       <c r="I98" s="29">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="P98" s="29" t="s">
         <v>9</v>
       </c>
       <c r="Q98" s="12">
         <f>K89</f>
-        <v>-181.66</v>
+        <v>-191.66</v>
       </c>
       <c r="R98" s="40">
         <v>-200</v>
       </c>
       <c r="S98" s="12">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="T98" s="12">
         <f t="shared" si="2"/>
-        <v>273.17073170731709</v>
+        <v>268.68686868686871</v>
       </c>
       <c r="U98" s="12">
         <f t="shared" si="3"/>
-        <v>-108.48926829268288</v>
+        <v>-122.97313131313126</v>
       </c>
       <c r="V98" s="29" t="s">
         <v>9</v>
@@ -6440,32 +6464,34 @@
       <c r="G99" s="1">
         <v>3</v>
       </c>
-      <c r="H99" s="1"/>
+      <c r="H99" s="1">
+        <v>11</v>
+      </c>
       <c r="I99" s="29">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="P99" s="29" t="s">
         <v>12</v>
       </c>
       <c r="Q99" s="12">
         <f>N89</f>
-        <v>377.5</v>
+        <v>427.5</v>
       </c>
       <c r="R99" s="40">
         <v>-200</v>
       </c>
       <c r="S99" s="12">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="T99" s="12">
         <f t="shared" si="2"/>
-        <v>239.02439024390245</v>
+        <v>353.53535353535352</v>
       </c>
       <c r="U99" s="12">
         <f t="shared" si="3"/>
-        <v>416.52439024390242</v>
+        <v>581.03535353535358</v>
       </c>
       <c r="V99" s="29" t="s">
         <v>12</v>
@@ -6487,7 +6513,9 @@
       <c r="G100" s="1">
         <v>11</v>
       </c>
-      <c r="H100" s="1"/>
+      <c r="H100" s="1">
+        <v>0</v>
+      </c>
       <c r="I100" s="29">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -6508,11 +6536,11 @@
       </c>
       <c r="T100" s="12">
         <f t="shared" si="2"/>
-        <v>187.80487804878049</v>
+        <v>155.55555555555557</v>
       </c>
       <c r="U100" s="12">
         <f t="shared" si="3"/>
-        <v>146.13487804878048</v>
+        <v>113.88555555555556</v>
       </c>
       <c r="V100" s="29" t="s">
         <v>10</v>
@@ -6534,7 +6562,9 @@
       <c r="G101" s="1">
         <v>0</v>
       </c>
-      <c r="H101" s="1"/>
+      <c r="H101" s="1">
+        <v>0</v>
+      </c>
       <c r="I101" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6544,7 +6574,7 @@
       </c>
       <c r="Q101" s="12">
         <f>T89</f>
-        <v>-267.5</v>
+        <v>-282.5</v>
       </c>
       <c r="R101" s="40">
         <v>-200</v>
@@ -6559,7 +6589,7 @@
       </c>
       <c r="U101" s="12">
         <f t="shared" si="3"/>
-        <v>-467.5</v>
+        <v>-482.5</v>
       </c>
       <c r="V101" s="29" t="s">
         <v>17</v>
@@ -6581,7 +6611,9 @@
       <c r="G102" s="1">
         <v>25</v>
       </c>
-      <c r="H102" s="1"/>
+      <c r="H102" s="1">
+        <v>0</v>
+      </c>
       <c r="I102" s="29">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -6591,7 +6623,7 @@
       </c>
       <c r="Q102" s="12">
         <f>W89</f>
-        <v>-279.17</v>
+        <v>-304.17</v>
       </c>
       <c r="R102" s="40">
         <v>-200</v>
@@ -6602,11 +6634,11 @@
       </c>
       <c r="T102" s="12">
         <f t="shared" si="2"/>
-        <v>597.56097560975616</v>
-      </c>
-      <c r="U102" s="12">
+        <v>494.94949494949498</v>
+      </c>
+      <c r="U102" s="42">
         <f t="shared" si="3"/>
-        <v>118.39097560975614</v>
+        <v>-9.2205050505050394</v>
       </c>
       <c r="V102" s="29" t="s">
         <v>97</v>
@@ -7118,8 +7150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25E9A583-41BF-8143-84DF-F8B494A614D1}">
   <dimension ref="E6:J47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView showGridLines="0" topLeftCell="A24" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47:G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7445,7 +7477,9 @@
       <c r="I40" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="J40" s="7"/>
+      <c r="J40" s="7" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="41" spans="5:10" ht="19" x14ac:dyDescent="0.25">
       <c r="E41" s="29" t="s">
@@ -7460,7 +7494,9 @@
       <c r="I41" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="J41" s="7"/>
+      <c r="J41" s="7" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="42" spans="5:10" ht="19" x14ac:dyDescent="0.25">
       <c r="E42" s="29" t="s">

</xml_diff>